<commit_message>
io port doc updated
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="22635" windowHeight="11655"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="22635" windowHeight="11655" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
+    <sheet name="io port" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -35,6 +35,242 @@
   </si>
   <si>
     <t>emulated ppu renderer implementation on vga timing</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PPU</t>
+  </si>
+  <si>
+    <t>0x2000 (PPU制御レジスタ1)</t>
+  </si>
+  <si>
+    <t>W1 : PPUの基本設定を行います。</t>
+  </si>
+  <si>
+    <t>位置</t>
+  </si>
+  <si>
+    <t>内容</t>
+  </si>
+  <si>
+    <t>値</t>
+  </si>
+  <si>
+    <t>bit7</t>
+  </si>
+  <si>
+    <t>VBlank時にNMI割込を発生</t>
+  </si>
+  <si>
+    <t>0:オフ, 1:オン</t>
+  </si>
+  <si>
+    <t>bit6</t>
+  </si>
+  <si>
+    <t>PPU選択?</t>
+  </si>
+  <si>
+    <t>0:マスター, 1:スレーブ</t>
+  </si>
+  <si>
+    <t>bit5</t>
+  </si>
+  <si>
+    <t>スプライトサイズ</t>
+  </si>
+  <si>
+    <t>0:8x8ピクセル</t>
+  </si>
+  <si>
+    <t>1:8x16ピクセル</t>
+  </si>
+  <si>
+    <t>bit4</t>
+  </si>
+  <si>
+    <t>BG用キャラクタテーブルベース</t>
+  </si>
+  <si>
+    <t>0:0x0000, 1:0x1000</t>
+  </si>
+  <si>
+    <t>bit3</t>
+  </si>
+  <si>
+    <t>スプライト用キャラクタテーブルベース</t>
+  </si>
+  <si>
+    <t>bit2</t>
+  </si>
+  <si>
+    <t>VRAMアクセス時のアドレス増加値</t>
+  </si>
+  <si>
+    <t>0:1byte, 1:32byte</t>
+  </si>
+  <si>
+    <t>bit1-0</t>
+  </si>
+  <si>
+    <t>メインスクリーンアドレス</t>
+  </si>
+  <si>
+    <t>00:0x2000, 01:0x2400</t>
+  </si>
+  <si>
+    <t>10:0x2800, 11:0x2C00</t>
+  </si>
+  <si>
+    <t>0x2001 (PPU制御レジスタ2)</t>
+  </si>
+  <si>
+    <t>W1 : PPUの表示設定を行います。</t>
+  </si>
+  <si>
+    <t>赤色を強調</t>
+  </si>
+  <si>
+    <t>緑色を強調</t>
+  </si>
+  <si>
+    <t>青色を強調</t>
+  </si>
+  <si>
+    <t>スプライトの表示</t>
+  </si>
+  <si>
+    <t>BGの表示</t>
+  </si>
+  <si>
+    <t>画面左端8ピクセルのスプライトを表示</t>
+  </si>
+  <si>
+    <t>0:クリップ, 1:表示</t>
+  </si>
+  <si>
+    <t>bit1</t>
+  </si>
+  <si>
+    <t>画面左端8ピクセルのBGを表示</t>
+  </si>
+  <si>
+    <t>bit0</t>
+  </si>
+  <si>
+    <t>色設定</t>
+  </si>
+  <si>
+    <t>0:カラー, 1:モノクロ</t>
+  </si>
+  <si>
+    <t>0x2002 (PPUステータスレジスタ)</t>
+  </si>
+  <si>
+    <t>R1 : PPUの状態を取得します。</t>
+  </si>
+  <si>
+    <t>スクリーンの描画状況</t>
+  </si>
+  <si>
+    <t>0:スキャンライン描画中</t>
+  </si>
+  <si>
+    <t>1:VBlank中</t>
+  </si>
+  <si>
+    <t>描画スキャンラインの0番スプライトヒット</t>
+  </si>
+  <si>
+    <t>0:ヒットせず, 1:ヒット</t>
+  </si>
+  <si>
+    <t>描画スキャンラインのスプライト横並び数</t>
+  </si>
+  <si>
+    <t>0:8個以下, 1:9個以上</t>
+  </si>
+  <si>
+    <t>VRAM状態</t>
+  </si>
+  <si>
+    <t>0:書き込み可能</t>
+  </si>
+  <si>
+    <t>1:書き込み不可</t>
+  </si>
+  <si>
+    <t>bit3-0</t>
+  </si>
+  <si>
+    <t>未使用</t>
+  </si>
+  <si>
+    <t>0x2003 (スプライトアドレスレジスタ)</t>
+  </si>
+  <si>
+    <t>W1 : スプライトRAMへの書き込みアドレスを設定します。</t>
+  </si>
+  <si>
+    <t>bit7-0</t>
+  </si>
+  <si>
+    <t>スプライトRAMアドレス</t>
+  </si>
+  <si>
+    <t>データ値</t>
+  </si>
+  <si>
+    <t>0x2004 (スプライトアクセスレジスタ)</t>
+  </si>
+  <si>
+    <t>W1 : スプライトRAMへ書き込みを行います。</t>
+  </si>
+  <si>
+    <t>スプライトRAMへ書き込むデータ</t>
+  </si>
+  <si>
+    <t>0x2005 (スクロールレジスタ)</t>
+  </si>
+  <si>
+    <t>W2 : スクロールの設定を行います。このレジスタには2回連続で書き込みます。</t>
+  </si>
+  <si>
+    <t>(1)水平スクロール値</t>
+  </si>
+  <si>
+    <t>(2)垂直スクロール値</t>
+  </si>
+  <si>
+    <t>0x2006 (VRAMアドレスレジスタ)</t>
+  </si>
+  <si>
+    <t>W2 : VRAMへの書き込みアドレスを設定します。このレジスタには2回連続で書き込みます。</t>
+  </si>
+  <si>
+    <t>(1)VRAMアドレス上位8bit</t>
+  </si>
+  <si>
+    <t>(2)VRAMアドレス下位8bit</t>
+  </si>
+  <si>
+    <t>0x2007 (VRAMアクセスレジスタ)</t>
+  </si>
+  <si>
+    <t>R1 / W1 : VRAMに対してデータ読み込み、データ書き込みを行います。</t>
+  </si>
+  <si>
+    <t>(R)VRAMから読み込んだデータ</t>
+  </si>
+  <si>
+    <t>(W)VRAMへ書き込むデータ</t>
+  </si>
+  <si>
+    <t>ppu ctl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ppu mask</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -42,7 +278,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +294,32 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -67,12 +329,71 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF786054"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color rgb="FF584A44"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF804030"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF804030"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF804030"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF804030"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF804030"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF804030"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF804030"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF804030"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF804030"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF804030"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -81,9 +402,36 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="AO6:AO13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
@@ -1062,14 +1410,540 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C30" sqref="A29:XFD30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="59.25" customWidth="1"/>
+    <col min="2" max="2" width="42.625" customWidth="1"/>
+    <col min="3" max="3" width="64.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.25">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.25">
+      <c r="A13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1">
+      <c r="A17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1">
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1">
+      <c r="A26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25">
+      <c r="A29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1">
+      <c r="A31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1">
+      <c r="A32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25">
+      <c r="A33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1">
+      <c r="A35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1">
+      <c r="A36" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A37" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1">
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1">
+      <c r="A39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1">
+      <c r="A40" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A41" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1">
+      <c r="A42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1">
+      <c r="A43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1">
+      <c r="A44" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A45" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1">
+      <c r="A46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25">
+      <c r="A47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1">
+      <c r="A48" s="8"/>
+      <c r="B48" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1">
+      <c r="A49" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A50" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" thickBot="1">
+      <c r="A51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25">
+      <c r="A52" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="8"/>
+      <c r="B53" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1">
+      <c r="A54" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A55" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" thickBot="1">
+      <c r="A56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25">
+      <c r="A57" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" thickBot="1">
+      <c r="A58" s="8"/>
+      <c r="B58" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
vga disp diagram added
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="22635" windowHeight="11655" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="22635" windowHeight="11655" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
     <sheet name="io port" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="display" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -272,24 +277,39 @@
   <si>
     <t>ppu mask</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(scr_x, scr_y)</t>
+  </si>
+  <si>
+    <t>Virtual Screen</t>
+  </si>
+  <si>
+    <t>Horizontal Mirror</t>
+  </si>
+  <si>
+    <t>Vertical Mirror</t>
+  </si>
+  <si>
+    <t>60 frames per sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -329,7 +349,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -396,13 +416,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -424,21 +593,82 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCFF"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1083,8 +1313,1340 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1278427" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2419350" y="1905000"/>
+          <a:ext cx="1278427" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>VGA</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1165447" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943975" y="1238250"/>
+          <a:ext cx="1165447" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>NES</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943975" y="4686300"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11410950" y="4686300"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943975" y="6410325"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11410950" y="6410325"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886825" y="4705350"/>
+          <a:ext cx="2438400" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCFF">
+            <a:alpha val="30196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="7743825"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163175" y="7743825"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="9467850"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163175" y="9467850"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7610475" y="7762875"/>
+          <a:ext cx="2019300" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCFF">
+            <a:alpha val="30196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="7762875"/>
+          <a:ext cx="476250" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCFF">
+            <a:alpha val="30196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>7096</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>167482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Right Arrow 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9455896" y="8597107"/>
+          <a:ext cx="231029" cy="118268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>207453</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Right Arrow 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="8601074"/>
+          <a:ext cx="207453" cy="114301"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="7743825"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038600" y="7743825"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="13687425"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="496674" cy="843757"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163175" y="13687425"/>
+          <a:ext cx="496674" cy="843757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="4800"/>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rectangle 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7610475" y="11982451"/>
+          <a:ext cx="2495550" cy="1238250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCFF">
+            <a:alpha val="30196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7610475" y="11496675"/>
+          <a:ext cx="2495550" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCFF">
+            <a:alpha val="30196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>76797</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>181160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>189903</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Down Arrow 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8725497" y="13020860"/>
+          <a:ext cx="113106" cy="209365"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>76797</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>189903</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>157299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Down Arrow 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8725497" y="11506200"/>
+          <a:ext cx="113106" cy="157299"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Connector 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5648325" y="771525"/>
+          <a:ext cx="3000375" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5648325" y="3267075"/>
+          <a:ext cx="3000375" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1126,7 +2688,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1158,9 +2720,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1192,6 +2755,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1367,14 +2931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AO6:AO13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AO15" sqref="AO15"/>
+      <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="6" spans="41:41">
       <c r="AO6" t="s">
@@ -1409,18 +2973,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C30" sqref="A29:XFD30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.25" customWidth="1"/>
-    <col min="2" max="2" width="42.625" customWidth="1"/>
-    <col min="3" max="3" width="64.25" customWidth="1"/>
+    <col min="1" max="1" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="15.75" thickBot="1">
@@ -1428,7 +2990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" thickBot="1">
+    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1436,12 +2998,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" thickBot="1">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1452,7 +3014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1463,7 +3025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1474,25 +3036,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +3065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1">
+    <row r="11" spans="1:3" ht="29.25" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -1514,7 +3076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1525,38 +3087,38 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" thickBot="1">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -1567,7 +3129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +3140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +3151,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +3162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1611,7 +3173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -1622,7 +3184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
+    <row r="23" spans="1:3" ht="29.25" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -1633,7 +3195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1644,7 +3206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
       <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
@@ -1655,17 +3217,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" thickBot="1">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
@@ -1676,25 +3238,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1">
+    <row r="31" spans="1:3" ht="29.25" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1705,7 +3267,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
+    <row r="32" spans="1:3" ht="29.25" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>17</v>
       </c>
@@ -1716,25 +3278,25 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1">
       <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
@@ -1743,17 +3305,17 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" thickBot="1">
+    <row r="37" spans="1:3" ht="15.75" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
@@ -1764,7 +3326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1">
+    <row r="39" spans="1:3" ht="15.75" thickBot="1">
       <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
@@ -1775,17 +3337,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" thickBot="1">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1">
+    <row r="42" spans="1:3" ht="15.75" thickBot="1">
       <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
@@ -1796,7 +3358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
@@ -1807,17 +3369,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1">
       <c r="A44" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="26.25" thickBot="1">
+    <row r="45" spans="1:3" ht="39" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1">
+    <row r="46" spans="1:3" ht="15.75" thickBot="1">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -1828,35 +3390,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1">
-      <c r="A48" s="8"/>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A48" s="9"/>
       <c r="B48" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="8"/>
-    </row>
-    <row r="49" spans="1:3" ht="15" thickBot="1">
+      <c r="C48" s="9"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
       <c r="A49" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="26.25" thickBot="1">
+    <row r="50" spans="1:3" ht="39" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1">
+    <row r="51" spans="1:3" ht="15.75" thickBot="1">
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
@@ -1867,35 +3429,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25">
-      <c r="A52" s="7" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1">
-      <c r="A53" s="8"/>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A53" s="9"/>
       <c r="B53" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="8"/>
-    </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1">
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" thickBot="1">
+    <row r="55" spans="1:3" ht="26.25" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1">
+    <row r="56" spans="1:3" ht="15.75" thickBot="1">
       <c r="A56" s="4" t="s">
         <v>8</v>
       </c>
@@ -1906,26 +3468,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25">
-      <c r="A57" s="7" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" thickBot="1">
-      <c r="A58" s="8"/>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A58" s="9"/>
       <c r="B58" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="8"/>
+      <c r="C58" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -1934,12 +3502,6 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1948,14 +3510,2126 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:AW78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="Y71" sqref="Y71"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:48">
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="4:48" ht="15.75" thickBot="1">
+      <c r="Z4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="4:48">
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11">
+        <v>640</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="20"/>
+    </row>
+    <row r="6" spans="4:48">
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="22"/>
+    </row>
+    <row r="7" spans="4:48">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="22"/>
+      <c r="AL7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="4:48" ht="15.75" thickBot="1">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="22"/>
+      <c r="AU8">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="4:48">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="22"/>
+      <c r="AJ9" s="10"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="11">
+        <v>256</v>
+      </c>
+      <c r="AM9" s="11"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="11"/>
+      <c r="AP9" s="11"/>
+      <c r="AQ9" s="11"/>
+      <c r="AR9" s="11"/>
+      <c r="AS9" s="12"/>
+      <c r="AT9" s="19"/>
+      <c r="AU9" s="19"/>
+      <c r="AV9" s="20"/>
+    </row>
+    <row r="10" spans="4:48">
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="22"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="14"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="14"/>
+      <c r="AR10" s="14"/>
+      <c r="AS10" s="15"/>
+      <c r="AT10" s="14"/>
+      <c r="AU10" s="14"/>
+      <c r="AV10" s="22"/>
+    </row>
+    <row r="11" spans="4:48">
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="22"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="14"/>
+      <c r="AM11" s="14"/>
+      <c r="AN11" s="14"/>
+      <c r="AO11" s="14"/>
+      <c r="AP11" s="14"/>
+      <c r="AQ11" s="14"/>
+      <c r="AR11" s="14"/>
+      <c r="AS11" s="15"/>
+      <c r="AT11" s="14"/>
+      <c r="AU11" s="14"/>
+      <c r="AV11" s="22"/>
+    </row>
+    <row r="12" spans="4:48">
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="22"/>
+      <c r="AJ12" s="13">
+        <v>240</v>
+      </c>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="14"/>
+      <c r="AN12" s="14"/>
+      <c r="AO12" s="14"/>
+      <c r="AP12" s="14"/>
+      <c r="AQ12" s="14"/>
+      <c r="AR12" s="14"/>
+      <c r="AS12" s="15"/>
+      <c r="AT12" s="14"/>
+      <c r="AU12" s="14"/>
+      <c r="AV12" s="22"/>
+    </row>
+    <row r="13" spans="4:48">
+      <c r="D13" s="13">
+        <v>480</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="22"/>
+      <c r="AJ13" s="13"/>
+      <c r="AK13" s="14"/>
+      <c r="AL13" s="14"/>
+      <c r="AM13" s="14"/>
+      <c r="AN13" s="14"/>
+      <c r="AO13" s="14"/>
+      <c r="AP13" s="14"/>
+      <c r="AQ13" s="14"/>
+      <c r="AR13" s="14"/>
+      <c r="AS13" s="15"/>
+      <c r="AT13" s="14"/>
+      <c r="AU13" s="14"/>
+      <c r="AV13" s="22"/>
+    </row>
+    <row r="14" spans="4:48">
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="22"/>
+      <c r="AJ14" s="13"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
+      <c r="AN14" s="14"/>
+      <c r="AO14" s="14"/>
+      <c r="AP14" s="14"/>
+      <c r="AQ14" s="14"/>
+      <c r="AR14" s="14"/>
+      <c r="AS14" s="15"/>
+      <c r="AT14" s="14"/>
+      <c r="AU14" s="14"/>
+      <c r="AV14" s="22"/>
+    </row>
+    <row r="15" spans="4:48">
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="22"/>
+      <c r="AJ15" s="13"/>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="14"/>
+      <c r="AM15" s="14"/>
+      <c r="AN15" s="14"/>
+      <c r="AO15" s="14"/>
+      <c r="AP15" s="14"/>
+      <c r="AQ15" s="14"/>
+      <c r="AR15" s="14"/>
+      <c r="AS15" s="15"/>
+      <c r="AT15" s="14"/>
+      <c r="AU15" s="14"/>
+      <c r="AV15" s="22"/>
+    </row>
+    <row r="16" spans="4:48">
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="22"/>
+      <c r="AJ16" s="13"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="14"/>
+      <c r="AP16" s="14"/>
+      <c r="AQ16" s="14"/>
+      <c r="AR16" s="14"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="14"/>
+      <c r="AU16" s="14"/>
+      <c r="AV16" s="22"/>
+    </row>
+    <row r="17" spans="3:48" ht="15.75" thickBot="1">
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="22"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="17"/>
+      <c r="AL17" s="17"/>
+      <c r="AM17" s="17"/>
+      <c r="AN17" s="17"/>
+      <c r="AO17" s="17"/>
+      <c r="AP17" s="17"/>
+      <c r="AQ17" s="17"/>
+      <c r="AR17" s="17"/>
+      <c r="AS17" s="18"/>
+      <c r="AT17" s="14"/>
+      <c r="AU17" s="14"/>
+      <c r="AV17" s="22"/>
+    </row>
+    <row r="18" spans="3:48">
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="22"/>
+      <c r="AJ18" s="21"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14"/>
+      <c r="AP18" s="14"/>
+      <c r="AQ18" s="14"/>
+      <c r="AR18" s="14"/>
+      <c r="AS18" s="14"/>
+      <c r="AT18" s="14"/>
+      <c r="AU18" s="14"/>
+      <c r="AV18" s="22"/>
+    </row>
+    <row r="19" spans="3:48">
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="22"/>
+      <c r="AI19">
+        <v>262</v>
+      </c>
+      <c r="AJ19" s="21"/>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="14"/>
+      <c r="AM19" s="14"/>
+      <c r="AN19" s="14"/>
+      <c r="AO19" s="14"/>
+      <c r="AP19" s="14"/>
+      <c r="AQ19" s="14"/>
+      <c r="AR19" s="14"/>
+      <c r="AS19" s="14"/>
+      <c r="AT19" s="14"/>
+      <c r="AU19" s="14"/>
+      <c r="AV19" s="22"/>
+    </row>
+    <row r="20" spans="3:48">
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="22"/>
+      <c r="AJ20" s="21"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="14"/>
+      <c r="AM20" s="14"/>
+      <c r="AN20" s="14"/>
+      <c r="AO20" s="14"/>
+      <c r="AP20" s="14"/>
+      <c r="AQ20" s="14"/>
+      <c r="AR20" s="14"/>
+      <c r="AS20" s="14"/>
+      <c r="AT20" s="14"/>
+      <c r="AU20" s="14"/>
+      <c r="AV20" s="22"/>
+    </row>
+    <row r="21" spans="3:48">
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="14"/>
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="22"/>
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="24"/>
+      <c r="AL21" s="24"/>
+      <c r="AM21" s="24"/>
+      <c r="AN21" s="24"/>
+      <c r="AO21" s="24"/>
+      <c r="AP21" s="24"/>
+      <c r="AQ21" s="24"/>
+      <c r="AR21" s="24"/>
+      <c r="AS21" s="24"/>
+      <c r="AT21" s="24"/>
+      <c r="AU21" s="24"/>
+      <c r="AV21" s="25"/>
+    </row>
+    <row r="22" spans="3:48" ht="15.75" thickBot="1">
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="22"/>
+    </row>
+    <row r="23" spans="3:48">
+      <c r="D23" s="21"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="22"/>
+    </row>
+    <row r="24" spans="3:48">
+      <c r="D24" s="21"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="22"/>
+    </row>
+    <row r="25" spans="3:48">
+      <c r="D25" s="21"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="14"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="22"/>
+    </row>
+    <row r="26" spans="3:48">
+      <c r="C26">
+        <v>600</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="14"/>
+      <c r="W26" s="14"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="14"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="22"/>
+    </row>
+    <row r="27" spans="3:48">
+      <c r="D27" s="21"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="14"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="22"/>
+    </row>
+    <row r="28" spans="3:48">
+      <c r="D28" s="21"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="22"/>
+    </row>
+    <row r="29" spans="3:48">
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="24"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="24"/>
+      <c r="Z29" s="24"/>
+      <c r="AA29" s="24"/>
+      <c r="AB29" s="24"/>
+      <c r="AC29" s="24"/>
+      <c r="AD29" s="25"/>
+    </row>
+    <row r="35" spans="3:49">
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="3:49">
+      <c r="AD37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="3:49" ht="15.75" thickBot="1"/>
+    <row r="39" spans="3:49">
+      <c r="E39" s="10"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="12"/>
+      <c r="AD39" s="10"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="11"/>
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="11"/>
+      <c r="AI39" s="11"/>
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="11"/>
+      <c r="AM39" s="12"/>
+      <c r="AN39" s="10"/>
+      <c r="AO39" s="11"/>
+      <c r="AP39" s="11"/>
+      <c r="AQ39" s="11"/>
+      <c r="AR39" s="11"/>
+      <c r="AS39" s="11"/>
+      <c r="AT39" s="11"/>
+      <c r="AU39" s="11"/>
+      <c r="AV39" s="11"/>
+      <c r="AW39" s="12"/>
+    </row>
+    <row r="40" spans="3:49">
+      <c r="E40" s="13"/>
+      <c r="F40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="15"/>
+      <c r="AD40" s="13"/>
+      <c r="AE40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF40" s="14"/>
+      <c r="AG40" s="14"/>
+      <c r="AH40" s="14"/>
+      <c r="AI40" s="14"/>
+      <c r="AJ40" s="14"/>
+      <c r="AK40" s="14"/>
+      <c r="AL40" s="14"/>
+      <c r="AM40" s="15"/>
+      <c r="AN40" s="13"/>
+      <c r="AO40" s="14"/>
+      <c r="AP40" s="14"/>
+      <c r="AQ40" s="14"/>
+      <c r="AR40" s="14"/>
+      <c r="AS40" s="14"/>
+      <c r="AT40" s="14"/>
+      <c r="AU40" s="14"/>
+      <c r="AV40" s="14"/>
+      <c r="AW40" s="15"/>
+    </row>
+    <row r="41" spans="3:49">
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="15"/>
+      <c r="AD41" s="13"/>
+      <c r="AE41" s="14"/>
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="14"/>
+      <c r="AH41" s="14"/>
+      <c r="AI41" s="14"/>
+      <c r="AJ41" s="14"/>
+      <c r="AK41" s="14"/>
+      <c r="AL41" s="14"/>
+      <c r="AM41" s="15"/>
+      <c r="AN41" s="13"/>
+      <c r="AO41" s="14"/>
+      <c r="AP41" s="14"/>
+      <c r="AQ41" s="14"/>
+      <c r="AR41" s="14"/>
+      <c r="AS41" s="14"/>
+      <c r="AT41" s="14"/>
+      <c r="AU41" s="14"/>
+      <c r="AV41" s="14"/>
+      <c r="AW41" s="15"/>
+    </row>
+    <row r="42" spans="3:49">
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="15"/>
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="14"/>
+      <c r="AF42" s="14"/>
+      <c r="AG42" s="14"/>
+      <c r="AH42" s="14"/>
+      <c r="AI42" s="14"/>
+      <c r="AJ42" s="14"/>
+      <c r="AK42" s="14"/>
+      <c r="AL42" s="14"/>
+      <c r="AM42" s="15"/>
+      <c r="AN42" s="13"/>
+      <c r="AO42" s="14"/>
+      <c r="AP42" s="14"/>
+      <c r="AQ42" s="14"/>
+      <c r="AR42" s="14"/>
+      <c r="AS42" s="14"/>
+      <c r="AT42" s="14"/>
+      <c r="AU42" s="14"/>
+      <c r="AV42" s="14"/>
+      <c r="AW42" s="15"/>
+    </row>
+    <row r="43" spans="3:49">
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="15"/>
+      <c r="AD43" s="13"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="14"/>
+      <c r="AI43" s="14"/>
+      <c r="AJ43" s="14"/>
+      <c r="AK43" s="14"/>
+      <c r="AL43" s="14"/>
+      <c r="AM43" s="15"/>
+      <c r="AN43" s="13"/>
+      <c r="AO43" s="14"/>
+      <c r="AP43" s="14"/>
+      <c r="AQ43" s="14"/>
+      <c r="AR43" s="14"/>
+      <c r="AS43" s="14"/>
+      <c r="AT43" s="14"/>
+      <c r="AU43" s="14"/>
+      <c r="AV43" s="14"/>
+      <c r="AW43" s="15"/>
+    </row>
+    <row r="44" spans="3:49">
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="15"/>
+      <c r="AD44" s="13"/>
+      <c r="AE44" s="14"/>
+      <c r="AF44" s="14"/>
+      <c r="AG44" s="14"/>
+      <c r="AH44" s="14"/>
+      <c r="AI44" s="14"/>
+      <c r="AJ44" s="14"/>
+      <c r="AK44" s="14"/>
+      <c r="AL44" s="14"/>
+      <c r="AM44" s="15"/>
+      <c r="AN44" s="13"/>
+      <c r="AO44" s="14"/>
+      <c r="AP44" s="14"/>
+      <c r="AQ44" s="14"/>
+      <c r="AR44" s="14"/>
+      <c r="AS44" s="14"/>
+      <c r="AT44" s="14"/>
+      <c r="AU44" s="14"/>
+      <c r="AV44" s="14"/>
+      <c r="AW44" s="15"/>
+    </row>
+    <row r="45" spans="3:49">
+      <c r="E45" s="13"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="15"/>
+      <c r="AD45" s="13"/>
+      <c r="AE45" s="14"/>
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
+      <c r="AH45" s="14"/>
+      <c r="AI45" s="14"/>
+      <c r="AJ45" s="14"/>
+      <c r="AK45" s="14"/>
+      <c r="AL45" s="14"/>
+      <c r="AM45" s="15"/>
+      <c r="AN45" s="13"/>
+      <c r="AO45" s="14"/>
+      <c r="AP45" s="14"/>
+      <c r="AQ45" s="14"/>
+      <c r="AR45" s="14"/>
+      <c r="AS45" s="14"/>
+      <c r="AT45" s="14"/>
+      <c r="AU45" s="14"/>
+      <c r="AV45" s="14"/>
+      <c r="AW45" s="15"/>
+    </row>
+    <row r="46" spans="3:49">
+      <c r="E46" s="13"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="15"/>
+      <c r="AD46" s="13"/>
+      <c r="AE46" s="14"/>
+      <c r="AF46" s="14"/>
+      <c r="AG46" s="14"/>
+      <c r="AH46" s="14"/>
+      <c r="AI46" s="14"/>
+      <c r="AJ46" s="14"/>
+      <c r="AK46" s="14"/>
+      <c r="AL46" s="14"/>
+      <c r="AM46" s="15"/>
+      <c r="AN46" s="13"/>
+      <c r="AO46" s="14"/>
+      <c r="AP46" s="14"/>
+      <c r="AQ46" s="14"/>
+      <c r="AR46" s="14"/>
+      <c r="AS46" s="14"/>
+      <c r="AT46" s="14"/>
+      <c r="AU46" s="14"/>
+      <c r="AV46" s="14"/>
+      <c r="AW46" s="15"/>
+    </row>
+    <row r="47" spans="3:49" ht="15.75" thickBot="1">
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="18"/>
+      <c r="AD47" s="16"/>
+      <c r="AE47" s="17"/>
+      <c r="AF47" s="17"/>
+      <c r="AG47" s="17"/>
+      <c r="AH47" s="17"/>
+      <c r="AI47" s="17"/>
+      <c r="AJ47" s="17"/>
+      <c r="AK47" s="17"/>
+      <c r="AL47" s="17"/>
+      <c r="AM47" s="18"/>
+      <c r="AN47" s="16"/>
+      <c r="AO47" s="17"/>
+      <c r="AP47" s="17"/>
+      <c r="AQ47" s="17"/>
+      <c r="AR47" s="17"/>
+      <c r="AS47" s="17"/>
+      <c r="AT47" s="17"/>
+      <c r="AU47" s="17"/>
+      <c r="AV47" s="17"/>
+      <c r="AW47" s="18"/>
+    </row>
+    <row r="48" spans="3:49">
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="12"/>
+      <c r="AD48" s="10"/>
+      <c r="AE48" s="11"/>
+      <c r="AF48" s="11"/>
+      <c r="AG48" s="11"/>
+      <c r="AH48" s="11"/>
+      <c r="AI48" s="11"/>
+      <c r="AJ48" s="11"/>
+      <c r="AK48" s="11"/>
+      <c r="AL48" s="11"/>
+      <c r="AM48" s="12"/>
+      <c r="AN48" s="10"/>
+      <c r="AO48" s="11"/>
+      <c r="AP48" s="11"/>
+      <c r="AQ48" s="11"/>
+      <c r="AR48" s="11"/>
+      <c r="AS48" s="11"/>
+      <c r="AT48" s="11"/>
+      <c r="AU48" s="11"/>
+      <c r="AV48" s="11"/>
+      <c r="AW48" s="12"/>
+    </row>
+    <row r="49" spans="5:49">
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="15"/>
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="14"/>
+      <c r="AF49" s="14"/>
+      <c r="AG49" s="14"/>
+      <c r="AH49" s="14"/>
+      <c r="AI49" s="14"/>
+      <c r="AJ49" s="14"/>
+      <c r="AK49" s="14"/>
+      <c r="AL49" s="14"/>
+      <c r="AM49" s="15"/>
+      <c r="AN49" s="13"/>
+      <c r="AO49" s="14"/>
+      <c r="AP49" s="14"/>
+      <c r="AQ49" s="14"/>
+      <c r="AR49" s="14"/>
+      <c r="AS49" s="14"/>
+      <c r="AT49" s="14"/>
+      <c r="AU49" s="14"/>
+      <c r="AV49" s="14"/>
+      <c r="AW49" s="15"/>
+    </row>
+    <row r="50" spans="5:49">
+      <c r="E50" s="13"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="14"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="14"/>
+      <c r="X50" s="15"/>
+      <c r="AD50" s="13"/>
+      <c r="AE50" s="14"/>
+      <c r="AF50" s="14"/>
+      <c r="AG50" s="14"/>
+      <c r="AH50" s="14"/>
+      <c r="AI50" s="14"/>
+      <c r="AJ50" s="14"/>
+      <c r="AK50" s="14"/>
+      <c r="AL50" s="14"/>
+      <c r="AM50" s="15"/>
+      <c r="AN50" s="13"/>
+      <c r="AO50" s="14"/>
+      <c r="AP50" s="14"/>
+      <c r="AQ50" s="14"/>
+      <c r="AR50" s="14"/>
+      <c r="AS50" s="14"/>
+      <c r="AT50" s="14"/>
+      <c r="AU50" s="14"/>
+      <c r="AV50" s="14"/>
+      <c r="AW50" s="15"/>
+    </row>
+    <row r="51" spans="5:49">
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="15"/>
+      <c r="AD51" s="13"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+      <c r="AH51" s="14"/>
+      <c r="AI51" s="14"/>
+      <c r="AJ51" s="14"/>
+      <c r="AK51" s="14"/>
+      <c r="AL51" s="14"/>
+      <c r="AM51" s="15"/>
+      <c r="AN51" s="13"/>
+      <c r="AO51" s="14"/>
+      <c r="AP51" s="14"/>
+      <c r="AQ51" s="14"/>
+      <c r="AR51" s="14"/>
+      <c r="AS51" s="14"/>
+      <c r="AT51" s="14"/>
+      <c r="AU51" s="14"/>
+      <c r="AV51" s="14"/>
+      <c r="AW51" s="15"/>
+    </row>
+    <row r="52" spans="5:49">
+      <c r="E52" s="13"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="14"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="14"/>
+      <c r="X52" s="15"/>
+      <c r="AD52" s="13"/>
+      <c r="AE52" s="14"/>
+      <c r="AF52" s="14"/>
+      <c r="AG52" s="14"/>
+      <c r="AH52" s="14"/>
+      <c r="AI52" s="14"/>
+      <c r="AJ52" s="14"/>
+      <c r="AK52" s="14"/>
+      <c r="AL52" s="14"/>
+      <c r="AM52" s="15"/>
+      <c r="AN52" s="13"/>
+      <c r="AO52" s="14"/>
+      <c r="AP52" s="14"/>
+      <c r="AQ52" s="14"/>
+      <c r="AR52" s="14"/>
+      <c r="AS52" s="14"/>
+      <c r="AT52" s="14"/>
+      <c r="AU52" s="14"/>
+      <c r="AV52" s="14"/>
+      <c r="AW52" s="15"/>
+    </row>
+    <row r="53" spans="5:49">
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="13"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="14"/>
+      <c r="X53" s="15"/>
+      <c r="AD53" s="13"/>
+      <c r="AE53" s="14"/>
+      <c r="AF53" s="14"/>
+      <c r="AG53" s="14"/>
+      <c r="AH53" s="14"/>
+      <c r="AI53" s="14"/>
+      <c r="AJ53" s="14"/>
+      <c r="AK53" s="14"/>
+      <c r="AL53" s="14"/>
+      <c r="AM53" s="15"/>
+      <c r="AN53" s="13"/>
+      <c r="AO53" s="14"/>
+      <c r="AP53" s="14"/>
+      <c r="AQ53" s="14"/>
+      <c r="AR53" s="14"/>
+      <c r="AS53" s="14"/>
+      <c r="AT53" s="14"/>
+      <c r="AU53" s="14"/>
+      <c r="AV53" s="14"/>
+      <c r="AW53" s="15"/>
+    </row>
+    <row r="54" spans="5:49">
+      <c r="E54" s="13"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="13"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="14"/>
+      <c r="W54" s="14"/>
+      <c r="X54" s="15"/>
+      <c r="AD54" s="13"/>
+      <c r="AE54" s="14"/>
+      <c r="AF54" s="14"/>
+      <c r="AG54" s="14"/>
+      <c r="AH54" s="14"/>
+      <c r="AI54" s="14"/>
+      <c r="AJ54" s="14"/>
+      <c r="AK54" s="14"/>
+      <c r="AL54" s="14"/>
+      <c r="AM54" s="15"/>
+      <c r="AN54" s="13"/>
+      <c r="AO54" s="14"/>
+      <c r="AP54" s="14"/>
+      <c r="AQ54" s="14"/>
+      <c r="AR54" s="14"/>
+      <c r="AS54" s="14"/>
+      <c r="AT54" s="14"/>
+      <c r="AU54" s="14"/>
+      <c r="AV54" s="14"/>
+      <c r="AW54" s="15"/>
+    </row>
+    <row r="55" spans="5:49">
+      <c r="E55" s="13"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="14"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="14"/>
+      <c r="X55" s="15"/>
+      <c r="AD55" s="13"/>
+      <c r="AE55" s="14"/>
+      <c r="AF55" s="14"/>
+      <c r="AG55" s="14"/>
+      <c r="AH55" s="14"/>
+      <c r="AI55" s="14"/>
+      <c r="AJ55" s="14"/>
+      <c r="AK55" s="14"/>
+      <c r="AL55" s="14"/>
+      <c r="AM55" s="15"/>
+      <c r="AN55" s="13"/>
+      <c r="AO55" s="14"/>
+      <c r="AP55" s="14"/>
+      <c r="AQ55" s="14"/>
+      <c r="AR55" s="14"/>
+      <c r="AS55" s="14"/>
+      <c r="AT55" s="14"/>
+      <c r="AU55" s="14"/>
+      <c r="AV55" s="14"/>
+      <c r="AW55" s="15"/>
+    </row>
+    <row r="56" spans="5:49" ht="15.75" thickBot="1">
+      <c r="E56" s="16"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="17"/>
+      <c r="W56" s="17"/>
+      <c r="X56" s="18"/>
+      <c r="AD56" s="16"/>
+      <c r="AE56" s="17"/>
+      <c r="AF56" s="17"/>
+      <c r="AG56" s="17"/>
+      <c r="AH56" s="17"/>
+      <c r="AI56" s="17"/>
+      <c r="AJ56" s="17"/>
+      <c r="AK56" s="17"/>
+      <c r="AL56" s="17"/>
+      <c r="AM56" s="18"/>
+      <c r="AN56" s="16"/>
+      <c r="AO56" s="17"/>
+      <c r="AP56" s="17"/>
+      <c r="AQ56" s="17"/>
+      <c r="AR56" s="17"/>
+      <c r="AS56" s="17"/>
+      <c r="AT56" s="17"/>
+      <c r="AU56" s="17"/>
+      <c r="AV56" s="17"/>
+      <c r="AW56" s="18"/>
+    </row>
+    <row r="59" spans="5:49">
+      <c r="AD59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="5:49" ht="15.75" thickBot="1"/>
+    <row r="61" spans="5:49">
+      <c r="AD61" s="10"/>
+      <c r="AE61" s="11"/>
+      <c r="AF61" s="11"/>
+      <c r="AG61" s="11"/>
+      <c r="AH61" s="11"/>
+      <c r="AI61" s="11"/>
+      <c r="AJ61" s="11"/>
+      <c r="AK61" s="11"/>
+      <c r="AL61" s="11"/>
+      <c r="AM61" s="12"/>
+      <c r="AN61" s="10"/>
+      <c r="AO61" s="11"/>
+      <c r="AP61" s="11"/>
+      <c r="AQ61" s="11"/>
+      <c r="AR61" s="11"/>
+      <c r="AS61" s="11"/>
+      <c r="AT61" s="11"/>
+      <c r="AU61" s="11"/>
+      <c r="AV61" s="11"/>
+      <c r="AW61" s="12"/>
+    </row>
+    <row r="62" spans="5:49">
+      <c r="AD62" s="13"/>
+      <c r="AE62" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF62" s="14"/>
+      <c r="AG62" s="14"/>
+      <c r="AH62" s="14"/>
+      <c r="AI62" s="14"/>
+      <c r="AJ62" s="14"/>
+      <c r="AK62" s="14"/>
+      <c r="AL62" s="14"/>
+      <c r="AM62" s="15"/>
+      <c r="AN62" s="13"/>
+      <c r="AO62" s="14"/>
+      <c r="AP62" s="14"/>
+      <c r="AQ62" s="14"/>
+      <c r="AR62" s="14"/>
+      <c r="AS62" s="14"/>
+      <c r="AT62" s="14"/>
+      <c r="AU62" s="14"/>
+      <c r="AV62" s="14"/>
+      <c r="AW62" s="15"/>
+    </row>
+    <row r="63" spans="5:49">
+      <c r="AD63" s="13"/>
+      <c r="AE63" s="14"/>
+      <c r="AF63" s="14"/>
+      <c r="AG63" s="14"/>
+      <c r="AH63" s="14"/>
+      <c r="AI63" s="14"/>
+      <c r="AJ63" s="14"/>
+      <c r="AK63" s="14"/>
+      <c r="AL63" s="14"/>
+      <c r="AM63" s="15"/>
+      <c r="AN63" s="13"/>
+      <c r="AO63" s="14"/>
+      <c r="AP63" s="14"/>
+      <c r="AQ63" s="14"/>
+      <c r="AR63" s="14"/>
+      <c r="AS63" s="14"/>
+      <c r="AT63" s="14"/>
+      <c r="AU63" s="14"/>
+      <c r="AV63" s="14"/>
+      <c r="AW63" s="15"/>
+    </row>
+    <row r="64" spans="5:49">
+      <c r="AD64" s="13"/>
+      <c r="AE64" s="14"/>
+      <c r="AF64" s="14"/>
+      <c r="AG64" s="14"/>
+      <c r="AH64" s="14"/>
+      <c r="AI64" s="14"/>
+      <c r="AJ64" s="14"/>
+      <c r="AK64" s="14"/>
+      <c r="AL64" s="14"/>
+      <c r="AM64" s="15"/>
+      <c r="AN64" s="13"/>
+      <c r="AO64" s="14"/>
+      <c r="AP64" s="14"/>
+      <c r="AQ64" s="14"/>
+      <c r="AR64" s="14"/>
+      <c r="AS64" s="14"/>
+      <c r="AT64" s="14"/>
+      <c r="AU64" s="14"/>
+      <c r="AV64" s="14"/>
+      <c r="AW64" s="15"/>
+    </row>
+    <row r="65" spans="30:49">
+      <c r="AD65" s="13"/>
+      <c r="AE65" s="14"/>
+      <c r="AF65" s="14"/>
+      <c r="AG65" s="14"/>
+      <c r="AH65" s="14"/>
+      <c r="AI65" s="14"/>
+      <c r="AJ65" s="14"/>
+      <c r="AK65" s="14"/>
+      <c r="AL65" s="14"/>
+      <c r="AM65" s="15"/>
+      <c r="AN65" s="13"/>
+      <c r="AO65" s="14"/>
+      <c r="AP65" s="14"/>
+      <c r="AQ65" s="14"/>
+      <c r="AR65" s="14"/>
+      <c r="AS65" s="14"/>
+      <c r="AT65" s="14"/>
+      <c r="AU65" s="14"/>
+      <c r="AV65" s="14"/>
+      <c r="AW65" s="15"/>
+    </row>
+    <row r="66" spans="30:49">
+      <c r="AD66" s="13"/>
+      <c r="AE66" s="14"/>
+      <c r="AF66" s="14"/>
+      <c r="AG66" s="14"/>
+      <c r="AH66" s="14"/>
+      <c r="AI66" s="14"/>
+      <c r="AJ66" s="14"/>
+      <c r="AK66" s="14"/>
+      <c r="AL66" s="14"/>
+      <c r="AM66" s="15"/>
+      <c r="AN66" s="13"/>
+      <c r="AO66" s="14"/>
+      <c r="AP66" s="14"/>
+      <c r="AQ66" s="14"/>
+      <c r="AR66" s="14"/>
+      <c r="AS66" s="14"/>
+      <c r="AT66" s="14"/>
+      <c r="AU66" s="14"/>
+      <c r="AV66" s="14"/>
+      <c r="AW66" s="15"/>
+    </row>
+    <row r="67" spans="30:49">
+      <c r="AD67" s="13"/>
+      <c r="AE67" s="14"/>
+      <c r="AF67" s="14"/>
+      <c r="AG67" s="14"/>
+      <c r="AH67" s="14"/>
+      <c r="AI67" s="14"/>
+      <c r="AJ67" s="14"/>
+      <c r="AK67" s="14"/>
+      <c r="AL67" s="14"/>
+      <c r="AM67" s="15"/>
+      <c r="AN67" s="13"/>
+      <c r="AO67" s="14"/>
+      <c r="AP67" s="14"/>
+      <c r="AQ67" s="14"/>
+      <c r="AR67" s="14"/>
+      <c r="AS67" s="14"/>
+      <c r="AT67" s="14"/>
+      <c r="AU67" s="14"/>
+      <c r="AV67" s="14"/>
+      <c r="AW67" s="15"/>
+    </row>
+    <row r="68" spans="30:49">
+      <c r="AD68" s="13"/>
+      <c r="AE68" s="14"/>
+      <c r="AF68" s="14"/>
+      <c r="AG68" s="14"/>
+      <c r="AH68" s="14"/>
+      <c r="AI68" s="14"/>
+      <c r="AJ68" s="14"/>
+      <c r="AK68" s="14"/>
+      <c r="AL68" s="14"/>
+      <c r="AM68" s="15"/>
+      <c r="AN68" s="13"/>
+      <c r="AO68" s="14"/>
+      <c r="AP68" s="14"/>
+      <c r="AQ68" s="14"/>
+      <c r="AR68" s="14"/>
+      <c r="AS68" s="14"/>
+      <c r="AT68" s="14"/>
+      <c r="AU68" s="14"/>
+      <c r="AV68" s="14"/>
+      <c r="AW68" s="15"/>
+    </row>
+    <row r="69" spans="30:49" ht="15.75" thickBot="1">
+      <c r="AD69" s="16"/>
+      <c r="AE69" s="17"/>
+      <c r="AF69" s="17"/>
+      <c r="AG69" s="17"/>
+      <c r="AH69" s="17"/>
+      <c r="AI69" s="17"/>
+      <c r="AJ69" s="17"/>
+      <c r="AK69" s="17"/>
+      <c r="AL69" s="17"/>
+      <c r="AM69" s="18"/>
+      <c r="AN69" s="16"/>
+      <c r="AO69" s="17"/>
+      <c r="AP69" s="17"/>
+      <c r="AQ69" s="17"/>
+      <c r="AR69" s="17"/>
+      <c r="AS69" s="17"/>
+      <c r="AT69" s="17"/>
+      <c r="AU69" s="17"/>
+      <c r="AV69" s="17"/>
+      <c r="AW69" s="18"/>
+    </row>
+    <row r="70" spans="30:49">
+      <c r="AD70" s="10"/>
+      <c r="AE70" s="11"/>
+      <c r="AF70" s="11"/>
+      <c r="AG70" s="11"/>
+      <c r="AH70" s="11"/>
+      <c r="AI70" s="11"/>
+      <c r="AJ70" s="11"/>
+      <c r="AK70" s="11"/>
+      <c r="AL70" s="11"/>
+      <c r="AM70" s="12"/>
+      <c r="AN70" s="10"/>
+      <c r="AO70" s="11"/>
+      <c r="AP70" s="11"/>
+      <c r="AQ70" s="11"/>
+      <c r="AR70" s="11"/>
+      <c r="AS70" s="11"/>
+      <c r="AT70" s="11"/>
+      <c r="AU70" s="11"/>
+      <c r="AV70" s="11"/>
+      <c r="AW70" s="12"/>
+    </row>
+    <row r="71" spans="30:49">
+      <c r="AD71" s="13"/>
+      <c r="AE71" s="14"/>
+      <c r="AF71" s="14"/>
+      <c r="AG71" s="14"/>
+      <c r="AH71" s="14"/>
+      <c r="AI71" s="14"/>
+      <c r="AJ71" s="14"/>
+      <c r="AK71" s="14"/>
+      <c r="AL71" s="14"/>
+      <c r="AM71" s="15"/>
+      <c r="AN71" s="13"/>
+      <c r="AO71" s="14"/>
+      <c r="AP71" s="14"/>
+      <c r="AQ71" s="14"/>
+      <c r="AR71" s="14"/>
+      <c r="AS71" s="14"/>
+      <c r="AT71" s="14"/>
+      <c r="AU71" s="14"/>
+      <c r="AV71" s="14"/>
+      <c r="AW71" s="15"/>
+    </row>
+    <row r="72" spans="30:49">
+      <c r="AD72" s="13"/>
+      <c r="AE72" s="14"/>
+      <c r="AF72" s="14"/>
+      <c r="AG72" s="14"/>
+      <c r="AH72" s="14"/>
+      <c r="AI72" s="14"/>
+      <c r="AJ72" s="14"/>
+      <c r="AK72" s="14"/>
+      <c r="AL72" s="14"/>
+      <c r="AM72" s="15"/>
+      <c r="AN72" s="13"/>
+      <c r="AO72" s="14"/>
+      <c r="AP72" s="14"/>
+      <c r="AQ72" s="14"/>
+      <c r="AR72" s="14"/>
+      <c r="AS72" s="14"/>
+      <c r="AT72" s="14"/>
+      <c r="AU72" s="14"/>
+      <c r="AV72" s="14"/>
+      <c r="AW72" s="15"/>
+    </row>
+    <row r="73" spans="30:49">
+      <c r="AD73" s="13"/>
+      <c r="AE73" s="14"/>
+      <c r="AF73" s="14"/>
+      <c r="AG73" s="14"/>
+      <c r="AH73" s="14"/>
+      <c r="AI73" s="14"/>
+      <c r="AJ73" s="14"/>
+      <c r="AK73" s="14"/>
+      <c r="AL73" s="14"/>
+      <c r="AM73" s="15"/>
+      <c r="AN73" s="13"/>
+      <c r="AO73" s="14"/>
+      <c r="AP73" s="14"/>
+      <c r="AQ73" s="14"/>
+      <c r="AR73" s="14"/>
+      <c r="AS73" s="14"/>
+      <c r="AT73" s="14"/>
+      <c r="AU73" s="14"/>
+      <c r="AV73" s="14"/>
+      <c r="AW73" s="15"/>
+    </row>
+    <row r="74" spans="30:49">
+      <c r="AD74" s="13"/>
+      <c r="AE74" s="14"/>
+      <c r="AF74" s="14"/>
+      <c r="AG74" s="14"/>
+      <c r="AH74" s="14"/>
+      <c r="AI74" s="14"/>
+      <c r="AJ74" s="14"/>
+      <c r="AK74" s="14"/>
+      <c r="AL74" s="14"/>
+      <c r="AM74" s="15"/>
+      <c r="AN74" s="13"/>
+      <c r="AO74" s="14"/>
+      <c r="AP74" s="14"/>
+      <c r="AQ74" s="14"/>
+      <c r="AR74" s="14"/>
+      <c r="AS74" s="14"/>
+      <c r="AT74" s="14"/>
+      <c r="AU74" s="14"/>
+      <c r="AV74" s="14"/>
+      <c r="AW74" s="15"/>
+    </row>
+    <row r="75" spans="30:49">
+      <c r="AD75" s="13"/>
+      <c r="AE75" s="14"/>
+      <c r="AF75" s="14"/>
+      <c r="AG75" s="14"/>
+      <c r="AH75" s="14"/>
+      <c r="AI75" s="14"/>
+      <c r="AJ75" s="14"/>
+      <c r="AK75" s="14"/>
+      <c r="AL75" s="14"/>
+      <c r="AM75" s="15"/>
+      <c r="AN75" s="13"/>
+      <c r="AO75" s="14"/>
+      <c r="AP75" s="14"/>
+      <c r="AQ75" s="14"/>
+      <c r="AR75" s="14"/>
+      <c r="AS75" s="14"/>
+      <c r="AT75" s="14"/>
+      <c r="AU75" s="14"/>
+      <c r="AV75" s="14"/>
+      <c r="AW75" s="15"/>
+    </row>
+    <row r="76" spans="30:49">
+      <c r="AD76" s="13"/>
+      <c r="AE76" s="14"/>
+      <c r="AF76" s="14"/>
+      <c r="AG76" s="14"/>
+      <c r="AH76" s="14"/>
+      <c r="AI76" s="14"/>
+      <c r="AJ76" s="14"/>
+      <c r="AK76" s="14"/>
+      <c r="AL76" s="14"/>
+      <c r="AM76" s="15"/>
+      <c r="AN76" s="13"/>
+      <c r="AO76" s="14"/>
+      <c r="AP76" s="14"/>
+      <c r="AQ76" s="14"/>
+      <c r="AR76" s="14"/>
+      <c r="AS76" s="14"/>
+      <c r="AT76" s="14"/>
+      <c r="AU76" s="14"/>
+      <c r="AV76" s="14"/>
+      <c r="AW76" s="15"/>
+    </row>
+    <row r="77" spans="30:49">
+      <c r="AD77" s="13"/>
+      <c r="AE77" s="14"/>
+      <c r="AF77" s="14"/>
+      <c r="AG77" s="14"/>
+      <c r="AH77" s="14"/>
+      <c r="AI77" s="14"/>
+      <c r="AJ77" s="14"/>
+      <c r="AK77" s="14"/>
+      <c r="AL77" s="14"/>
+      <c r="AM77" s="15"/>
+      <c r="AN77" s="13"/>
+      <c r="AO77" s="14"/>
+      <c r="AP77" s="14"/>
+      <c r="AQ77" s="14"/>
+      <c r="AR77" s="14"/>
+      <c r="AS77" s="14"/>
+      <c r="AT77" s="14"/>
+      <c r="AU77" s="14"/>
+      <c r="AV77" s="14"/>
+      <c r="AW77" s="15"/>
+    </row>
+    <row r="78" spans="30:49" ht="15.75" thickBot="1">
+      <c r="AD78" s="16"/>
+      <c r="AE78" s="17"/>
+      <c r="AF78" s="17"/>
+      <c r="AG78" s="17"/>
+      <c r="AH78" s="17"/>
+      <c r="AI78" s="17"/>
+      <c r="AJ78" s="17"/>
+      <c r="AK78" s="17"/>
+      <c r="AL78" s="17"/>
+      <c r="AM78" s="18"/>
+      <c r="AN78" s="16"/>
+      <c r="AO78" s="17"/>
+      <c r="AP78" s="17"/>
+      <c r="AQ78" s="17"/>
+      <c r="AR78" s="17"/>
+      <c r="AS78" s="17"/>
+      <c r="AT78" s="17"/>
+      <c r="AU78" s="17"/>
+      <c r="AV78" s="17"/>
+      <c r="AW78" s="18"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
scroll bug fixed, but still not correct.
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="22635" windowHeight="11655" activeTab="2"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="io port" sheetId="2" r:id="rId2"/>
     <sheet name="display" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -292,24 +287,44 @@
   </si>
   <si>
     <t>60 frames per sec</t>
+  </si>
+  <si>
+    <t>constant HSCAN_MAX    : integer := 341;</t>
+  </si>
+  <si>
+    <t>constant VSCAN_MAX    : integer := 262;</t>
+  </si>
+  <si>
+    <t>constant HSCAN        : integer := 257;</t>
+  </si>
+  <si>
+    <t>constant VSCAN        : integer := 240;</t>
+  </si>
+  <si>
+    <t>2c00</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>32 x 30 tiles</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -571,7 +586,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -594,12 +609,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
@@ -650,9 +659,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2646,7 +2664,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2688,7 +2706,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2720,10 +2738,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2755,7 +2772,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2931,14 +2947,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="AO6:AO13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="6" spans="41:41">
       <c r="AO6" t="s">
@@ -2973,16 +2989,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="59.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.25" customWidth="1"/>
+    <col min="2" max="2" width="42.625" customWidth="1"/>
+    <col min="3" max="3" width="64.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="15.75" thickBot="1">
@@ -2990,7 +3006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2998,12 +3014,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1">
+    <row r="4" spans="1:3" ht="14.25" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1">
+    <row r="5" spans="1:3" ht="15" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -3014,7 +3030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1">
+    <row r="6" spans="1:3" ht="15" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -3025,7 +3041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1">
+    <row r="7" spans="1:3" ht="15" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -3036,25 +3052,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" ht="14.25">
+      <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+    <row r="9" spans="1:3" ht="15" thickBot="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
+    <row r="10" spans="1:3" ht="15" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -3065,7 +3081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29.25" thickBot="1">
+    <row r="11" spans="1:3" ht="15" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -3076,7 +3092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1">
+    <row r="12" spans="1:3" ht="15" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -3087,25 +3103,25 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" ht="14.25">
+      <c r="A13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+    <row r="14" spans="1:3" ht="15" thickBot="1">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+    <row r="15" spans="1:3" ht="15" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -3113,12 +3129,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1">
+    <row r="16" spans="1:3" ht="14.25" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1">
+    <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -3129,7 +3145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1">
+    <row r="18" spans="1:3" ht="15" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -3140,7 +3156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1">
+    <row r="19" spans="1:3" ht="15" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -3151,7 +3167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1">
+    <row r="20" spans="1:3" ht="15" thickBot="1">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
@@ -3162,7 +3178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1">
+    <row r="21" spans="1:3" ht="15" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -3173,7 +3189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1">
+    <row r="22" spans="1:3" ht="15" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -3184,7 +3200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29.25" thickBot="1">
+    <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -3195,7 +3211,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+    <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -3206,7 +3222,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+    <row r="25" spans="1:3" ht="15" thickBot="1">
       <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
@@ -3217,17 +3233,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1">
+    <row r="26" spans="1:3" ht="15" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+    <row r="27" spans="1:3" ht="14.25" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1">
+    <row r="28" spans="1:3" ht="15" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
@@ -3238,25 +3254,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:3" ht="14.25">
+      <c r="A29" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="24" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
+    <row r="30" spans="1:3" ht="15" thickBot="1">
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="29.25" thickBot="1">
+    <row r="31" spans="1:3" ht="15" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -3267,7 +3283,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="29.25" thickBot="1">
+    <row r="32" spans="1:3" ht="15" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>17</v>
       </c>
@@ -3278,25 +3294,25 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:3" ht="14.25">
+      <c r="A33" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="24" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+    <row r="34" spans="1:3" ht="15" thickBot="1">
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1">
+    <row r="35" spans="1:3" ht="15" thickBot="1">
       <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
@@ -3305,17 +3321,17 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+    <row r="36" spans="1:3" ht="15" thickBot="1">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1">
+    <row r="37" spans="1:3" ht="14.25" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1">
+    <row r="38" spans="1:3" ht="15" thickBot="1">
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
@@ -3326,7 +3342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1">
+    <row r="39" spans="1:3" ht="15" thickBot="1">
       <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
@@ -3337,17 +3353,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1">
+    <row r="40" spans="1:3" ht="15" thickBot="1">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1">
+    <row r="41" spans="1:3" ht="14.25" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1">
+    <row r="42" spans="1:3" ht="15" thickBot="1">
       <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
@@ -3358,7 +3374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1">
+    <row r="43" spans="1:3" ht="15" thickBot="1">
       <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
@@ -3369,17 +3385,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1">
+    <row r="44" spans="1:3" ht="15" thickBot="1">
       <c r="A44" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="39" thickBot="1">
+    <row r="45" spans="1:3" ht="26.25" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1">
+    <row r="46" spans="1:3" ht="15" thickBot="1">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -3390,35 +3406,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:3" ht="14.25">
+      <c r="A47" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A48" s="9"/>
+    <row r="48" spans="1:3" ht="15" thickBot="1">
+      <c r="A48" s="25"/>
       <c r="B48" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="9"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+      <c r="C48" s="25"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="39" thickBot="1">
+    <row r="50" spans="1:3" ht="26.25" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1">
+    <row r="51" spans="1:3" ht="15" thickBot="1">
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
@@ -3429,35 +3445,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:3" ht="14.25">
+      <c r="A52" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A53" s="9"/>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="25"/>
       <c r="B53" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="9"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1">
+      <c r="C53" s="25"/>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="26.25" thickBot="1">
+    <row r="55" spans="1:3" ht="14.25" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1">
+    <row r="56" spans="1:3" ht="15" thickBot="1">
       <c r="A56" s="4" t="s">
         <v>8</v>
       </c>
@@ -3468,23 +3484,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:3" ht="14.25">
+      <c r="A57" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A58" s="9"/>
+    <row r="58" spans="1:3" ht="15" thickBot="1">
+      <c r="A58" s="25"/>
       <c r="B58" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="9"/>
+      <c r="C58" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3510,19 +3526,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:AW78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Y71" sqref="Y71"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
     <col min="33" max="38" width="4" bestFit="1" customWidth="1"/>
     <col min="45" max="47" width="4" bestFit="1" customWidth="1"/>
@@ -3533,924 +3551,938 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="4:48" ht="15.75" thickBot="1">
+    <row r="4" spans="4:48" ht="14.25" thickBot="1">
       <c r="Z4">
         <v>800</v>
       </c>
     </row>
     <row r="5" spans="4:48">
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9">
         <v>640</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="20"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="4:48">
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="22"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="20"/>
     </row>
     <row r="7" spans="4:48">
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="22"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="20"/>
       <c r="AL7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="4:48" ht="15.75" thickBot="1">
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="22"/>
+    <row r="8" spans="4:48" ht="14.25" thickBot="1">
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="20"/>
       <c r="AU8">
         <v>341</v>
       </c>
     </row>
     <row r="9" spans="4:48">
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="22"/>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="11">
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="20"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9">
         <v>256</v>
       </c>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="11"/>
-      <c r="AR9" s="11"/>
-      <c r="AS9" s="12"/>
-      <c r="AT9" s="19"/>
-      <c r="AU9" s="19"/>
-      <c r="AV9" s="20"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="10"/>
+      <c r="AT9" s="17"/>
+      <c r="AU9" s="17"/>
+      <c r="AV9" s="18"/>
     </row>
     <row r="10" spans="4:48">
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="22"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AM10" s="14"/>
-      <c r="AN10" s="14"/>
-      <c r="AO10" s="14"/>
-      <c r="AP10" s="14"/>
-      <c r="AQ10" s="14"/>
-      <c r="AR10" s="14"/>
-      <c r="AS10" s="15"/>
-      <c r="AT10" s="14"/>
-      <c r="AU10" s="14"/>
-      <c r="AV10" s="22"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="20"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="12"/>
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="12"/>
+      <c r="AU10" s="12"/>
+      <c r="AV10" s="20"/>
     </row>
     <row r="11" spans="4:48">
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="22"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
-      <c r="AN11" s="14"/>
-      <c r="AO11" s="14"/>
-      <c r="AP11" s="14"/>
-      <c r="AQ11" s="14"/>
-      <c r="AR11" s="14"/>
-      <c r="AS11" s="15"/>
-      <c r="AT11" s="14"/>
-      <c r="AU11" s="14"/>
-      <c r="AV11" s="22"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="20"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="12"/>
+      <c r="AM11" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN11" s="12"/>
+      <c r="AO11" s="12"/>
+      <c r="AP11" s="12"/>
+      <c r="AQ11" s="12"/>
+      <c r="AR11" s="12"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="12"/>
+      <c r="AU11" s="12"/>
+      <c r="AV11" s="20"/>
     </row>
     <row r="12" spans="4:48">
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="22"/>
-      <c r="AJ12" s="13">
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="20"/>
+      <c r="AJ12" s="11">
         <v>240</v>
       </c>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14"/>
-      <c r="AO12" s="14"/>
-      <c r="AP12" s="14"/>
-      <c r="AQ12" s="14"/>
-      <c r="AR12" s="14"/>
-      <c r="AS12" s="15"/>
-      <c r="AT12" s="14"/>
-      <c r="AU12" s="14"/>
-      <c r="AV12" s="22"/>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="12"/>
+      <c r="AN12" s="12"/>
+      <c r="AO12" s="12"/>
+      <c r="AP12" s="12"/>
+      <c r="AQ12" s="12"/>
+      <c r="AR12" s="12"/>
+      <c r="AS12" s="13"/>
+      <c r="AT12" s="12"/>
+      <c r="AU12" s="12"/>
+      <c r="AV12" s="20"/>
     </row>
     <row r="13" spans="4:48">
-      <c r="D13" s="13">
+      <c r="D13" s="11">
         <v>480</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="22"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="14"/>
-      <c r="AL13" s="14"/>
-      <c r="AM13" s="14"/>
-      <c r="AN13" s="14"/>
-      <c r="AO13" s="14"/>
-      <c r="AP13" s="14"/>
-      <c r="AQ13" s="14"/>
-      <c r="AR13" s="14"/>
-      <c r="AS13" s="15"/>
-      <c r="AT13" s="14"/>
-      <c r="AU13" s="14"/>
-      <c r="AV13" s="22"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="20"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="12"/>
+      <c r="AL13" s="12"/>
+      <c r="AM13" s="12"/>
+      <c r="AN13" s="12"/>
+      <c r="AO13" s="12"/>
+      <c r="AP13" s="12"/>
+      <c r="AQ13" s="12"/>
+      <c r="AR13" s="12"/>
+      <c r="AS13" s="13"/>
+      <c r="AT13" s="12"/>
+      <c r="AU13" s="12"/>
+      <c r="AV13" s="20"/>
     </row>
     <row r="14" spans="4:48">
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="22"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="14"/>
-      <c r="AL14" s="14"/>
-      <c r="AM14" s="14"/>
-      <c r="AN14" s="14"/>
-      <c r="AO14" s="14"/>
-      <c r="AP14" s="14"/>
-      <c r="AQ14" s="14"/>
-      <c r="AR14" s="14"/>
-      <c r="AS14" s="15"/>
-      <c r="AT14" s="14"/>
-      <c r="AU14" s="14"/>
-      <c r="AV14" s="22"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="20"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="12"/>
+      <c r="AL14" s="12"/>
+      <c r="AM14" s="12"/>
+      <c r="AN14" s="12"/>
+      <c r="AO14" s="12"/>
+      <c r="AP14" s="12"/>
+      <c r="AQ14" s="12"/>
+      <c r="AR14" s="12"/>
+      <c r="AS14" s="13"/>
+      <c r="AT14" s="12"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="20"/>
     </row>
     <row r="15" spans="4:48">
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="22"/>
-      <c r="AJ15" s="13"/>
-      <c r="AK15" s="14"/>
-      <c r="AL15" s="14"/>
-      <c r="AM15" s="14"/>
-      <c r="AN15" s="14"/>
-      <c r="AO15" s="14"/>
-      <c r="AP15" s="14"/>
-      <c r="AQ15" s="14"/>
-      <c r="AR15" s="14"/>
-      <c r="AS15" s="15"/>
-      <c r="AT15" s="14"/>
-      <c r="AU15" s="14"/>
-      <c r="AV15" s="22"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="20"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="12"/>
+      <c r="AL15" s="12"/>
+      <c r="AM15" s="12"/>
+      <c r="AN15" s="12"/>
+      <c r="AO15" s="12"/>
+      <c r="AP15" s="12"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="12"/>
+      <c r="AS15" s="13"/>
+      <c r="AT15" s="12"/>
+      <c r="AU15" s="12"/>
+      <c r="AV15" s="20"/>
     </row>
     <row r="16" spans="4:48">
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="22"/>
-      <c r="AJ16" s="13"/>
-      <c r="AK16" s="14"/>
-      <c r="AL16" s="14"/>
-      <c r="AM16" s="14"/>
-      <c r="AN16" s="14"/>
-      <c r="AO16" s="14"/>
-      <c r="AP16" s="14"/>
-      <c r="AQ16" s="14"/>
-      <c r="AR16" s="14"/>
-      <c r="AS16" s="15"/>
-      <c r="AT16" s="14"/>
-      <c r="AU16" s="14"/>
-      <c r="AV16" s="22"/>
-    </row>
-    <row r="17" spans="3:48" ht="15.75" thickBot="1">
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="22"/>
-      <c r="AJ17" s="16"/>
-      <c r="AK17" s="17"/>
-      <c r="AL17" s="17"/>
-      <c r="AM17" s="17"/>
-      <c r="AN17" s="17"/>
-      <c r="AO17" s="17"/>
-      <c r="AP17" s="17"/>
-      <c r="AQ17" s="17"/>
-      <c r="AR17" s="17"/>
-      <c r="AS17" s="18"/>
-      <c r="AT17" s="14"/>
-      <c r="AU17" s="14"/>
-      <c r="AV17" s="22"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="20"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="12"/>
+      <c r="AL16" s="12"/>
+      <c r="AM16" s="12"/>
+      <c r="AN16" s="12"/>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="13"/>
+      <c r="AT16" s="12"/>
+      <c r="AU16" s="12"/>
+      <c r="AV16" s="20"/>
+    </row>
+    <row r="17" spans="3:48" ht="14.25" thickBot="1">
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="20"/>
+      <c r="AJ17" s="14"/>
+      <c r="AK17" s="15"/>
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="15"/>
+      <c r="AQ17" s="15"/>
+      <c r="AR17" s="15"/>
+      <c r="AS17" s="16"/>
+      <c r="AT17" s="12"/>
+      <c r="AU17" s="12"/>
+      <c r="AV17" s="20"/>
     </row>
     <row r="18" spans="3:48">
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="22"/>
-      <c r="AJ18" s="21"/>
-      <c r="AK18" s="14"/>
-      <c r="AL18" s="14"/>
-      <c r="AM18" s="14"/>
-      <c r="AN18" s="14"/>
-      <c r="AO18" s="14"/>
-      <c r="AP18" s="14"/>
-      <c r="AQ18" s="14"/>
-      <c r="AR18" s="14"/>
-      <c r="AS18" s="14"/>
-      <c r="AT18" s="14"/>
-      <c r="AU18" s="14"/>
-      <c r="AV18" s="22"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="12"/>
+      <c r="AC18" s="12"/>
+      <c r="AD18" s="20"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="12"/>
+      <c r="AL18" s="12"/>
+      <c r="AM18" s="12"/>
+      <c r="AN18" s="12"/>
+      <c r="AO18" s="12"/>
+      <c r="AP18" s="12"/>
+      <c r="AQ18" s="12"/>
+      <c r="AR18" s="12"/>
+      <c r="AS18" s="12"/>
+      <c r="AT18" s="12"/>
+      <c r="AU18" s="12"/>
+      <c r="AV18" s="20"/>
     </row>
     <row r="19" spans="3:48">
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="22"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="20"/>
       <c r="AI19">
         <v>262</v>
       </c>
-      <c r="AJ19" s="21"/>
-      <c r="AK19" s="14"/>
-      <c r="AL19" s="14"/>
-      <c r="AM19" s="14"/>
-      <c r="AN19" s="14"/>
-      <c r="AO19" s="14"/>
-      <c r="AP19" s="14"/>
-      <c r="AQ19" s="14"/>
-      <c r="AR19" s="14"/>
-      <c r="AS19" s="14"/>
-      <c r="AT19" s="14"/>
-      <c r="AU19" s="14"/>
-      <c r="AV19" s="22"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+      <c r="AM19" s="12"/>
+      <c r="AN19" s="12"/>
+      <c r="AO19" s="12"/>
+      <c r="AP19" s="12"/>
+      <c r="AQ19" s="12"/>
+      <c r="AR19" s="12"/>
+      <c r="AS19" s="12"/>
+      <c r="AT19" s="12"/>
+      <c r="AU19" s="12"/>
+      <c r="AV19" s="20"/>
     </row>
     <row r="20" spans="3:48">
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-      <c r="AB20" s="14"/>
-      <c r="AC20" s="14"/>
-      <c r="AD20" s="22"/>
-      <c r="AJ20" s="21"/>
-      <c r="AK20" s="14"/>
-      <c r="AL20" s="14"/>
-      <c r="AM20" s="14"/>
-      <c r="AN20" s="14"/>
-      <c r="AO20" s="14"/>
-      <c r="AP20" s="14"/>
-      <c r="AQ20" s="14"/>
-      <c r="AR20" s="14"/>
-      <c r="AS20" s="14"/>
-      <c r="AT20" s="14"/>
-      <c r="AU20" s="14"/>
-      <c r="AV20" s="22"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
+      <c r="AD20" s="20"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="12"/>
+      <c r="AL20" s="12"/>
+      <c r="AM20" s="12"/>
+      <c r="AN20" s="12"/>
+      <c r="AO20" s="12"/>
+      <c r="AP20" s="12"/>
+      <c r="AQ20" s="12"/>
+      <c r="AR20" s="12"/>
+      <c r="AS20" s="12"/>
+      <c r="AT20" s="12"/>
+      <c r="AU20" s="12"/>
+      <c r="AV20" s="20"/>
     </row>
     <row r="21" spans="3:48">
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="14"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="14"/>
-      <c r="AC21" s="14"/>
-      <c r="AD21" s="22"/>
-      <c r="AJ21" s="23"/>
-      <c r="AK21" s="24"/>
-      <c r="AL21" s="24"/>
-      <c r="AM21" s="24"/>
-      <c r="AN21" s="24"/>
-      <c r="AO21" s="24"/>
-      <c r="AP21" s="24"/>
-      <c r="AQ21" s="24"/>
-      <c r="AR21" s="24"/>
-      <c r="AS21" s="24"/>
-      <c r="AT21" s="24"/>
-      <c r="AU21" s="24"/>
-      <c r="AV21" s="25"/>
-    </row>
-    <row r="22" spans="3:48" ht="15.75" thickBot="1">
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="14"/>
-      <c r="AA22" s="14"/>
-      <c r="AB22" s="14"/>
-      <c r="AC22" s="14"/>
-      <c r="AD22" s="22"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="12"/>
+      <c r="AC21" s="12"/>
+      <c r="AD21" s="20"/>
+      <c r="AJ21" s="21"/>
+      <c r="AK21" s="22"/>
+      <c r="AL21" s="22"/>
+      <c r="AM21" s="22"/>
+      <c r="AN21" s="22"/>
+      <c r="AO21" s="22"/>
+      <c r="AP21" s="22"/>
+      <c r="AQ21" s="22"/>
+      <c r="AR21" s="22"/>
+      <c r="AS21" s="22"/>
+      <c r="AT21" s="22"/>
+      <c r="AU21" s="22"/>
+      <c r="AV21" s="23"/>
+    </row>
+    <row r="22" spans="3:48" ht="14.25" thickBot="1">
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="20"/>
     </row>
     <row r="23" spans="3:48">
-      <c r="D23" s="21"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
-      <c r="Z23" s="14"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
-      <c r="AC23" s="14"/>
-      <c r="AD23" s="22"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="20"/>
+      <c r="AL23" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="24" spans="3:48">
-      <c r="D24" s="21"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
-      <c r="AC24" s="14"/>
-      <c r="AD24" s="22"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="12"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="12"/>
+      <c r="AD24" s="20"/>
+      <c r="AL24" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="3:48">
-      <c r="D25" s="21"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="14"/>
-      <c r="AB25" s="14"/>
-      <c r="AC25" s="14"/>
-      <c r="AD25" s="22"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="12"/>
+      <c r="AD25" s="20"/>
+      <c r="AL25" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="26" spans="3:48">
       <c r="C26">
         <v>600</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="14"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
-      <c r="AD26" s="22"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="20"/>
+      <c r="AL26" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27" spans="3:48">
-      <c r="D27" s="21"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="14"/>
-      <c r="AD27" s="22"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="20"/>
     </row>
     <row r="28" spans="3:48">
-      <c r="D28" s="21"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="14"/>
-      <c r="Z28" s="14"/>
-      <c r="AA28" s="14"/>
-      <c r="AB28" s="14"/>
-      <c r="AC28" s="14"/>
-      <c r="AD28" s="22"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="20"/>
     </row>
     <row r="29" spans="3:48">
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="24"/>
-      <c r="AB29" s="24"/>
-      <c r="AC29" s="24"/>
-      <c r="AD29" s="25"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="23"/>
     </row>
     <row r="35" spans="3:49">
       <c r="C35" t="s">
@@ -4462,1170 +4494,1178 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="3:49" ht="15.75" thickBot="1"/>
+    <row r="38" spans="3:49" ht="14.25" thickBot="1"/>
     <row r="39" spans="3:49">
-      <c r="E39" s="10"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
-      <c r="V39" s="11"/>
-      <c r="W39" s="11"/>
-      <c r="X39" s="12"/>
-      <c r="AD39" s="10"/>
-      <c r="AE39" s="11"/>
-      <c r="AF39" s="11"/>
-      <c r="AG39" s="11"/>
-      <c r="AH39" s="11"/>
-      <c r="AI39" s="11"/>
-      <c r="AJ39" s="11"/>
-      <c r="AK39" s="11"/>
-      <c r="AL39" s="11"/>
-      <c r="AM39" s="12"/>
-      <c r="AN39" s="10"/>
-      <c r="AO39" s="11"/>
-      <c r="AP39" s="11"/>
-      <c r="AQ39" s="11"/>
-      <c r="AR39" s="11"/>
-      <c r="AS39" s="11"/>
-      <c r="AT39" s="11"/>
-      <c r="AU39" s="11"/>
-      <c r="AV39" s="11"/>
-      <c r="AW39" s="12"/>
+      <c r="E39" s="26">
+        <v>2000</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="8">
+        <v>2400</v>
+      </c>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="10"/>
+      <c r="AD39" s="8"/>
+      <c r="AE39" s="9"/>
+      <c r="AF39" s="9"/>
+      <c r="AG39" s="9"/>
+      <c r="AH39" s="9"/>
+      <c r="AI39" s="9"/>
+      <c r="AJ39" s="9"/>
+      <c r="AK39" s="9"/>
+      <c r="AL39" s="9"/>
+      <c r="AM39" s="10"/>
+      <c r="AN39" s="8"/>
+      <c r="AO39" s="9"/>
+      <c r="AP39" s="9"/>
+      <c r="AQ39" s="9"/>
+      <c r="AR39" s="9"/>
+      <c r="AS39" s="9"/>
+      <c r="AT39" s="9"/>
+      <c r="AU39" s="9"/>
+      <c r="AV39" s="9"/>
+      <c r="AW39" s="10"/>
     </row>
     <row r="40" spans="3:49">
-      <c r="E40" s="13"/>
-      <c r="F40" s="14" t="s">
+      <c r="E40" s="11"/>
+      <c r="F40" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="15"/>
-      <c r="AD40" s="13"/>
-      <c r="AE40" s="14" t="s">
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12"/>
+      <c r="V40" s="12"/>
+      <c r="W40" s="12"/>
+      <c r="X40" s="13"/>
+      <c r="AD40" s="11"/>
+      <c r="AE40" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AF40" s="14"/>
-      <c r="AG40" s="14"/>
-      <c r="AH40" s="14"/>
-      <c r="AI40" s="14"/>
-      <c r="AJ40" s="14"/>
-      <c r="AK40" s="14"/>
-      <c r="AL40" s="14"/>
-      <c r="AM40" s="15"/>
-      <c r="AN40" s="13"/>
-      <c r="AO40" s="14"/>
-      <c r="AP40" s="14"/>
-      <c r="AQ40" s="14"/>
-      <c r="AR40" s="14"/>
-      <c r="AS40" s="14"/>
-      <c r="AT40" s="14"/>
-      <c r="AU40" s="14"/>
-      <c r="AV40" s="14"/>
-      <c r="AW40" s="15"/>
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+      <c r="AH40" s="12"/>
+      <c r="AI40" s="12"/>
+      <c r="AJ40" s="12"/>
+      <c r="AK40" s="12"/>
+      <c r="AL40" s="12"/>
+      <c r="AM40" s="13"/>
+      <c r="AN40" s="11"/>
+      <c r="AO40" s="12"/>
+      <c r="AP40" s="12"/>
+      <c r="AQ40" s="12"/>
+      <c r="AR40" s="12"/>
+      <c r="AS40" s="12"/>
+      <c r="AT40" s="12"/>
+      <c r="AU40" s="12"/>
+      <c r="AV40" s="12"/>
+      <c r="AW40" s="13"/>
     </row>
     <row r="41" spans="3:49">
-      <c r="E41" s="13"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="14"/>
-      <c r="V41" s="14"/>
-      <c r="W41" s="14"/>
-      <c r="X41" s="15"/>
-      <c r="AD41" s="13"/>
-      <c r="AE41" s="14"/>
-      <c r="AF41" s="14"/>
-      <c r="AG41" s="14"/>
-      <c r="AH41" s="14"/>
-      <c r="AI41" s="14"/>
-      <c r="AJ41" s="14"/>
-      <c r="AK41" s="14"/>
-      <c r="AL41" s="14"/>
-      <c r="AM41" s="15"/>
-      <c r="AN41" s="13"/>
-      <c r="AO41" s="14"/>
-      <c r="AP41" s="14"/>
-      <c r="AQ41" s="14"/>
-      <c r="AR41" s="14"/>
-      <c r="AS41" s="14"/>
-      <c r="AT41" s="14"/>
-      <c r="AU41" s="14"/>
-      <c r="AV41" s="14"/>
-      <c r="AW41" s="15"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="13"/>
+      <c r="AD41" s="11"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="12"/>
+      <c r="AH41" s="12"/>
+      <c r="AI41" s="12"/>
+      <c r="AJ41" s="12"/>
+      <c r="AK41" s="12"/>
+      <c r="AL41" s="12"/>
+      <c r="AM41" s="13"/>
+      <c r="AN41" s="11"/>
+      <c r="AO41" s="12"/>
+      <c r="AP41" s="12"/>
+      <c r="AQ41" s="12"/>
+      <c r="AR41" s="12"/>
+      <c r="AS41" s="12"/>
+      <c r="AT41" s="12"/>
+      <c r="AU41" s="12"/>
+      <c r="AV41" s="12"/>
+      <c r="AW41" s="13"/>
     </row>
     <row r="42" spans="3:49">
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="15"/>
-      <c r="AD42" s="13"/>
-      <c r="AE42" s="14"/>
-      <c r="AF42" s="14"/>
-      <c r="AG42" s="14"/>
-      <c r="AH42" s="14"/>
-      <c r="AI42" s="14"/>
-      <c r="AJ42" s="14"/>
-      <c r="AK42" s="14"/>
-      <c r="AL42" s="14"/>
-      <c r="AM42" s="15"/>
-      <c r="AN42" s="13"/>
-      <c r="AO42" s="14"/>
-      <c r="AP42" s="14"/>
-      <c r="AQ42" s="14"/>
-      <c r="AR42" s="14"/>
-      <c r="AS42" s="14"/>
-      <c r="AT42" s="14"/>
-      <c r="AU42" s="14"/>
-      <c r="AV42" s="14"/>
-      <c r="AW42" s="15"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12"/>
+      <c r="V42" s="12"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="13"/>
+      <c r="AD42" s="11"/>
+      <c r="AE42" s="12"/>
+      <c r="AF42" s="12"/>
+      <c r="AG42" s="12"/>
+      <c r="AH42" s="12"/>
+      <c r="AI42" s="12"/>
+      <c r="AJ42" s="12"/>
+      <c r="AK42" s="12"/>
+      <c r="AL42" s="12"/>
+      <c r="AM42" s="13"/>
+      <c r="AN42" s="11"/>
+      <c r="AO42" s="12"/>
+      <c r="AP42" s="12"/>
+      <c r="AQ42" s="12"/>
+      <c r="AR42" s="12"/>
+      <c r="AS42" s="12"/>
+      <c r="AT42" s="12"/>
+      <c r="AU42" s="12"/>
+      <c r="AV42" s="12"/>
+      <c r="AW42" s="13"/>
     </row>
     <row r="43" spans="3:49">
-      <c r="E43" s="13"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="15"/>
-      <c r="AD43" s="13"/>
-      <c r="AE43" s="14"/>
-      <c r="AF43" s="14"/>
-      <c r="AG43" s="14"/>
-      <c r="AH43" s="14"/>
-      <c r="AI43" s="14"/>
-      <c r="AJ43" s="14"/>
-      <c r="AK43" s="14"/>
-      <c r="AL43" s="14"/>
-      <c r="AM43" s="15"/>
-      <c r="AN43" s="13"/>
-      <c r="AO43" s="14"/>
-      <c r="AP43" s="14"/>
-      <c r="AQ43" s="14"/>
-      <c r="AR43" s="14"/>
-      <c r="AS43" s="14"/>
-      <c r="AT43" s="14"/>
-      <c r="AU43" s="14"/>
-      <c r="AV43" s="14"/>
-      <c r="AW43" s="15"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
+      <c r="S43" s="12"/>
+      <c r="T43" s="12"/>
+      <c r="U43" s="12"/>
+      <c r="V43" s="12"/>
+      <c r="W43" s="12"/>
+      <c r="X43" s="13"/>
+      <c r="AD43" s="11"/>
+      <c r="AE43" s="12"/>
+      <c r="AF43" s="12"/>
+      <c r="AG43" s="12"/>
+      <c r="AH43" s="12"/>
+      <c r="AI43" s="12"/>
+      <c r="AJ43" s="12"/>
+      <c r="AK43" s="12"/>
+      <c r="AL43" s="12"/>
+      <c r="AM43" s="13"/>
+      <c r="AN43" s="11"/>
+      <c r="AO43" s="12"/>
+      <c r="AP43" s="12"/>
+      <c r="AQ43" s="12"/>
+      <c r="AR43" s="12"/>
+      <c r="AS43" s="12"/>
+      <c r="AT43" s="12"/>
+      <c r="AU43" s="12"/>
+      <c r="AV43" s="12"/>
+      <c r="AW43" s="13"/>
     </row>
     <row r="44" spans="3:49">
-      <c r="E44" s="13"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="15"/>
-      <c r="AD44" s="13"/>
-      <c r="AE44" s="14"/>
-      <c r="AF44" s="14"/>
-      <c r="AG44" s="14"/>
-      <c r="AH44" s="14"/>
-      <c r="AI44" s="14"/>
-      <c r="AJ44" s="14"/>
-      <c r="AK44" s="14"/>
-      <c r="AL44" s="14"/>
-      <c r="AM44" s="15"/>
-      <c r="AN44" s="13"/>
-      <c r="AO44" s="14"/>
-      <c r="AP44" s="14"/>
-      <c r="AQ44" s="14"/>
-      <c r="AR44" s="14"/>
-      <c r="AS44" s="14"/>
-      <c r="AT44" s="14"/>
-      <c r="AU44" s="14"/>
-      <c r="AV44" s="14"/>
-      <c r="AW44" s="15"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="13"/>
+      <c r="AD44" s="11"/>
+      <c r="AE44" s="12"/>
+      <c r="AF44" s="12"/>
+      <c r="AG44" s="12"/>
+      <c r="AH44" s="12"/>
+      <c r="AI44" s="12"/>
+      <c r="AJ44" s="12"/>
+      <c r="AK44" s="12"/>
+      <c r="AL44" s="12"/>
+      <c r="AM44" s="13"/>
+      <c r="AN44" s="11"/>
+      <c r="AO44" s="12"/>
+      <c r="AP44" s="12"/>
+      <c r="AQ44" s="12"/>
+      <c r="AR44" s="12"/>
+      <c r="AS44" s="12"/>
+      <c r="AT44" s="12"/>
+      <c r="AU44" s="12"/>
+      <c r="AV44" s="12"/>
+      <c r="AW44" s="13"/>
     </row>
     <row r="45" spans="3:49">
-      <c r="E45" s="13"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="14"/>
-      <c r="V45" s="14"/>
-      <c r="W45" s="14"/>
-      <c r="X45" s="15"/>
-      <c r="AD45" s="13"/>
-      <c r="AE45" s="14"/>
-      <c r="AF45" s="14"/>
-      <c r="AG45" s="14"/>
-      <c r="AH45" s="14"/>
-      <c r="AI45" s="14"/>
-      <c r="AJ45" s="14"/>
-      <c r="AK45" s="14"/>
-      <c r="AL45" s="14"/>
-      <c r="AM45" s="15"/>
-      <c r="AN45" s="13"/>
-      <c r="AO45" s="14"/>
-      <c r="AP45" s="14"/>
-      <c r="AQ45" s="14"/>
-      <c r="AR45" s="14"/>
-      <c r="AS45" s="14"/>
-      <c r="AT45" s="14"/>
-      <c r="AU45" s="14"/>
-      <c r="AV45" s="14"/>
-      <c r="AW45" s="15"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="13"/>
+      <c r="AD45" s="11"/>
+      <c r="AE45" s="12"/>
+      <c r="AF45" s="12"/>
+      <c r="AG45" s="12"/>
+      <c r="AH45" s="12"/>
+      <c r="AI45" s="12"/>
+      <c r="AJ45" s="12"/>
+      <c r="AK45" s="12"/>
+      <c r="AL45" s="12"/>
+      <c r="AM45" s="13"/>
+      <c r="AN45" s="11"/>
+      <c r="AO45" s="12"/>
+      <c r="AP45" s="12"/>
+      <c r="AQ45" s="12"/>
+      <c r="AR45" s="12"/>
+      <c r="AS45" s="12"/>
+      <c r="AT45" s="12"/>
+      <c r="AU45" s="12"/>
+      <c r="AV45" s="12"/>
+      <c r="AW45" s="13"/>
     </row>
     <row r="46" spans="3:49">
-      <c r="E46" s="13"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="14"/>
-      <c r="U46" s="14"/>
-      <c r="V46" s="14"/>
-      <c r="W46" s="14"/>
-      <c r="X46" s="15"/>
-      <c r="AD46" s="13"/>
-      <c r="AE46" s="14"/>
-      <c r="AF46" s="14"/>
-      <c r="AG46" s="14"/>
-      <c r="AH46" s="14"/>
-      <c r="AI46" s="14"/>
-      <c r="AJ46" s="14"/>
-      <c r="AK46" s="14"/>
-      <c r="AL46" s="14"/>
-      <c r="AM46" s="15"/>
-      <c r="AN46" s="13"/>
-      <c r="AO46" s="14"/>
-      <c r="AP46" s="14"/>
-      <c r="AQ46" s="14"/>
-      <c r="AR46" s="14"/>
-      <c r="AS46" s="14"/>
-      <c r="AT46" s="14"/>
-      <c r="AU46" s="14"/>
-      <c r="AV46" s="14"/>
-      <c r="AW46" s="15"/>
-    </row>
-    <row r="47" spans="3:49" ht="15.75" thickBot="1">
-      <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="17"/>
-      <c r="R47" s="17"/>
-      <c r="S47" s="17"/>
-      <c r="T47" s="17"/>
-      <c r="U47" s="17"/>
-      <c r="V47" s="17"/>
-      <c r="W47" s="17"/>
-      <c r="X47" s="18"/>
-      <c r="AD47" s="16"/>
-      <c r="AE47" s="17"/>
-      <c r="AF47" s="17"/>
-      <c r="AG47" s="17"/>
-      <c r="AH47" s="17"/>
-      <c r="AI47" s="17"/>
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
-      <c r="AL47" s="17"/>
-      <c r="AM47" s="18"/>
-      <c r="AN47" s="16"/>
-      <c r="AO47" s="17"/>
-      <c r="AP47" s="17"/>
-      <c r="AQ47" s="17"/>
-      <c r="AR47" s="17"/>
-      <c r="AS47" s="17"/>
-      <c r="AT47" s="17"/>
-      <c r="AU47" s="17"/>
-      <c r="AV47" s="17"/>
-      <c r="AW47" s="18"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="13"/>
+      <c r="AD46" s="11"/>
+      <c r="AE46" s="12"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AH46" s="12"/>
+      <c r="AI46" s="12"/>
+      <c r="AJ46" s="12"/>
+      <c r="AK46" s="12"/>
+      <c r="AL46" s="12"/>
+      <c r="AM46" s="13"/>
+      <c r="AN46" s="11"/>
+      <c r="AO46" s="12"/>
+      <c r="AP46" s="12"/>
+      <c r="AQ46" s="12"/>
+      <c r="AR46" s="12"/>
+      <c r="AS46" s="12"/>
+      <c r="AT46" s="12"/>
+      <c r="AU46" s="12"/>
+      <c r="AV46" s="12"/>
+      <c r="AW46" s="13"/>
+    </row>
+    <row r="47" spans="3:49" ht="14.25" thickBot="1">
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="16"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="15"/>
+      <c r="AF47" s="15"/>
+      <c r="AG47" s="15"/>
+      <c r="AH47" s="15"/>
+      <c r="AI47" s="15"/>
+      <c r="AJ47" s="15"/>
+      <c r="AK47" s="15"/>
+      <c r="AL47" s="15"/>
+      <c r="AM47" s="16"/>
+      <c r="AN47" s="14"/>
+      <c r="AO47" s="15"/>
+      <c r="AP47" s="15"/>
+      <c r="AQ47" s="15"/>
+      <c r="AR47" s="15"/>
+      <c r="AS47" s="15"/>
+      <c r="AT47" s="15"/>
+      <c r="AU47" s="15"/>
+      <c r="AV47" s="15"/>
+      <c r="AW47" s="16"/>
     </row>
     <row r="48" spans="3:49">
-      <c r="E48" s="10"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
-      <c r="V48" s="11"/>
-      <c r="W48" s="11"/>
-      <c r="X48" s="12"/>
-      <c r="AD48" s="10"/>
-      <c r="AE48" s="11"/>
-      <c r="AF48" s="11"/>
-      <c r="AG48" s="11"/>
-      <c r="AH48" s="11"/>
-      <c r="AI48" s="11"/>
-      <c r="AJ48" s="11"/>
-      <c r="AK48" s="11"/>
-      <c r="AL48" s="11"/>
-      <c r="AM48" s="12"/>
-      <c r="AN48" s="10"/>
-      <c r="AO48" s="11"/>
-      <c r="AP48" s="11"/>
-      <c r="AQ48" s="11"/>
-      <c r="AR48" s="11"/>
-      <c r="AS48" s="11"/>
-      <c r="AT48" s="11"/>
-      <c r="AU48" s="11"/>
-      <c r="AV48" s="11"/>
-      <c r="AW48" s="12"/>
+      <c r="E48" s="8">
+        <v>2800</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="10"/>
+      <c r="AD48" s="8"/>
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="9"/>
+      <c r="AG48" s="9"/>
+      <c r="AH48" s="9"/>
+      <c r="AI48" s="9"/>
+      <c r="AJ48" s="9"/>
+      <c r="AK48" s="9"/>
+      <c r="AL48" s="9"/>
+      <c r="AM48" s="10"/>
+      <c r="AN48" s="8"/>
+      <c r="AO48" s="9"/>
+      <c r="AP48" s="9"/>
+      <c r="AQ48" s="9"/>
+      <c r="AR48" s="9"/>
+      <c r="AS48" s="9"/>
+      <c r="AT48" s="9"/>
+      <c r="AU48" s="9"/>
+      <c r="AV48" s="9"/>
+      <c r="AW48" s="10"/>
     </row>
     <row r="49" spans="5:49">
-      <c r="E49" s="13"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="14"/>
-      <c r="V49" s="14"/>
-      <c r="W49" s="14"/>
-      <c r="X49" s="15"/>
-      <c r="AD49" s="13"/>
-      <c r="AE49" s="14"/>
-      <c r="AF49" s="14"/>
-      <c r="AG49" s="14"/>
-      <c r="AH49" s="14"/>
-      <c r="AI49" s="14"/>
-      <c r="AJ49" s="14"/>
-      <c r="AK49" s="14"/>
-      <c r="AL49" s="14"/>
-      <c r="AM49" s="15"/>
-      <c r="AN49" s="13"/>
-      <c r="AO49" s="14"/>
-      <c r="AP49" s="14"/>
-      <c r="AQ49" s="14"/>
-      <c r="AR49" s="14"/>
-      <c r="AS49" s="14"/>
-      <c r="AT49" s="14"/>
-      <c r="AU49" s="14"/>
-      <c r="AV49" s="14"/>
-      <c r="AW49" s="15"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="12"/>
+      <c r="V49" s="12"/>
+      <c r="W49" s="12"/>
+      <c r="X49" s="13"/>
+      <c r="AD49" s="11"/>
+      <c r="AE49" s="12"/>
+      <c r="AF49" s="12"/>
+      <c r="AG49" s="12"/>
+      <c r="AH49" s="12"/>
+      <c r="AI49" s="12"/>
+      <c r="AJ49" s="12"/>
+      <c r="AK49" s="12"/>
+      <c r="AL49" s="12"/>
+      <c r="AM49" s="13"/>
+      <c r="AN49" s="11"/>
+      <c r="AO49" s="12"/>
+      <c r="AP49" s="12"/>
+      <c r="AQ49" s="12"/>
+      <c r="AR49" s="12"/>
+      <c r="AS49" s="12"/>
+      <c r="AT49" s="12"/>
+      <c r="AU49" s="12"/>
+      <c r="AV49" s="12"/>
+      <c r="AW49" s="13"/>
     </row>
     <row r="50" spans="5:49">
-      <c r="E50" s="13"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
-      <c r="T50" s="14"/>
-      <c r="U50" s="14"/>
-      <c r="V50" s="14"/>
-      <c r="W50" s="14"/>
-      <c r="X50" s="15"/>
-      <c r="AD50" s="13"/>
-      <c r="AE50" s="14"/>
-      <c r="AF50" s="14"/>
-      <c r="AG50" s="14"/>
-      <c r="AH50" s="14"/>
-      <c r="AI50" s="14"/>
-      <c r="AJ50" s="14"/>
-      <c r="AK50" s="14"/>
-      <c r="AL50" s="14"/>
-      <c r="AM50" s="15"/>
-      <c r="AN50" s="13"/>
-      <c r="AO50" s="14"/>
-      <c r="AP50" s="14"/>
-      <c r="AQ50" s="14"/>
-      <c r="AR50" s="14"/>
-      <c r="AS50" s="14"/>
-      <c r="AT50" s="14"/>
-      <c r="AU50" s="14"/>
-      <c r="AV50" s="14"/>
-      <c r="AW50" s="15"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="12"/>
+      <c r="V50" s="12"/>
+      <c r="W50" s="12"/>
+      <c r="X50" s="13"/>
+      <c r="AD50" s="11"/>
+      <c r="AE50" s="12"/>
+      <c r="AF50" s="12"/>
+      <c r="AG50" s="12"/>
+      <c r="AH50" s="12"/>
+      <c r="AI50" s="12"/>
+      <c r="AJ50" s="12"/>
+      <c r="AK50" s="12"/>
+      <c r="AL50" s="12"/>
+      <c r="AM50" s="13"/>
+      <c r="AN50" s="11"/>
+      <c r="AO50" s="12"/>
+      <c r="AP50" s="12"/>
+      <c r="AQ50" s="12"/>
+      <c r="AR50" s="12"/>
+      <c r="AS50" s="12"/>
+      <c r="AT50" s="12"/>
+      <c r="AU50" s="12"/>
+      <c r="AV50" s="12"/>
+      <c r="AW50" s="13"/>
     </row>
     <row r="51" spans="5:49">
-      <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
-      <c r="T51" s="14"/>
-      <c r="U51" s="14"/>
-      <c r="V51" s="14"/>
-      <c r="W51" s="14"/>
-      <c r="X51" s="15"/>
-      <c r="AD51" s="13"/>
-      <c r="AE51" s="14"/>
-      <c r="AF51" s="14"/>
-      <c r="AG51" s="14"/>
-      <c r="AH51" s="14"/>
-      <c r="AI51" s="14"/>
-      <c r="AJ51" s="14"/>
-      <c r="AK51" s="14"/>
-      <c r="AL51" s="14"/>
-      <c r="AM51" s="15"/>
-      <c r="AN51" s="13"/>
-      <c r="AO51" s="14"/>
-      <c r="AP51" s="14"/>
-      <c r="AQ51" s="14"/>
-      <c r="AR51" s="14"/>
-      <c r="AS51" s="14"/>
-      <c r="AT51" s="14"/>
-      <c r="AU51" s="14"/>
-      <c r="AV51" s="14"/>
-      <c r="AW51" s="15"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="X51" s="13"/>
+      <c r="AD51" s="11"/>
+      <c r="AE51" s="12"/>
+      <c r="AF51" s="12"/>
+      <c r="AG51" s="12"/>
+      <c r="AH51" s="12"/>
+      <c r="AI51" s="12"/>
+      <c r="AJ51" s="12"/>
+      <c r="AK51" s="12"/>
+      <c r="AL51" s="12"/>
+      <c r="AM51" s="13"/>
+      <c r="AN51" s="11"/>
+      <c r="AO51" s="12"/>
+      <c r="AP51" s="12"/>
+      <c r="AQ51" s="12"/>
+      <c r="AR51" s="12"/>
+      <c r="AS51" s="12"/>
+      <c r="AT51" s="12"/>
+      <c r="AU51" s="12"/>
+      <c r="AV51" s="12"/>
+      <c r="AW51" s="13"/>
     </row>
     <row r="52" spans="5:49">
-      <c r="E52" s="13"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="13"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="14"/>
-      <c r="U52" s="14"/>
-      <c r="V52" s="14"/>
-      <c r="W52" s="14"/>
-      <c r="X52" s="15"/>
-      <c r="AD52" s="13"/>
-      <c r="AE52" s="14"/>
-      <c r="AF52" s="14"/>
-      <c r="AG52" s="14"/>
-      <c r="AH52" s="14"/>
-      <c r="AI52" s="14"/>
-      <c r="AJ52" s="14"/>
-      <c r="AK52" s="14"/>
-      <c r="AL52" s="14"/>
-      <c r="AM52" s="15"/>
-      <c r="AN52" s="13"/>
-      <c r="AO52" s="14"/>
-      <c r="AP52" s="14"/>
-      <c r="AQ52" s="14"/>
-      <c r="AR52" s="14"/>
-      <c r="AS52" s="14"/>
-      <c r="AT52" s="14"/>
-      <c r="AU52" s="14"/>
-      <c r="AV52" s="14"/>
-      <c r="AW52" s="15"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="12"/>
+      <c r="X52" s="13"/>
+      <c r="AD52" s="11"/>
+      <c r="AE52" s="12"/>
+      <c r="AF52" s="12"/>
+      <c r="AG52" s="12"/>
+      <c r="AH52" s="12"/>
+      <c r="AI52" s="12"/>
+      <c r="AJ52" s="12"/>
+      <c r="AK52" s="12"/>
+      <c r="AL52" s="12"/>
+      <c r="AM52" s="13"/>
+      <c r="AN52" s="11"/>
+      <c r="AO52" s="12"/>
+      <c r="AP52" s="12"/>
+      <c r="AQ52" s="12"/>
+      <c r="AR52" s="12"/>
+      <c r="AS52" s="12"/>
+      <c r="AT52" s="12"/>
+      <c r="AU52" s="12"/>
+      <c r="AV52" s="12"/>
+      <c r="AW52" s="13"/>
     </row>
     <row r="53" spans="5:49">
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="14"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="14"/>
-      <c r="T53" s="14"/>
-      <c r="U53" s="14"/>
-      <c r="V53" s="14"/>
-      <c r="W53" s="14"/>
-      <c r="X53" s="15"/>
-      <c r="AD53" s="13"/>
-      <c r="AE53" s="14"/>
-      <c r="AF53" s="14"/>
-      <c r="AG53" s="14"/>
-      <c r="AH53" s="14"/>
-      <c r="AI53" s="14"/>
-      <c r="AJ53" s="14"/>
-      <c r="AK53" s="14"/>
-      <c r="AL53" s="14"/>
-      <c r="AM53" s="15"/>
-      <c r="AN53" s="13"/>
-      <c r="AO53" s="14"/>
-      <c r="AP53" s="14"/>
-      <c r="AQ53" s="14"/>
-      <c r="AR53" s="14"/>
-      <c r="AS53" s="14"/>
-      <c r="AT53" s="14"/>
-      <c r="AU53" s="14"/>
-      <c r="AV53" s="14"/>
-      <c r="AW53" s="15"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="12"/>
+      <c r="T53" s="12"/>
+      <c r="U53" s="12"/>
+      <c r="V53" s="12"/>
+      <c r="W53" s="12"/>
+      <c r="X53" s="13"/>
+      <c r="AD53" s="11"/>
+      <c r="AE53" s="12"/>
+      <c r="AF53" s="12"/>
+      <c r="AG53" s="12"/>
+      <c r="AH53" s="12"/>
+      <c r="AI53" s="12"/>
+      <c r="AJ53" s="12"/>
+      <c r="AK53" s="12"/>
+      <c r="AL53" s="12"/>
+      <c r="AM53" s="13"/>
+      <c r="AN53" s="11"/>
+      <c r="AO53" s="12"/>
+      <c r="AP53" s="12"/>
+      <c r="AQ53" s="12"/>
+      <c r="AR53" s="12"/>
+      <c r="AS53" s="12"/>
+      <c r="AT53" s="12"/>
+      <c r="AU53" s="12"/>
+      <c r="AV53" s="12"/>
+      <c r="AW53" s="13"/>
     </row>
     <row r="54" spans="5:49">
-      <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="13"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="14"/>
-      <c r="U54" s="14"/>
-      <c r="V54" s="14"/>
-      <c r="W54" s="14"/>
-      <c r="X54" s="15"/>
-      <c r="AD54" s="13"/>
-      <c r="AE54" s="14"/>
-      <c r="AF54" s="14"/>
-      <c r="AG54" s="14"/>
-      <c r="AH54" s="14"/>
-      <c r="AI54" s="14"/>
-      <c r="AJ54" s="14"/>
-      <c r="AK54" s="14"/>
-      <c r="AL54" s="14"/>
-      <c r="AM54" s="15"/>
-      <c r="AN54" s="13"/>
-      <c r="AO54" s="14"/>
-      <c r="AP54" s="14"/>
-      <c r="AQ54" s="14"/>
-      <c r="AR54" s="14"/>
-      <c r="AS54" s="14"/>
-      <c r="AT54" s="14"/>
-      <c r="AU54" s="14"/>
-      <c r="AV54" s="14"/>
-      <c r="AW54" s="15"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="12"/>
+      <c r="T54" s="12"/>
+      <c r="U54" s="12"/>
+      <c r="V54" s="12"/>
+      <c r="W54" s="12"/>
+      <c r="X54" s="13"/>
+      <c r="AD54" s="11"/>
+      <c r="AE54" s="12"/>
+      <c r="AF54" s="12"/>
+      <c r="AG54" s="12"/>
+      <c r="AH54" s="12"/>
+      <c r="AI54" s="12"/>
+      <c r="AJ54" s="12"/>
+      <c r="AK54" s="12"/>
+      <c r="AL54" s="12"/>
+      <c r="AM54" s="13"/>
+      <c r="AN54" s="11"/>
+      <c r="AO54" s="12"/>
+      <c r="AP54" s="12"/>
+      <c r="AQ54" s="12"/>
+      <c r="AR54" s="12"/>
+      <c r="AS54" s="12"/>
+      <c r="AT54" s="12"/>
+      <c r="AU54" s="12"/>
+      <c r="AV54" s="12"/>
+      <c r="AW54" s="13"/>
     </row>
     <row r="55" spans="5:49">
-      <c r="E55" s="13"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="14"/>
-      <c r="T55" s="14"/>
-      <c r="U55" s="14"/>
-      <c r="V55" s="14"/>
-      <c r="W55" s="14"/>
-      <c r="X55" s="15"/>
-      <c r="AD55" s="13"/>
-      <c r="AE55" s="14"/>
-      <c r="AF55" s="14"/>
-      <c r="AG55" s="14"/>
-      <c r="AH55" s="14"/>
-      <c r="AI55" s="14"/>
-      <c r="AJ55" s="14"/>
-      <c r="AK55" s="14"/>
-      <c r="AL55" s="14"/>
-      <c r="AM55" s="15"/>
-      <c r="AN55" s="13"/>
-      <c r="AO55" s="14"/>
-      <c r="AP55" s="14"/>
-      <c r="AQ55" s="14"/>
-      <c r="AR55" s="14"/>
-      <c r="AS55" s="14"/>
-      <c r="AT55" s="14"/>
-      <c r="AU55" s="14"/>
-      <c r="AV55" s="14"/>
-      <c r="AW55" s="15"/>
-    </row>
-    <row r="56" spans="5:49" ht="15.75" thickBot="1">
-      <c r="E56" s="16"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="17"/>
-      <c r="T56" s="17"/>
-      <c r="U56" s="17"/>
-      <c r="V56" s="17"/>
-      <c r="W56" s="17"/>
-      <c r="X56" s="18"/>
-      <c r="AD56" s="16"/>
-      <c r="AE56" s="17"/>
-      <c r="AF56" s="17"/>
-      <c r="AG56" s="17"/>
-      <c r="AH56" s="17"/>
-      <c r="AI56" s="17"/>
-      <c r="AJ56" s="17"/>
-      <c r="AK56" s="17"/>
-      <c r="AL56" s="17"/>
-      <c r="AM56" s="18"/>
-      <c r="AN56" s="16"/>
-      <c r="AO56" s="17"/>
-      <c r="AP56" s="17"/>
-      <c r="AQ56" s="17"/>
-      <c r="AR56" s="17"/>
-      <c r="AS56" s="17"/>
-      <c r="AT56" s="17"/>
-      <c r="AU56" s="17"/>
-      <c r="AV56" s="17"/>
-      <c r="AW56" s="18"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="12"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="12"/>
+      <c r="V55" s="12"/>
+      <c r="W55" s="12"/>
+      <c r="X55" s="13"/>
+      <c r="AD55" s="11"/>
+      <c r="AE55" s="12"/>
+      <c r="AF55" s="12"/>
+      <c r="AG55" s="12"/>
+      <c r="AH55" s="12"/>
+      <c r="AI55" s="12"/>
+      <c r="AJ55" s="12"/>
+      <c r="AK55" s="12"/>
+      <c r="AL55" s="12"/>
+      <c r="AM55" s="13"/>
+      <c r="AN55" s="11"/>
+      <c r="AO55" s="12"/>
+      <c r="AP55" s="12"/>
+      <c r="AQ55" s="12"/>
+      <c r="AR55" s="12"/>
+      <c r="AS55" s="12"/>
+      <c r="AT55" s="12"/>
+      <c r="AU55" s="12"/>
+      <c r="AV55" s="12"/>
+      <c r="AW55" s="13"/>
+    </row>
+    <row r="56" spans="5:49" ht="14.25" thickBot="1">
+      <c r="E56" s="14"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="14"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="15"/>
+      <c r="R56" s="15"/>
+      <c r="S56" s="15"/>
+      <c r="T56" s="15"/>
+      <c r="U56" s="15"/>
+      <c r="V56" s="15"/>
+      <c r="W56" s="15"/>
+      <c r="X56" s="16"/>
+      <c r="AD56" s="14"/>
+      <c r="AE56" s="15"/>
+      <c r="AF56" s="15"/>
+      <c r="AG56" s="15"/>
+      <c r="AH56" s="15"/>
+      <c r="AI56" s="15"/>
+      <c r="AJ56" s="15"/>
+      <c r="AK56" s="15"/>
+      <c r="AL56" s="15"/>
+      <c r="AM56" s="16"/>
+      <c r="AN56" s="14"/>
+      <c r="AO56" s="15"/>
+      <c r="AP56" s="15"/>
+      <c r="AQ56" s="15"/>
+      <c r="AR56" s="15"/>
+      <c r="AS56" s="15"/>
+      <c r="AT56" s="15"/>
+      <c r="AU56" s="15"/>
+      <c r="AV56" s="15"/>
+      <c r="AW56" s="16"/>
     </row>
     <row r="59" spans="5:49">
       <c r="AD59" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="5:49" ht="15.75" thickBot="1"/>
+    <row r="60" spans="5:49" ht="14.25" thickBot="1"/>
     <row r="61" spans="5:49">
-      <c r="AD61" s="10"/>
-      <c r="AE61" s="11"/>
-      <c r="AF61" s="11"/>
-      <c r="AG61" s="11"/>
-      <c r="AH61" s="11"/>
-      <c r="AI61" s="11"/>
-      <c r="AJ61" s="11"/>
-      <c r="AK61" s="11"/>
-      <c r="AL61" s="11"/>
-      <c r="AM61" s="12"/>
-      <c r="AN61" s="10"/>
-      <c r="AO61" s="11"/>
-      <c r="AP61" s="11"/>
-      <c r="AQ61" s="11"/>
-      <c r="AR61" s="11"/>
-      <c r="AS61" s="11"/>
-      <c r="AT61" s="11"/>
-      <c r="AU61" s="11"/>
-      <c r="AV61" s="11"/>
-      <c r="AW61" s="12"/>
+      <c r="AD61" s="8"/>
+      <c r="AE61" s="9"/>
+      <c r="AF61" s="9"/>
+      <c r="AG61" s="9"/>
+      <c r="AH61" s="9"/>
+      <c r="AI61" s="9"/>
+      <c r="AJ61" s="9"/>
+      <c r="AK61" s="9"/>
+      <c r="AL61" s="9"/>
+      <c r="AM61" s="10"/>
+      <c r="AN61" s="8"/>
+      <c r="AO61" s="9"/>
+      <c r="AP61" s="9"/>
+      <c r="AQ61" s="9"/>
+      <c r="AR61" s="9"/>
+      <c r="AS61" s="9"/>
+      <c r="AT61" s="9"/>
+      <c r="AU61" s="9"/>
+      <c r="AV61" s="9"/>
+      <c r="AW61" s="10"/>
     </row>
     <row r="62" spans="5:49">
-      <c r="AD62" s="13"/>
-      <c r="AE62" s="14" t="s">
+      <c r="AD62" s="11"/>
+      <c r="AE62" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AF62" s="14"/>
-      <c r="AG62" s="14"/>
-      <c r="AH62" s="14"/>
-      <c r="AI62" s="14"/>
-      <c r="AJ62" s="14"/>
-      <c r="AK62" s="14"/>
-      <c r="AL62" s="14"/>
-      <c r="AM62" s="15"/>
-      <c r="AN62" s="13"/>
-      <c r="AO62" s="14"/>
-      <c r="AP62" s="14"/>
-      <c r="AQ62" s="14"/>
-      <c r="AR62" s="14"/>
-      <c r="AS62" s="14"/>
-      <c r="AT62" s="14"/>
-      <c r="AU62" s="14"/>
-      <c r="AV62" s="14"/>
-      <c r="AW62" s="15"/>
+      <c r="AF62" s="12"/>
+      <c r="AG62" s="12"/>
+      <c r="AH62" s="12"/>
+      <c r="AI62" s="12"/>
+      <c r="AJ62" s="12"/>
+      <c r="AK62" s="12"/>
+      <c r="AL62" s="12"/>
+      <c r="AM62" s="13"/>
+      <c r="AN62" s="11"/>
+      <c r="AO62" s="12"/>
+      <c r="AP62" s="12"/>
+      <c r="AQ62" s="12"/>
+      <c r="AR62" s="12"/>
+      <c r="AS62" s="12"/>
+      <c r="AT62" s="12"/>
+      <c r="AU62" s="12"/>
+      <c r="AV62" s="12"/>
+      <c r="AW62" s="13"/>
     </row>
     <row r="63" spans="5:49">
-      <c r="AD63" s="13"/>
-      <c r="AE63" s="14"/>
-      <c r="AF63" s="14"/>
-      <c r="AG63" s="14"/>
-      <c r="AH63" s="14"/>
-      <c r="AI63" s="14"/>
-      <c r="AJ63" s="14"/>
-      <c r="AK63" s="14"/>
-      <c r="AL63" s="14"/>
-      <c r="AM63" s="15"/>
-      <c r="AN63" s="13"/>
-      <c r="AO63" s="14"/>
-      <c r="AP63" s="14"/>
-      <c r="AQ63" s="14"/>
-      <c r="AR63" s="14"/>
-      <c r="AS63" s="14"/>
-      <c r="AT63" s="14"/>
-      <c r="AU63" s="14"/>
-      <c r="AV63" s="14"/>
-      <c r="AW63" s="15"/>
+      <c r="AD63" s="11"/>
+      <c r="AE63" s="12"/>
+      <c r="AF63" s="12"/>
+      <c r="AG63" s="12"/>
+      <c r="AH63" s="12"/>
+      <c r="AI63" s="12"/>
+      <c r="AJ63" s="12"/>
+      <c r="AK63" s="12"/>
+      <c r="AL63" s="12"/>
+      <c r="AM63" s="13"/>
+      <c r="AN63" s="11"/>
+      <c r="AO63" s="12"/>
+      <c r="AP63" s="12"/>
+      <c r="AQ63" s="12"/>
+      <c r="AR63" s="12"/>
+      <c r="AS63" s="12"/>
+      <c r="AT63" s="12"/>
+      <c r="AU63" s="12"/>
+      <c r="AV63" s="12"/>
+      <c r="AW63" s="13"/>
     </row>
     <row r="64" spans="5:49">
-      <c r="AD64" s="13"/>
-      <c r="AE64" s="14"/>
-      <c r="AF64" s="14"/>
-      <c r="AG64" s="14"/>
-      <c r="AH64" s="14"/>
-      <c r="AI64" s="14"/>
-      <c r="AJ64" s="14"/>
-      <c r="AK64" s="14"/>
-      <c r="AL64" s="14"/>
-      <c r="AM64" s="15"/>
-      <c r="AN64" s="13"/>
-      <c r="AO64" s="14"/>
-      <c r="AP64" s="14"/>
-      <c r="AQ64" s="14"/>
-      <c r="AR64" s="14"/>
-      <c r="AS64" s="14"/>
-      <c r="AT64" s="14"/>
-      <c r="AU64" s="14"/>
-      <c r="AV64" s="14"/>
-      <c r="AW64" s="15"/>
+      <c r="AD64" s="11"/>
+      <c r="AE64" s="12"/>
+      <c r="AF64" s="12"/>
+      <c r="AG64" s="12"/>
+      <c r="AH64" s="12"/>
+      <c r="AI64" s="12"/>
+      <c r="AJ64" s="12"/>
+      <c r="AK64" s="12"/>
+      <c r="AL64" s="12"/>
+      <c r="AM64" s="13"/>
+      <c r="AN64" s="11"/>
+      <c r="AO64" s="12"/>
+      <c r="AP64" s="12"/>
+      <c r="AQ64" s="12"/>
+      <c r="AR64" s="12"/>
+      <c r="AS64" s="12"/>
+      <c r="AT64" s="12"/>
+      <c r="AU64" s="12"/>
+      <c r="AV64" s="12"/>
+      <c r="AW64" s="13"/>
     </row>
     <row r="65" spans="30:49">
-      <c r="AD65" s="13"/>
-      <c r="AE65" s="14"/>
-      <c r="AF65" s="14"/>
-      <c r="AG65" s="14"/>
-      <c r="AH65" s="14"/>
-      <c r="AI65" s="14"/>
-      <c r="AJ65" s="14"/>
-      <c r="AK65" s="14"/>
-      <c r="AL65" s="14"/>
-      <c r="AM65" s="15"/>
-      <c r="AN65" s="13"/>
-      <c r="AO65" s="14"/>
-      <c r="AP65" s="14"/>
-      <c r="AQ65" s="14"/>
-      <c r="AR65" s="14"/>
-      <c r="AS65" s="14"/>
-      <c r="AT65" s="14"/>
-      <c r="AU65" s="14"/>
-      <c r="AV65" s="14"/>
-      <c r="AW65" s="15"/>
+      <c r="AD65" s="11"/>
+      <c r="AE65" s="12"/>
+      <c r="AF65" s="12"/>
+      <c r="AG65" s="12"/>
+      <c r="AH65" s="12"/>
+      <c r="AI65" s="12"/>
+      <c r="AJ65" s="12"/>
+      <c r="AK65" s="12"/>
+      <c r="AL65" s="12"/>
+      <c r="AM65" s="13"/>
+      <c r="AN65" s="11"/>
+      <c r="AO65" s="12"/>
+      <c r="AP65" s="12"/>
+      <c r="AQ65" s="12"/>
+      <c r="AR65" s="12"/>
+      <c r="AS65" s="12"/>
+      <c r="AT65" s="12"/>
+      <c r="AU65" s="12"/>
+      <c r="AV65" s="12"/>
+      <c r="AW65" s="13"/>
     </row>
     <row r="66" spans="30:49">
-      <c r="AD66" s="13"/>
-      <c r="AE66" s="14"/>
-      <c r="AF66" s="14"/>
-      <c r="AG66" s="14"/>
-      <c r="AH66" s="14"/>
-      <c r="AI66" s="14"/>
-      <c r="AJ66" s="14"/>
-      <c r="AK66" s="14"/>
-      <c r="AL66" s="14"/>
-      <c r="AM66" s="15"/>
-      <c r="AN66" s="13"/>
-      <c r="AO66" s="14"/>
-      <c r="AP66" s="14"/>
-      <c r="AQ66" s="14"/>
-      <c r="AR66" s="14"/>
-      <c r="AS66" s="14"/>
-      <c r="AT66" s="14"/>
-      <c r="AU66" s="14"/>
-      <c r="AV66" s="14"/>
-      <c r="AW66" s="15"/>
+      <c r="AD66" s="11"/>
+      <c r="AE66" s="12"/>
+      <c r="AF66" s="12"/>
+      <c r="AG66" s="12"/>
+      <c r="AH66" s="12"/>
+      <c r="AI66" s="12"/>
+      <c r="AJ66" s="12"/>
+      <c r="AK66" s="12"/>
+      <c r="AL66" s="12"/>
+      <c r="AM66" s="13"/>
+      <c r="AN66" s="11"/>
+      <c r="AO66" s="12"/>
+      <c r="AP66" s="12"/>
+      <c r="AQ66" s="12"/>
+      <c r="AR66" s="12"/>
+      <c r="AS66" s="12"/>
+      <c r="AT66" s="12"/>
+      <c r="AU66" s="12"/>
+      <c r="AV66" s="12"/>
+      <c r="AW66" s="13"/>
     </row>
     <row r="67" spans="30:49">
-      <c r="AD67" s="13"/>
-      <c r="AE67" s="14"/>
-      <c r="AF67" s="14"/>
-      <c r="AG67" s="14"/>
-      <c r="AH67" s="14"/>
-      <c r="AI67" s="14"/>
-      <c r="AJ67" s="14"/>
-      <c r="AK67" s="14"/>
-      <c r="AL67" s="14"/>
-      <c r="AM67" s="15"/>
-      <c r="AN67" s="13"/>
-      <c r="AO67" s="14"/>
-      <c r="AP67" s="14"/>
-      <c r="AQ67" s="14"/>
-      <c r="AR67" s="14"/>
-      <c r="AS67" s="14"/>
-      <c r="AT67" s="14"/>
-      <c r="AU67" s="14"/>
-      <c r="AV67" s="14"/>
-      <c r="AW67" s="15"/>
+      <c r="AD67" s="11"/>
+      <c r="AE67" s="12"/>
+      <c r="AF67" s="12"/>
+      <c r="AG67" s="12"/>
+      <c r="AH67" s="12"/>
+      <c r="AI67" s="12"/>
+      <c r="AJ67" s="12"/>
+      <c r="AK67" s="12"/>
+      <c r="AL67" s="12"/>
+      <c r="AM67" s="13"/>
+      <c r="AN67" s="11"/>
+      <c r="AO67" s="12"/>
+      <c r="AP67" s="12"/>
+      <c r="AQ67" s="12"/>
+      <c r="AR67" s="12"/>
+      <c r="AS67" s="12"/>
+      <c r="AT67" s="12"/>
+      <c r="AU67" s="12"/>
+      <c r="AV67" s="12"/>
+      <c r="AW67" s="13"/>
     </row>
     <row r="68" spans="30:49">
-      <c r="AD68" s="13"/>
-      <c r="AE68" s="14"/>
-      <c r="AF68" s="14"/>
-      <c r="AG68" s="14"/>
-      <c r="AH68" s="14"/>
-      <c r="AI68" s="14"/>
-      <c r="AJ68" s="14"/>
-      <c r="AK68" s="14"/>
-      <c r="AL68" s="14"/>
-      <c r="AM68" s="15"/>
-      <c r="AN68" s="13"/>
-      <c r="AO68" s="14"/>
-      <c r="AP68" s="14"/>
-      <c r="AQ68" s="14"/>
-      <c r="AR68" s="14"/>
-      <c r="AS68" s="14"/>
-      <c r="AT68" s="14"/>
-      <c r="AU68" s="14"/>
-      <c r="AV68" s="14"/>
-      <c r="AW68" s="15"/>
-    </row>
-    <row r="69" spans="30:49" ht="15.75" thickBot="1">
-      <c r="AD69" s="16"/>
-      <c r="AE69" s="17"/>
-      <c r="AF69" s="17"/>
-      <c r="AG69" s="17"/>
-      <c r="AH69" s="17"/>
-      <c r="AI69" s="17"/>
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
-      <c r="AL69" s="17"/>
-      <c r="AM69" s="18"/>
-      <c r="AN69" s="16"/>
-      <c r="AO69" s="17"/>
-      <c r="AP69" s="17"/>
-      <c r="AQ69" s="17"/>
-      <c r="AR69" s="17"/>
-      <c r="AS69" s="17"/>
-      <c r="AT69" s="17"/>
-      <c r="AU69" s="17"/>
-      <c r="AV69" s="17"/>
-      <c r="AW69" s="18"/>
+      <c r="AD68" s="11"/>
+      <c r="AE68" s="12"/>
+      <c r="AF68" s="12"/>
+      <c r="AG68" s="12"/>
+      <c r="AH68" s="12"/>
+      <c r="AI68" s="12"/>
+      <c r="AJ68" s="12"/>
+      <c r="AK68" s="12"/>
+      <c r="AL68" s="12"/>
+      <c r="AM68" s="13"/>
+      <c r="AN68" s="11"/>
+      <c r="AO68" s="12"/>
+      <c r="AP68" s="12"/>
+      <c r="AQ68" s="12"/>
+      <c r="AR68" s="12"/>
+      <c r="AS68" s="12"/>
+      <c r="AT68" s="12"/>
+      <c r="AU68" s="12"/>
+      <c r="AV68" s="12"/>
+      <c r="AW68" s="13"/>
+    </row>
+    <row r="69" spans="30:49" ht="14.25" thickBot="1">
+      <c r="AD69" s="14"/>
+      <c r="AE69" s="15"/>
+      <c r="AF69" s="15"/>
+      <c r="AG69" s="15"/>
+      <c r="AH69" s="15"/>
+      <c r="AI69" s="15"/>
+      <c r="AJ69" s="15"/>
+      <c r="AK69" s="15"/>
+      <c r="AL69" s="15"/>
+      <c r="AM69" s="16"/>
+      <c r="AN69" s="14"/>
+      <c r="AO69" s="15"/>
+      <c r="AP69" s="15"/>
+      <c r="AQ69" s="15"/>
+      <c r="AR69" s="15"/>
+      <c r="AS69" s="15"/>
+      <c r="AT69" s="15"/>
+      <c r="AU69" s="15"/>
+      <c r="AV69" s="15"/>
+      <c r="AW69" s="16"/>
     </row>
     <row r="70" spans="30:49">
-      <c r="AD70" s="10"/>
-      <c r="AE70" s="11"/>
-      <c r="AF70" s="11"/>
-      <c r="AG70" s="11"/>
-      <c r="AH70" s="11"/>
-      <c r="AI70" s="11"/>
-      <c r="AJ70" s="11"/>
-      <c r="AK70" s="11"/>
-      <c r="AL70" s="11"/>
-      <c r="AM70" s="12"/>
-      <c r="AN70" s="10"/>
-      <c r="AO70" s="11"/>
-      <c r="AP70" s="11"/>
-      <c r="AQ70" s="11"/>
-      <c r="AR70" s="11"/>
-      <c r="AS70" s="11"/>
-      <c r="AT70" s="11"/>
-      <c r="AU70" s="11"/>
-      <c r="AV70" s="11"/>
-      <c r="AW70" s="12"/>
+      <c r="AD70" s="8"/>
+      <c r="AE70" s="9"/>
+      <c r="AF70" s="9"/>
+      <c r="AG70" s="9"/>
+      <c r="AH70" s="9"/>
+      <c r="AI70" s="9"/>
+      <c r="AJ70" s="9"/>
+      <c r="AK70" s="9"/>
+      <c r="AL70" s="9"/>
+      <c r="AM70" s="10"/>
+      <c r="AN70" s="8"/>
+      <c r="AO70" s="9"/>
+      <c r="AP70" s="9"/>
+      <c r="AQ70" s="9"/>
+      <c r="AR70" s="9"/>
+      <c r="AS70" s="9"/>
+      <c r="AT70" s="9"/>
+      <c r="AU70" s="9"/>
+      <c r="AV70" s="9"/>
+      <c r="AW70" s="10"/>
     </row>
     <row r="71" spans="30:49">
-      <c r="AD71" s="13"/>
-      <c r="AE71" s="14"/>
-      <c r="AF71" s="14"/>
-      <c r="AG71" s="14"/>
-      <c r="AH71" s="14"/>
-      <c r="AI71" s="14"/>
-      <c r="AJ71" s="14"/>
-      <c r="AK71" s="14"/>
-      <c r="AL71" s="14"/>
-      <c r="AM71" s="15"/>
-      <c r="AN71" s="13"/>
-      <c r="AO71" s="14"/>
-      <c r="AP71" s="14"/>
-      <c r="AQ71" s="14"/>
-      <c r="AR71" s="14"/>
-      <c r="AS71" s="14"/>
-      <c r="AT71" s="14"/>
-      <c r="AU71" s="14"/>
-      <c r="AV71" s="14"/>
-      <c r="AW71" s="15"/>
+      <c r="AD71" s="11"/>
+      <c r="AE71" s="12"/>
+      <c r="AF71" s="12"/>
+      <c r="AG71" s="12"/>
+      <c r="AH71" s="12"/>
+      <c r="AI71" s="12"/>
+      <c r="AJ71" s="12"/>
+      <c r="AK71" s="12"/>
+      <c r="AL71" s="12"/>
+      <c r="AM71" s="13"/>
+      <c r="AN71" s="11"/>
+      <c r="AO71" s="12"/>
+      <c r="AP71" s="12"/>
+      <c r="AQ71" s="12"/>
+      <c r="AR71" s="12"/>
+      <c r="AS71" s="12"/>
+      <c r="AT71" s="12"/>
+      <c r="AU71" s="12"/>
+      <c r="AV71" s="12"/>
+      <c r="AW71" s="13"/>
     </row>
     <row r="72" spans="30:49">
-      <c r="AD72" s="13"/>
-      <c r="AE72" s="14"/>
-      <c r="AF72" s="14"/>
-      <c r="AG72" s="14"/>
-      <c r="AH72" s="14"/>
-      <c r="AI72" s="14"/>
-      <c r="AJ72" s="14"/>
-      <c r="AK72" s="14"/>
-      <c r="AL72" s="14"/>
-      <c r="AM72" s="15"/>
-      <c r="AN72" s="13"/>
-      <c r="AO72" s="14"/>
-      <c r="AP72" s="14"/>
-      <c r="AQ72" s="14"/>
-      <c r="AR72" s="14"/>
-      <c r="AS72" s="14"/>
-      <c r="AT72" s="14"/>
-      <c r="AU72" s="14"/>
-      <c r="AV72" s="14"/>
-      <c r="AW72" s="15"/>
+      <c r="AD72" s="11"/>
+      <c r="AE72" s="12"/>
+      <c r="AF72" s="12"/>
+      <c r="AG72" s="12"/>
+      <c r="AH72" s="12"/>
+      <c r="AI72" s="12"/>
+      <c r="AJ72" s="12"/>
+      <c r="AK72" s="12"/>
+      <c r="AL72" s="12"/>
+      <c r="AM72" s="13"/>
+      <c r="AN72" s="11"/>
+      <c r="AO72" s="12"/>
+      <c r="AP72" s="12"/>
+      <c r="AQ72" s="12"/>
+      <c r="AR72" s="12"/>
+      <c r="AS72" s="12"/>
+      <c r="AT72" s="12"/>
+      <c r="AU72" s="12"/>
+      <c r="AV72" s="12"/>
+      <c r="AW72" s="13"/>
     </row>
     <row r="73" spans="30:49">
-      <c r="AD73" s="13"/>
-      <c r="AE73" s="14"/>
-      <c r="AF73" s="14"/>
-      <c r="AG73" s="14"/>
-      <c r="AH73" s="14"/>
-      <c r="AI73" s="14"/>
-      <c r="AJ73" s="14"/>
-      <c r="AK73" s="14"/>
-      <c r="AL73" s="14"/>
-      <c r="AM73" s="15"/>
-      <c r="AN73" s="13"/>
-      <c r="AO73" s="14"/>
-      <c r="AP73" s="14"/>
-      <c r="AQ73" s="14"/>
-      <c r="AR73" s="14"/>
-      <c r="AS73" s="14"/>
-      <c r="AT73" s="14"/>
-      <c r="AU73" s="14"/>
-      <c r="AV73" s="14"/>
-      <c r="AW73" s="15"/>
+      <c r="AD73" s="11"/>
+      <c r="AE73" s="12"/>
+      <c r="AF73" s="12"/>
+      <c r="AG73" s="12"/>
+      <c r="AH73" s="12"/>
+      <c r="AI73" s="12"/>
+      <c r="AJ73" s="12"/>
+      <c r="AK73" s="12"/>
+      <c r="AL73" s="12"/>
+      <c r="AM73" s="13"/>
+      <c r="AN73" s="11"/>
+      <c r="AO73" s="12"/>
+      <c r="AP73" s="12"/>
+      <c r="AQ73" s="12"/>
+      <c r="AR73" s="12"/>
+      <c r="AS73" s="12"/>
+      <c r="AT73" s="12"/>
+      <c r="AU73" s="12"/>
+      <c r="AV73" s="12"/>
+      <c r="AW73" s="13"/>
     </row>
     <row r="74" spans="30:49">
-      <c r="AD74" s="13"/>
-      <c r="AE74" s="14"/>
-      <c r="AF74" s="14"/>
-      <c r="AG74" s="14"/>
-      <c r="AH74" s="14"/>
-      <c r="AI74" s="14"/>
-      <c r="AJ74" s="14"/>
-      <c r="AK74" s="14"/>
-      <c r="AL74" s="14"/>
-      <c r="AM74" s="15"/>
-      <c r="AN74" s="13"/>
-      <c r="AO74" s="14"/>
-      <c r="AP74" s="14"/>
-      <c r="AQ74" s="14"/>
-      <c r="AR74" s="14"/>
-      <c r="AS74" s="14"/>
-      <c r="AT74" s="14"/>
-      <c r="AU74" s="14"/>
-      <c r="AV74" s="14"/>
-      <c r="AW74" s="15"/>
+      <c r="AD74" s="11"/>
+      <c r="AE74" s="12"/>
+      <c r="AF74" s="12"/>
+      <c r="AG74" s="12"/>
+      <c r="AH74" s="12"/>
+      <c r="AI74" s="12"/>
+      <c r="AJ74" s="12"/>
+      <c r="AK74" s="12"/>
+      <c r="AL74" s="12"/>
+      <c r="AM74" s="13"/>
+      <c r="AN74" s="11"/>
+      <c r="AO74" s="12"/>
+      <c r="AP74" s="12"/>
+      <c r="AQ74" s="12"/>
+      <c r="AR74" s="12"/>
+      <c r="AS74" s="12"/>
+      <c r="AT74" s="12"/>
+      <c r="AU74" s="12"/>
+      <c r="AV74" s="12"/>
+      <c r="AW74" s="13"/>
     </row>
     <row r="75" spans="30:49">
-      <c r="AD75" s="13"/>
-      <c r="AE75" s="14"/>
-      <c r="AF75" s="14"/>
-      <c r="AG75" s="14"/>
-      <c r="AH75" s="14"/>
-      <c r="AI75" s="14"/>
-      <c r="AJ75" s="14"/>
-      <c r="AK75" s="14"/>
-      <c r="AL75" s="14"/>
-      <c r="AM75" s="15"/>
-      <c r="AN75" s="13"/>
-      <c r="AO75" s="14"/>
-      <c r="AP75" s="14"/>
-      <c r="AQ75" s="14"/>
-      <c r="AR75" s="14"/>
-      <c r="AS75" s="14"/>
-      <c r="AT75" s="14"/>
-      <c r="AU75" s="14"/>
-      <c r="AV75" s="14"/>
-      <c r="AW75" s="15"/>
+      <c r="AD75" s="11"/>
+      <c r="AE75" s="12"/>
+      <c r="AF75" s="12"/>
+      <c r="AG75" s="12"/>
+      <c r="AH75" s="12"/>
+      <c r="AI75" s="12"/>
+      <c r="AJ75" s="12"/>
+      <c r="AK75" s="12"/>
+      <c r="AL75" s="12"/>
+      <c r="AM75" s="13"/>
+      <c r="AN75" s="11"/>
+      <c r="AO75" s="12"/>
+      <c r="AP75" s="12"/>
+      <c r="AQ75" s="12"/>
+      <c r="AR75" s="12"/>
+      <c r="AS75" s="12"/>
+      <c r="AT75" s="12"/>
+      <c r="AU75" s="12"/>
+      <c r="AV75" s="12"/>
+      <c r="AW75" s="13"/>
     </row>
     <row r="76" spans="30:49">
-      <c r="AD76" s="13"/>
-      <c r="AE76" s="14"/>
-      <c r="AF76" s="14"/>
-      <c r="AG76" s="14"/>
-      <c r="AH76" s="14"/>
-      <c r="AI76" s="14"/>
-      <c r="AJ76" s="14"/>
-      <c r="AK76" s="14"/>
-      <c r="AL76" s="14"/>
-      <c r="AM76" s="15"/>
-      <c r="AN76" s="13"/>
-      <c r="AO76" s="14"/>
-      <c r="AP76" s="14"/>
-      <c r="AQ76" s="14"/>
-      <c r="AR76" s="14"/>
-      <c r="AS76" s="14"/>
-      <c r="AT76" s="14"/>
-      <c r="AU76" s="14"/>
-      <c r="AV76" s="14"/>
-      <c r="AW76" s="15"/>
+      <c r="AD76" s="11"/>
+      <c r="AE76" s="12"/>
+      <c r="AF76" s="12"/>
+      <c r="AG76" s="12"/>
+      <c r="AH76" s="12"/>
+      <c r="AI76" s="12"/>
+      <c r="AJ76" s="12"/>
+      <c r="AK76" s="12"/>
+      <c r="AL76" s="12"/>
+      <c r="AM76" s="13"/>
+      <c r="AN76" s="11"/>
+      <c r="AO76" s="12"/>
+      <c r="AP76" s="12"/>
+      <c r="AQ76" s="12"/>
+      <c r="AR76" s="12"/>
+      <c r="AS76" s="12"/>
+      <c r="AT76" s="12"/>
+      <c r="AU76" s="12"/>
+      <c r="AV76" s="12"/>
+      <c r="AW76" s="13"/>
     </row>
     <row r="77" spans="30:49">
-      <c r="AD77" s="13"/>
-      <c r="AE77" s="14"/>
-      <c r="AF77" s="14"/>
-      <c r="AG77" s="14"/>
-      <c r="AH77" s="14"/>
-      <c r="AI77" s="14"/>
-      <c r="AJ77" s="14"/>
-      <c r="AK77" s="14"/>
-      <c r="AL77" s="14"/>
-      <c r="AM77" s="15"/>
-      <c r="AN77" s="13"/>
-      <c r="AO77" s="14"/>
-      <c r="AP77" s="14"/>
-      <c r="AQ77" s="14"/>
-      <c r="AR77" s="14"/>
-      <c r="AS77" s="14"/>
-      <c r="AT77" s="14"/>
-      <c r="AU77" s="14"/>
-      <c r="AV77" s="14"/>
-      <c r="AW77" s="15"/>
-    </row>
-    <row r="78" spans="30:49" ht="15.75" thickBot="1">
-      <c r="AD78" s="16"/>
-      <c r="AE78" s="17"/>
-      <c r="AF78" s="17"/>
-      <c r="AG78" s="17"/>
-      <c r="AH78" s="17"/>
-      <c r="AI78" s="17"/>
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
-      <c r="AL78" s="17"/>
-      <c r="AM78" s="18"/>
-      <c r="AN78" s="16"/>
-      <c r="AO78" s="17"/>
-      <c r="AP78" s="17"/>
-      <c r="AQ78" s="17"/>
-      <c r="AR78" s="17"/>
-      <c r="AS78" s="17"/>
-      <c r="AT78" s="17"/>
-      <c r="AU78" s="17"/>
-      <c r="AV78" s="17"/>
-      <c r="AW78" s="18"/>
+      <c r="AD77" s="11"/>
+      <c r="AE77" s="12"/>
+      <c r="AF77" s="12"/>
+      <c r="AG77" s="12"/>
+      <c r="AH77" s="12"/>
+      <c r="AI77" s="12"/>
+      <c r="AJ77" s="12"/>
+      <c r="AK77" s="12"/>
+      <c r="AL77" s="12"/>
+      <c r="AM77" s="13"/>
+      <c r="AN77" s="11"/>
+      <c r="AO77" s="12"/>
+      <c r="AP77" s="12"/>
+      <c r="AQ77" s="12"/>
+      <c r="AR77" s="12"/>
+      <c r="AS77" s="12"/>
+      <c r="AT77" s="12"/>
+      <c r="AU77" s="12"/>
+      <c r="AV77" s="12"/>
+      <c r="AW77" s="13"/>
+    </row>
+    <row r="78" spans="30:49" ht="14.25" thickBot="1">
+      <c r="AD78" s="14"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+      <c r="AI78" s="15"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="15"/>
+      <c r="AL78" s="15"/>
+      <c r="AM78" s="16"/>
+      <c r="AN78" s="14"/>
+      <c r="AO78" s="15"/>
+      <c r="AP78" s="15"/>
+      <c r="AQ78" s="15"/>
+      <c r="AR78" s="15"/>
+      <c r="AS78" s="15"/>
+      <c r="AT78" s="15"/>
+      <c r="AU78" s="15"/>
+      <c r="AV78" s="15"/>
+      <c r="AW78" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
sprite ok on the test rom.
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="display" sheetId="3" r:id="rId3"/>
     <sheet name="motones vga" sheetId="4" r:id="rId4"/>
     <sheet name="pattern fetch" sheetId="5" r:id="rId5"/>
+    <sheet name="vram access" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="144">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -496,6 +497,14 @@
   </si>
   <si>
     <t>D6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name table write</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sprite pattern read</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -992,30 +1001,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1036,6 +1021,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3454,46 +3463,6 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>8282</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>49696</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>103533</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>154472</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="207065" y="5093805"/>
-          <a:ext cx="12486033" cy="5148884"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
@@ -3604,27 +3573,126 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="419100" y="6619875"/>
+          <a:ext cx="12801600" cy="7010400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="371475"/>
+          <a:ext cx="12801600" cy="7010400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>124241</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>66262</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>382244</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>173936</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>91112</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>120513</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>24436</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="角丸四角形吹き出し 5"/>
+        <xdr:cNvPr id="3" name="角丸四角形吹き出し 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6485284" y="8067262"/>
+          <a:off x="5868644" y="4792732"/>
           <a:ext cx="1109869" cy="546654"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
@@ -3670,31 +3738,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>110987</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>102706</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>302730</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>136664</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>99392</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>135835</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>509795</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="角丸四角形吹き出し 6"/>
+        <xdr:cNvPr id="4" name="角丸四角形吹き出し 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4881770" y="9669119"/>
-          <a:ext cx="1578665" cy="380999"/>
+          <a:off x="4417530" y="6308864"/>
+          <a:ext cx="1578665" cy="577711"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -55254"/>
-            <a:gd name="adj2" fmla="val -143164"/>
+            <a:gd name="adj1" fmla="val -51634"/>
+            <a:gd name="adj2" fmla="val -120082"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -3720,7 +3788,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>data 45 written @ 203C</a:t>
+            <a:t>data 45 is written @ 203B</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -3730,25 +3798,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>106017</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>64605</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>551622</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>33959</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>140804</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>24847</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>29817</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>6625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="角丸四角形吹き出し 8"/>
+        <xdr:cNvPr id="5" name="角丸四角形吹き出し 4"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6930887" y="9109214"/>
+          <a:off x="7409622" y="5691809"/>
           <a:ext cx="2221395" cy="829916"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
@@ -3807,31 +3875,91 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>188844</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>89454</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>106017</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>122584</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>320538</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>46797</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="角丸四角形吹き出し 9"/>
+        <xdr:cNvPr id="6" name="角丸四角形吹き出し 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3170583" y="8960128"/>
+          <a:off x="1952626" y="5666548"/>
+          <a:ext cx="1796912" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40930"/>
+            <a:gd name="adj2" fmla="val -455448"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>addr is already latched</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>376444</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="角丸四角形吹き出し 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7496175" y="12277725"/>
           <a:ext cx="1109869" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -57235"/>
-            <a:gd name="adj2" fmla="val -427948"/>
+            <a:gd name="adj1" fmla="val 54332"/>
+            <a:gd name="adj2" fmla="val -180447"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -3858,6 +3986,70 @@
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>addr is latched</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>500269</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="角丸四角形吹き出し 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8991600" y="12887325"/>
+          <a:ext cx="1109869" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -41787"/>
+            <a:gd name="adj2" fmla="val -222947"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> read</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -4253,10 +4445,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -4264,8 +4456,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
@@ -4304,10 +4496,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="49" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -4315,8 +4507,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
@@ -4455,10 +4647,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="49" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -4466,8 +4658,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
@@ -4495,10 +4687,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="49" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -4506,8 +4698,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="6" t="s">
         <v>57</v>
       </c>
@@ -4607,22 +4799,22 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="49" t="s">
         <v>62</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="42" t="s">
+      <c r="C47" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" thickBot="1">
-      <c r="A48" s="43"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="43"/>
+      <c r="C48" s="50"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="2" t="s">
@@ -4646,22 +4838,22 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="49" t="s">
         <v>62</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="42" t="s">
+      <c r="C52" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" thickBot="1">
-      <c r="A53" s="43"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="43"/>
+      <c r="C53" s="50"/>
     </row>
     <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="2" t="s">
@@ -4685,31 +4877,25 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25">
-      <c r="A57" s="42" t="s">
+      <c r="A57" s="49" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1">
-      <c r="A58" s="43"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="43"/>
+      <c r="C58" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -4718,6 +4904,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4729,7 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:BX117"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -9469,62 +9661,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="44" t="s">
+      <c r="K33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44" t="s">
+      <c r="L33" s="51"/>
+      <c r="M33" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="44"/>
-      <c r="O33" s="44" t="s">
+      <c r="N33" s="51"/>
+      <c r="O33" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44" t="s">
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44" t="s">
+      <c r="R33" s="51"/>
+      <c r="S33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="44"/>
-      <c r="U33" s="44" t="s">
+      <c r="T33" s="51"/>
+      <c r="U33" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="44"/>
-      <c r="W33" s="44" t="s">
+      <c r="V33" s="51"/>
+      <c r="W33" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="44"/>
-      <c r="Y33" s="44" t="s">
+      <c r="X33" s="51"/>
+      <c r="Y33" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="44"/>
-      <c r="AA33" s="44" t="s">
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="44"/>
+      <c r="AB33" s="51"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="44" t="s">
+      <c r="AG33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="44"/>
-      <c r="AI33" s="44" t="s">
+      <c r="AH33" s="51"/>
+      <c r="AI33" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="44"/>
-      <c r="AK33" s="44" t="s">
+      <c r="AJ33" s="51"/>
+      <c r="AK33" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="44"/>
-      <c r="AM33" s="44" t="s">
+      <c r="AL33" s="51"/>
+      <c r="AM33" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="44"/>
+      <c r="AN33" s="51"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -9541,50 +9733,50 @@
       <c r="BD33" s="34"/>
       <c r="BF33" s="34"/>
       <c r="BG33" s="34"/>
-      <c r="BI33" s="44" t="s">
+      <c r="BI33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BJ33" s="44"/>
-      <c r="BK33" s="44" t="s">
+      <c r="BJ33" s="51"/>
+      <c r="BK33" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BL33" s="44"/>
-      <c r="BM33" s="44" t="s">
+      <c r="BL33" s="51"/>
+      <c r="BM33" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BN33" s="44"/>
-      <c r="BO33" s="44" t="s">
+      <c r="BN33" s="51"/>
+      <c r="BO33" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BP33" s="44"/>
-      <c r="BQ33" s="44" t="s">
+      <c r="BP33" s="51"/>
+      <c r="BQ33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BR33" s="44"/>
-      <c r="BS33" s="44" t="s">
+      <c r="BR33" s="51"/>
+      <c r="BS33" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BT33" s="44"/>
-      <c r="BU33" s="44" t="s">
+      <c r="BT33" s="51"/>
+      <c r="BU33" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BV33" s="44"/>
-      <c r="BW33" s="44" t="s">
+      <c r="BV33" s="51"/>
+      <c r="BW33" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BX33" s="44"/>
-      <c r="BY33" s="44" t="s">
+      <c r="BX33" s="51"/>
+      <c r="BY33" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BZ33" s="44"/>
-      <c r="CA33" s="44" t="s">
+      <c r="BZ33" s="51"/>
+      <c r="CA33" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="CB33" s="44"/>
-      <c r="CC33" s="44" t="s">
+      <c r="CB33" s="51"/>
+      <c r="CC33" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="CD33" s="44"/>
+      <c r="CD33" s="51"/>
       <c r="CE33" s="41" t="s">
         <v>121</v>
       </c>
@@ -9595,62 +9787,62 @@
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="44" t="s">
+      <c r="K34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="44"/>
-      <c r="M34" s="44" t="s">
+      <c r="L34" s="51"/>
+      <c r="M34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="44"/>
-      <c r="O34" s="44" t="s">
+      <c r="N34" s="51"/>
+      <c r="O34" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="44"/>
-      <c r="Q34" s="44" t="s">
+      <c r="P34" s="51"/>
+      <c r="Q34" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="44"/>
-      <c r="S34" s="44" t="s">
+      <c r="R34" s="51"/>
+      <c r="S34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="44"/>
-      <c r="U34" s="44" t="s">
+      <c r="T34" s="51"/>
+      <c r="U34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="44"/>
-      <c r="W34" s="44" t="s">
+      <c r="V34" s="51"/>
+      <c r="W34" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="44"/>
-      <c r="Y34" s="44" t="s">
+      <c r="X34" s="51"/>
+      <c r="Y34" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="44"/>
-      <c r="AA34" s="44" t="s">
+      <c r="Z34" s="51"/>
+      <c r="AA34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="44"/>
+      <c r="AB34" s="51"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="44" t="s">
+      <c r="AG34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="44"/>
-      <c r="AI34" s="44" t="s">
+      <c r="AH34" s="51"/>
+      <c r="AI34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="44"/>
-      <c r="AK34" s="44" t="s">
+      <c r="AJ34" s="51"/>
+      <c r="AK34" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="44"/>
-      <c r="AM34" s="44" t="s">
+      <c r="AL34" s="51"/>
+      <c r="AM34" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="44"/>
+      <c r="AN34" s="51"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -9667,50 +9859,50 @@
       <c r="BD34" s="34"/>
       <c r="BF34" s="34"/>
       <c r="BG34" s="34"/>
-      <c r="BI34" s="44" t="s">
+      <c r="BI34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BJ34" s="44"/>
-      <c r="BK34" s="44" t="s">
+      <c r="BJ34" s="51"/>
+      <c r="BK34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BL34" s="44"/>
-      <c r="BM34" s="44" t="s">
+      <c r="BL34" s="51"/>
+      <c r="BM34" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BN34" s="44"/>
-      <c r="BO34" s="44" t="s">
+      <c r="BN34" s="51"/>
+      <c r="BO34" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BP34" s="44"/>
-      <c r="BQ34" s="44" t="s">
+      <c r="BP34" s="51"/>
+      <c r="BQ34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BR34" s="44"/>
-      <c r="BS34" s="44" t="s">
+      <c r="BR34" s="51"/>
+      <c r="BS34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BT34" s="44"/>
-      <c r="BU34" s="44" t="s">
+      <c r="BT34" s="51"/>
+      <c r="BU34" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BV34" s="44"/>
-      <c r="BW34" s="44" t="s">
+      <c r="BV34" s="51"/>
+      <c r="BW34" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BX34" s="44"/>
-      <c r="BY34" s="44" t="s">
+      <c r="BX34" s="51"/>
+      <c r="BY34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BZ34" s="44"/>
-      <c r="CA34" s="44" t="s">
+      <c r="BZ34" s="51"/>
+      <c r="CA34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="CB34" s="44"/>
-      <c r="CC34" s="44" t="s">
+      <c r="CB34" s="51"/>
+      <c r="CC34" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="CD34" s="44"/>
+      <c r="CD34" s="51"/>
       <c r="CE34" s="41" t="s">
         <v>121</v>
       </c>
@@ -9728,62 +9920,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="45" t="s">
+      <c r="K36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45" t="s">
+      <c r="L36" s="56"/>
+      <c r="M36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45" t="s">
+      <c r="N36" s="56"/>
+      <c r="O36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45" t="s">
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45" t="s">
+      <c r="R36" s="56"/>
+      <c r="S36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45" t="s">
+      <c r="T36" s="56"/>
+      <c r="U36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="45"/>
-      <c r="W36" s="45" t="s">
+      <c r="V36" s="56"/>
+      <c r="W36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="45" t="s">
+      <c r="X36" s="56"/>
+      <c r="Y36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="45"/>
-      <c r="AA36" s="45" t="s">
+      <c r="Z36" s="56"/>
+      <c r="AA36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="45"/>
+      <c r="AB36" s="56"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="45" t="s">
+      <c r="AG36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="45"/>
-      <c r="AI36" s="45" t="s">
+      <c r="AH36" s="56"/>
+      <c r="AI36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="45"/>
-      <c r="AK36" s="45" t="s">
+      <c r="AJ36" s="56"/>
+      <c r="AK36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="45"/>
-      <c r="AM36" s="45" t="s">
+      <c r="AL36" s="56"/>
+      <c r="AM36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="45"/>
+      <c r="AN36" s="56"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -9800,50 +9992,50 @@
       <c r="BD36" s="36"/>
       <c r="BF36" s="34"/>
       <c r="BG36" s="34"/>
-      <c r="BI36" s="44" t="s">
+      <c r="BI36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BJ36" s="44"/>
-      <c r="BK36" s="44" t="s">
+      <c r="BJ36" s="51"/>
+      <c r="BK36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BL36" s="44"/>
-      <c r="BM36" s="44" t="s">
+      <c r="BL36" s="51"/>
+      <c r="BM36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BN36" s="44"/>
-      <c r="BO36" s="44" t="s">
+      <c r="BN36" s="51"/>
+      <c r="BO36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BP36" s="44"/>
-      <c r="BQ36" s="44" t="s">
+      <c r="BP36" s="51"/>
+      <c r="BQ36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BR36" s="44"/>
-      <c r="BS36" s="44" t="s">
+      <c r="BR36" s="51"/>
+      <c r="BS36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BT36" s="44"/>
-      <c r="BU36" s="44" t="s">
+      <c r="BT36" s="51"/>
+      <c r="BU36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BV36" s="44"/>
-      <c r="BW36" s="44" t="s">
+      <c r="BV36" s="51"/>
+      <c r="BW36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BX36" s="44"/>
-      <c r="BY36" s="44" t="s">
+      <c r="BX36" s="51"/>
+      <c r="BY36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BZ36" s="44"/>
-      <c r="CA36" s="44" t="s">
+      <c r="BZ36" s="51"/>
+      <c r="CA36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="CB36" s="44"/>
-      <c r="CC36" s="44" t="s">
+      <c r="CB36" s="51"/>
+      <c r="CC36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="CD36" s="44"/>
+      <c r="CD36" s="51"/>
       <c r="CE36" s="41" t="s">
         <v>121</v>
       </c>
@@ -10183,58 +10375,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="44" t="s">
+      <c r="M42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="44"/>
-      <c r="O42" s="44" t="s">
+      <c r="N42" s="51"/>
+      <c r="O42" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44" t="s">
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="44"/>
-      <c r="S42" s="44" t="s">
+      <c r="R42" s="51"/>
+      <c r="S42" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="44"/>
-      <c r="U42" s="44" t="s">
+      <c r="T42" s="51"/>
+      <c r="U42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="44"/>
-      <c r="W42" s="44" t="s">
+      <c r="V42" s="51"/>
+      <c r="W42" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="44"/>
-      <c r="Y42" s="44" t="s">
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="44"/>
-      <c r="AA42" s="44" t="s">
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="44"/>
+      <c r="AB42" s="51"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="44" t="s">
+      <c r="AG42" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="44"/>
-      <c r="AI42" s="44" t="s">
+      <c r="AH42" s="51"/>
+      <c r="AI42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="44"/>
-      <c r="AK42" s="44" t="s">
+      <c r="AJ42" s="51"/>
+      <c r="AK42" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="44"/>
-      <c r="AM42" s="44" t="s">
+      <c r="AL42" s="51"/>
+      <c r="AM42" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="44"/>
+      <c r="AN42" s="51"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -10251,50 +10443,50 @@
       <c r="BD42" s="34"/>
       <c r="BF42" s="34"/>
       <c r="BG42" s="34"/>
-      <c r="BI42" s="44" t="s">
+      <c r="BI42" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BJ42" s="44"/>
-      <c r="BK42" s="44" t="s">
+      <c r="BJ42" s="51"/>
+      <c r="BK42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BL42" s="44"/>
-      <c r="BM42" s="44" t="s">
+      <c r="BL42" s="51"/>
+      <c r="BM42" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BN42" s="44"/>
-      <c r="BO42" s="44" t="s">
+      <c r="BN42" s="51"/>
+      <c r="BO42" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BP42" s="44"/>
-      <c r="BQ42" s="44" t="s">
+      <c r="BP42" s="51"/>
+      <c r="BQ42" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BR42" s="44"/>
-      <c r="BS42" s="44" t="s">
+      <c r="BR42" s="51"/>
+      <c r="BS42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="BT42" s="44"/>
-      <c r="BU42" s="44" t="s">
+      <c r="BT42" s="51"/>
+      <c r="BU42" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="BV42" s="44"/>
-      <c r="BW42" s="44" t="s">
+      <c r="BV42" s="51"/>
+      <c r="BW42" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="BX42" s="44"/>
-      <c r="BY42" s="44" t="s">
+      <c r="BX42" s="51"/>
+      <c r="BY42" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="BZ42" s="44"/>
-      <c r="CA42" s="44" t="s">
+      <c r="BZ42" s="51"/>
+      <c r="CA42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="CB42" s="44"/>
-      <c r="CC42" s="44" t="s">
+      <c r="CB42" s="51"/>
+      <c r="CC42" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="CD42" s="44"/>
+      <c r="CD42" s="51"/>
       <c r="CE42" s="41" t="s">
         <v>121</v>
       </c>
@@ -10332,71 +10524,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="49" t="s">
+      <c r="K46" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="49"/>
-      <c r="M46" s="49"/>
-      <c r="N46" s="49"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="49"/>
-      <c r="R46" s="49"/>
-      <c r="S46" s="49"/>
-      <c r="T46" s="49"/>
-      <c r="U46" s="49"/>
-      <c r="V46" s="49"/>
-      <c r="W46" s="49"/>
-      <c r="X46" s="49"/>
-      <c r="Y46" s="49"/>
-      <c r="Z46" s="49"/>
-      <c r="AA46" s="49"/>
-      <c r="AB46" s="49"/>
-      <c r="AC46" s="49"/>
-      <c r="AD46" s="49"/>
-      <c r="AE46" s="49" t="s">
+      <c r="L46" s="55"/>
+      <c r="M46" s="55"/>
+      <c r="N46" s="55"/>
+      <c r="O46" s="55"/>
+      <c r="P46" s="55"/>
+      <c r="Q46" s="55"/>
+      <c r="R46" s="55"/>
+      <c r="S46" s="55"/>
+      <c r="T46" s="55"/>
+      <c r="U46" s="55"/>
+      <c r="V46" s="55"/>
+      <c r="W46" s="55"/>
+      <c r="X46" s="55"/>
+      <c r="Y46" s="55"/>
+      <c r="Z46" s="55"/>
+      <c r="AA46" s="55"/>
+      <c r="AB46" s="55"/>
+      <c r="AC46" s="55"/>
+      <c r="AD46" s="55"/>
+      <c r="AE46" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="49"/>
-      <c r="AG46" s="49"/>
-      <c r="AH46" s="49"/>
-      <c r="AI46" s="49"/>
-      <c r="AJ46" s="49"/>
-      <c r="AK46" s="49"/>
-      <c r="AL46" s="49"/>
-      <c r="AM46" s="49"/>
-      <c r="AN46" s="49"/>
-      <c r="AO46" s="44" t="s">
+      <c r="AF46" s="55"/>
+      <c r="AG46" s="55"/>
+      <c r="AH46" s="55"/>
+      <c r="AI46" s="55"/>
+      <c r="AJ46" s="55"/>
+      <c r="AK46" s="55"/>
+      <c r="AL46" s="55"/>
+      <c r="AM46" s="55"/>
+      <c r="AN46" s="55"/>
+      <c r="AO46" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="44"/>
-      <c r="AQ46" s="44" t="s">
+      <c r="AP46" s="51"/>
+      <c r="AQ46" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="44"/>
-      <c r="AS46" s="44" t="s">
+      <c r="AR46" s="51"/>
+      <c r="AS46" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="44"/>
-      <c r="AU46" s="44" t="s">
+      <c r="AT46" s="51"/>
+      <c r="AU46" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="44"/>
-      <c r="AW46" s="46" t="s">
+      <c r="AV46" s="51"/>
+      <c r="AW46" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="47"/>
-      <c r="AY46" s="47"/>
-      <c r="AZ46" s="47"/>
-      <c r="BA46" s="47"/>
-      <c r="BB46" s="47"/>
-      <c r="BC46" s="47"/>
-      <c r="BD46" s="47"/>
-      <c r="BE46" s="48"/>
-      <c r="BF46" s="44" t="s">
+      <c r="AX46" s="53"/>
+      <c r="AY46" s="53"/>
+      <c r="AZ46" s="53"/>
+      <c r="BA46" s="53"/>
+      <c r="BB46" s="53"/>
+      <c r="BC46" s="53"/>
+      <c r="BD46" s="53"/>
+      <c r="BE46" s="54"/>
+      <c r="BF46" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="44"/>
+      <c r="BG46" s="51"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -13958,74 +14150,20 @@
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BK42:BL42"/>
-    <mergeCell ref="BM42:BN42"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="BK36:BL36"/>
-    <mergeCell ref="BM36:BN36"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BY36:BZ36"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BK33:BL33"/>
-    <mergeCell ref="BM33:BN33"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BK34:BL34"/>
-    <mergeCell ref="BM34:BN34"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BI42:BJ42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="BI36:BJ36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="BI33:BJ33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U33:V33"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="O36:P36"/>
@@ -14047,20 +14185,74 @@
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="BI33:BJ33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="BI42:BJ42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="BI36:BJ36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="BK33:BL33"/>
+    <mergeCell ref="BM33:BN33"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BK34:BL34"/>
+    <mergeCell ref="BM34:BN34"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BK42:BL42"/>
+    <mergeCell ref="BM42:BN42"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="BK36:BL36"/>
+    <mergeCell ref="BM36:BN36"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BY36:BZ36"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14072,8 +14264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="G2:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AM25" sqref="AM25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -14126,28 +14318,28 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="52"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="44"/>
     </row>
     <row r="7" spans="9:25">
       <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="51"/>
-      <c r="U7" s="52"/>
-      <c r="Y7" s="50" t="s">
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="44"/>
+      <c r="Y7" s="42" t="s">
         <v>128</v>
       </c>
     </row>
@@ -14155,15 +14347,15 @@
       <c r="M8">
         <v>2</v>
       </c>
-      <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="52"/>
-      <c r="Y8" s="52" t="s">
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="44"/>
+      <c r="Y8" s="44" t="s">
         <v>129</v>
       </c>
     </row>
@@ -14171,15 +14363,15 @@
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="52"/>
-      <c r="Y9" s="53" t="s">
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="44"/>
+      <c r="Y9" s="45" t="s">
         <v>130</v>
       </c>
     </row>
@@ -14187,15 +14379,15 @@
       <c r="M10">
         <v>4</v>
       </c>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="51"/>
-      <c r="T10" s="51"/>
-      <c r="U10" s="52"/>
-      <c r="Y10" s="51" t="s">
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="44"/>
+      <c r="Y10" s="43" t="s">
         <v>131</v>
       </c>
     </row>
@@ -14203,46 +14395,46 @@
       <c r="M11">
         <v>5</v>
       </c>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="52"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="44"/>
     </row>
     <row r="12" spans="9:25">
       <c r="M12">
         <v>6</v>
       </c>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="52"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="44"/>
     </row>
     <row r="13" spans="9:25">
       <c r="M13">
         <v>7</v>
       </c>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
     </row>
     <row r="18" spans="7:34">
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="Y18" s="54" t="s">
+      <c r="Y18" s="46" t="s">
         <v>138</v>
       </c>
     </row>
@@ -14300,29 +14492,29 @@
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
       <c r="P20" t="s">
         <v>132</v>
       </c>
       <c r="Y20">
         <v>0</v>
       </c>
-      <c r="Z20" s="53"/>
-      <c r="AA20" s="53"/>
-      <c r="AB20" s="50"/>
-      <c r="AC20" s="50"/>
-      <c r="AD20" s="50"/>
-      <c r="AE20" s="53"/>
-      <c r="AF20" s="53"/>
-      <c r="AG20" s="50"/>
-      <c r="AH20" s="55" t="s">
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="45"/>
+      <c r="AB20" s="42"/>
+      <c r="AC20" s="42"/>
+      <c r="AD20" s="42"/>
+      <c r="AE20" s="45"/>
+      <c r="AF20" s="45"/>
+      <c r="AG20" s="42"/>
+      <c r="AH20" s="47" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14330,29 +14522,29 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
-      <c r="O21" s="52"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
       <c r="P21" t="s">
         <v>132</v>
       </c>
       <c r="Y21">
         <v>1</v>
       </c>
-      <c r="Z21" s="53"/>
-      <c r="AA21" s="53"/>
-      <c r="AB21" s="50"/>
-      <c r="AC21" s="50"/>
-      <c r="AD21" s="50"/>
-      <c r="AE21" s="53"/>
-      <c r="AF21" s="53"/>
-      <c r="AG21" s="50"/>
-      <c r="AH21" s="55" t="s">
+      <c r="Z21" s="45"/>
+      <c r="AA21" s="45"/>
+      <c r="AB21" s="42"/>
+      <c r="AC21" s="42"/>
+      <c r="AD21" s="42"/>
+      <c r="AE21" s="45"/>
+      <c r="AF21" s="45"/>
+      <c r="AG21" s="42"/>
+      <c r="AH21" s="47" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14360,29 +14552,29 @@
       <c r="G22">
         <v>2</v>
       </c>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
       <c r="P22" t="s">
         <v>133</v>
       </c>
       <c r="Y22">
         <v>2</v>
       </c>
-      <c r="Z22" s="53"/>
-      <c r="AA22" s="53"/>
-      <c r="AB22" s="53"/>
-      <c r="AC22" s="50"/>
-      <c r="AD22" s="53"/>
-      <c r="AE22" s="53"/>
-      <c r="AF22" s="53"/>
-      <c r="AG22" s="50"/>
-      <c r="AH22" s="55" t="s">
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="45"/>
+      <c r="AB22" s="45"/>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="45"/>
+      <c r="AE22" s="45"/>
+      <c r="AF22" s="45"/>
+      <c r="AG22" s="42"/>
+      <c r="AH22" s="47" t="s">
         <v>140</v>
       </c>
     </row>
@@ -14390,29 +14582,29 @@
       <c r="G23">
         <v>3</v>
       </c>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
       <c r="P23" t="s">
         <v>133</v>
       </c>
       <c r="Y23">
         <v>3</v>
       </c>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="53"/>
-      <c r="AD23" s="50"/>
-      <c r="AE23" s="53"/>
-      <c r="AF23" s="53"/>
-      <c r="AG23" s="50"/>
-      <c r="AH23" s="55" t="s">
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="42"/>
+      <c r="AC23" s="45"/>
+      <c r="AD23" s="42"/>
+      <c r="AE23" s="45"/>
+      <c r="AF23" s="45"/>
+      <c r="AG23" s="42"/>
+      <c r="AH23" s="47" t="s">
         <v>141</v>
       </c>
     </row>
@@ -14420,29 +14612,29 @@
       <c r="G24">
         <v>4</v>
       </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
       <c r="P24" t="s">
         <v>133</v>
       </c>
       <c r="Y24">
         <v>4</v>
       </c>
-      <c r="Z24" s="53"/>
-      <c r="AA24" s="53"/>
-      <c r="AB24" s="50"/>
-      <c r="AC24" s="50"/>
-      <c r="AD24" s="50"/>
-      <c r="AE24" s="53"/>
-      <c r="AF24" s="53"/>
-      <c r="AG24" s="50"/>
-      <c r="AH24" s="55" t="s">
+      <c r="Z24" s="45"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="45"/>
+      <c r="AF24" s="45"/>
+      <c r="AG24" s="42"/>
+      <c r="AH24" s="47" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14450,29 +14642,29 @@
       <c r="G25">
         <v>5</v>
       </c>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
       <c r="P25" t="s">
         <v>132</v>
       </c>
       <c r="Y25">
         <v>5</v>
       </c>
-      <c r="Z25" s="53"/>
-      <c r="AA25" s="53"/>
-      <c r="AB25" s="50"/>
-      <c r="AC25" s="50"/>
-      <c r="AD25" s="50"/>
-      <c r="AE25" s="53"/>
-      <c r="AF25" s="53"/>
-      <c r="AG25" s="50"/>
-      <c r="AH25" s="55" t="s">
+      <c r="Z25" s="45"/>
+      <c r="AA25" s="45"/>
+      <c r="AB25" s="42"/>
+      <c r="AC25" s="42"/>
+      <c r="AD25" s="42"/>
+      <c r="AE25" s="45"/>
+      <c r="AF25" s="45"/>
+      <c r="AG25" s="42"/>
+      <c r="AH25" s="47" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14480,29 +14672,29 @@
       <c r="G26">
         <v>6</v>
       </c>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="52"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
       <c r="P26" t="s">
         <v>132</v>
       </c>
       <c r="Y26">
         <v>6</v>
       </c>
-      <c r="Z26" s="53"/>
-      <c r="AA26" s="53"/>
-      <c r="AB26" s="50"/>
-      <c r="AC26" s="50"/>
-      <c r="AD26" s="50"/>
-      <c r="AE26" s="53"/>
-      <c r="AF26" s="53"/>
-      <c r="AG26" s="50"/>
-      <c r="AH26" s="55" t="s">
+      <c r="Z26" s="45"/>
+      <c r="AA26" s="45"/>
+      <c r="AB26" s="42"/>
+      <c r="AC26" s="42"/>
+      <c r="AD26" s="42"/>
+      <c r="AE26" s="45"/>
+      <c r="AF26" s="45"/>
+      <c r="AG26" s="42"/>
+      <c r="AH26" s="47" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14510,30 +14702,57 @@
       <c r="G27">
         <v>7</v>
       </c>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
       <c r="P27" t="s">
         <v>132</v>
       </c>
       <c r="Y27">
         <v>7</v>
       </c>
-      <c r="Z27" s="50"/>
-      <c r="AA27" s="50"/>
-      <c r="AB27" s="50"/>
-      <c r="AC27" s="50"/>
-      <c r="AD27" s="50"/>
-      <c r="AE27" s="50"/>
-      <c r="AF27" s="50"/>
-      <c r="AG27" s="50"/>
-      <c r="AH27" s="56" t="s">
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="42"/>
+      <c r="AC27" s="42"/>
+      <c r="AD27" s="42"/>
+      <c r="AE27" s="42"/>
+      <c r="AF27" s="42"/>
+      <c r="AG27" s="42"/>
+      <c r="AH27" s="48" t="s">
         <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:B50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="T71" sqref="T71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sprite next line bug working..
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="154">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -505,6 +505,46 @@
   </si>
   <si>
     <t>sprite pattern read</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>@0x04f0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>@0x04f8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on y=6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on y=7</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1031,6 +1071,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1041,9 +1084,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4057,6 +4097,147 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="638175" y="16773525"/>
+          <a:ext cx="12868275" cy="7715250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2053" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13716000" y="16802100"/>
+          <a:ext cx="12868275" cy="7715250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2054" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13716000" y="24860250"/>
+          <a:ext cx="12868275" cy="7715250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4896,6 +5077,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -4904,12 +5091,6 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9920,62 +10101,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="56" t="s">
+      <c r="K36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56" t="s">
+      <c r="L36" s="52"/>
+      <c r="M36" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56" t="s">
+      <c r="N36" s="52"/>
+      <c r="O36" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56" t="s">
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56" t="s">
+      <c r="R36" s="52"/>
+      <c r="S36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56" t="s">
+      <c r="T36" s="52"/>
+      <c r="U36" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="56"/>
-      <c r="W36" s="56" t="s">
+      <c r="V36" s="52"/>
+      <c r="W36" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="56"/>
-      <c r="Y36" s="56" t="s">
+      <c r="X36" s="52"/>
+      <c r="Y36" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="56"/>
-      <c r="AA36" s="56" t="s">
+      <c r="Z36" s="52"/>
+      <c r="AA36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="56"/>
+      <c r="AB36" s="52"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="56" t="s">
+      <c r="AG36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="56"/>
-      <c r="AI36" s="56" t="s">
+      <c r="AH36" s="52"/>
+      <c r="AI36" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="56"/>
-      <c r="AK36" s="56" t="s">
+      <c r="AJ36" s="52"/>
+      <c r="AK36" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="56"/>
-      <c r="AM36" s="56" t="s">
+      <c r="AL36" s="52"/>
+      <c r="AM36" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="56"/>
+      <c r="AN36" s="52"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -10524,40 +10705,40 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="55" t="s">
+      <c r="K46" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="55"/>
-      <c r="M46" s="55"/>
-      <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="P46" s="55"/>
-      <c r="Q46" s="55"/>
-      <c r="R46" s="55"/>
-      <c r="S46" s="55"/>
-      <c r="T46" s="55"/>
-      <c r="U46" s="55"/>
-      <c r="V46" s="55"/>
-      <c r="W46" s="55"/>
-      <c r="X46" s="55"/>
-      <c r="Y46" s="55"/>
-      <c r="Z46" s="55"/>
-      <c r="AA46" s="55"/>
-      <c r="AB46" s="55"/>
-      <c r="AC46" s="55"/>
-      <c r="AD46" s="55"/>
-      <c r="AE46" s="55" t="s">
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="56"/>
+      <c r="U46" s="56"/>
+      <c r="V46" s="56"/>
+      <c r="W46" s="56"/>
+      <c r="X46" s="56"/>
+      <c r="Y46" s="56"/>
+      <c r="Z46" s="56"/>
+      <c r="AA46" s="56"/>
+      <c r="AB46" s="56"/>
+      <c r="AC46" s="56"/>
+      <c r="AD46" s="56"/>
+      <c r="AE46" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="55"/>
-      <c r="AG46" s="55"/>
-      <c r="AH46" s="55"/>
-      <c r="AI46" s="55"/>
-      <c r="AJ46" s="55"/>
-      <c r="AK46" s="55"/>
-      <c r="AL46" s="55"/>
-      <c r="AM46" s="55"/>
-      <c r="AN46" s="55"/>
+      <c r="AF46" s="56"/>
+      <c r="AG46" s="56"/>
+      <c r="AH46" s="56"/>
+      <c r="AI46" s="56"/>
+      <c r="AJ46" s="56"/>
+      <c r="AK46" s="56"/>
+      <c r="AL46" s="56"/>
+      <c r="AM46" s="56"/>
+      <c r="AN46" s="56"/>
       <c r="AO46" s="51" t="s">
         <v>111</v>
       </c>
@@ -10574,17 +10755,17 @@
         <v>118</v>
       </c>
       <c r="AV46" s="51"/>
-      <c r="AW46" s="52" t="s">
+      <c r="AW46" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="53"/>
-      <c r="AY46" s="53"/>
-      <c r="AZ46" s="53"/>
-      <c r="BA46" s="53"/>
-      <c r="BB46" s="53"/>
-      <c r="BC46" s="53"/>
-      <c r="BD46" s="53"/>
-      <c r="BE46" s="54"/>
+      <c r="AX46" s="54"/>
+      <c r="AY46" s="54"/>
+      <c r="AZ46" s="54"/>
+      <c r="BA46" s="54"/>
+      <c r="BB46" s="54"/>
+      <c r="BC46" s="54"/>
+      <c r="BD46" s="54"/>
+      <c r="BE46" s="55"/>
       <c r="BF46" s="51" t="s">
         <v>118</v>
       </c>
@@ -14150,20 +14331,74 @@
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="BI33:BJ33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BK42:BL42"/>
+    <mergeCell ref="BM42:BN42"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="BK36:BL36"/>
+    <mergeCell ref="BM36:BN36"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="BK33:BL33"/>
+    <mergeCell ref="BM33:BN33"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BK34:BL34"/>
+    <mergeCell ref="BM34:BN34"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BI42:BJ42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="BI36:BJ36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="AI36:AJ36"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="O36:P36"/>
@@ -14185,74 +14420,20 @@
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="BI42:BJ42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="BI36:BJ36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BK33:BL33"/>
-    <mergeCell ref="BM33:BN33"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BK34:BL34"/>
-    <mergeCell ref="BM34:BN34"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BK42:BL42"/>
-    <mergeCell ref="BM42:BN42"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="BK36:BL36"/>
-    <mergeCell ref="BM36:BN36"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="BI33:BJ33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U33:V33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14262,10 +14443,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="G2:AH27"/>
+  <dimension ref="G2:AW27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -14275,17 +14456,17 @@
     <col min="34" max="34" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:25">
+    <row r="2" spans="9:49">
       <c r="I2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="9:25">
+    <row r="3" spans="9:49">
       <c r="I3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="9:25">
+    <row r="5" spans="9:49">
       <c r="N5">
         <v>7</v>
       </c>
@@ -14310,8 +14491,32 @@
       <c r="U5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="9:25">
+      <c r="AP5">
+        <v>7</v>
+      </c>
+      <c r="AQ5">
+        <v>6</v>
+      </c>
+      <c r="AR5">
+        <v>5</v>
+      </c>
+      <c r="AS5">
+        <v>4</v>
+      </c>
+      <c r="AT5">
+        <v>3</v>
+      </c>
+      <c r="AU5">
+        <v>2</v>
+      </c>
+      <c r="AV5">
+        <v>1</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="9:49">
       <c r="I6" t="s">
         <v>134</v>
       </c>
@@ -14326,8 +14531,19 @@
       <c r="S6" s="43"/>
       <c r="T6" s="43"/>
       <c r="U6" s="44"/>
-    </row>
-    <row r="7" spans="9:25">
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="42"/>
+      <c r="AQ6" s="43"/>
+      <c r="AR6" s="43"/>
+      <c r="AS6" s="43"/>
+      <c r="AT6" s="43"/>
+      <c r="AU6" s="43"/>
+      <c r="AV6" s="44"/>
+      <c r="AW6" s="42"/>
+    </row>
+    <row r="7" spans="9:49">
       <c r="M7">
         <v>1</v>
       </c>
@@ -14342,8 +14558,19 @@
       <c r="Y7" s="42" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="8" spans="9:25">
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="43"/>
+      <c r="AQ7" s="43"/>
+      <c r="AR7" s="44"/>
+      <c r="AS7" s="44"/>
+      <c r="AT7" s="44"/>
+      <c r="AU7" s="43"/>
+      <c r="AV7" s="43"/>
+      <c r="AW7" s="44"/>
+    </row>
+    <row r="8" spans="9:49">
       <c r="M8">
         <v>2</v>
       </c>
@@ -14358,8 +14585,19 @@
       <c r="Y8" s="44" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="9:25">
+      <c r="AO8">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="43"/>
+      <c r="AQ8" s="43"/>
+      <c r="AR8" s="44"/>
+      <c r="AS8" s="42"/>
+      <c r="AT8" s="42"/>
+      <c r="AU8" s="43"/>
+      <c r="AV8" s="43"/>
+      <c r="AW8" s="44"/>
+    </row>
+    <row r="9" spans="9:49">
       <c r="M9">
         <v>3</v>
       </c>
@@ -14374,8 +14612,19 @@
       <c r="Y9" s="45" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="9:25">
+      <c r="AO9">
+        <v>3</v>
+      </c>
+      <c r="AP9" s="43"/>
+      <c r="AQ9" s="43"/>
+      <c r="AR9" s="44"/>
+      <c r="AS9" s="42"/>
+      <c r="AT9" s="42"/>
+      <c r="AU9" s="43"/>
+      <c r="AV9" s="43"/>
+      <c r="AW9" s="44"/>
+    </row>
+    <row r="10" spans="9:49">
       <c r="M10">
         <v>4</v>
       </c>
@@ -14390,8 +14639,19 @@
       <c r="Y10" s="43" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="9:25">
+      <c r="AO10">
+        <v>4</v>
+      </c>
+      <c r="AP10" s="43"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="44"/>
+      <c r="AS10" s="42"/>
+      <c r="AT10" s="42"/>
+      <c r="AU10" s="43"/>
+      <c r="AV10" s="43"/>
+      <c r="AW10" s="44"/>
+    </row>
+    <row r="11" spans="9:49">
       <c r="M11">
         <v>5</v>
       </c>
@@ -14403,8 +14663,19 @@
       <c r="S11" s="43"/>
       <c r="T11" s="43"/>
       <c r="U11" s="44"/>
-    </row>
-    <row r="12" spans="9:25">
+      <c r="AO11">
+        <v>5</v>
+      </c>
+      <c r="AP11" s="43"/>
+      <c r="AQ11" s="43"/>
+      <c r="AR11" s="44"/>
+      <c r="AS11" s="42"/>
+      <c r="AT11" s="42"/>
+      <c r="AU11" s="43"/>
+      <c r="AV11" s="43"/>
+      <c r="AW11" s="44"/>
+    </row>
+    <row r="12" spans="9:49">
       <c r="M12">
         <v>6</v>
       </c>
@@ -14416,8 +14687,19 @@
       <c r="S12" s="43"/>
       <c r="T12" s="43"/>
       <c r="U12" s="44"/>
-    </row>
-    <row r="13" spans="9:25">
+      <c r="AO12">
+        <v>6</v>
+      </c>
+      <c r="AP12" s="44"/>
+      <c r="AQ12" s="43"/>
+      <c r="AR12" s="43"/>
+      <c r="AS12" s="43"/>
+      <c r="AT12" s="43"/>
+      <c r="AU12" s="43"/>
+      <c r="AV12" s="44"/>
+      <c r="AW12" s="44"/>
+    </row>
+    <row r="13" spans="9:49">
       <c r="M13">
         <v>7</v>
       </c>
@@ -14429,16 +14711,33 @@
       <c r="S13" s="44"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
-    </row>
-    <row r="18" spans="7:34">
+      <c r="AO13">
+        <v>7</v>
+      </c>
+      <c r="AP13" s="42"/>
+      <c r="AQ13" s="44"/>
+      <c r="AR13" s="44"/>
+      <c r="AS13" s="44"/>
+      <c r="AT13" s="44"/>
+      <c r="AU13" s="44"/>
+      <c r="AV13" s="44"/>
+      <c r="AW13" s="42"/>
+    </row>
+    <row r="18" spans="7:46">
       <c r="G18" s="46" t="s">
         <v>137</v>
       </c>
       <c r="Y18" s="46" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="19" spans="7:34">
+      <c r="AO18" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="AS18" s="46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="7:46">
       <c r="H19">
         <v>7</v>
       </c>
@@ -14488,7 +14787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:34">
+    <row r="20" spans="7:46">
       <c r="G20">
         <v>0</v>
       </c>
@@ -14517,8 +14816,17 @@
       <c r="AH20" s="47" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="21" spans="7:34">
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="7:46">
       <c r="G21">
         <v>1</v>
       </c>
@@ -14547,8 +14855,17 @@
       <c r="AH21" s="47" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="22" spans="7:34">
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="7:46">
       <c r="G22">
         <v>2</v>
       </c>
@@ -14577,8 +14894,17 @@
       <c r="AH22" s="47" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="23" spans="7:34">
+      <c r="AO22">
+        <v>2</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="7:46">
       <c r="G23">
         <v>3</v>
       </c>
@@ -14607,8 +14933,17 @@
       <c r="AH23" s="47" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="24" spans="7:34">
+      <c r="AO23">
+        <v>3</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="7:46">
       <c r="G24">
         <v>4</v>
       </c>
@@ -14637,8 +14972,17 @@
       <c r="AH24" s="47" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="25" spans="7:34">
+      <c r="AO24">
+        <v>4</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="7:46">
       <c r="G25">
         <v>5</v>
       </c>
@@ -14667,8 +15011,17 @@
       <c r="AH25" s="47" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="26" spans="7:34">
+      <c r="AO25">
+        <v>5</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="7:46">
       <c r="G26">
         <v>6</v>
       </c>
@@ -14697,8 +15050,17 @@
       <c r="AH26" s="47" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="27" spans="7:34">
+      <c r="AO26">
+        <v>6</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="7:46">
       <c r="G27">
         <v>7</v>
       </c>
@@ -14727,6 +15089,16 @@
       <c r="AH27" s="48" t="s">
         <v>128</v>
       </c>
+      <c r="AO27">
+        <v>7</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS27" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT27" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -14737,10 +15109,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:B50"/>
+  <dimension ref="B1:B146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="T71" sqref="T71"/>
+    <sheetView tabSelected="1" topLeftCell="Q115" workbookViewId="0">
+      <selection activeCell="U146" sqref="U146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -14755,6 +15127,16 @@
         <v>143</v>
       </c>
     </row>
+    <row r="96" spans="2:2">
+      <c r="B96" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sprite bug fix, but nmi doesn't work in de1-cv...
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -540,11 +540,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>on y=6</t>
+    <t>ale=1 &gt;&gt; latch</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>on y=7</t>
+    <t>ale=0 &gt;&gt; read/write</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1071,9 +1071,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1084,6 +1081,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3620,20 +3620,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="7" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3647,8 +3647,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="419100" y="6619875"/>
-          <a:ext cx="12801600" cy="7010400"/>
+          <a:off x="704850" y="8753475"/>
+          <a:ext cx="12868275" cy="7715250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3975,16 +3975,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>376444</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>624094</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3993,7 +3993,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7496175" y="12277725"/>
+          <a:off x="4314825" y="14801850"/>
           <a:ext cx="1109869" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
@@ -4035,16 +4035,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>500269</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>100219</xdr:colOff>
       <xdr:row>89</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4053,7 +4053,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8991600" y="12887325"/>
+          <a:off x="5848350" y="14916150"/>
           <a:ext cx="1109869" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
@@ -4095,147 +4095,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2050" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="638175" y="16773525"/>
-          <a:ext cx="12868275" cy="7715250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2053" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13716000" y="16802100"/>
-          <a:ext cx="12868275" cy="7715250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>190</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2054" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13716000" y="24860250"/>
-          <a:ext cx="12868275" cy="7715250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5077,12 +4936,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -5091,6 +4944,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10101,62 +9960,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="52" t="s">
+      <c r="K36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="52"/>
-      <c r="M36" s="52" t="s">
+      <c r="L36" s="56"/>
+      <c r="M36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="52"/>
-      <c r="O36" s="52" t="s">
+      <c r="N36" s="56"/>
+      <c r="O36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="52" t="s">
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="52"/>
-      <c r="S36" s="52" t="s">
+      <c r="R36" s="56"/>
+      <c r="S36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="52"/>
-      <c r="U36" s="52" t="s">
+      <c r="T36" s="56"/>
+      <c r="U36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="52"/>
-      <c r="W36" s="52" t="s">
+      <c r="V36" s="56"/>
+      <c r="W36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="52"/>
-      <c r="Y36" s="52" t="s">
+      <c r="X36" s="56"/>
+      <c r="Y36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="52"/>
-      <c r="AA36" s="52" t="s">
+      <c r="Z36" s="56"/>
+      <c r="AA36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="52"/>
+      <c r="AB36" s="56"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="52" t="s">
+      <c r="AG36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="52"/>
-      <c r="AI36" s="52" t="s">
+      <c r="AH36" s="56"/>
+      <c r="AI36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="52"/>
-      <c r="AK36" s="52" t="s">
+      <c r="AJ36" s="56"/>
+      <c r="AK36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="52"/>
-      <c r="AM36" s="52" t="s">
+      <c r="AL36" s="56"/>
+      <c r="AM36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="52"/>
+      <c r="AN36" s="56"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -10705,40 +10564,40 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="56" t="s">
+      <c r="K46" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
-      <c r="T46" s="56"/>
-      <c r="U46" s="56"/>
-      <c r="V46" s="56"/>
-      <c r="W46" s="56"/>
-      <c r="X46" s="56"/>
-      <c r="Y46" s="56"/>
-      <c r="Z46" s="56"/>
-      <c r="AA46" s="56"/>
-      <c r="AB46" s="56"/>
-      <c r="AC46" s="56"/>
-      <c r="AD46" s="56"/>
-      <c r="AE46" s="56" t="s">
+      <c r="L46" s="55"/>
+      <c r="M46" s="55"/>
+      <c r="N46" s="55"/>
+      <c r="O46" s="55"/>
+      <c r="P46" s="55"/>
+      <c r="Q46" s="55"/>
+      <c r="R46" s="55"/>
+      <c r="S46" s="55"/>
+      <c r="T46" s="55"/>
+      <c r="U46" s="55"/>
+      <c r="V46" s="55"/>
+      <c r="W46" s="55"/>
+      <c r="X46" s="55"/>
+      <c r="Y46" s="55"/>
+      <c r="Z46" s="55"/>
+      <c r="AA46" s="55"/>
+      <c r="AB46" s="55"/>
+      <c r="AC46" s="55"/>
+      <c r="AD46" s="55"/>
+      <c r="AE46" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="56"/>
-      <c r="AG46" s="56"/>
-      <c r="AH46" s="56"/>
-      <c r="AI46" s="56"/>
-      <c r="AJ46" s="56"/>
-      <c r="AK46" s="56"/>
-      <c r="AL46" s="56"/>
-      <c r="AM46" s="56"/>
-      <c r="AN46" s="56"/>
+      <c r="AF46" s="55"/>
+      <c r="AG46" s="55"/>
+      <c r="AH46" s="55"/>
+      <c r="AI46" s="55"/>
+      <c r="AJ46" s="55"/>
+      <c r="AK46" s="55"/>
+      <c r="AL46" s="55"/>
+      <c r="AM46" s="55"/>
+      <c r="AN46" s="55"/>
       <c r="AO46" s="51" t="s">
         <v>111</v>
       </c>
@@ -10755,17 +10614,17 @@
         <v>118</v>
       </c>
       <c r="AV46" s="51"/>
-      <c r="AW46" s="53" t="s">
+      <c r="AW46" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="54"/>
-      <c r="AY46" s="54"/>
-      <c r="AZ46" s="54"/>
-      <c r="BA46" s="54"/>
-      <c r="BB46" s="54"/>
-      <c r="BC46" s="54"/>
-      <c r="BD46" s="54"/>
-      <c r="BE46" s="55"/>
+      <c r="AX46" s="53"/>
+      <c r="AY46" s="53"/>
+      <c r="AZ46" s="53"/>
+      <c r="BA46" s="53"/>
+      <c r="BB46" s="53"/>
+      <c r="BC46" s="53"/>
+      <c r="BD46" s="53"/>
+      <c r="BE46" s="54"/>
       <c r="BF46" s="51" t="s">
         <v>118</v>
       </c>
@@ -14331,74 +14190,20 @@
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BK42:BL42"/>
-    <mergeCell ref="BM42:BN42"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="BK36:BL36"/>
-    <mergeCell ref="BM36:BN36"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BY36:BZ36"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BK33:BL33"/>
-    <mergeCell ref="BM33:BN33"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BK34:BL34"/>
-    <mergeCell ref="BM34:BN34"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BI42:BJ42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="BI36:BJ36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="BI33:BJ33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U33:V33"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="O36:P36"/>
@@ -14420,20 +14225,74 @@
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="BI33:BJ33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="BI42:BJ42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="BI36:BJ36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="BK33:BL33"/>
+    <mergeCell ref="BM33:BN33"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BK34:BL34"/>
+    <mergeCell ref="BM34:BN34"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BK42:BL42"/>
+    <mergeCell ref="BM42:BN42"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="BK36:BL36"/>
+    <mergeCell ref="BM36:BN36"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BY36:BZ36"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14446,7 +14305,7 @@
   <dimension ref="G2:AW27"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -15109,10 +14968,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:B146"/>
+  <dimension ref="B1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q115" workbookViewId="0">
-      <selection activeCell="U146" sqref="U146"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U83" sqref="U83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -15122,19 +14981,19 @@
         <v>142</v>
       </c>
     </row>
+    <row r="45" spans="6:6">
+      <c r="F45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6">
+      <c r="F46" t="s">
+        <v>153</v>
+      </c>
+    </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2">
-      <c r="B96" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2">
-      <c r="B146" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bg edge display bug fixed. scrolling sitll not correct.
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="153">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -417,10 +417,6 @@
   </si>
   <si>
     <t>0 - 239, 262</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HGB</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -651,7 +647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -908,13 +904,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1038,9 +1047,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1071,6 +1077,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1083,7 +1092,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3390,16 +3402,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>76</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>82</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>82</xdr:col>
-      <xdr:colOff>201082</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>26561</xdr:rowOff>
+      <xdr:col>84</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>148170</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3408,8 +3420,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="18369440" y="6849585"/>
-          <a:ext cx="195894" cy="1440391"/>
+          <a:off x="19145248" y="7323669"/>
+          <a:ext cx="148168" cy="444500"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst>
@@ -4485,10 +4497,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -4496,8 +4508,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
@@ -4536,10 +4548,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -4547,8 +4559,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
@@ -4687,10 +4699,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="48" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -4698,8 +4710,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1">
-      <c r="A30" s="50"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
@@ -4727,10 +4739,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="48" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -4738,8 +4750,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="6" t="s">
         <v>57</v>
       </c>
@@ -4839,22 +4851,22 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="48" t="s">
         <v>62</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="48" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" thickBot="1">
-      <c r="A48" s="50"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="50"/>
+      <c r="C48" s="49"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="2" t="s">
@@ -4878,22 +4890,22 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="48" t="s">
         <v>62</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="49" t="s">
+      <c r="C52" s="48" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" thickBot="1">
-      <c r="A53" s="50"/>
+      <c r="A53" s="49"/>
       <c r="B53" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="50"/>
+      <c r="C53" s="49"/>
     </row>
     <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="2" t="s">
@@ -4917,25 +4929,31 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="48" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="48" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1">
-      <c r="A58" s="50"/>
+      <c r="A58" s="49"/>
       <c r="B58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="50"/>
+      <c r="C58" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -4944,12 +4962,6 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9452,8 +9464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CF125"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AS32" sqref="AS32:AT32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BO33" sqref="BO33:BP33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -9483,6 +9495,7 @@
     <col min="69" max="69" width="4.5" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="4.5" bestFit="1" customWidth="1"/>
     <col min="78" max="79" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
@@ -9490,7 +9503,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="10:83" s="27" customFormat="1" ht="42">
+    <row r="32" spans="10:84" s="27" customFormat="1" ht="42">
       <c r="J32" s="27">
         <v>0</v>
       </c>
@@ -9694,6 +9707,9 @@
       </c>
       <c r="CE32" s="27">
         <v>399</v>
+      </c>
+      <c r="CF32" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="6:84">
@@ -9701,62 +9717,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="51" t="s">
+      <c r="K33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51" t="s">
+      <c r="L33" s="50"/>
+      <c r="M33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51" t="s">
+      <c r="N33" s="50"/>
+      <c r="O33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51" t="s">
+      <c r="P33" s="50"/>
+      <c r="Q33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="51"/>
-      <c r="S33" s="51" t="s">
+      <c r="R33" s="50"/>
+      <c r="S33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="51"/>
-      <c r="U33" s="51" t="s">
+      <c r="T33" s="50"/>
+      <c r="U33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="51"/>
-      <c r="W33" s="51" t="s">
+      <c r="V33" s="50"/>
+      <c r="W33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="51"/>
-      <c r="Y33" s="51" t="s">
+      <c r="X33" s="50"/>
+      <c r="Y33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="51"/>
-      <c r="AA33" s="51" t="s">
+      <c r="Z33" s="50"/>
+      <c r="AA33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="51"/>
+      <c r="AB33" s="50"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="51" t="s">
+      <c r="AG33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="51"/>
-      <c r="AI33" s="51" t="s">
+      <c r="AH33" s="50"/>
+      <c r="AI33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="51"/>
-      <c r="AK33" s="51" t="s">
+      <c r="AJ33" s="50"/>
+      <c r="AK33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="51"/>
-      <c r="AM33" s="51" t="s">
+      <c r="AL33" s="50"/>
+      <c r="AM33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="51"/>
+      <c r="AN33" s="50"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -9773,116 +9789,110 @@
       <c r="BD33" s="34"/>
       <c r="BF33" s="34"/>
       <c r="BG33" s="34"/>
-      <c r="BI33" s="51" t="s">
+      <c r="BI33" s="34"/>
+      <c r="BJ33" s="34"/>
+      <c r="BK33" s="34"/>
+      <c r="BL33" s="34"/>
+      <c r="BM33" s="34"/>
+      <c r="BN33" s="34"/>
+      <c r="BO33" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BJ33" s="51"/>
-      <c r="BK33" s="51" t="s">
+      <c r="BP33" s="57"/>
+      <c r="BQ33" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BL33" s="51"/>
-      <c r="BM33" s="51" t="s">
+      <c r="BR33" s="57"/>
+      <c r="BS33" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BN33" s="51"/>
-      <c r="BO33" s="51" t="s">
+      <c r="BT33" s="57"/>
+      <c r="BU33" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BP33" s="51"/>
-      <c r="BQ33" s="51" t="s">
+      <c r="BV33" s="57"/>
+      <c r="BW33" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BR33" s="51"/>
-      <c r="BS33" s="51" t="s">
+      <c r="BX33" s="57"/>
+      <c r="BY33" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BT33" s="51"/>
-      <c r="BU33" s="51" t="s">
+      <c r="BZ33" s="57"/>
+      <c r="CA33" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BV33" s="51"/>
-      <c r="BW33" s="51" t="s">
+      <c r="CB33" s="57"/>
+      <c r="CC33" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BX33" s="51"/>
-      <c r="BY33" s="51" t="s">
+      <c r="CD33" s="57"/>
+      <c r="CE33" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BZ33" s="51"/>
-      <c r="CA33" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="CB33" s="51"/>
-      <c r="CC33" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="CD33" s="51"/>
-      <c r="CE33" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="CF33" s="27"/>
+      <c r="CF33" s="57"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="51" t="s">
+      <c r="K34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51" t="s">
+      <c r="L34" s="50"/>
+      <c r="M34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51" t="s">
+      <c r="N34" s="50"/>
+      <c r="O34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51" t="s">
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="51"/>
-      <c r="S34" s="51" t="s">
+      <c r="R34" s="50"/>
+      <c r="S34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="51"/>
-      <c r="U34" s="51" t="s">
+      <c r="T34" s="50"/>
+      <c r="U34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="51"/>
-      <c r="W34" s="51" t="s">
+      <c r="V34" s="50"/>
+      <c r="W34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="51"/>
-      <c r="Y34" s="51" t="s">
+      <c r="X34" s="50"/>
+      <c r="Y34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="51"/>
-      <c r="AA34" s="51" t="s">
+      <c r="Z34" s="50"/>
+      <c r="AA34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="51"/>
+      <c r="AB34" s="50"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="51" t="s">
+      <c r="AG34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="51"/>
-      <c r="AI34" s="51" t="s">
+      <c r="AH34" s="50"/>
+      <c r="AI34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="51"/>
-      <c r="AK34" s="51" t="s">
+      <c r="AJ34" s="50"/>
+      <c r="AK34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="51"/>
-      <c r="AM34" s="51" t="s">
+      <c r="AL34" s="50"/>
+      <c r="AM34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="51"/>
+      <c r="AN34" s="50"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -9899,54 +9909,48 @@
       <c r="BD34" s="34"/>
       <c r="BF34" s="34"/>
       <c r="BG34" s="34"/>
-      <c r="BI34" s="51" t="s">
+      <c r="BI34" s="34"/>
+      <c r="BJ34" s="34"/>
+      <c r="BK34" s="34"/>
+      <c r="BL34" s="34"/>
+      <c r="BM34" s="34"/>
+      <c r="BN34" s="34"/>
+      <c r="BO34" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BJ34" s="51"/>
-      <c r="BK34" s="51" t="s">
+      <c r="BP34" s="57"/>
+      <c r="BQ34" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BL34" s="51"/>
-      <c r="BM34" s="51" t="s">
+      <c r="BR34" s="57"/>
+      <c r="BS34" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BN34" s="51"/>
-      <c r="BO34" s="51" t="s">
+      <c r="BT34" s="57"/>
+      <c r="BU34" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BP34" s="51"/>
-      <c r="BQ34" s="51" t="s">
+      <c r="BV34" s="57"/>
+      <c r="BW34" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BR34" s="51"/>
-      <c r="BS34" s="51" t="s">
+      <c r="BX34" s="57"/>
+      <c r="BY34" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BT34" s="51"/>
-      <c r="BU34" s="51" t="s">
+      <c r="BZ34" s="57"/>
+      <c r="CA34" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BV34" s="51"/>
-      <c r="BW34" s="51" t="s">
+      <c r="CB34" s="57"/>
+      <c r="CC34" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BX34" s="51"/>
-      <c r="BY34" s="51" t="s">
+      <c r="CD34" s="57"/>
+      <c r="CE34" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BZ34" s="51"/>
-      <c r="CA34" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="CB34" s="51"/>
-      <c r="CC34" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="CD34" s="51"/>
-      <c r="CE34" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="CF34" s="27"/>
+      <c r="CF34" s="57"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -9960,62 +9964,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="56" t="s">
+      <c r="K36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56" t="s">
+      <c r="L36" s="51"/>
+      <c r="M36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56" t="s">
+      <c r="N36" s="51"/>
+      <c r="O36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56" t="s">
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56" t="s">
+      <c r="R36" s="51"/>
+      <c r="S36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56" t="s">
+      <c r="T36" s="51"/>
+      <c r="U36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="56"/>
-      <c r="W36" s="56" t="s">
+      <c r="V36" s="51"/>
+      <c r="W36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="56"/>
-      <c r="Y36" s="56" t="s">
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="56"/>
-      <c r="AA36" s="56" t="s">
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="56"/>
+      <c r="AB36" s="51"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="56" t="s">
+      <c r="AG36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="56"/>
-      <c r="AI36" s="56" t="s">
+      <c r="AH36" s="51"/>
+      <c r="AI36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="56"/>
-      <c r="AK36" s="56" t="s">
+      <c r="AJ36" s="51"/>
+      <c r="AK36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="56"/>
-      <c r="AM36" s="56" t="s">
+      <c r="AL36" s="51"/>
+      <c r="AM36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="56"/>
+      <c r="AN36" s="51"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -10032,54 +10036,48 @@
       <c r="BD36" s="36"/>
       <c r="BF36" s="34"/>
       <c r="BG36" s="34"/>
-      <c r="BI36" s="51" t="s">
+      <c r="BI36" s="34"/>
+      <c r="BJ36" s="34"/>
+      <c r="BK36" s="34"/>
+      <c r="BL36" s="34"/>
+      <c r="BM36" s="34"/>
+      <c r="BN36" s="34"/>
+      <c r="BO36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BJ36" s="51"/>
-      <c r="BK36" s="51" t="s">
+      <c r="BP36" s="57"/>
+      <c r="BQ36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BL36" s="51"/>
-      <c r="BM36" s="51" t="s">
+      <c r="BR36" s="57"/>
+      <c r="BS36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BN36" s="51"/>
-      <c r="BO36" s="51" t="s">
+      <c r="BT36" s="57"/>
+      <c r="BU36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BP36" s="51"/>
-      <c r="BQ36" s="51" t="s">
+      <c r="BV36" s="57"/>
+      <c r="BW36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BR36" s="51"/>
-      <c r="BS36" s="51" t="s">
+      <c r="BX36" s="57"/>
+      <c r="BY36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BT36" s="51"/>
-      <c r="BU36" s="51" t="s">
+      <c r="BZ36" s="57"/>
+      <c r="CA36" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BV36" s="51"/>
-      <c r="BW36" s="51" t="s">
+      <c r="CB36" s="57"/>
+      <c r="CC36" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BX36" s="51"/>
-      <c r="BY36" s="51" t="s">
+      <c r="CD36" s="57"/>
+      <c r="CE36" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BZ36" s="51"/>
-      <c r="CA36" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="CB36" s="51"/>
-      <c r="CC36" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="CD36" s="51"/>
-      <c r="CE36" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="CF36" s="27"/>
+      <c r="CF36" s="57"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -10415,58 +10413,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="51" t="s">
+      <c r="M42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="51"/>
-      <c r="O42" s="51" t="s">
+      <c r="N42" s="50"/>
+      <c r="O42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="51" t="s">
+      <c r="P42" s="50"/>
+      <c r="Q42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="51"/>
-      <c r="S42" s="51" t="s">
+      <c r="R42" s="50"/>
+      <c r="S42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="51"/>
-      <c r="U42" s="51" t="s">
+      <c r="T42" s="50"/>
+      <c r="U42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="51"/>
-      <c r="W42" s="51" t="s">
+      <c r="V42" s="50"/>
+      <c r="W42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="51" t="s">
+      <c r="X42" s="50"/>
+      <c r="Y42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="51"/>
-      <c r="AA42" s="51" t="s">
+      <c r="Z42" s="50"/>
+      <c r="AA42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="51"/>
+      <c r="AB42" s="50"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="51" t="s">
+      <c r="AG42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="51"/>
-      <c r="AI42" s="51" t="s">
+      <c r="AH42" s="50"/>
+      <c r="AI42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="51"/>
-      <c r="AK42" s="51" t="s">
+      <c r="AJ42" s="50"/>
+      <c r="AK42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="51"/>
-      <c r="AM42" s="51" t="s">
+      <c r="AL42" s="50"/>
+      <c r="AM42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="51"/>
+      <c r="AN42" s="50"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -10483,54 +10481,48 @@
       <c r="BD42" s="34"/>
       <c r="BF42" s="34"/>
       <c r="BG42" s="34"/>
-      <c r="BI42" s="51" t="s">
+      <c r="BI42" s="34"/>
+      <c r="BJ42" s="34"/>
+      <c r="BK42" s="34"/>
+      <c r="BL42" s="34"/>
+      <c r="BM42" s="34"/>
+      <c r="BN42" s="34"/>
+      <c r="BO42" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BJ42" s="51"/>
-      <c r="BK42" s="51" t="s">
+      <c r="BP42" s="57"/>
+      <c r="BQ42" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BL42" s="51"/>
-      <c r="BM42" s="51" t="s">
+      <c r="BR42" s="57"/>
+      <c r="BS42" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BN42" s="51"/>
-      <c r="BO42" s="51" t="s">
+      <c r="BT42" s="57"/>
+      <c r="BU42" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BP42" s="51"/>
-      <c r="BQ42" s="51" t="s">
+      <c r="BV42" s="57"/>
+      <c r="BW42" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BR42" s="51"/>
-      <c r="BS42" s="51" t="s">
+      <c r="BX42" s="57"/>
+      <c r="BY42" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="BT42" s="51"/>
-      <c r="BU42" s="51" t="s">
+      <c r="BZ42" s="57"/>
+      <c r="CA42" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="BV42" s="51"/>
-      <c r="BW42" s="51" t="s">
+      <c r="CB42" s="57"/>
+      <c r="CC42" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="BX42" s="51"/>
-      <c r="BY42" s="51" t="s">
+      <c r="CD42" s="57"/>
+      <c r="CE42" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="BZ42" s="51"/>
-      <c r="CA42" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="CB42" s="51"/>
-      <c r="CC42" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="CD42" s="51"/>
-      <c r="CE42" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="CF42" s="27"/>
+      <c r="CF42" s="57"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -10541,15 +10533,14 @@
     </row>
     <row r="44" spans="6:84">
       <c r="AK44" t="s">
-        <v>122</v>
-      </c>
-      <c r="CA44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="CB44" s="27"/>
       <c r="CC44" s="27"/>
       <c r="CD44" s="27"/>
-      <c r="CE44" s="27"/>
+      <c r="CE44" t="s">
+        <v>121</v>
+      </c>
       <c r="CF44" s="27"/>
     </row>
     <row r="45" spans="6:84">
@@ -10598,22 +10589,22 @@
       <c r="AL46" s="55"/>
       <c r="AM46" s="55"/>
       <c r="AN46" s="55"/>
-      <c r="AO46" s="51" t="s">
+      <c r="AO46" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="51"/>
-      <c r="AQ46" s="51" t="s">
+      <c r="AP46" s="50"/>
+      <c r="AQ46" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="51"/>
-      <c r="AS46" s="51" t="s">
+      <c r="AR46" s="50"/>
+      <c r="AS46" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="51"/>
-      <c r="AU46" s="51" t="s">
+      <c r="AT46" s="50"/>
+      <c r="AU46" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="51"/>
+      <c r="AV46" s="50"/>
       <c r="AW46" s="52" t="s">
         <v>119</v>
       </c>
@@ -10625,10 +10616,10 @@
       <c r="BC46" s="53"/>
       <c r="BD46" s="53"/>
       <c r="BE46" s="54"/>
-      <c r="BF46" s="51" t="s">
+      <c r="BF46" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="51"/>
+      <c r="BG46" s="50"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -10738,7 +10729,7 @@
       <c r="BP53" s="17"/>
       <c r="BQ53" s="18"/>
       <c r="BS53" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="5:71">
@@ -10872,7 +10863,7 @@
       <c r="BP55" s="12"/>
       <c r="BQ55" s="20"/>
       <c r="BS55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="5:71">
@@ -10939,7 +10930,7 @@
       <c r="BP56" s="12"/>
       <c r="BQ56" s="20"/>
       <c r="BS56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="5:71">
@@ -11006,7 +10997,7 @@
       <c r="BP57" s="12"/>
       <c r="BQ57" s="20"/>
       <c r="BS57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="5:71">
@@ -11073,7 +11064,7 @@
       <c r="BP58" s="12"/>
       <c r="BQ58" s="20"/>
       <c r="BS58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="5:71">
@@ -14189,60 +14180,40 @@
       <c r="AV125" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="103">
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="BI33:BJ33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="BQ34:BR34"/>
-    <mergeCell ref="BS34:BT34"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AG34:AH34"/>
-    <mergeCell ref="AI34:AJ34"/>
-    <mergeCell ref="AK34:AL34"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="BI34:BJ34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="BI42:BJ42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="BI36:BJ36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="AI36:AJ36"/>
+  <mergeCells count="95">
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
     <mergeCell ref="AS46:AT46"/>
     <mergeCell ref="AU46:AV46"/>
     <mergeCell ref="BF46:BG46"/>
@@ -14256,47 +14227,60 @@
     <mergeCell ref="AI42:AJ42"/>
     <mergeCell ref="AK42:AL42"/>
     <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BK33:BL33"/>
-    <mergeCell ref="BM33:BN33"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BK34:BL34"/>
-    <mergeCell ref="BM34:BN34"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BK42:BL42"/>
-    <mergeCell ref="BM42:BN42"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="BK36:BL36"/>
-    <mergeCell ref="BM36:BN36"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="BQ34:BR34"/>
+    <mergeCell ref="BS34:BT34"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AG34:AH34"/>
+    <mergeCell ref="AI34:AJ34"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U33:V33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14317,12 +14301,12 @@
   <sheetData>
     <row r="2" spans="9:49">
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="9:49">
       <c r="I3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="9:49">
@@ -14377,223 +14361,223 @@
     </row>
     <row r="6" spans="9:49">
       <c r="I6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="44"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="43"/>
       <c r="AO6">
         <v>0</v>
       </c>
-      <c r="AP6" s="42"/>
-      <c r="AQ6" s="43"/>
-      <c r="AR6" s="43"/>
-      <c r="AS6" s="43"/>
-      <c r="AT6" s="43"/>
-      <c r="AU6" s="43"/>
-      <c r="AV6" s="44"/>
-      <c r="AW6" s="42"/>
+      <c r="AP6" s="41"/>
+      <c r="AQ6" s="42"/>
+      <c r="AR6" s="42"/>
+      <c r="AS6" s="42"/>
+      <c r="AT6" s="42"/>
+      <c r="AU6" s="42"/>
+      <c r="AV6" s="43"/>
+      <c r="AW6" s="41"/>
     </row>
     <row r="7" spans="9:49">
       <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="44"/>
-      <c r="Y7" s="42" t="s">
-        <v>128</v>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="43"/>
+      <c r="Y7" s="41" t="s">
+        <v>127</v>
       </c>
       <c r="AO7">
         <v>1</v>
       </c>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="43"/>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="44"/>
-      <c r="AT7" s="44"/>
-      <c r="AU7" s="43"/>
-      <c r="AV7" s="43"/>
-      <c r="AW7" s="44"/>
+      <c r="AP7" s="42"/>
+      <c r="AQ7" s="42"/>
+      <c r="AR7" s="43"/>
+      <c r="AS7" s="43"/>
+      <c r="AT7" s="43"/>
+      <c r="AU7" s="42"/>
+      <c r="AV7" s="42"/>
+      <c r="AW7" s="43"/>
     </row>
     <row r="8" spans="9:49">
       <c r="M8">
         <v>2</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="44"/>
-      <c r="Y8" s="44" t="s">
-        <v>129</v>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="43"/>
+      <c r="Y8" s="43" t="s">
+        <v>128</v>
       </c>
       <c r="AO8">
         <v>2</v>
       </c>
-      <c r="AP8" s="43"/>
-      <c r="AQ8" s="43"/>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="42"/>
-      <c r="AT8" s="42"/>
-      <c r="AU8" s="43"/>
-      <c r="AV8" s="43"/>
-      <c r="AW8" s="44"/>
+      <c r="AP8" s="42"/>
+      <c r="AQ8" s="42"/>
+      <c r="AR8" s="43"/>
+      <c r="AS8" s="41"/>
+      <c r="AT8" s="41"/>
+      <c r="AU8" s="42"/>
+      <c r="AV8" s="42"/>
+      <c r="AW8" s="43"/>
     </row>
     <row r="9" spans="9:49">
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="44"/>
-      <c r="Y9" s="45" t="s">
-        <v>130</v>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="43"/>
+      <c r="Y9" s="44" t="s">
+        <v>129</v>
       </c>
       <c r="AO9">
         <v>3</v>
       </c>
-      <c r="AP9" s="43"/>
-      <c r="AQ9" s="43"/>
-      <c r="AR9" s="44"/>
-      <c r="AS9" s="42"/>
-      <c r="AT9" s="42"/>
-      <c r="AU9" s="43"/>
-      <c r="AV9" s="43"/>
-      <c r="AW9" s="44"/>
+      <c r="AP9" s="42"/>
+      <c r="AQ9" s="42"/>
+      <c r="AR9" s="43"/>
+      <c r="AS9" s="41"/>
+      <c r="AT9" s="41"/>
+      <c r="AU9" s="42"/>
+      <c r="AV9" s="42"/>
+      <c r="AW9" s="43"/>
     </row>
     <row r="10" spans="9:49">
       <c r="M10">
         <v>4</v>
       </c>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="44"/>
-      <c r="Y10" s="43" t="s">
-        <v>131</v>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="43"/>
+      <c r="Y10" s="42" t="s">
+        <v>130</v>
       </c>
       <c r="AO10">
         <v>4</v>
       </c>
-      <c r="AP10" s="43"/>
-      <c r="AQ10" s="43"/>
-      <c r="AR10" s="44"/>
-      <c r="AS10" s="42"/>
-      <c r="AT10" s="42"/>
-      <c r="AU10" s="43"/>
-      <c r="AV10" s="43"/>
-      <c r="AW10" s="44"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="42"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="41"/>
+      <c r="AT10" s="41"/>
+      <c r="AU10" s="42"/>
+      <c r="AV10" s="42"/>
+      <c r="AW10" s="43"/>
     </row>
     <row r="11" spans="9:49">
       <c r="M11">
         <v>5</v>
       </c>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="44"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="43"/>
       <c r="AO11">
         <v>5</v>
       </c>
-      <c r="AP11" s="43"/>
-      <c r="AQ11" s="43"/>
-      <c r="AR11" s="44"/>
-      <c r="AS11" s="42"/>
-      <c r="AT11" s="42"/>
-      <c r="AU11" s="43"/>
-      <c r="AV11" s="43"/>
-      <c r="AW11" s="44"/>
+      <c r="AP11" s="42"/>
+      <c r="AQ11" s="42"/>
+      <c r="AR11" s="43"/>
+      <c r="AS11" s="41"/>
+      <c r="AT11" s="41"/>
+      <c r="AU11" s="42"/>
+      <c r="AV11" s="42"/>
+      <c r="AW11" s="43"/>
     </row>
     <row r="12" spans="9:49">
       <c r="M12">
         <v>6</v>
       </c>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="44"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="43"/>
       <c r="AO12">
         <v>6</v>
       </c>
-      <c r="AP12" s="44"/>
-      <c r="AQ12" s="43"/>
-      <c r="AR12" s="43"/>
-      <c r="AS12" s="43"/>
-      <c r="AT12" s="43"/>
-      <c r="AU12" s="43"/>
-      <c r="AV12" s="44"/>
-      <c r="AW12" s="44"/>
+      <c r="AP12" s="43"/>
+      <c r="AQ12" s="42"/>
+      <c r="AR12" s="42"/>
+      <c r="AS12" s="42"/>
+      <c r="AT12" s="42"/>
+      <c r="AU12" s="42"/>
+      <c r="AV12" s="43"/>
+      <c r="AW12" s="43"/>
     </row>
     <row r="13" spans="9:49">
       <c r="M13">
         <v>7</v>
       </c>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
       <c r="AO13">
         <v>7</v>
       </c>
-      <c r="AP13" s="42"/>
-      <c r="AQ13" s="44"/>
-      <c r="AR13" s="44"/>
-      <c r="AS13" s="44"/>
-      <c r="AT13" s="44"/>
-      <c r="AU13" s="44"/>
-      <c r="AV13" s="44"/>
-      <c r="AW13" s="42"/>
+      <c r="AP13" s="41"/>
+      <c r="AQ13" s="43"/>
+      <c r="AR13" s="43"/>
+      <c r="AS13" s="43"/>
+      <c r="AT13" s="43"/>
+      <c r="AU13" s="43"/>
+      <c r="AV13" s="43"/>
+      <c r="AW13" s="41"/>
     </row>
     <row r="18" spans="7:46">
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y18" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="Y18" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="AO18" s="46" t="s">
+      <c r="AO18" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="AS18" s="45" t="s">
         <v>147</v>
-      </c>
-      <c r="AS18" s="46" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="7:46">
@@ -14650,314 +14634,314 @@
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
       <c r="P20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y20">
         <v>0</v>
       </c>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="45"/>
-      <c r="AB20" s="42"/>
-      <c r="AC20" s="42"/>
-      <c r="AD20" s="42"/>
-      <c r="AE20" s="45"/>
-      <c r="AF20" s="45"/>
-      <c r="AG20" s="42"/>
-      <c r="AH20" s="47" t="s">
-        <v>139</v>
+      <c r="Z20" s="44"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="41"/>
+      <c r="AC20" s="41"/>
+      <c r="AD20" s="41"/>
+      <c r="AE20" s="44"/>
+      <c r="AF20" s="44"/>
+      <c r="AG20" s="41"/>
+      <c r="AH20" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="AO20">
         <v>0</v>
       </c>
       <c r="AP20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AS20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="7:46">
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
       <c r="P21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y21">
         <v>1</v>
       </c>
-      <c r="Z21" s="45"/>
-      <c r="AA21" s="45"/>
-      <c r="AB21" s="42"/>
-      <c r="AC21" s="42"/>
-      <c r="AD21" s="42"/>
-      <c r="AE21" s="45"/>
-      <c r="AF21" s="45"/>
-      <c r="AG21" s="42"/>
-      <c r="AH21" s="47" t="s">
-        <v>139</v>
+      <c r="Z21" s="44"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="41"/>
+      <c r="AC21" s="41"/>
+      <c r="AD21" s="41"/>
+      <c r="AE21" s="44"/>
+      <c r="AF21" s="44"/>
+      <c r="AG21" s="41"/>
+      <c r="AH21" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="AO21">
         <v>1</v>
       </c>
       <c r="AP21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AS21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="7:46">
       <c r="G22">
         <v>2</v>
       </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
       <c r="P22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y22">
         <v>2</v>
       </c>
-      <c r="Z22" s="45"/>
-      <c r="AA22" s="45"/>
-      <c r="AB22" s="45"/>
-      <c r="AC22" s="42"/>
-      <c r="AD22" s="45"/>
-      <c r="AE22" s="45"/>
-      <c r="AF22" s="45"/>
-      <c r="AG22" s="42"/>
-      <c r="AH22" s="47" t="s">
-        <v>140</v>
+      <c r="Z22" s="44"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="41"/>
+      <c r="AD22" s="44"/>
+      <c r="AE22" s="44"/>
+      <c r="AF22" s="44"/>
+      <c r="AG22" s="41"/>
+      <c r="AH22" s="46" t="s">
+        <v>139</v>
       </c>
       <c r="AO22">
         <v>2</v>
       </c>
       <c r="AP22" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS22" t="s">
         <v>144</v>
-      </c>
-      <c r="AS22" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="23" spans="7:46">
       <c r="G23">
         <v>3</v>
       </c>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="44"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
       <c r="P23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y23">
         <v>3</v>
       </c>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="42"/>
-      <c r="AC23" s="45"/>
-      <c r="AD23" s="42"/>
-      <c r="AE23" s="45"/>
-      <c r="AF23" s="45"/>
-      <c r="AG23" s="42"/>
-      <c r="AH23" s="47" t="s">
-        <v>141</v>
+      <c r="Z23" s="44"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="41"/>
+      <c r="AC23" s="44"/>
+      <c r="AD23" s="41"/>
+      <c r="AE23" s="44"/>
+      <c r="AF23" s="44"/>
+      <c r="AG23" s="41"/>
+      <c r="AH23" s="46" t="s">
+        <v>140</v>
       </c>
       <c r="AO23">
         <v>3</v>
       </c>
       <c r="AP23" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS23" t="s">
         <v>144</v>
-      </c>
-      <c r="AS23" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="24" spans="7:46">
       <c r="G24">
         <v>4</v>
       </c>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
       <c r="P24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y24">
         <v>4</v>
       </c>
-      <c r="Z24" s="45"/>
-      <c r="AA24" s="45"/>
-      <c r="AB24" s="42"/>
-      <c r="AC24" s="42"/>
-      <c r="AD24" s="42"/>
-      <c r="AE24" s="45"/>
-      <c r="AF24" s="45"/>
-      <c r="AG24" s="42"/>
-      <c r="AH24" s="47" t="s">
-        <v>139</v>
+      <c r="Z24" s="44"/>
+      <c r="AA24" s="44"/>
+      <c r="AB24" s="41"/>
+      <c r="AC24" s="41"/>
+      <c r="AD24" s="41"/>
+      <c r="AE24" s="44"/>
+      <c r="AF24" s="44"/>
+      <c r="AG24" s="41"/>
+      <c r="AH24" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="AO24">
         <v>4</v>
       </c>
       <c r="AP24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS24" t="s">
         <v>144</v>
-      </c>
-      <c r="AS24" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="25" spans="7:46">
       <c r="G25">
         <v>5</v>
       </c>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
       <c r="P25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y25">
         <v>5</v>
       </c>
-      <c r="Z25" s="45"/>
-      <c r="AA25" s="45"/>
-      <c r="AB25" s="42"/>
-      <c r="AC25" s="42"/>
-      <c r="AD25" s="42"/>
-      <c r="AE25" s="45"/>
-      <c r="AF25" s="45"/>
-      <c r="AG25" s="42"/>
-      <c r="AH25" s="47" t="s">
-        <v>139</v>
+      <c r="Z25" s="44"/>
+      <c r="AA25" s="44"/>
+      <c r="AB25" s="41"/>
+      <c r="AC25" s="41"/>
+      <c r="AD25" s="41"/>
+      <c r="AE25" s="44"/>
+      <c r="AF25" s="44"/>
+      <c r="AG25" s="41"/>
+      <c r="AH25" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="AO25">
         <v>5</v>
       </c>
       <c r="AP25" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS25" t="s">
         <v>144</v>
-      </c>
-      <c r="AS25" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="26" spans="7:46">
       <c r="G26">
         <v>6</v>
       </c>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
       <c r="P26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y26">
         <v>6</v>
       </c>
-      <c r="Z26" s="45"/>
-      <c r="AA26" s="45"/>
-      <c r="AB26" s="42"/>
-      <c r="AC26" s="42"/>
-      <c r="AD26" s="42"/>
-      <c r="AE26" s="45"/>
-      <c r="AF26" s="45"/>
-      <c r="AG26" s="42"/>
-      <c r="AH26" s="47" t="s">
-        <v>139</v>
+      <c r="Z26" s="44"/>
+      <c r="AA26" s="44"/>
+      <c r="AB26" s="41"/>
+      <c r="AC26" s="41"/>
+      <c r="AD26" s="41"/>
+      <c r="AE26" s="44"/>
+      <c r="AF26" s="44"/>
+      <c r="AG26" s="41"/>
+      <c r="AH26" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="AO26">
         <v>6</v>
       </c>
       <c r="AP26" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS26" t="s">
         <v>150</v>
-      </c>
-      <c r="AS26" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="27" spans="7:46">
       <c r="G27">
         <v>7</v>
       </c>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
       <c r="P27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y27">
         <v>7</v>
       </c>
-      <c r="Z27" s="42"/>
-      <c r="AA27" s="42"/>
-      <c r="AB27" s="42"/>
-      <c r="AC27" s="42"/>
-      <c r="AD27" s="42"/>
-      <c r="AE27" s="42"/>
-      <c r="AF27" s="42"/>
-      <c r="AG27" s="42"/>
-      <c r="AH27" s="48" t="s">
-        <v>128</v>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="41"/>
+      <c r="AB27" s="41"/>
+      <c r="AC27" s="41"/>
+      <c r="AD27" s="41"/>
+      <c r="AE27" s="41"/>
+      <c r="AF27" s="41"/>
+      <c r="AG27" s="41"/>
+      <c r="AH27" s="47" t="s">
+        <v>127</v>
       </c>
       <c r="AO27">
         <v>7</v>
       </c>
       <c r="AP27" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS27" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="AT27" s="46"/>
+        <v>148</v>
+      </c>
+      <c r="AS27" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="AT27" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -14970,7 +14954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U83" sqref="U83"/>
     </sheetView>
   </sheetViews>
@@ -14978,22 +14962,22 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="6:6">
       <c r="F45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="6:6">
       <c r="F46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scrolling ok, but now scroll happens only 8 pix each... strange!
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -1074,10 +1074,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1092,10 +1095,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3402,16 +3402,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>82</xdr:col>
-      <xdr:colOff>10582</xdr:colOff>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>84</xdr:col>
       <xdr:colOff>10582</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>148170</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>10586</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3420,8 +3420,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="19145248" y="7323669"/>
-          <a:ext cx="148168" cy="444500"/>
+          <a:off x="19118790" y="7328961"/>
+          <a:ext cx="179918" cy="465666"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst>
@@ -4948,12 +4948,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -4962,6 +4956,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9464,8 +9464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CF125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BO33" sqref="BO33:BP33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CE36" sqref="CE36:CF36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -9717,62 +9717,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="50" t="s">
+      <c r="K33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50" t="s">
+      <c r="L33" s="52"/>
+      <c r="M33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50" t="s">
+      <c r="N33" s="52"/>
+      <c r="O33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50" t="s">
+      <c r="P33" s="52"/>
+      <c r="Q33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50" t="s">
+      <c r="R33" s="52"/>
+      <c r="S33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="50"/>
-      <c r="U33" s="50" t="s">
+      <c r="T33" s="52"/>
+      <c r="U33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="50"/>
-      <c r="W33" s="50" t="s">
+      <c r="V33" s="52"/>
+      <c r="W33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="50" t="s">
+      <c r="X33" s="52"/>
+      <c r="Y33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="50"/>
-      <c r="AA33" s="50" t="s">
+      <c r="Z33" s="52"/>
+      <c r="AA33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="50"/>
+      <c r="AB33" s="52"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="50" t="s">
+      <c r="AG33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="50"/>
-      <c r="AI33" s="50" t="s">
+      <c r="AH33" s="52"/>
+      <c r="AI33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="50"/>
-      <c r="AK33" s="50" t="s">
+      <c r="AJ33" s="52"/>
+      <c r="AK33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="50"/>
-      <c r="AM33" s="50" t="s">
+      <c r="AL33" s="52"/>
+      <c r="AM33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="50"/>
+      <c r="AN33" s="52"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -9795,104 +9795,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="56" t="s">
+      <c r="BO33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="57"/>
-      <c r="BQ33" s="56" t="s">
+      <c r="BP33" s="51"/>
+      <c r="BQ33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="57"/>
-      <c r="BS33" s="56" t="s">
+      <c r="BR33" s="51"/>
+      <c r="BS33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="57"/>
-      <c r="BU33" s="56" t="s">
+      <c r="BT33" s="51"/>
+      <c r="BU33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="57"/>
-      <c r="BW33" s="56" t="s">
+      <c r="BV33" s="51"/>
+      <c r="BW33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="57"/>
-      <c r="BY33" s="56" t="s">
+      <c r="BX33" s="51"/>
+      <c r="BY33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="57"/>
-      <c r="CA33" s="56" t="s">
+      <c r="BZ33" s="51"/>
+      <c r="CA33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="57"/>
-      <c r="CC33" s="56" t="s">
+      <c r="CB33" s="51"/>
+      <c r="CC33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="57"/>
-      <c r="CE33" s="56" t="s">
+      <c r="CD33" s="51"/>
+      <c r="CE33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="57"/>
+      <c r="CF33" s="51"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="50" t="s">
+      <c r="K34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50" t="s">
+      <c r="L34" s="52"/>
+      <c r="M34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50" t="s">
+      <c r="N34" s="52"/>
+      <c r="O34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50" t="s">
+      <c r="P34" s="52"/>
+      <c r="Q34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50" t="s">
+      <c r="R34" s="52"/>
+      <c r="S34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="50"/>
-      <c r="U34" s="50" t="s">
+      <c r="T34" s="52"/>
+      <c r="U34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="50"/>
-      <c r="W34" s="50" t="s">
+      <c r="V34" s="52"/>
+      <c r="W34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="50" t="s">
+      <c r="X34" s="52"/>
+      <c r="Y34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="50"/>
-      <c r="AA34" s="50" t="s">
+      <c r="Z34" s="52"/>
+      <c r="AA34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="50"/>
+      <c r="AB34" s="52"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="50" t="s">
+      <c r="AG34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="50"/>
-      <c r="AI34" s="50" t="s">
+      <c r="AH34" s="52"/>
+      <c r="AI34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="50"/>
-      <c r="AK34" s="50" t="s">
+      <c r="AJ34" s="52"/>
+      <c r="AK34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="50"/>
-      <c r="AM34" s="50" t="s">
+      <c r="AL34" s="52"/>
+      <c r="AM34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="50"/>
+      <c r="AN34" s="52"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -9915,42 +9915,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="56" t="s">
+      <c r="BO34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="57"/>
-      <c r="BQ34" s="56" t="s">
+      <c r="BP34" s="51"/>
+      <c r="BQ34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="57"/>
-      <c r="BS34" s="56" t="s">
+      <c r="BR34" s="51"/>
+      <c r="BS34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="57"/>
-      <c r="BU34" s="56" t="s">
+      <c r="BT34" s="51"/>
+      <c r="BU34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="57"/>
-      <c r="BW34" s="56" t="s">
+      <c r="BV34" s="51"/>
+      <c r="BW34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="57"/>
-      <c r="BY34" s="56" t="s">
+      <c r="BX34" s="51"/>
+      <c r="BY34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="57"/>
-      <c r="CA34" s="56" t="s">
+      <c r="BZ34" s="51"/>
+      <c r="CA34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="57"/>
-      <c r="CC34" s="56" t="s">
+      <c r="CB34" s="51"/>
+      <c r="CC34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="57"/>
-      <c r="CE34" s="56" t="s">
+      <c r="CD34" s="51"/>
+      <c r="CE34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="57"/>
+      <c r="CF34" s="51"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -9964,62 +9964,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="51" t="s">
+      <c r="K36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51" t="s">
+      <c r="L36" s="57"/>
+      <c r="M36" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="51"/>
-      <c r="O36" s="51" t="s">
+      <c r="N36" s="57"/>
+      <c r="O36" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="51" t="s">
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="51"/>
-      <c r="S36" s="51" t="s">
+      <c r="R36" s="57"/>
+      <c r="S36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="51"/>
-      <c r="U36" s="51" t="s">
+      <c r="T36" s="57"/>
+      <c r="U36" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="51"/>
-      <c r="W36" s="51" t="s">
+      <c r="V36" s="57"/>
+      <c r="W36" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="51"/>
-      <c r="Y36" s="51" t="s">
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="51"/>
-      <c r="AA36" s="51" t="s">
+      <c r="Z36" s="57"/>
+      <c r="AA36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="51"/>
+      <c r="AB36" s="57"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="51" t="s">
+      <c r="AG36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="51"/>
-      <c r="AI36" s="51" t="s">
+      <c r="AH36" s="57"/>
+      <c r="AI36" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="51"/>
-      <c r="AK36" s="51" t="s">
+      <c r="AJ36" s="57"/>
+      <c r="AK36" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="51"/>
-      <c r="AM36" s="51" t="s">
+      <c r="AL36" s="57"/>
+      <c r="AM36" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="51"/>
+      <c r="AN36" s="57"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -10042,42 +10042,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="56" t="s">
+      <c r="BO36" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="57"/>
-      <c r="BQ36" s="56" t="s">
+      <c r="BP36" s="51"/>
+      <c r="BQ36" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="57"/>
-      <c r="BS36" s="56" t="s">
+      <c r="BR36" s="51"/>
+      <c r="BS36" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="57"/>
-      <c r="BU36" s="56" t="s">
+      <c r="BT36" s="51"/>
+      <c r="BU36" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="57"/>
-      <c r="BW36" s="56" t="s">
+      <c r="BV36" s="51"/>
+      <c r="BW36" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="57"/>
-      <c r="BY36" s="56" t="s">
+      <c r="BX36" s="51"/>
+      <c r="BY36" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="57"/>
-      <c r="CA36" s="56" t="s">
+      <c r="BZ36" s="51"/>
+      <c r="CA36" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="57"/>
-      <c r="CC36" s="56" t="s">
+      <c r="CB36" s="51"/>
+      <c r="CC36" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="57"/>
-      <c r="CE36" s="56" t="s">
+      <c r="CD36" s="51"/>
+      <c r="CE36" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="57"/>
+      <c r="CF36" s="51"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -10413,58 +10413,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="50" t="s">
+      <c r="M42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50" t="s">
+      <c r="N42" s="52"/>
+      <c r="O42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50" t="s">
+      <c r="P42" s="52"/>
+      <c r="Q42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="50"/>
-      <c r="S42" s="50" t="s">
+      <c r="R42" s="52"/>
+      <c r="S42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="50"/>
-      <c r="U42" s="50" t="s">
+      <c r="T42" s="52"/>
+      <c r="U42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="50"/>
-      <c r="W42" s="50" t="s">
+      <c r="V42" s="52"/>
+      <c r="W42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="50"/>
-      <c r="Y42" s="50" t="s">
+      <c r="X42" s="52"/>
+      <c r="Y42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="50"/>
-      <c r="AA42" s="50" t="s">
+      <c r="Z42" s="52"/>
+      <c r="AA42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="50"/>
+      <c r="AB42" s="52"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="50" t="s">
+      <c r="AG42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="50"/>
-      <c r="AI42" s="50" t="s">
+      <c r="AH42" s="52"/>
+      <c r="AI42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="50"/>
-      <c r="AK42" s="50" t="s">
+      <c r="AJ42" s="52"/>
+      <c r="AK42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="50"/>
-      <c r="AM42" s="50" t="s">
+      <c r="AL42" s="52"/>
+      <c r="AM42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="50"/>
+      <c r="AN42" s="52"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -10487,42 +10487,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="56" t="s">
+      <c r="BO42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="57"/>
-      <c r="BQ42" s="56" t="s">
+      <c r="BP42" s="51"/>
+      <c r="BQ42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="57"/>
-      <c r="BS42" s="56" t="s">
+      <c r="BR42" s="51"/>
+      <c r="BS42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="57"/>
-      <c r="BU42" s="56" t="s">
+      <c r="BT42" s="51"/>
+      <c r="BU42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="57"/>
-      <c r="BW42" s="56" t="s">
+      <c r="BV42" s="51"/>
+      <c r="BW42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="57"/>
-      <c r="BY42" s="56" t="s">
+      <c r="BX42" s="51"/>
+      <c r="BY42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="57"/>
-      <c r="CA42" s="56" t="s">
+      <c r="BZ42" s="51"/>
+      <c r="CA42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="57"/>
-      <c r="CC42" s="56" t="s">
+      <c r="CB42" s="51"/>
+      <c r="CC42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="57"/>
-      <c r="CE42" s="56" t="s">
+      <c r="CD42" s="51"/>
+      <c r="CE42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="57"/>
+      <c r="CF42" s="51"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -10555,71 +10555,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="55" t="s">
+      <c r="K46" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="55"/>
-      <c r="M46" s="55"/>
-      <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="P46" s="55"/>
-      <c r="Q46" s="55"/>
-      <c r="R46" s="55"/>
-      <c r="S46" s="55"/>
-      <c r="T46" s="55"/>
-      <c r="U46" s="55"/>
-      <c r="V46" s="55"/>
-      <c r="W46" s="55"/>
-      <c r="X46" s="55"/>
-      <c r="Y46" s="55"/>
-      <c r="Z46" s="55"/>
-      <c r="AA46" s="55"/>
-      <c r="AB46" s="55"/>
-      <c r="AC46" s="55"/>
-      <c r="AD46" s="55"/>
-      <c r="AE46" s="55" t="s">
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="56"/>
+      <c r="U46" s="56"/>
+      <c r="V46" s="56"/>
+      <c r="W46" s="56"/>
+      <c r="X46" s="56"/>
+      <c r="Y46" s="56"/>
+      <c r="Z46" s="56"/>
+      <c r="AA46" s="56"/>
+      <c r="AB46" s="56"/>
+      <c r="AC46" s="56"/>
+      <c r="AD46" s="56"/>
+      <c r="AE46" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="55"/>
-      <c r="AG46" s="55"/>
-      <c r="AH46" s="55"/>
-      <c r="AI46" s="55"/>
-      <c r="AJ46" s="55"/>
-      <c r="AK46" s="55"/>
-      <c r="AL46" s="55"/>
-      <c r="AM46" s="55"/>
-      <c r="AN46" s="55"/>
-      <c r="AO46" s="50" t="s">
+      <c r="AF46" s="56"/>
+      <c r="AG46" s="56"/>
+      <c r="AH46" s="56"/>
+      <c r="AI46" s="56"/>
+      <c r="AJ46" s="56"/>
+      <c r="AK46" s="56"/>
+      <c r="AL46" s="56"/>
+      <c r="AM46" s="56"/>
+      <c r="AN46" s="56"/>
+      <c r="AO46" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="50"/>
-      <c r="AQ46" s="50" t="s">
+      <c r="AP46" s="52"/>
+      <c r="AQ46" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="50"/>
-      <c r="AS46" s="50" t="s">
+      <c r="AR46" s="52"/>
+      <c r="AS46" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="50"/>
-      <c r="AU46" s="50" t="s">
+      <c r="AT46" s="52"/>
+      <c r="AU46" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="50"/>
-      <c r="AW46" s="52" t="s">
+      <c r="AV46" s="52"/>
+      <c r="AW46" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="53"/>
-      <c r="AY46" s="53"/>
-      <c r="AZ46" s="53"/>
-      <c r="BA46" s="53"/>
-      <c r="BB46" s="53"/>
-      <c r="BC46" s="53"/>
-      <c r="BD46" s="53"/>
-      <c r="BE46" s="54"/>
-      <c r="BF46" s="50" t="s">
+      <c r="AX46" s="54"/>
+      <c r="AY46" s="54"/>
+      <c r="AZ46" s="54"/>
+      <c r="BA46" s="54"/>
+      <c r="BB46" s="54"/>
+      <c r="BC46" s="54"/>
+      <c r="BD46" s="54"/>
+      <c r="BE46" s="55"/>
+      <c r="BF46" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="50"/>
+      <c r="BG46" s="52"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -14181,85 +14181,11 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BY36:BZ36"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="BQ34:BR34"/>
-    <mergeCell ref="BS34:BT34"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AG34:AH34"/>
-    <mergeCell ref="AI34:AJ34"/>
-    <mergeCell ref="AK34:AL34"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
@@ -14270,12 +14196,86 @@
     <mergeCell ref="AG33:AH33"/>
     <mergeCell ref="AI33:AJ33"/>
     <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
     <mergeCell ref="U33:V33"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AG34:AH34"/>
+    <mergeCell ref="AI34:AJ34"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="BQ34:BR34"/>
+    <mergeCell ref="BS34:BT34"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rtl sim ok for sprite. testbench update
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="167">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -576,6 +576,30 @@
     <t>(nesx + scr) % 8=1</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ph</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -1107,16 +1131,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1129,6 +1150,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5261,12 +5285,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -5275,6 +5293,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9777,8 +9801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CF125"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AU47" sqref="AU47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -10030,62 +10054,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="50" t="s">
+      <c r="K33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50" t="s">
+      <c r="L33" s="52"/>
+      <c r="M33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50" t="s">
+      <c r="N33" s="52"/>
+      <c r="O33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50" t="s">
+      <c r="P33" s="52"/>
+      <c r="Q33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50" t="s">
+      <c r="R33" s="52"/>
+      <c r="S33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="50"/>
-      <c r="U33" s="50" t="s">
+      <c r="T33" s="52"/>
+      <c r="U33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="50"/>
-      <c r="W33" s="50" t="s">
+      <c r="V33" s="52"/>
+      <c r="W33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="50" t="s">
+      <c r="X33" s="52"/>
+      <c r="Y33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="50"/>
-      <c r="AA33" s="50" t="s">
+      <c r="Z33" s="52"/>
+      <c r="AA33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="50"/>
+      <c r="AB33" s="52"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="50" t="s">
+      <c r="AG33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="50"/>
-      <c r="AI33" s="50" t="s">
+      <c r="AH33" s="52"/>
+      <c r="AI33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="50"/>
-      <c r="AK33" s="50" t="s">
+      <c r="AJ33" s="52"/>
+      <c r="AK33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="50"/>
-      <c r="AM33" s="50" t="s">
+      <c r="AL33" s="52"/>
+      <c r="AM33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="50"/>
+      <c r="AN33" s="52"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -10108,104 +10132,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="52" t="s">
+      <c r="BO33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="53"/>
-      <c r="BQ33" s="52" t="s">
+      <c r="BP33" s="51"/>
+      <c r="BQ33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="53"/>
-      <c r="BS33" s="52" t="s">
+      <c r="BR33" s="51"/>
+      <c r="BS33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="53"/>
-      <c r="BU33" s="52" t="s">
+      <c r="BT33" s="51"/>
+      <c r="BU33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="53"/>
-      <c r="BW33" s="52" t="s">
+      <c r="BV33" s="51"/>
+      <c r="BW33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="53"/>
-      <c r="BY33" s="52" t="s">
+      <c r="BX33" s="51"/>
+      <c r="BY33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="53"/>
-      <c r="CA33" s="52" t="s">
+      <c r="BZ33" s="51"/>
+      <c r="CA33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="53"/>
-      <c r="CC33" s="52" t="s">
+      <c r="CB33" s="51"/>
+      <c r="CC33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="53"/>
-      <c r="CE33" s="52" t="s">
+      <c r="CD33" s="51"/>
+      <c r="CE33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="53"/>
+      <c r="CF33" s="51"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="50" t="s">
+      <c r="K34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50" t="s">
+      <c r="L34" s="52"/>
+      <c r="M34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50" t="s">
+      <c r="N34" s="52"/>
+      <c r="O34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50" t="s">
+      <c r="P34" s="52"/>
+      <c r="Q34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50" t="s">
+      <c r="R34" s="52"/>
+      <c r="S34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="50"/>
-      <c r="U34" s="50" t="s">
+      <c r="T34" s="52"/>
+      <c r="U34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="50"/>
-      <c r="W34" s="50" t="s">
+      <c r="V34" s="52"/>
+      <c r="W34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="50" t="s">
+      <c r="X34" s="52"/>
+      <c r="Y34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="50"/>
-      <c r="AA34" s="50" t="s">
+      <c r="Z34" s="52"/>
+      <c r="AA34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="50"/>
+      <c r="AB34" s="52"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="50" t="s">
+      <c r="AG34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="50"/>
-      <c r="AI34" s="50" t="s">
+      <c r="AH34" s="52"/>
+      <c r="AI34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="50"/>
-      <c r="AK34" s="50" t="s">
+      <c r="AJ34" s="52"/>
+      <c r="AK34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="50"/>
-      <c r="AM34" s="50" t="s">
+      <c r="AL34" s="52"/>
+      <c r="AM34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="50"/>
+      <c r="AN34" s="52"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -10228,42 +10252,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="52" t="s">
+      <c r="BO34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="53"/>
-      <c r="BQ34" s="52" t="s">
+      <c r="BP34" s="51"/>
+      <c r="BQ34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="53"/>
-      <c r="BS34" s="52" t="s">
+      <c r="BR34" s="51"/>
+      <c r="BS34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="53"/>
-      <c r="BU34" s="52" t="s">
+      <c r="BT34" s="51"/>
+      <c r="BU34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="53"/>
-      <c r="BW34" s="52" t="s">
+      <c r="BV34" s="51"/>
+      <c r="BW34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="53"/>
-      <c r="BY34" s="52" t="s">
+      <c r="BX34" s="51"/>
+      <c r="BY34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="53"/>
-      <c r="CA34" s="52" t="s">
+      <c r="BZ34" s="51"/>
+      <c r="CA34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="53"/>
-      <c r="CC34" s="52" t="s">
+      <c r="CB34" s="51"/>
+      <c r="CC34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="53"/>
-      <c r="CE34" s="52" t="s">
+      <c r="CD34" s="51"/>
+      <c r="CE34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="53"/>
+      <c r="CF34" s="51"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -10277,62 +10301,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="51" t="s">
+      <c r="K36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51" t="s">
+      <c r="L36" s="57"/>
+      <c r="M36" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="51"/>
-      <c r="O36" s="51" t="s">
+      <c r="N36" s="57"/>
+      <c r="O36" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="51" t="s">
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="51"/>
-      <c r="S36" s="51" t="s">
+      <c r="R36" s="57"/>
+      <c r="S36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="51"/>
-      <c r="U36" s="51" t="s">
+      <c r="T36" s="57"/>
+      <c r="U36" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="51"/>
-      <c r="W36" s="51" t="s">
+      <c r="V36" s="57"/>
+      <c r="W36" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="51"/>
-      <c r="Y36" s="51" t="s">
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="51"/>
-      <c r="AA36" s="51" t="s">
+      <c r="Z36" s="57"/>
+      <c r="AA36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="51"/>
+      <c r="AB36" s="57"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="51" t="s">
+      <c r="AG36" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="51"/>
-      <c r="AI36" s="51" t="s">
+      <c r="AH36" s="57"/>
+      <c r="AI36" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="51"/>
-      <c r="AK36" s="51" t="s">
+      <c r="AJ36" s="57"/>
+      <c r="AK36" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="51"/>
-      <c r="AM36" s="51" t="s">
+      <c r="AL36" s="57"/>
+      <c r="AM36" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="51"/>
+      <c r="AN36" s="57"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -10355,42 +10379,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="52" t="s">
+      <c r="BO36" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="53"/>
-      <c r="BQ36" s="52" t="s">
+      <c r="BP36" s="51"/>
+      <c r="BQ36" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="53"/>
-      <c r="BS36" s="52" t="s">
+      <c r="BR36" s="51"/>
+      <c r="BS36" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="53"/>
-      <c r="BU36" s="52" t="s">
+      <c r="BT36" s="51"/>
+      <c r="BU36" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="53"/>
-      <c r="BW36" s="52" t="s">
+      <c r="BV36" s="51"/>
+      <c r="BW36" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="53"/>
-      <c r="BY36" s="52" t="s">
+      <c r="BX36" s="51"/>
+      <c r="BY36" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="53"/>
-      <c r="CA36" s="52" t="s">
+      <c r="BZ36" s="51"/>
+      <c r="CA36" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="53"/>
-      <c r="CC36" s="52" t="s">
+      <c r="CB36" s="51"/>
+      <c r="CC36" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="53"/>
-      <c r="CE36" s="52" t="s">
+      <c r="CD36" s="51"/>
+      <c r="CE36" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="53"/>
+      <c r="CF36" s="51"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -10726,58 +10750,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="50" t="s">
+      <c r="M42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50" t="s">
+      <c r="N42" s="52"/>
+      <c r="O42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50" t="s">
+      <c r="P42" s="52"/>
+      <c r="Q42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="50"/>
-      <c r="S42" s="50" t="s">
+      <c r="R42" s="52"/>
+      <c r="S42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="50"/>
-      <c r="U42" s="50" t="s">
+      <c r="T42" s="52"/>
+      <c r="U42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="50"/>
-      <c r="W42" s="50" t="s">
+      <c r="V42" s="52"/>
+      <c r="W42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="50"/>
-      <c r="Y42" s="50" t="s">
+      <c r="X42" s="52"/>
+      <c r="Y42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="50"/>
-      <c r="AA42" s="50" t="s">
+      <c r="Z42" s="52"/>
+      <c r="AA42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="50"/>
+      <c r="AB42" s="52"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="50" t="s">
+      <c r="AG42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="50"/>
-      <c r="AI42" s="50" t="s">
+      <c r="AH42" s="52"/>
+      <c r="AI42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="50"/>
-      <c r="AK42" s="50" t="s">
+      <c r="AJ42" s="52"/>
+      <c r="AK42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="50"/>
-      <c r="AM42" s="50" t="s">
+      <c r="AL42" s="52"/>
+      <c r="AM42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="50"/>
+      <c r="AN42" s="52"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -10800,42 +10824,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="52" t="s">
+      <c r="BO42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="53"/>
-      <c r="BQ42" s="52" t="s">
+      <c r="BP42" s="51"/>
+      <c r="BQ42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="53"/>
-      <c r="BS42" s="52" t="s">
+      <c r="BR42" s="51"/>
+      <c r="BS42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="53"/>
-      <c r="BU42" s="52" t="s">
+      <c r="BT42" s="51"/>
+      <c r="BU42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="53"/>
-      <c r="BW42" s="52" t="s">
+      <c r="BV42" s="51"/>
+      <c r="BW42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="53"/>
-      <c r="BY42" s="52" t="s">
+      <c r="BX42" s="51"/>
+      <c r="BY42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="53"/>
-      <c r="CA42" s="52" t="s">
+      <c r="BZ42" s="51"/>
+      <c r="CA42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="53"/>
-      <c r="CC42" s="52" t="s">
+      <c r="CB42" s="51"/>
+      <c r="CC42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="53"/>
-      <c r="CE42" s="52" t="s">
+      <c r="CD42" s="51"/>
+      <c r="CE42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="53"/>
+      <c r="CF42" s="51"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -10868,71 +10892,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="57" t="s">
+      <c r="K46" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="57"/>
-      <c r="O46" s="57"/>
-      <c r="P46" s="57"/>
-      <c r="Q46" s="57"/>
-      <c r="R46" s="57"/>
-      <c r="S46" s="57"/>
-      <c r="T46" s="57"/>
-      <c r="U46" s="57"/>
-      <c r="V46" s="57"/>
-      <c r="W46" s="57"/>
-      <c r="X46" s="57"/>
-      <c r="Y46" s="57"/>
-      <c r="Z46" s="57"/>
-      <c r="AA46" s="57"/>
-      <c r="AB46" s="57"/>
-      <c r="AC46" s="57"/>
-      <c r="AD46" s="57"/>
-      <c r="AE46" s="57" t="s">
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="56"/>
+      <c r="U46" s="56"/>
+      <c r="V46" s="56"/>
+      <c r="W46" s="56"/>
+      <c r="X46" s="56"/>
+      <c r="Y46" s="56"/>
+      <c r="Z46" s="56"/>
+      <c r="AA46" s="56"/>
+      <c r="AB46" s="56"/>
+      <c r="AC46" s="56"/>
+      <c r="AD46" s="56"/>
+      <c r="AE46" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="57"/>
-      <c r="AG46" s="57"/>
-      <c r="AH46" s="57"/>
-      <c r="AI46" s="57"/>
-      <c r="AJ46" s="57"/>
-      <c r="AK46" s="57"/>
-      <c r="AL46" s="57"/>
-      <c r="AM46" s="57"/>
-      <c r="AN46" s="57"/>
-      <c r="AO46" s="50" t="s">
+      <c r="AF46" s="56"/>
+      <c r="AG46" s="56"/>
+      <c r="AH46" s="56"/>
+      <c r="AI46" s="56"/>
+      <c r="AJ46" s="56"/>
+      <c r="AK46" s="56"/>
+      <c r="AL46" s="56"/>
+      <c r="AM46" s="56"/>
+      <c r="AN46" s="56"/>
+      <c r="AO46" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="50"/>
-      <c r="AQ46" s="50" t="s">
+      <c r="AP46" s="52"/>
+      <c r="AQ46" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="50"/>
-      <c r="AS46" s="50" t="s">
+      <c r="AR46" s="52"/>
+      <c r="AS46" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="50"/>
-      <c r="AU46" s="50" t="s">
+      <c r="AT46" s="52"/>
+      <c r="AU46" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="50"/>
-      <c r="AW46" s="54" t="s">
+      <c r="AV46" s="52"/>
+      <c r="AW46" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="55"/>
-      <c r="AY46" s="55"/>
-      <c r="AZ46" s="55"/>
-      <c r="BA46" s="55"/>
-      <c r="BB46" s="55"/>
-      <c r="BC46" s="55"/>
-      <c r="BD46" s="55"/>
-      <c r="BE46" s="56"/>
-      <c r="BF46" s="50" t="s">
+      <c r="AX46" s="54"/>
+      <c r="AY46" s="54"/>
+      <c r="AZ46" s="54"/>
+      <c r="BA46" s="54"/>
+      <c r="BB46" s="54"/>
+      <c r="BC46" s="54"/>
+      <c r="BD46" s="54"/>
+      <c r="BE46" s="55"/>
+      <c r="BF46" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="50"/>
+      <c r="BG46" s="52"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -10957,6 +10981,26 @@
       <c r="CD46" s="38"/>
       <c r="CE46" s="38"/>
       <c r="CF46" s="27"/>
+    </row>
+    <row r="47" spans="6:84">
+      <c r="AO47" t="s">
+        <v>162</v>
+      </c>
+      <c r="AP47" t="s">
+        <v>164</v>
+      </c>
+      <c r="AQ47" t="s">
+        <v>163</v>
+      </c>
+      <c r="AR47" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS47" t="s">
+        <v>165</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="52" spans="5:71" ht="14.25" thickBot="1">
       <c r="E52" t="s">
@@ -14494,21 +14538,70 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BY36:BZ36"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AG34:AH34"/>
+    <mergeCell ref="AI34:AJ34"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
     <mergeCell ref="BO33:BP33"/>
     <mergeCell ref="BO34:BP34"/>
     <mergeCell ref="CA33:CB33"/>
@@ -14525,70 +14618,21 @@
     <mergeCell ref="BY34:BZ34"/>
     <mergeCell ref="CA34:CB34"/>
     <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AG34:AH34"/>
-    <mergeCell ref="AI34:AJ34"/>
-    <mergeCell ref="AK34:AL34"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BY36:BZ36"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15304,11 +15348,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:CB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AK37" sqref="AK37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:80" s="27" customFormat="1" ht="42">
       <c r="F2" s="27">
@@ -15524,62 +15571,62 @@
         <v>0</v>
       </c>
       <c r="F3" s="39"/>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50" t="s">
+      <c r="H3" s="52"/>
+      <c r="I3" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50" t="s">
+      <c r="J3" s="52"/>
+      <c r="K3" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50" t="s">
+      <c r="L3" s="52"/>
+      <c r="M3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50" t="s">
+      <c r="N3" s="52"/>
+      <c r="O3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50" t="s">
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50" t="s">
+      <c r="R3" s="52"/>
+      <c r="S3" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50" t="s">
+      <c r="T3" s="52"/>
+      <c r="U3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50" t="s">
+      <c r="V3" s="52"/>
+      <c r="W3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="X3" s="50"/>
+      <c r="X3" s="52"/>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="50" t="s">
+      <c r="AC3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="50"/>
-      <c r="AE3" s="50" t="s">
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="50" t="s">
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="50"/>
-      <c r="AI3" s="50" t="s">
+      <c r="AH3" s="52"/>
+      <c r="AI3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AJ3" s="50"/>
+      <c r="AJ3" s="52"/>
       <c r="AK3" s="34"/>
       <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
@@ -15602,104 +15649,104 @@
       <c r="BH3" s="34"/>
       <c r="BI3" s="34"/>
       <c r="BJ3" s="34"/>
-      <c r="BK3" s="52" t="s">
+      <c r="BK3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="52" t="s">
+      <c r="BL3" s="51"/>
+      <c r="BM3" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="52" t="s">
+      <c r="BN3" s="51"/>
+      <c r="BO3" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="52" t="s">
+      <c r="BP3" s="51"/>
+      <c r="BQ3" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="52" t="s">
+      <c r="BR3" s="51"/>
+      <c r="BS3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="52" t="s">
+      <c r="BT3" s="51"/>
+      <c r="BU3" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="52" t="s">
+      <c r="BV3" s="51"/>
+      <c r="BW3" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BX3" s="53"/>
-      <c r="BY3" s="52" t="s">
+      <c r="BX3" s="51"/>
+      <c r="BY3" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BZ3" s="53"/>
-      <c r="CA3" s="52" t="s">
+      <c r="BZ3" s="51"/>
+      <c r="CA3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CB3" s="53"/>
+      <c r="CB3" s="51"/>
     </row>
     <row r="4" spans="2:80">
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="34"/>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50" t="s">
+      <c r="H4" s="52"/>
+      <c r="I4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50" t="s">
+      <c r="J4" s="52"/>
+      <c r="K4" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50" t="s">
+      <c r="L4" s="52"/>
+      <c r="M4" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50" t="s">
+      <c r="N4" s="52"/>
+      <c r="O4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50" t="s">
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50" t="s">
+      <c r="R4" s="52"/>
+      <c r="S4" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50" t="s">
+      <c r="T4" s="52"/>
+      <c r="U4" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50" t="s">
+      <c r="V4" s="52"/>
+      <c r="W4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="50"/>
+      <c r="X4" s="52"/>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="50" t="s">
+      <c r="AC4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="50" t="s">
+      <c r="AD4" s="52"/>
+      <c r="AE4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50" t="s">
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50" t="s">
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="50"/>
+      <c r="AJ4" s="52"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
@@ -15722,42 +15769,42 @@
       <c r="BH4" s="34"/>
       <c r="BI4" s="34"/>
       <c r="BJ4" s="34"/>
-      <c r="BK4" s="52" t="s">
+      <c r="BK4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BL4" s="53"/>
-      <c r="BM4" s="52" t="s">
+      <c r="BL4" s="51"/>
+      <c r="BM4" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BN4" s="53"/>
-      <c r="BO4" s="52" t="s">
+      <c r="BN4" s="51"/>
+      <c r="BO4" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BP4" s="53"/>
-      <c r="BQ4" s="52" t="s">
+      <c r="BP4" s="51"/>
+      <c r="BQ4" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BR4" s="53"/>
-      <c r="BS4" s="52" t="s">
+      <c r="BR4" s="51"/>
+      <c r="BS4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BT4" s="53"/>
-      <c r="BU4" s="52" t="s">
+      <c r="BT4" s="51"/>
+      <c r="BU4" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BV4" s="53"/>
-      <c r="BW4" s="52" t="s">
+      <c r="BV4" s="51"/>
+      <c r="BW4" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="53"/>
-      <c r="BY4" s="52" t="s">
+      <c r="BX4" s="51"/>
+      <c r="BY4" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BZ4" s="53"/>
-      <c r="CA4" s="52" t="s">
+      <c r="BZ4" s="51"/>
+      <c r="CA4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CB4" s="53"/>
+      <c r="CB4" s="51"/>
     </row>
     <row r="5" spans="2:80">
       <c r="BX5" s="27"/>
@@ -15771,62 +15818,62 @@
         <v>239</v>
       </c>
       <c r="F6" s="36"/>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51" t="s">
+      <c r="H6" s="57"/>
+      <c r="I6" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51" t="s">
+      <c r="J6" s="57"/>
+      <c r="K6" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51" t="s">
+      <c r="L6" s="57"/>
+      <c r="M6" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51" t="s">
+      <c r="N6" s="57"/>
+      <c r="O6" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="51" t="s">
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="R6" s="51"/>
-      <c r="S6" s="51" t="s">
+      <c r="R6" s="57"/>
+      <c r="S6" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="51"/>
-      <c r="U6" s="51" t="s">
+      <c r="T6" s="57"/>
+      <c r="U6" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51" t="s">
+      <c r="V6" s="57"/>
+      <c r="W6" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="X6" s="51"/>
+      <c r="X6" s="57"/>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AC6" s="51" t="s">
+      <c r="AC6" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" s="51"/>
-      <c r="AE6" s="51" t="s">
+      <c r="AD6" s="57"/>
+      <c r="AE6" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51" t="s">
+      <c r="AF6" s="57"/>
+      <c r="AG6" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="AH6" s="51"/>
-      <c r="AI6" s="51" t="s">
+      <c r="AH6" s="57"/>
+      <c r="AI6" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="AJ6" s="51"/>
+      <c r="AJ6" s="57"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -15849,42 +15896,42 @@
       <c r="BH6" s="34"/>
       <c r="BI6" s="34"/>
       <c r="BJ6" s="34"/>
-      <c r="BK6" s="52" t="s">
+      <c r="BK6" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BL6" s="53"/>
-      <c r="BM6" s="52" t="s">
+      <c r="BL6" s="51"/>
+      <c r="BM6" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BN6" s="53"/>
-      <c r="BO6" s="52" t="s">
+      <c r="BN6" s="51"/>
+      <c r="BO6" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BP6" s="53"/>
-      <c r="BQ6" s="52" t="s">
+      <c r="BP6" s="51"/>
+      <c r="BQ6" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BR6" s="53"/>
-      <c r="BS6" s="52" t="s">
+      <c r="BR6" s="51"/>
+      <c r="BS6" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BT6" s="53"/>
-      <c r="BU6" s="52" t="s">
+      <c r="BT6" s="51"/>
+      <c r="BU6" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BV6" s="53"/>
-      <c r="BW6" s="52" t="s">
+      <c r="BV6" s="51"/>
+      <c r="BW6" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BX6" s="53"/>
-      <c r="BY6" s="52" t="s">
+      <c r="BX6" s="51"/>
+      <c r="BY6" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BZ6" s="53"/>
-      <c r="CA6" s="52" t="s">
+      <c r="BZ6" s="51"/>
+      <c r="CA6" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CB6" s="53"/>
+      <c r="CB6" s="51"/>
     </row>
     <row r="7" spans="2:80">
       <c r="E7">
@@ -16220,58 +16267,58 @@
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="50" t="s">
+      <c r="I12" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50" t="s">
+      <c r="J12" s="52"/>
+      <c r="K12" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50" t="s">
+      <c r="L12" s="52"/>
+      <c r="M12" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50" t="s">
+      <c r="N12" s="52"/>
+      <c r="O12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50" t="s">
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50" t="s">
+      <c r="R12" s="52"/>
+      <c r="S12" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50" t="s">
+      <c r="T12" s="52"/>
+      <c r="U12" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50" t="s">
+      <c r="V12" s="52"/>
+      <c r="W12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="50"/>
+      <c r="X12" s="52"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="50" t="s">
+      <c r="AC12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="50"/>
-      <c r="AE12" s="50" t="s">
+      <c r="AD12" s="52"/>
+      <c r="AE12" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AF12" s="50"/>
-      <c r="AG12" s="50" t="s">
+      <c r="AF12" s="52"/>
+      <c r="AG12" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AH12" s="50"/>
-      <c r="AI12" s="50" t="s">
+      <c r="AH12" s="52"/>
+      <c r="AI12" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AJ12" s="50"/>
+      <c r="AJ12" s="52"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="34"/>
       <c r="AM12" s="34"/>
@@ -16294,42 +16341,42 @@
       <c r="BH12" s="34"/>
       <c r="BI12" s="34"/>
       <c r="BJ12" s="34"/>
-      <c r="BK12" s="52" t="s">
+      <c r="BK12" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BL12" s="53"/>
-      <c r="BM12" s="52" t="s">
+      <c r="BL12" s="51"/>
+      <c r="BM12" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BN12" s="53"/>
-      <c r="BO12" s="52" t="s">
+      <c r="BN12" s="51"/>
+      <c r="BO12" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BP12" s="53"/>
-      <c r="BQ12" s="52" t="s">
+      <c r="BP12" s="51"/>
+      <c r="BQ12" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BR12" s="53"/>
-      <c r="BS12" s="52" t="s">
+      <c r="BR12" s="51"/>
+      <c r="BS12" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BT12" s="53"/>
-      <c r="BU12" s="52" t="s">
+      <c r="BT12" s="51"/>
+      <c r="BU12" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="BV12" s="53"/>
-      <c r="BW12" s="52" t="s">
+      <c r="BV12" s="51"/>
+      <c r="BW12" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BX12" s="53"/>
-      <c r="BY12" s="52" t="s">
+      <c r="BX12" s="51"/>
+      <c r="BY12" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="BZ12" s="53"/>
-      <c r="CA12" s="52" t="s">
+      <c r="BZ12" s="51"/>
+      <c r="CA12" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="CB12" s="53"/>
+      <c r="CB12" s="51"/>
     </row>
     <row r="13" spans="2:80">
       <c r="BX13" s="27"/>
@@ -16362,71 +16409,71 @@
         <v>120</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="57" t="s">
+      <c r="G16" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
-      <c r="U16" s="57"/>
-      <c r="V16" s="57"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
-      <c r="Y16" s="57"/>
-      <c r="Z16" s="57"/>
-      <c r="AA16" s="57" t="s">
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="AB16" s="57"/>
-      <c r="AC16" s="57"/>
-      <c r="AD16" s="57"/>
-      <c r="AE16" s="57"/>
-      <c r="AF16" s="57"/>
-      <c r="AG16" s="57"/>
-      <c r="AH16" s="57"/>
-      <c r="AI16" s="57"/>
-      <c r="AJ16" s="57"/>
-      <c r="AK16" s="50" t="s">
+      <c r="AB16" s="56"/>
+      <c r="AC16" s="56"/>
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="56"/>
+      <c r="AH16" s="56"/>
+      <c r="AI16" s="56"/>
+      <c r="AJ16" s="56"/>
+      <c r="AK16" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="AL16" s="50"/>
-      <c r="AM16" s="50" t="s">
+      <c r="AL16" s="52"/>
+      <c r="AM16" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="AN16" s="50"/>
-      <c r="AO16" s="50" t="s">
+      <c r="AN16" s="52"/>
+      <c r="AO16" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="AP16" s="50"/>
-      <c r="AQ16" s="50" t="s">
+      <c r="AP16" s="52"/>
+      <c r="AQ16" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="AR16" s="50"/>
-      <c r="AS16" s="54" t="s">
+      <c r="AR16" s="52"/>
+      <c r="AS16" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="AT16" s="55"/>
-      <c r="AU16" s="55"/>
-      <c r="AV16" s="55"/>
-      <c r="AW16" s="55"/>
-      <c r="AX16" s="55"/>
-      <c r="AY16" s="55"/>
-      <c r="AZ16" s="55"/>
-      <c r="BA16" s="56"/>
-      <c r="BB16" s="50" t="s">
+      <c r="AT16" s="54"/>
+      <c r="AU16" s="54"/>
+      <c r="AV16" s="54"/>
+      <c r="AW16" s="54"/>
+      <c r="AX16" s="54"/>
+      <c r="AY16" s="54"/>
+      <c r="AZ16" s="54"/>
+      <c r="BA16" s="55"/>
+      <c r="BB16" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="BC16" s="50"/>
+      <c r="BC16" s="52"/>
       <c r="BE16" s="38"/>
       <c r="BF16" s="38"/>
       <c r="BG16" s="38"/>
@@ -16975,6 +17022,85 @@
     </row>
   </sheetData>
   <mergeCells count="95">
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="BU3:BV3"/>
+    <mergeCell ref="BW3:BX3"/>
+    <mergeCell ref="BY3:BZ3"/>
+    <mergeCell ref="CA3:CB3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
     <mergeCell ref="BB16:BC16"/>
     <mergeCell ref="BW12:BX12"/>
     <mergeCell ref="BY12:BZ12"/>
@@ -16991,85 +17117,6 @@
     <mergeCell ref="BO12:BP12"/>
     <mergeCell ref="BQ12:BR12"/>
     <mergeCell ref="BS12:BT12"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="BU3:BV3"/>
-    <mergeCell ref="BW3:BX3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="CA3:CB3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
debug sprite on gate leve
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="display" sheetId="3" r:id="rId3"/>
     <sheet name="motones vga" sheetId="4" r:id="rId4"/>
     <sheet name="pattern fetch" sheetId="5" r:id="rId5"/>
-    <sheet name="vram access" sheetId="6" r:id="rId6"/>
-    <sheet name="scroll" sheetId="7" r:id="rId7"/>
+    <sheet name="scroll" sheetId="7" r:id="rId6"/>
+    <sheet name="vram access" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1131,13 +1131,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1150,9 +1153,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3687,6 +3687,286 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10586</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="右中かっこ 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="19054761" y="7424740"/>
+          <a:ext cx="182034" cy="458258"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 69079"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>26559</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="右中かっこ 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8216321" y="6728405"/>
+          <a:ext cx="198008" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 69079"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047750" y="4486275"/>
+          <a:ext cx="3352800" cy="2390775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="4476750"/>
+          <a:ext cx="3352800" cy="2390775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6286500" y="4476750"/>
+          <a:ext cx="3352800" cy="2390775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -4166,284 +4446,51 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>77</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>80</xdr:col>
-      <xdr:colOff>10582</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>10586</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="右中かっこ 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="19054761" y="7424740"/>
-          <a:ext cx="182034" cy="458258"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightBrace">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 69079"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>26559</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="右中かっこ 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="8216321" y="6728405"/>
-          <a:ext cx="198008" cy="1866900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightBrace">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 69079"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="正方形/長方形 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1047750" y="4486275"/>
-          <a:ext cx="3352800" cy="2390775"/>
+          <a:off x="685800" y="17316450"/>
+          <a:ext cx="12868275" cy="7715250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6076950" y="4476750"/>
-          <a:ext cx="3352800" cy="2390775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>70</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="正方形/長方形 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6286500" y="4476750"/>
-          <a:ext cx="3352800" cy="2390775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5285,6 +5332,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -5293,12 +5346,6 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9801,7 +9848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CF125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AU47" sqref="AU47"/>
     </sheetView>
   </sheetViews>
@@ -10054,62 +10101,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="52" t="s">
+      <c r="K33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52" t="s">
+      <c r="L33" s="50"/>
+      <c r="M33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52" t="s">
+      <c r="N33" s="50"/>
+      <c r="O33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52" t="s">
+      <c r="P33" s="50"/>
+      <c r="Q33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52" t="s">
+      <c r="R33" s="50"/>
+      <c r="S33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52" t="s">
+      <c r="T33" s="50"/>
+      <c r="U33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52" t="s">
+      <c r="V33" s="50"/>
+      <c r="W33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52" t="s">
+      <c r="X33" s="50"/>
+      <c r="Y33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="52" t="s">
+      <c r="Z33" s="50"/>
+      <c r="AA33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="52"/>
+      <c r="AB33" s="50"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="52" t="s">
+      <c r="AG33" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="52"/>
-      <c r="AI33" s="52" t="s">
+      <c r="AH33" s="50"/>
+      <c r="AI33" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="52"/>
-      <c r="AK33" s="52" t="s">
+      <c r="AJ33" s="50"/>
+      <c r="AK33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="52"/>
-      <c r="AM33" s="52" t="s">
+      <c r="AL33" s="50"/>
+      <c r="AM33" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="52"/>
+      <c r="AN33" s="50"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -10132,104 +10179,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="50" t="s">
+      <c r="BO33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="51"/>
-      <c r="BQ33" s="50" t="s">
+      <c r="BP33" s="53"/>
+      <c r="BQ33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="51"/>
-      <c r="BS33" s="50" t="s">
+      <c r="BR33" s="53"/>
+      <c r="BS33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="51"/>
-      <c r="BU33" s="50" t="s">
+      <c r="BT33" s="53"/>
+      <c r="BU33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="51"/>
-      <c r="BW33" s="50" t="s">
+      <c r="BV33" s="53"/>
+      <c r="BW33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="51"/>
-      <c r="BY33" s="50" t="s">
+      <c r="BX33" s="53"/>
+      <c r="BY33" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="51"/>
-      <c r="CA33" s="50" t="s">
+      <c r="BZ33" s="53"/>
+      <c r="CA33" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="51"/>
-      <c r="CC33" s="50" t="s">
+      <c r="CB33" s="53"/>
+      <c r="CC33" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="51"/>
-      <c r="CE33" s="50" t="s">
+      <c r="CD33" s="53"/>
+      <c r="CE33" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="51"/>
+      <c r="CF33" s="53"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="52" t="s">
+      <c r="K34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52" t="s">
+      <c r="L34" s="50"/>
+      <c r="M34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52" t="s">
+      <c r="N34" s="50"/>
+      <c r="O34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52" t="s">
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52" t="s">
+      <c r="R34" s="50"/>
+      <c r="S34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52" t="s">
+      <c r="T34" s="50"/>
+      <c r="U34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="52"/>
-      <c r="W34" s="52" t="s">
+      <c r="V34" s="50"/>
+      <c r="W34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52" t="s">
+      <c r="X34" s="50"/>
+      <c r="Y34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="52" t="s">
+      <c r="Z34" s="50"/>
+      <c r="AA34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="52"/>
+      <c r="AB34" s="50"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="52" t="s">
+      <c r="AG34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="52"/>
-      <c r="AI34" s="52" t="s">
+      <c r="AH34" s="50"/>
+      <c r="AI34" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="52"/>
-      <c r="AK34" s="52" t="s">
+      <c r="AJ34" s="50"/>
+      <c r="AK34" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="52"/>
-      <c r="AM34" s="52" t="s">
+      <c r="AL34" s="50"/>
+      <c r="AM34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="52"/>
+      <c r="AN34" s="50"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -10252,42 +10299,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="50" t="s">
+      <c r="BO34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="51"/>
-      <c r="BQ34" s="50" t="s">
+      <c r="BP34" s="53"/>
+      <c r="BQ34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="51"/>
-      <c r="BS34" s="50" t="s">
+      <c r="BR34" s="53"/>
+      <c r="BS34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="51"/>
-      <c r="BU34" s="50" t="s">
+      <c r="BT34" s="53"/>
+      <c r="BU34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="51"/>
-      <c r="BW34" s="50" t="s">
+      <c r="BV34" s="53"/>
+      <c r="BW34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="51"/>
-      <c r="BY34" s="50" t="s">
+      <c r="BX34" s="53"/>
+      <c r="BY34" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="51"/>
-      <c r="CA34" s="50" t="s">
+      <c r="BZ34" s="53"/>
+      <c r="CA34" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="51"/>
-      <c r="CC34" s="50" t="s">
+      <c r="CB34" s="53"/>
+      <c r="CC34" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="51"/>
-      <c r="CE34" s="50" t="s">
+      <c r="CD34" s="53"/>
+      <c r="CE34" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="51"/>
+      <c r="CF34" s="53"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -10301,62 +10348,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="57" t="s">
+      <c r="K36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57" t="s">
+      <c r="L36" s="51"/>
+      <c r="M36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57" t="s">
+      <c r="N36" s="51"/>
+      <c r="O36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57" t="s">
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="57"/>
-      <c r="S36" s="57" t="s">
+      <c r="R36" s="51"/>
+      <c r="S36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="57"/>
-      <c r="U36" s="57" t="s">
+      <c r="T36" s="51"/>
+      <c r="U36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="57"/>
-      <c r="W36" s="57" t="s">
+      <c r="V36" s="51"/>
+      <c r="W36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="57"/>
-      <c r="Y36" s="57" t="s">
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="57"/>
-      <c r="AA36" s="57" t="s">
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="57"/>
+      <c r="AB36" s="51"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="57" t="s">
+      <c r="AG36" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="57"/>
-      <c r="AI36" s="57" t="s">
+      <c r="AH36" s="51"/>
+      <c r="AI36" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="57"/>
-      <c r="AK36" s="57" t="s">
+      <c r="AJ36" s="51"/>
+      <c r="AK36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="57"/>
-      <c r="AM36" s="57" t="s">
+      <c r="AL36" s="51"/>
+      <c r="AM36" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="57"/>
+      <c r="AN36" s="51"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -10379,42 +10426,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="50" t="s">
+      <c r="BO36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="51"/>
-      <c r="BQ36" s="50" t="s">
+      <c r="BP36" s="53"/>
+      <c r="BQ36" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="51"/>
-      <c r="BS36" s="50" t="s">
+      <c r="BR36" s="53"/>
+      <c r="BS36" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="51"/>
-      <c r="BU36" s="50" t="s">
+      <c r="BT36" s="53"/>
+      <c r="BU36" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="51"/>
-      <c r="BW36" s="50" t="s">
+      <c r="BV36" s="53"/>
+      <c r="BW36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="51"/>
-      <c r="BY36" s="50" t="s">
+      <c r="BX36" s="53"/>
+      <c r="BY36" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="51"/>
-      <c r="CA36" s="50" t="s">
+      <c r="BZ36" s="53"/>
+      <c r="CA36" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="51"/>
-      <c r="CC36" s="50" t="s">
+      <c r="CB36" s="53"/>
+      <c r="CC36" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="51"/>
-      <c r="CE36" s="50" t="s">
+      <c r="CD36" s="53"/>
+      <c r="CE36" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="51"/>
+      <c r="CF36" s="53"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -10750,58 +10797,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="52" t="s">
+      <c r="M42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52" t="s">
+      <c r="N42" s="50"/>
+      <c r="O42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52" t="s">
+      <c r="P42" s="50"/>
+      <c r="Q42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="52"/>
-      <c r="S42" s="52" t="s">
+      <c r="R42" s="50"/>
+      <c r="S42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52" t="s">
+      <c r="T42" s="50"/>
+      <c r="U42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="52"/>
-      <c r="W42" s="52" t="s">
+      <c r="V42" s="50"/>
+      <c r="W42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="52"/>
-      <c r="Y42" s="52" t="s">
+      <c r="X42" s="50"/>
+      <c r="Y42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="52" t="s">
+      <c r="Z42" s="50"/>
+      <c r="AA42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="52"/>
+      <c r="AB42" s="50"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="52" t="s">
+      <c r="AG42" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="52"/>
-      <c r="AI42" s="52" t="s">
+      <c r="AH42" s="50"/>
+      <c r="AI42" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="52"/>
-      <c r="AK42" s="52" t="s">
+      <c r="AJ42" s="50"/>
+      <c r="AK42" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="52"/>
-      <c r="AM42" s="52" t="s">
+      <c r="AL42" s="50"/>
+      <c r="AM42" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="52"/>
+      <c r="AN42" s="50"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -10824,42 +10871,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="50" t="s">
+      <c r="BO42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="51"/>
-      <c r="BQ42" s="50" t="s">
+      <c r="BP42" s="53"/>
+      <c r="BQ42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="51"/>
-      <c r="BS42" s="50" t="s">
+      <c r="BR42" s="53"/>
+      <c r="BS42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="51"/>
-      <c r="BU42" s="50" t="s">
+      <c r="BT42" s="53"/>
+      <c r="BU42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="51"/>
-      <c r="BW42" s="50" t="s">
+      <c r="BV42" s="53"/>
+      <c r="BW42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="51"/>
-      <c r="BY42" s="50" t="s">
+      <c r="BX42" s="53"/>
+      <c r="BY42" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="51"/>
-      <c r="CA42" s="50" t="s">
+      <c r="BZ42" s="53"/>
+      <c r="CA42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="51"/>
-      <c r="CC42" s="50" t="s">
+      <c r="CB42" s="53"/>
+      <c r="CC42" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="51"/>
-      <c r="CE42" s="50" t="s">
+      <c r="CD42" s="53"/>
+      <c r="CE42" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="51"/>
+      <c r="CF42" s="53"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -10892,71 +10939,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="56" t="s">
+      <c r="K46" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
-      <c r="T46" s="56"/>
-      <c r="U46" s="56"/>
-      <c r="V46" s="56"/>
-      <c r="W46" s="56"/>
-      <c r="X46" s="56"/>
-      <c r="Y46" s="56"/>
-      <c r="Z46" s="56"/>
-      <c r="AA46" s="56"/>
-      <c r="AB46" s="56"/>
-      <c r="AC46" s="56"/>
-      <c r="AD46" s="56"/>
-      <c r="AE46" s="56" t="s">
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="57"/>
+      <c r="R46" s="57"/>
+      <c r="S46" s="57"/>
+      <c r="T46" s="57"/>
+      <c r="U46" s="57"/>
+      <c r="V46" s="57"/>
+      <c r="W46" s="57"/>
+      <c r="X46" s="57"/>
+      <c r="Y46" s="57"/>
+      <c r="Z46" s="57"/>
+      <c r="AA46" s="57"/>
+      <c r="AB46" s="57"/>
+      <c r="AC46" s="57"/>
+      <c r="AD46" s="57"/>
+      <c r="AE46" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="56"/>
-      <c r="AG46" s="56"/>
-      <c r="AH46" s="56"/>
-      <c r="AI46" s="56"/>
-      <c r="AJ46" s="56"/>
-      <c r="AK46" s="56"/>
-      <c r="AL46" s="56"/>
-      <c r="AM46" s="56"/>
-      <c r="AN46" s="56"/>
-      <c r="AO46" s="52" t="s">
+      <c r="AF46" s="57"/>
+      <c r="AG46" s="57"/>
+      <c r="AH46" s="57"/>
+      <c r="AI46" s="57"/>
+      <c r="AJ46" s="57"/>
+      <c r="AK46" s="57"/>
+      <c r="AL46" s="57"/>
+      <c r="AM46" s="57"/>
+      <c r="AN46" s="57"/>
+      <c r="AO46" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="52"/>
-      <c r="AQ46" s="52" t="s">
+      <c r="AP46" s="50"/>
+      <c r="AQ46" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="52"/>
-      <c r="AS46" s="52" t="s">
+      <c r="AR46" s="50"/>
+      <c r="AS46" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="52"/>
-      <c r="AU46" s="52" t="s">
+      <c r="AT46" s="50"/>
+      <c r="AU46" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="52"/>
-      <c r="AW46" s="53" t="s">
+      <c r="AV46" s="50"/>
+      <c r="AW46" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="54"/>
-      <c r="AY46" s="54"/>
-      <c r="AZ46" s="54"/>
-      <c r="BA46" s="54"/>
-      <c r="BB46" s="54"/>
-      <c r="BC46" s="54"/>
-      <c r="BD46" s="54"/>
-      <c r="BE46" s="55"/>
-      <c r="BF46" s="52" t="s">
+      <c r="AX46" s="55"/>
+      <c r="AY46" s="55"/>
+      <c r="AZ46" s="55"/>
+      <c r="BA46" s="55"/>
+      <c r="BB46" s="55"/>
+      <c r="BC46" s="55"/>
+      <c r="BD46" s="55"/>
+      <c r="BE46" s="56"/>
+      <c r="BF46" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="52"/>
+      <c r="BG46" s="50"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -14538,11 +14585,80 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="BQ34:BR34"/>
+    <mergeCell ref="BS34:BT34"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
@@ -14559,80 +14675,11 @@
     <mergeCell ref="AI34:AJ34"/>
     <mergeCell ref="AK34:AL34"/>
     <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="BQ34:BR34"/>
-    <mergeCell ref="BS34:BT34"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15309,43 +15356,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F50"/>
-  <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U83" sqref="U83"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="2:2">
-      <c r="B1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="6:6">
-      <c r="F45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="6:6">
-      <c r="F46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:CB37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15571,62 +15581,62 @@
         <v>0</v>
       </c>
       <c r="F3" s="39"/>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52" t="s">
+      <c r="H3" s="50"/>
+      <c r="I3" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52" t="s">
+      <c r="L3" s="50"/>
+      <c r="M3" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52" t="s">
+      <c r="N3" s="50"/>
+      <c r="O3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52" t="s">
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52" t="s">
+      <c r="R3" s="50"/>
+      <c r="S3" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52" t="s">
+      <c r="T3" s="50"/>
+      <c r="U3" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52" t="s">
+      <c r="V3" s="50"/>
+      <c r="W3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="X3" s="52"/>
+      <c r="X3" s="50"/>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="52" t="s">
+      <c r="AC3" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="52" t="s">
+      <c r="AD3" s="50"/>
+      <c r="AE3" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="52" t="s">
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="52"/>
-      <c r="AI3" s="52" t="s">
+      <c r="AH3" s="50"/>
+      <c r="AI3" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AJ3" s="52"/>
+      <c r="AJ3" s="50"/>
       <c r="AK3" s="34"/>
       <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
@@ -15649,104 +15659,104 @@
       <c r="BH3" s="34"/>
       <c r="BI3" s="34"/>
       <c r="BJ3" s="34"/>
-      <c r="BK3" s="50" t="s">
+      <c r="BK3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BL3" s="51"/>
-      <c r="BM3" s="50" t="s">
+      <c r="BL3" s="53"/>
+      <c r="BM3" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BN3" s="51"/>
-      <c r="BO3" s="50" t="s">
+      <c r="BN3" s="53"/>
+      <c r="BO3" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" s="51"/>
-      <c r="BQ3" s="50" t="s">
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BR3" s="51"/>
-      <c r="BS3" s="50" t="s">
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="51"/>
-      <c r="BU3" s="50" t="s">
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BV3" s="51"/>
-      <c r="BW3" s="50" t="s">
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BX3" s="51"/>
-      <c r="BY3" s="50" t="s">
+      <c r="BX3" s="53"/>
+      <c r="BY3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BZ3" s="51"/>
-      <c r="CA3" s="50" t="s">
+      <c r="BZ3" s="53"/>
+      <c r="CA3" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CB3" s="51"/>
+      <c r="CB3" s="53"/>
     </row>
     <row r="4" spans="2:80">
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="34"/>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52" t="s">
+      <c r="H4" s="50"/>
+      <c r="I4" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52" t="s">
+      <c r="J4" s="50"/>
+      <c r="K4" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="50"/>
+      <c r="M4" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52" t="s">
+      <c r="N4" s="50"/>
+      <c r="O4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52" t="s">
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52" t="s">
+      <c r="R4" s="50"/>
+      <c r="S4" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52" t="s">
+      <c r="T4" s="50"/>
+      <c r="U4" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52" t="s">
+      <c r="V4" s="50"/>
+      <c r="W4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="52"/>
+      <c r="X4" s="50"/>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="52" t="s">
+      <c r="AC4" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="52" t="s">
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="52" t="s">
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="52" t="s">
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="52"/>
+      <c r="AJ4" s="50"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
@@ -15769,42 +15779,42 @@
       <c r="BH4" s="34"/>
       <c r="BI4" s="34"/>
       <c r="BJ4" s="34"/>
-      <c r="BK4" s="50" t="s">
+      <c r="BK4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BL4" s="51"/>
-      <c r="BM4" s="50" t="s">
+      <c r="BL4" s="53"/>
+      <c r="BM4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BN4" s="51"/>
-      <c r="BO4" s="50" t="s">
+      <c r="BN4" s="53"/>
+      <c r="BO4" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BP4" s="51"/>
-      <c r="BQ4" s="50" t="s">
+      <c r="BP4" s="53"/>
+      <c r="BQ4" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BR4" s="51"/>
-      <c r="BS4" s="50" t="s">
+      <c r="BR4" s="53"/>
+      <c r="BS4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BT4" s="51"/>
-      <c r="BU4" s="50" t="s">
+      <c r="BT4" s="53"/>
+      <c r="BU4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BV4" s="51"/>
-      <c r="BW4" s="50" t="s">
+      <c r="BV4" s="53"/>
+      <c r="BW4" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="51"/>
-      <c r="BY4" s="50" t="s">
+      <c r="BX4" s="53"/>
+      <c r="BY4" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BZ4" s="51"/>
-      <c r="CA4" s="50" t="s">
+      <c r="BZ4" s="53"/>
+      <c r="CA4" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CB4" s="51"/>
+      <c r="CB4" s="53"/>
     </row>
     <row r="5" spans="2:80">
       <c r="BX5" s="27"/>
@@ -15818,62 +15828,62 @@
         <v>239</v>
       </c>
       <c r="F6" s="36"/>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57" t="s">
+      <c r="H6" s="51"/>
+      <c r="I6" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57" t="s">
+      <c r="J6" s="51"/>
+      <c r="K6" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57" t="s">
+      <c r="L6" s="51"/>
+      <c r="M6" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57" t="s">
+      <c r="N6" s="51"/>
+      <c r="O6" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57" t="s">
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57" t="s">
+      <c r="R6" s="51"/>
+      <c r="S6" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57" t="s">
+      <c r="T6" s="51"/>
+      <c r="U6" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="V6" s="57"/>
-      <c r="W6" s="57" t="s">
+      <c r="V6" s="51"/>
+      <c r="W6" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="X6" s="57"/>
+      <c r="X6" s="51"/>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AC6" s="57" t="s">
+      <c r="AC6" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="57" t="s">
+      <c r="AD6" s="51"/>
+      <c r="AE6" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="57"/>
-      <c r="AG6" s="57" t="s">
+      <c r="AF6" s="51"/>
+      <c r="AG6" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="AH6" s="57"/>
-      <c r="AI6" s="57" t="s">
+      <c r="AH6" s="51"/>
+      <c r="AI6" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="AJ6" s="57"/>
+      <c r="AJ6" s="51"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -15896,42 +15906,42 @@
       <c r="BH6" s="34"/>
       <c r="BI6" s="34"/>
       <c r="BJ6" s="34"/>
-      <c r="BK6" s="50" t="s">
+      <c r="BK6" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BL6" s="51"/>
-      <c r="BM6" s="50" t="s">
+      <c r="BL6" s="53"/>
+      <c r="BM6" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BN6" s="51"/>
-      <c r="BO6" s="50" t="s">
+      <c r="BN6" s="53"/>
+      <c r="BO6" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BP6" s="51"/>
-      <c r="BQ6" s="50" t="s">
+      <c r="BP6" s="53"/>
+      <c r="BQ6" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BR6" s="51"/>
-      <c r="BS6" s="50" t="s">
+      <c r="BR6" s="53"/>
+      <c r="BS6" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="50" t="s">
+      <c r="BT6" s="53"/>
+      <c r="BU6" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BV6" s="51"/>
-      <c r="BW6" s="50" t="s">
+      <c r="BV6" s="53"/>
+      <c r="BW6" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BX6" s="51"/>
-      <c r="BY6" s="50" t="s">
+      <c r="BX6" s="53"/>
+      <c r="BY6" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BZ6" s="51"/>
-      <c r="CA6" s="50" t="s">
+      <c r="BZ6" s="53"/>
+      <c r="CA6" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CB6" s="51"/>
+      <c r="CB6" s="53"/>
     </row>
     <row r="7" spans="2:80">
       <c r="E7">
@@ -16267,58 +16277,58 @@
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52" t="s">
+      <c r="J12" s="50"/>
+      <c r="K12" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52" t="s">
+      <c r="L12" s="50"/>
+      <c r="M12" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52" t="s">
+      <c r="N12" s="50"/>
+      <c r="O12" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52" t="s">
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52" t="s">
+      <c r="R12" s="50"/>
+      <c r="S12" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52" t="s">
+      <c r="T12" s="50"/>
+      <c r="U12" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="52"/>
-      <c r="W12" s="52" t="s">
+      <c r="V12" s="50"/>
+      <c r="W12" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="52"/>
+      <c r="X12" s="50"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="52" t="s">
+      <c r="AC12" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="52"/>
-      <c r="AE12" s="52" t="s">
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AF12" s="52"/>
-      <c r="AG12" s="52" t="s">
+      <c r="AF12" s="50"/>
+      <c r="AG12" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="52" t="s">
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="AJ12" s="52"/>
+      <c r="AJ12" s="50"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="34"/>
       <c r="AM12" s="34"/>
@@ -16341,42 +16351,42 @@
       <c r="BH12" s="34"/>
       <c r="BI12" s="34"/>
       <c r="BJ12" s="34"/>
-      <c r="BK12" s="50" t="s">
+      <c r="BK12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BL12" s="51"/>
-      <c r="BM12" s="50" t="s">
+      <c r="BL12" s="53"/>
+      <c r="BM12" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BN12" s="51"/>
-      <c r="BO12" s="50" t="s">
+      <c r="BN12" s="53"/>
+      <c r="BO12" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BP12" s="51"/>
-      <c r="BQ12" s="50" t="s">
+      <c r="BP12" s="53"/>
+      <c r="BQ12" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BR12" s="51"/>
-      <c r="BS12" s="50" t="s">
+      <c r="BR12" s="53"/>
+      <c r="BS12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="BT12" s="51"/>
-      <c r="BU12" s="50" t="s">
+      <c r="BT12" s="53"/>
+      <c r="BU12" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="BV12" s="51"/>
-      <c r="BW12" s="50" t="s">
+      <c r="BV12" s="53"/>
+      <c r="BW12" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="BX12" s="51"/>
-      <c r="BY12" s="50" t="s">
+      <c r="BX12" s="53"/>
+      <c r="BY12" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="BZ12" s="51"/>
-      <c r="CA12" s="50" t="s">
+      <c r="BZ12" s="53"/>
+      <c r="CA12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="CB12" s="51"/>
+      <c r="CB12" s="53"/>
     </row>
     <row r="13" spans="2:80">
       <c r="BX13" s="27"/>
@@ -16409,71 +16419,71 @@
         <v>120</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
-      <c r="Z16" s="56"/>
-      <c r="AA16" s="56" t="s">
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="AB16" s="56"/>
-      <c r="AC16" s="56"/>
-      <c r="AD16" s="56"/>
-      <c r="AE16" s="56"/>
-      <c r="AF16" s="56"/>
-      <c r="AG16" s="56"/>
-      <c r="AH16" s="56"/>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="52" t="s">
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="57"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="57"/>
+      <c r="AI16" s="57"/>
+      <c r="AJ16" s="57"/>
+      <c r="AK16" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="AL16" s="52"/>
-      <c r="AM16" s="52" t="s">
+      <c r="AL16" s="50"/>
+      <c r="AM16" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="AN16" s="52"/>
-      <c r="AO16" s="52" t="s">
+      <c r="AN16" s="50"/>
+      <c r="AO16" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="AP16" s="52"/>
-      <c r="AQ16" s="52" t="s">
+      <c r="AP16" s="50"/>
+      <c r="AQ16" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="AR16" s="52"/>
-      <c r="AS16" s="53" t="s">
+      <c r="AR16" s="50"/>
+      <c r="AS16" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="AT16" s="54"/>
-      <c r="AU16" s="54"/>
-      <c r="AV16" s="54"/>
-      <c r="AW16" s="54"/>
-      <c r="AX16" s="54"/>
-      <c r="AY16" s="54"/>
-      <c r="AZ16" s="54"/>
-      <c r="BA16" s="55"/>
-      <c r="BB16" s="52" t="s">
+      <c r="AT16" s="55"/>
+      <c r="AU16" s="55"/>
+      <c r="AV16" s="55"/>
+      <c r="AW16" s="55"/>
+      <c r="AX16" s="55"/>
+      <c r="AY16" s="55"/>
+      <c r="AZ16" s="55"/>
+      <c r="BA16" s="56"/>
+      <c r="BB16" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="BC16" s="52"/>
+      <c r="BC16" s="50"/>
       <c r="BE16" s="38"/>
       <c r="BF16" s="38"/>
       <c r="BG16" s="38"/>
@@ -17022,18 +17032,73 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="BB16:BC16"/>
+    <mergeCell ref="BW12:BX12"/>
+    <mergeCell ref="BY12:BZ12"/>
+    <mergeCell ref="CA12:CB12"/>
+    <mergeCell ref="G16:Z16"/>
+    <mergeCell ref="AA16:AJ16"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AM16:AN16"/>
+    <mergeCell ref="AO16:AP16"/>
+    <mergeCell ref="AQ16:AR16"/>
+    <mergeCell ref="AS16:BA16"/>
+    <mergeCell ref="BK12:BL12"/>
+    <mergeCell ref="BM12:BN12"/>
+    <mergeCell ref="BO12:BP12"/>
+    <mergeCell ref="BQ12:BR12"/>
+    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AC6:AD6"/>
     <mergeCell ref="BU3:BV3"/>
     <mergeCell ref="BW3:BX3"/>
     <mergeCell ref="BY3:BZ3"/>
@@ -17050,77 +17115,59 @@
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="BQ3:BR3"/>
     <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="BB16:BC16"/>
-    <mergeCell ref="BW12:BX12"/>
-    <mergeCell ref="BY12:BZ12"/>
-    <mergeCell ref="CA12:CB12"/>
-    <mergeCell ref="G16:Z16"/>
-    <mergeCell ref="AA16:AJ16"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AM16:AN16"/>
-    <mergeCell ref="AO16:AP16"/>
-    <mergeCell ref="AQ16:AR16"/>
-    <mergeCell ref="AS16:BA16"/>
-    <mergeCell ref="BK12:BL12"/>
-    <mergeCell ref="BM12:BN12"/>
-    <mergeCell ref="BO12:BP12"/>
-    <mergeCell ref="BQ12:BR12"/>
-    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:F50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6">
+      <c r="F45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6">
+      <c r="F46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sprite reg update enabler timing changed..
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="238">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -791,6 +791,38 @@
   </si>
   <si>
     <t>spr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ff</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sprite plt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5bit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ph</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>at=3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -801,7 +833,7 @@
   <numFmts count="1">
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,6 +898,15 @@
       <color rgb="FFFFFFFF"/>
       <name val="MS PGothic"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="64">
@@ -1248,7 +1289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1542,13 +1583,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1692,36 +1746,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1900,8 +1924,50 @@
     <xf numFmtId="24" fontId="8" fillId="10" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5725,10 +5791,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="107" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -5736,8 +5802,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="108"/>
+      <c r="B9" s="108"/>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
@@ -5776,10 +5842,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="107" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -5787,8 +5853,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="108"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
@@ -5927,10 +5993,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="107" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -5938,8 +6004,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1">
-      <c r="A30" s="49"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="108"/>
+      <c r="B30" s="108"/>
       <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
@@ -5967,10 +6033,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="107" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -5978,8 +6044,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1">
-      <c r="A34" s="49"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="108"/>
+      <c r="B34" s="108"/>
       <c r="C34" s="6" t="s">
         <v>57</v>
       </c>
@@ -6079,22 +6145,22 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="107" t="s">
         <v>62</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="48" t="s">
+      <c r="C47" s="107" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" thickBot="1">
-      <c r="A48" s="49"/>
+      <c r="A48" s="108"/>
       <c r="B48" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="49"/>
+      <c r="C48" s="108"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="2" t="s">
@@ -6118,22 +6184,22 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25">
-      <c r="A52" s="48" t="s">
+      <c r="A52" s="107" t="s">
         <v>62</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="48" t="s">
+      <c r="C52" s="107" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" thickBot="1">
-      <c r="A53" s="49"/>
+      <c r="A53" s="108"/>
       <c r="B53" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="49"/>
+      <c r="C53" s="108"/>
     </row>
     <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="2" t="s">
@@ -6157,25 +6223,31 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25">
-      <c r="A57" s="48" t="s">
+      <c r="A57" s="107" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="48" t="s">
+      <c r="C57" s="107" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1">
-      <c r="A58" s="49"/>
+      <c r="A58" s="108"/>
       <c r="B58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="49"/>
+      <c r="C58" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -6184,12 +6256,6 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10945,62 +11011,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="52" t="s">
+      <c r="K33" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52" t="s">
+      <c r="L33" s="109"/>
+      <c r="M33" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52" t="s">
+      <c r="N33" s="109"/>
+      <c r="O33" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52" t="s">
+      <c r="P33" s="109"/>
+      <c r="Q33" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52" t="s">
+      <c r="R33" s="109"/>
+      <c r="S33" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52" t="s">
+      <c r="T33" s="109"/>
+      <c r="U33" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52" t="s">
+      <c r="V33" s="109"/>
+      <c r="W33" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52" t="s">
+      <c r="X33" s="109"/>
+      <c r="Y33" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="52" t="s">
+      <c r="Z33" s="109"/>
+      <c r="AA33" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="52"/>
+      <c r="AB33" s="109"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="52" t="s">
+      <c r="AG33" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="52"/>
-      <c r="AI33" s="52" t="s">
+      <c r="AH33" s="109"/>
+      <c r="AI33" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="52"/>
-      <c r="AK33" s="52" t="s">
+      <c r="AJ33" s="109"/>
+      <c r="AK33" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="52"/>
-      <c r="AM33" s="52" t="s">
+      <c r="AL33" s="109"/>
+      <c r="AM33" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="52"/>
+      <c r="AN33" s="109"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -11023,104 +11089,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="50" t="s">
+      <c r="BO33" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="51"/>
-      <c r="BQ33" s="50" t="s">
+      <c r="BP33" s="112"/>
+      <c r="BQ33" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="51"/>
-      <c r="BS33" s="50" t="s">
+      <c r="BR33" s="112"/>
+      <c r="BS33" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="51"/>
-      <c r="BU33" s="50" t="s">
+      <c r="BT33" s="112"/>
+      <c r="BU33" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="51"/>
-      <c r="BW33" s="50" t="s">
+      <c r="BV33" s="112"/>
+      <c r="BW33" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="51"/>
-      <c r="BY33" s="50" t="s">
+      <c r="BX33" s="112"/>
+      <c r="BY33" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="51"/>
-      <c r="CA33" s="50" t="s">
+      <c r="BZ33" s="112"/>
+      <c r="CA33" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="51"/>
-      <c r="CC33" s="50" t="s">
+      <c r="CB33" s="112"/>
+      <c r="CC33" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="51"/>
-      <c r="CE33" s="50" t="s">
+      <c r="CD33" s="112"/>
+      <c r="CE33" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="51"/>
+      <c r="CF33" s="112"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="52" t="s">
+      <c r="K34" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52" t="s">
+      <c r="L34" s="109"/>
+      <c r="M34" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52" t="s">
+      <c r="N34" s="109"/>
+      <c r="O34" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52" t="s">
+      <c r="P34" s="109"/>
+      <c r="Q34" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52" t="s">
+      <c r="R34" s="109"/>
+      <c r="S34" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52" t="s">
+      <c r="T34" s="109"/>
+      <c r="U34" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="52"/>
-      <c r="W34" s="52" t="s">
+      <c r="V34" s="109"/>
+      <c r="W34" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52" t="s">
+      <c r="X34" s="109"/>
+      <c r="Y34" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="52" t="s">
+      <c r="Z34" s="109"/>
+      <c r="AA34" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="52"/>
+      <c r="AB34" s="109"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="52" t="s">
+      <c r="AG34" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="52"/>
-      <c r="AI34" s="52" t="s">
+      <c r="AH34" s="109"/>
+      <c r="AI34" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="52"/>
-      <c r="AK34" s="52" t="s">
+      <c r="AJ34" s="109"/>
+      <c r="AK34" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="52"/>
-      <c r="AM34" s="52" t="s">
+      <c r="AL34" s="109"/>
+      <c r="AM34" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="52"/>
+      <c r="AN34" s="109"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -11143,42 +11209,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="50" t="s">
+      <c r="BO34" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="51"/>
-      <c r="BQ34" s="50" t="s">
+      <c r="BP34" s="112"/>
+      <c r="BQ34" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="51"/>
-      <c r="BS34" s="50" t="s">
+      <c r="BR34" s="112"/>
+      <c r="BS34" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="51"/>
-      <c r="BU34" s="50" t="s">
+      <c r="BT34" s="112"/>
+      <c r="BU34" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="51"/>
-      <c r="BW34" s="50" t="s">
+      <c r="BV34" s="112"/>
+      <c r="BW34" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="51"/>
-      <c r="BY34" s="50" t="s">
+      <c r="BX34" s="112"/>
+      <c r="BY34" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="51"/>
-      <c r="CA34" s="50" t="s">
+      <c r="BZ34" s="112"/>
+      <c r="CA34" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="51"/>
-      <c r="CC34" s="50" t="s">
+      <c r="CB34" s="112"/>
+      <c r="CC34" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="51"/>
-      <c r="CE34" s="50" t="s">
+      <c r="CD34" s="112"/>
+      <c r="CE34" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="51"/>
+      <c r="CF34" s="112"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -11192,62 +11258,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="57" t="s">
+      <c r="K36" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57" t="s">
+      <c r="L36" s="110"/>
+      <c r="M36" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57" t="s">
+      <c r="N36" s="110"/>
+      <c r="O36" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57" t="s">
+      <c r="P36" s="110"/>
+      <c r="Q36" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="57"/>
-      <c r="S36" s="57" t="s">
+      <c r="R36" s="110"/>
+      <c r="S36" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="57"/>
-      <c r="U36" s="57" t="s">
+      <c r="T36" s="110"/>
+      <c r="U36" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="57"/>
-      <c r="W36" s="57" t="s">
+      <c r="V36" s="110"/>
+      <c r="W36" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="57"/>
-      <c r="Y36" s="57" t="s">
+      <c r="X36" s="110"/>
+      <c r="Y36" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="57"/>
-      <c r="AA36" s="57" t="s">
+      <c r="Z36" s="110"/>
+      <c r="AA36" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="57"/>
+      <c r="AB36" s="110"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="57" t="s">
+      <c r="AG36" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="57"/>
-      <c r="AI36" s="57" t="s">
+      <c r="AH36" s="110"/>
+      <c r="AI36" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="57"/>
-      <c r="AK36" s="57" t="s">
+      <c r="AJ36" s="110"/>
+      <c r="AK36" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="57"/>
-      <c r="AM36" s="57" t="s">
+      <c r="AL36" s="110"/>
+      <c r="AM36" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="57"/>
+      <c r="AN36" s="110"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -11270,42 +11336,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="50" t="s">
+      <c r="BO36" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="51"/>
-      <c r="BQ36" s="50" t="s">
+      <c r="BP36" s="112"/>
+      <c r="BQ36" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="51"/>
-      <c r="BS36" s="50" t="s">
+      <c r="BR36" s="112"/>
+      <c r="BS36" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="51"/>
-      <c r="BU36" s="50" t="s">
+      <c r="BT36" s="112"/>
+      <c r="BU36" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="51"/>
-      <c r="BW36" s="50" t="s">
+      <c r="BV36" s="112"/>
+      <c r="BW36" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="51"/>
-      <c r="BY36" s="50" t="s">
+      <c r="BX36" s="112"/>
+      <c r="BY36" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="51"/>
-      <c r="CA36" s="50" t="s">
+      <c r="BZ36" s="112"/>
+      <c r="CA36" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="51"/>
-      <c r="CC36" s="50" t="s">
+      <c r="CB36" s="112"/>
+      <c r="CC36" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="51"/>
-      <c r="CE36" s="50" t="s">
+      <c r="CD36" s="112"/>
+      <c r="CE36" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="51"/>
+      <c r="CF36" s="112"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -11641,58 +11707,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="52" t="s">
+      <c r="M42" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52" t="s">
+      <c r="N42" s="109"/>
+      <c r="O42" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52" t="s">
+      <c r="P42" s="109"/>
+      <c r="Q42" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="52"/>
-      <c r="S42" s="52" t="s">
+      <c r="R42" s="109"/>
+      <c r="S42" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52" t="s">
+      <c r="T42" s="109"/>
+      <c r="U42" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="52"/>
-      <c r="W42" s="52" t="s">
+      <c r="V42" s="109"/>
+      <c r="W42" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="52"/>
-      <c r="Y42" s="52" t="s">
+      <c r="X42" s="109"/>
+      <c r="Y42" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="52" t="s">
+      <c r="Z42" s="109"/>
+      <c r="AA42" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="52"/>
+      <c r="AB42" s="109"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="52" t="s">
+      <c r="AG42" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="52"/>
-      <c r="AI42" s="52" t="s">
+      <c r="AH42" s="109"/>
+      <c r="AI42" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="52"/>
-      <c r="AK42" s="52" t="s">
+      <c r="AJ42" s="109"/>
+      <c r="AK42" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="52"/>
-      <c r="AM42" s="52" t="s">
+      <c r="AL42" s="109"/>
+      <c r="AM42" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="52"/>
+      <c r="AN42" s="109"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -11715,42 +11781,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="50" t="s">
+      <c r="BO42" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="51"/>
-      <c r="BQ42" s="50" t="s">
+      <c r="BP42" s="112"/>
+      <c r="BQ42" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="51"/>
-      <c r="BS42" s="50" t="s">
+      <c r="BR42" s="112"/>
+      <c r="BS42" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="51"/>
-      <c r="BU42" s="50" t="s">
+      <c r="BT42" s="112"/>
+      <c r="BU42" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="51"/>
-      <c r="BW42" s="50" t="s">
+      <c r="BV42" s="112"/>
+      <c r="BW42" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="51"/>
-      <c r="BY42" s="50" t="s">
+      <c r="BX42" s="112"/>
+      <c r="BY42" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="51"/>
-      <c r="CA42" s="50" t="s">
+      <c r="BZ42" s="112"/>
+      <c r="CA42" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="51"/>
-      <c r="CC42" s="50" t="s">
+      <c r="CB42" s="112"/>
+      <c r="CC42" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="51"/>
-      <c r="CE42" s="50" t="s">
+      <c r="CD42" s="112"/>
+      <c r="CE42" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="51"/>
+      <c r="CF42" s="112"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -11783,71 +11849,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="56" t="s">
+      <c r="K46" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
-      <c r="T46" s="56"/>
-      <c r="U46" s="56"/>
-      <c r="V46" s="56"/>
-      <c r="W46" s="56"/>
-      <c r="X46" s="56"/>
-      <c r="Y46" s="56"/>
-      <c r="Z46" s="56"/>
-      <c r="AA46" s="56"/>
-      <c r="AB46" s="56"/>
-      <c r="AC46" s="56"/>
-      <c r="AD46" s="56"/>
-      <c r="AE46" s="56" t="s">
+      <c r="L46" s="116"/>
+      <c r="M46" s="116"/>
+      <c r="N46" s="116"/>
+      <c r="O46" s="116"/>
+      <c r="P46" s="116"/>
+      <c r="Q46" s="116"/>
+      <c r="R46" s="116"/>
+      <c r="S46" s="116"/>
+      <c r="T46" s="116"/>
+      <c r="U46" s="116"/>
+      <c r="V46" s="116"/>
+      <c r="W46" s="116"/>
+      <c r="X46" s="116"/>
+      <c r="Y46" s="116"/>
+      <c r="Z46" s="116"/>
+      <c r="AA46" s="116"/>
+      <c r="AB46" s="116"/>
+      <c r="AC46" s="116"/>
+      <c r="AD46" s="116"/>
+      <c r="AE46" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="56"/>
-      <c r="AG46" s="56"/>
-      <c r="AH46" s="56"/>
-      <c r="AI46" s="56"/>
-      <c r="AJ46" s="56"/>
-      <c r="AK46" s="56"/>
-      <c r="AL46" s="56"/>
-      <c r="AM46" s="56"/>
-      <c r="AN46" s="56"/>
-      <c r="AO46" s="52" t="s">
+      <c r="AF46" s="116"/>
+      <c r="AG46" s="116"/>
+      <c r="AH46" s="116"/>
+      <c r="AI46" s="116"/>
+      <c r="AJ46" s="116"/>
+      <c r="AK46" s="116"/>
+      <c r="AL46" s="116"/>
+      <c r="AM46" s="116"/>
+      <c r="AN46" s="116"/>
+      <c r="AO46" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="52"/>
-      <c r="AQ46" s="52" t="s">
+      <c r="AP46" s="109"/>
+      <c r="AQ46" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="52"/>
-      <c r="AS46" s="52" t="s">
+      <c r="AR46" s="109"/>
+      <c r="AS46" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="52"/>
-      <c r="AU46" s="52" t="s">
+      <c r="AT46" s="109"/>
+      <c r="AU46" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="52"/>
-      <c r="AW46" s="53" t="s">
+      <c r="AV46" s="109"/>
+      <c r="AW46" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="54"/>
-      <c r="AY46" s="54"/>
-      <c r="AZ46" s="54"/>
-      <c r="BA46" s="54"/>
-      <c r="BB46" s="54"/>
-      <c r="BC46" s="54"/>
-      <c r="BD46" s="54"/>
-      <c r="BE46" s="55"/>
-      <c r="BF46" s="52" t="s">
+      <c r="AX46" s="114"/>
+      <c r="AY46" s="114"/>
+      <c r="AZ46" s="114"/>
+      <c r="BA46" s="114"/>
+      <c r="BB46" s="114"/>
+      <c r="BC46" s="114"/>
+      <c r="BD46" s="114"/>
+      <c r="BE46" s="115"/>
+      <c r="BF46" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="52"/>
+      <c r="BG46" s="109"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -15429,11 +15495,80 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="BQ34:BR34"/>
+    <mergeCell ref="BS34:BT34"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
@@ -15450,80 +15585,11 @@
     <mergeCell ref="AI34:AJ34"/>
     <mergeCell ref="AK34:AL34"/>
     <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="BQ34:BR34"/>
-    <mergeCell ref="BS34:BT34"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16425,62 +16491,62 @@
         <v>0</v>
       </c>
       <c r="F3" s="39"/>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52" t="s">
+      <c r="H3" s="109"/>
+      <c r="I3" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52" t="s">
+      <c r="J3" s="109"/>
+      <c r="K3" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52" t="s">
+      <c r="L3" s="109"/>
+      <c r="M3" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52" t="s">
+      <c r="N3" s="109"/>
+      <c r="O3" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52" t="s">
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52" t="s">
+      <c r="R3" s="109"/>
+      <c r="S3" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52" t="s">
+      <c r="T3" s="109"/>
+      <c r="U3" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52" t="s">
+      <c r="V3" s="109"/>
+      <c r="W3" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="X3" s="52"/>
+      <c r="X3" s="109"/>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="52" t="s">
+      <c r="AC3" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="52" t="s">
+      <c r="AD3" s="109"/>
+      <c r="AE3" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="52" t="s">
+      <c r="AF3" s="109"/>
+      <c r="AG3" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="52"/>
-      <c r="AI3" s="52" t="s">
+      <c r="AH3" s="109"/>
+      <c r="AI3" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="AJ3" s="52"/>
+      <c r="AJ3" s="109"/>
       <c r="AK3" s="34"/>
       <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
@@ -16503,104 +16569,104 @@
       <c r="BH3" s="34"/>
       <c r="BI3" s="34"/>
       <c r="BJ3" s="34"/>
-      <c r="BK3" s="50" t="s">
+      <c r="BK3" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BL3" s="51"/>
-      <c r="BM3" s="50" t="s">
+      <c r="BL3" s="112"/>
+      <c r="BM3" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BN3" s="51"/>
-      <c r="BO3" s="50" t="s">
+      <c r="BN3" s="112"/>
+      <c r="BO3" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" s="51"/>
-      <c r="BQ3" s="50" t="s">
+      <c r="BP3" s="112"/>
+      <c r="BQ3" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BR3" s="51"/>
-      <c r="BS3" s="50" t="s">
+      <c r="BR3" s="112"/>
+      <c r="BS3" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="51"/>
-      <c r="BU3" s="50" t="s">
+      <c r="BT3" s="112"/>
+      <c r="BU3" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BV3" s="51"/>
-      <c r="BW3" s="50" t="s">
+      <c r="BV3" s="112"/>
+      <c r="BW3" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BX3" s="51"/>
-      <c r="BY3" s="50" t="s">
+      <c r="BX3" s="112"/>
+      <c r="BY3" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BZ3" s="51"/>
-      <c r="CA3" s="50" t="s">
+      <c r="BZ3" s="112"/>
+      <c r="CA3" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CB3" s="51"/>
+      <c r="CB3" s="112"/>
     </row>
     <row r="4" spans="2:80">
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="34"/>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52" t="s">
+      <c r="H4" s="109"/>
+      <c r="I4" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52" t="s">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="109"/>
+      <c r="M4" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52" t="s">
+      <c r="N4" s="109"/>
+      <c r="O4" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52" t="s">
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52" t="s">
+      <c r="R4" s="109"/>
+      <c r="S4" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52" t="s">
+      <c r="T4" s="109"/>
+      <c r="U4" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52" t="s">
+      <c r="V4" s="109"/>
+      <c r="W4" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="52"/>
+      <c r="X4" s="109"/>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="52" t="s">
+      <c r="AC4" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="52" t="s">
+      <c r="AD4" s="109"/>
+      <c r="AE4" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="52" t="s">
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="52" t="s">
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="52"/>
+      <c r="AJ4" s="109"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
@@ -16623,42 +16689,42 @@
       <c r="BH4" s="34"/>
       <c r="BI4" s="34"/>
       <c r="BJ4" s="34"/>
-      <c r="BK4" s="50" t="s">
+      <c r="BK4" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BL4" s="51"/>
-      <c r="BM4" s="50" t="s">
+      <c r="BL4" s="112"/>
+      <c r="BM4" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BN4" s="51"/>
-      <c r="BO4" s="50" t="s">
+      <c r="BN4" s="112"/>
+      <c r="BO4" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BP4" s="51"/>
-      <c r="BQ4" s="50" t="s">
+      <c r="BP4" s="112"/>
+      <c r="BQ4" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BR4" s="51"/>
-      <c r="BS4" s="50" t="s">
+      <c r="BR4" s="112"/>
+      <c r="BS4" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BT4" s="51"/>
-      <c r="BU4" s="50" t="s">
+      <c r="BT4" s="112"/>
+      <c r="BU4" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BV4" s="51"/>
-      <c r="BW4" s="50" t="s">
+      <c r="BV4" s="112"/>
+      <c r="BW4" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="51"/>
-      <c r="BY4" s="50" t="s">
+      <c r="BX4" s="112"/>
+      <c r="BY4" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BZ4" s="51"/>
-      <c r="CA4" s="50" t="s">
+      <c r="BZ4" s="112"/>
+      <c r="CA4" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CB4" s="51"/>
+      <c r="CB4" s="112"/>
     </row>
     <row r="5" spans="2:80">
       <c r="BX5" s="27"/>
@@ -16672,62 +16738,62 @@
         <v>239</v>
       </c>
       <c r="F6" s="36"/>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57" t="s">
+      <c r="H6" s="110"/>
+      <c r="I6" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57" t="s">
+      <c r="J6" s="110"/>
+      <c r="K6" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57" t="s">
+      <c r="L6" s="110"/>
+      <c r="M6" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57" t="s">
+      <c r="N6" s="110"/>
+      <c r="O6" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57" t="s">
+      <c r="P6" s="110"/>
+      <c r="Q6" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57" t="s">
+      <c r="R6" s="110"/>
+      <c r="S6" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57" t="s">
+      <c r="T6" s="110"/>
+      <c r="U6" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="V6" s="57"/>
-      <c r="W6" s="57" t="s">
+      <c r="V6" s="110"/>
+      <c r="W6" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="X6" s="57"/>
+      <c r="X6" s="110"/>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AC6" s="57" t="s">
+      <c r="AC6" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="57" t="s">
+      <c r="AD6" s="110"/>
+      <c r="AE6" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="57"/>
-      <c r="AG6" s="57" t="s">
+      <c r="AF6" s="110"/>
+      <c r="AG6" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="AH6" s="57"/>
-      <c r="AI6" s="57" t="s">
+      <c r="AH6" s="110"/>
+      <c r="AI6" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="AJ6" s="57"/>
+      <c r="AJ6" s="110"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -16750,42 +16816,42 @@
       <c r="BH6" s="34"/>
       <c r="BI6" s="34"/>
       <c r="BJ6" s="34"/>
-      <c r="BK6" s="50" t="s">
+      <c r="BK6" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BL6" s="51"/>
-      <c r="BM6" s="50" t="s">
+      <c r="BL6" s="112"/>
+      <c r="BM6" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BN6" s="51"/>
-      <c r="BO6" s="50" t="s">
+      <c r="BN6" s="112"/>
+      <c r="BO6" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BP6" s="51"/>
-      <c r="BQ6" s="50" t="s">
+      <c r="BP6" s="112"/>
+      <c r="BQ6" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BR6" s="51"/>
-      <c r="BS6" s="50" t="s">
+      <c r="BR6" s="112"/>
+      <c r="BS6" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="50" t="s">
+      <c r="BT6" s="112"/>
+      <c r="BU6" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BV6" s="51"/>
-      <c r="BW6" s="50" t="s">
+      <c r="BV6" s="112"/>
+      <c r="BW6" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BX6" s="51"/>
-      <c r="BY6" s="50" t="s">
+      <c r="BX6" s="112"/>
+      <c r="BY6" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BZ6" s="51"/>
-      <c r="CA6" s="50" t="s">
+      <c r="BZ6" s="112"/>
+      <c r="CA6" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CB6" s="51"/>
+      <c r="CB6" s="112"/>
     </row>
     <row r="7" spans="2:80">
       <c r="E7">
@@ -17121,58 +17187,58 @@
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52" t="s">
+      <c r="J12" s="109"/>
+      <c r="K12" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52" t="s">
+      <c r="L12" s="109"/>
+      <c r="M12" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52" t="s">
+      <c r="N12" s="109"/>
+      <c r="O12" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52" t="s">
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52" t="s">
+      <c r="R12" s="109"/>
+      <c r="S12" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52" t="s">
+      <c r="T12" s="109"/>
+      <c r="U12" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="52"/>
-      <c r="W12" s="52" t="s">
+      <c r="V12" s="109"/>
+      <c r="W12" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="52"/>
+      <c r="X12" s="109"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="52" t="s">
+      <c r="AC12" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="52"/>
-      <c r="AE12" s="52" t="s">
+      <c r="AD12" s="109"/>
+      <c r="AE12" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AF12" s="52"/>
-      <c r="AG12" s="52" t="s">
+      <c r="AF12" s="109"/>
+      <c r="AG12" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="52" t="s">
+      <c r="AH12" s="109"/>
+      <c r="AI12" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="AJ12" s="52"/>
+      <c r="AJ12" s="109"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="34"/>
       <c r="AM12" s="34"/>
@@ -17195,42 +17261,42 @@
       <c r="BH12" s="34"/>
       <c r="BI12" s="34"/>
       <c r="BJ12" s="34"/>
-      <c r="BK12" s="50" t="s">
+      <c r="BK12" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BL12" s="51"/>
-      <c r="BM12" s="50" t="s">
+      <c r="BL12" s="112"/>
+      <c r="BM12" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BN12" s="51"/>
-      <c r="BO12" s="50" t="s">
+      <c r="BN12" s="112"/>
+      <c r="BO12" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BP12" s="51"/>
-      <c r="BQ12" s="50" t="s">
+      <c r="BP12" s="112"/>
+      <c r="BQ12" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BR12" s="51"/>
-      <c r="BS12" s="50" t="s">
+      <c r="BR12" s="112"/>
+      <c r="BS12" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="BT12" s="51"/>
-      <c r="BU12" s="50" t="s">
+      <c r="BT12" s="112"/>
+      <c r="BU12" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BV12" s="51"/>
-      <c r="BW12" s="50" t="s">
+      <c r="BV12" s="112"/>
+      <c r="BW12" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="BX12" s="51"/>
-      <c r="BY12" s="50" t="s">
+      <c r="BX12" s="112"/>
+      <c r="BY12" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="BZ12" s="51"/>
-      <c r="CA12" s="50" t="s">
+      <c r="BZ12" s="112"/>
+      <c r="CA12" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="CB12" s="51"/>
+      <c r="CB12" s="112"/>
     </row>
     <row r="13" spans="2:80">
       <c r="BX13" s="27"/>
@@ -17263,71 +17329,71 @@
         <v>120</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
-      <c r="Z16" s="56"/>
-      <c r="AA16" s="56" t="s">
+      <c r="H16" s="116"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
+      <c r="L16" s="116"/>
+      <c r="M16" s="116"/>
+      <c r="N16" s="116"/>
+      <c r="O16" s="116"/>
+      <c r="P16" s="116"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="116"/>
+      <c r="S16" s="116"/>
+      <c r="T16" s="116"/>
+      <c r="U16" s="116"/>
+      <c r="V16" s="116"/>
+      <c r="W16" s="116"/>
+      <c r="X16" s="116"/>
+      <c r="Y16" s="116"/>
+      <c r="Z16" s="116"/>
+      <c r="AA16" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="AB16" s="56"/>
-      <c r="AC16" s="56"/>
-      <c r="AD16" s="56"/>
-      <c r="AE16" s="56"/>
-      <c r="AF16" s="56"/>
-      <c r="AG16" s="56"/>
-      <c r="AH16" s="56"/>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="52" t="s">
+      <c r="AB16" s="116"/>
+      <c r="AC16" s="116"/>
+      <c r="AD16" s="116"/>
+      <c r="AE16" s="116"/>
+      <c r="AF16" s="116"/>
+      <c r="AG16" s="116"/>
+      <c r="AH16" s="116"/>
+      <c r="AI16" s="116"/>
+      <c r="AJ16" s="116"/>
+      <c r="AK16" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="AL16" s="52"/>
-      <c r="AM16" s="52" t="s">
+      <c r="AL16" s="109"/>
+      <c r="AM16" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="AN16" s="52"/>
-      <c r="AO16" s="52" t="s">
+      <c r="AN16" s="109"/>
+      <c r="AO16" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="AP16" s="52"/>
-      <c r="AQ16" s="52" t="s">
+      <c r="AP16" s="109"/>
+      <c r="AQ16" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="AR16" s="52"/>
-      <c r="AS16" s="53" t="s">
+      <c r="AR16" s="109"/>
+      <c r="AS16" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="AT16" s="54"/>
-      <c r="AU16" s="54"/>
-      <c r="AV16" s="54"/>
-      <c r="AW16" s="54"/>
-      <c r="AX16" s="54"/>
-      <c r="AY16" s="54"/>
-      <c r="AZ16" s="54"/>
-      <c r="BA16" s="55"/>
-      <c r="BB16" s="52" t="s">
+      <c r="AT16" s="114"/>
+      <c r="AU16" s="114"/>
+      <c r="AV16" s="114"/>
+      <c r="AW16" s="114"/>
+      <c r="AX16" s="114"/>
+      <c r="AY16" s="114"/>
+      <c r="AZ16" s="114"/>
+      <c r="BA16" s="115"/>
+      <c r="BB16" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="BC16" s="52"/>
+      <c r="BC16" s="109"/>
       <c r="BE16" s="38"/>
       <c r="BF16" s="38"/>
       <c r="BG16" s="38"/>
@@ -17876,18 +17942,73 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="BB16:BC16"/>
+    <mergeCell ref="BW12:BX12"/>
+    <mergeCell ref="BY12:BZ12"/>
+    <mergeCell ref="CA12:CB12"/>
+    <mergeCell ref="G16:Z16"/>
+    <mergeCell ref="AA16:AJ16"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AM16:AN16"/>
+    <mergeCell ref="AO16:AP16"/>
+    <mergeCell ref="AQ16:AR16"/>
+    <mergeCell ref="AS16:BA16"/>
+    <mergeCell ref="BK12:BL12"/>
+    <mergeCell ref="BM12:BN12"/>
+    <mergeCell ref="BO12:BP12"/>
+    <mergeCell ref="BQ12:BR12"/>
+    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AC6:AD6"/>
     <mergeCell ref="BU3:BV3"/>
     <mergeCell ref="BW3:BX3"/>
     <mergeCell ref="BY3:BZ3"/>
@@ -17904,73 +18025,18 @@
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="BQ3:BR3"/>
     <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="BB16:BC16"/>
-    <mergeCell ref="BW12:BX12"/>
-    <mergeCell ref="BY12:BZ12"/>
-    <mergeCell ref="CA12:CB12"/>
-    <mergeCell ref="G16:Z16"/>
-    <mergeCell ref="AA16:AJ16"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AM16:AN16"/>
-    <mergeCell ref="AO16:AP16"/>
-    <mergeCell ref="AQ16:AR16"/>
-    <mergeCell ref="AS16:BA16"/>
-    <mergeCell ref="BK12:BL12"/>
-    <mergeCell ref="BM12:BN12"/>
-    <mergeCell ref="BO12:BP12"/>
-    <mergeCell ref="BQ12:BR12"/>
-    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18018,292 +18084,400 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:R10"/>
+  <dimension ref="A4:AB16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="20" max="20" width="5.125" customWidth="1"/>
+    <col min="21" max="28" width="3.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25">
-      <c r="A5" s="58"/>
-    </row>
-    <row r="6" spans="1:18" ht="14.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60">
+    <row r="5" spans="1:28" ht="17.25">
+      <c r="A5" s="48"/>
+    </row>
+    <row r="6" spans="1:28" ht="14.25">
+      <c r="A6" s="49"/>
+      <c r="B6" s="50">
         <v>0</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="50">
         <v>1</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="50">
         <v>2</v>
       </c>
-      <c r="E6" s="60">
+      <c r="E6" s="50">
         <v>3</v>
       </c>
-      <c r="F6" s="60">
+      <c r="F6" s="50">
         <v>4</v>
       </c>
-      <c r="G6" s="60">
+      <c r="G6" s="50">
         <v>5</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="50">
         <v>6</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="50">
         <v>7</v>
       </c>
-      <c r="J6" s="60">
+      <c r="J6" s="50">
         <v>8</v>
       </c>
-      <c r="K6" s="60">
+      <c r="K6" s="50">
         <v>9</v>
       </c>
-      <c r="L6" s="61" t="s">
+      <c r="L6" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="61" t="s">
+      <c r="M6" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="N6" s="61" t="s">
+      <c r="N6" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="O6" s="61" t="s">
+      <c r="O6" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="P6" s="61" t="s">
+      <c r="P6" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="Q6" s="61" t="s">
+      <c r="Q6" s="51" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.25">
-      <c r="A7" s="116" t="s">
+    <row r="7" spans="1:28" ht="14.25">
+      <c r="A7" s="106" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="56" t="s">
         <v>177</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="H7" s="68" t="s">
+      <c r="H7" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="J7" s="70" t="s">
+      <c r="J7" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="K7" s="71" t="s">
+      <c r="K7" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="L7" s="72" t="s">
+      <c r="L7" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="M7" s="73" t="s">
+      <c r="M7" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="N7" s="74" t="s">
+      <c r="N7" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="O7" s="75" t="s">
+      <c r="O7" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="P7" s="75" t="s">
+      <c r="P7" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="Q7" s="75" t="s">
+      <c r="Q7" s="65" t="s">
         <v>186</v>
       </c>
       <c r="R7" s="117" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.25">
-      <c r="A8" s="60">
+    <row r="8" spans="1:28" ht="14.25">
+      <c r="A8" s="50">
         <v>10</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="67" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="E8" s="79" t="s">
+      <c r="E8" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="70" t="s">
         <v>191</v>
       </c>
-      <c r="G8" s="81" t="s">
+      <c r="G8" s="71" t="s">
         <v>192</v>
       </c>
-      <c r="H8" s="82" t="s">
+      <c r="H8" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="74" t="s">
         <v>195</v>
       </c>
-      <c r="K8" s="85" t="s">
+      <c r="K8" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="L8" s="86" t="s">
+      <c r="L8" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="M8" s="87" t="s">
+      <c r="M8" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="N8" s="88" t="s">
+      <c r="N8" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="O8" s="75" t="s">
+      <c r="O8" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="P8" s="75" t="s">
+      <c r="P8" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="Q8" s="75" t="s">
+      <c r="Q8" s="65" t="s">
         <v>186</v>
       </c>
       <c r="R8" s="117"/>
     </row>
-    <row r="9" spans="1:18" ht="14.25">
-      <c r="A9" s="60">
+    <row r="9" spans="1:28" ht="14.25">
+      <c r="A9" s="50">
         <v>20</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="79" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="91" t="s">
+      <c r="D9" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="F9" s="93" t="s">
+      <c r="F9" s="83" t="s">
         <v>204</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="H9" s="95" t="s">
+      <c r="H9" s="85" t="s">
         <v>206</v>
       </c>
-      <c r="I9" s="96" t="s">
+      <c r="I9" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="J9" s="97" t="s">
+      <c r="J9" s="87" t="s">
         <v>208</v>
       </c>
-      <c r="K9" s="98" t="s">
+      <c r="K9" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="L9" s="99" t="s">
+      <c r="L9" s="89" t="s">
         <v>210</v>
       </c>
-      <c r="M9" s="100" t="s">
+      <c r="M9" s="90" t="s">
         <v>211</v>
       </c>
-      <c r="N9" s="101" t="s">
+      <c r="N9" s="91" t="s">
         <v>212</v>
       </c>
-      <c r="O9" s="102" t="s">
+      <c r="O9" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="P9" s="75" t="s">
+      <c r="P9" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="Q9" s="75" t="s">
+      <c r="Q9" s="65" t="s">
         <v>186</v>
       </c>
       <c r="R9" s="117" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.25">
-      <c r="A10" s="60">
+    <row r="10" spans="1:28" ht="14.25">
+      <c r="A10" s="50">
         <v>30</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="79" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="93" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="E10" s="105" t="s">
+      <c r="E10" s="95" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="106" t="s">
+      <c r="F10" s="96" t="s">
         <v>216</v>
       </c>
-      <c r="G10" s="107" t="s">
+      <c r="G10" s="97" t="s">
         <v>217</v>
       </c>
-      <c r="H10" s="108" t="s">
+      <c r="H10" s="98" t="s">
         <v>218</v>
       </c>
-      <c r="I10" s="109" t="s">
+      <c r="I10" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="J10" s="110" t="s">
+      <c r="J10" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="K10" s="111" t="s">
+      <c r="K10" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="L10" s="112" t="s">
+      <c r="L10" s="102" t="s">
         <v>222</v>
       </c>
-      <c r="M10" s="113" t="s">
+      <c r="M10" s="103" t="s">
         <v>223</v>
       </c>
-      <c r="N10" s="114" t="s">
+      <c r="N10" s="104" t="s">
         <v>224</v>
       </c>
-      <c r="O10" s="115" t="s">
+      <c r="O10" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="P10" s="75" t="s">
+      <c r="P10" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="Q10" s="75" t="s">
+      <c r="Q10" s="65" t="s">
         <v>186</v>
       </c>
       <c r="R10" s="117"/>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="AB11" s="121"/>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="T12" s="118" t="s">
+        <v>230</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="12">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
+      <c r="T13" s="118">
+        <v>63</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="12">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28">
+      <c r="S15" t="s">
+        <v>233</v>
+      </c>
+      <c r="T15" t="s">
+        <v>234</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" t="s">
+        <v>231</v>
+      </c>
+      <c r="W15" t="s">
+        <v>232</v>
+      </c>
+      <c r="X15" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="S16" t="s">
+        <v>237</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
sprite pix processing ok!!!
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="461">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -1518,27 +1513,59 @@
   </si>
   <si>
     <t>v-ram</t>
+  </si>
+  <si>
+    <t>sprite</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cur y = N</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>spr y = M</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>prefetch &gt;&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>N - M + 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>flip vertically</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fetch =</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M - N + 6</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
   </numFmts>
   <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1597,7 +1624,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -2655,7 +2682,7 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="24" fontId="8" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2823,7 +2850,7 @@
     <xf numFmtId="0" fontId="7" fillId="63" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="24" fontId="8" fillId="10" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2979,13 +3006,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2998,9 +3028,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3017,7 +3044,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6453,7 +6480,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6495,7 +6522,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6527,10 +6554,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6562,7 +6588,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6738,14 +6763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="AO6:AO11"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="6" spans="41:41">
       <c r="AO6" t="s">
@@ -6775,16 +6800,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="59.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.25" customWidth="1"/>
+    <col min="2" max="2" width="42.625" customWidth="1"/>
+    <col min="3" max="3" width="64.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="15.75" thickBot="1">
@@ -6792,7 +6819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -6800,12 +6827,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1">
+    <row r="4" spans="1:3" ht="14.25" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1">
+    <row r="5" spans="1:3" ht="15" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -6816,7 +6843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1">
+    <row r="6" spans="1:3" ht="15" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -6827,7 +6854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1">
+    <row r="7" spans="1:3" ht="15" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -6838,7 +6865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="14.25">
       <c r="A8" s="156" t="s">
         <v>16</v>
       </c>
@@ -6849,14 +6876,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+    <row r="9" spans="1:3" ht="15" thickBot="1">
       <c r="A9" s="157"/>
       <c r="B9" s="157"/>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
+    <row r="10" spans="1:3" ht="15" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -6867,7 +6894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29.25" thickBot="1">
+    <row r="11" spans="1:3" ht="15" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -6878,7 +6905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1">
+    <row r="12" spans="1:3" ht="15" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -6889,7 +6916,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="14.25">
       <c r="A13" s="156" t="s">
         <v>28</v>
       </c>
@@ -6900,14 +6927,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+    <row r="14" spans="1:3" ht="15" thickBot="1">
       <c r="A14" s="157"/>
       <c r="B14" s="157"/>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+    <row r="15" spans="1:3" ht="15" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -6915,12 +6942,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1">
+    <row r="16" spans="1:3" ht="14.25" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1">
+    <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -6931,7 +6958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1">
+    <row r="18" spans="1:3" ht="15" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -6942,7 +6969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1">
+    <row r="19" spans="1:3" ht="15" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -6953,7 +6980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1">
+    <row r="20" spans="1:3" ht="15" thickBot="1">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -6964,7 +6991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1">
+    <row r="21" spans="1:3" ht="15" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -6975,7 +7002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1">
+    <row r="22" spans="1:3" ht="15" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
@@ -6986,7 +7013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29.25" thickBot="1">
+    <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -6997,7 +7024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+    <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>41</v>
       </c>
@@ -7008,7 +7035,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+    <row r="25" spans="1:3" ht="15" thickBot="1">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
@@ -7019,17 +7046,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1">
+    <row r="26" spans="1:3" ht="15" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+    <row r="27" spans="1:3" ht="14.25" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1">
+    <row r="28" spans="1:3" ht="15" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -7040,7 +7067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="14.25">
       <c r="A29" s="156" t="s">
         <v>10</v>
       </c>
@@ -7051,14 +7078,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1">
+    <row r="30" spans="1:3" ht="15" thickBot="1">
       <c r="A30" s="157"/>
       <c r="B30" s="157"/>
       <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="29.25" thickBot="1">
+    <row r="31" spans="1:3" ht="15" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>13</v>
       </c>
@@ -7069,7 +7096,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="29.25" thickBot="1">
+    <row r="32" spans="1:3" ht="15" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -7080,7 +7107,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" ht="14.25">
       <c r="A33" s="156" t="s">
         <v>20</v>
       </c>
@@ -7091,14 +7118,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1">
+    <row r="34" spans="1:3" ht="15" thickBot="1">
       <c r="A34" s="157"/>
       <c r="B34" s="157"/>
       <c r="C34" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1">
+    <row r="35" spans="1:3" ht="15" thickBot="1">
       <c r="A35" s="4" t="s">
         <v>58</v>
       </c>
@@ -7107,17 +7134,17 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+    <row r="36" spans="1:3" ht="15" thickBot="1">
       <c r="A36" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1">
+    <row r="37" spans="1:3" ht="14.25" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1">
+    <row r="38" spans="1:3" ht="15" thickBot="1">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -7128,7 +7155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1">
+    <row r="39" spans="1:3" ht="15" thickBot="1">
       <c r="A39" s="4" t="s">
         <v>62</v>
       </c>
@@ -7139,17 +7166,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1">
+    <row r="40" spans="1:3" ht="15" thickBot="1">
       <c r="A40" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1">
+    <row r="41" spans="1:3" ht="14.25" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1">
+    <row r="42" spans="1:3" ht="15" thickBot="1">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -7160,7 +7187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1">
+    <row r="43" spans="1:3" ht="15" thickBot="1">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -7171,17 +7198,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1">
+    <row r="44" spans="1:3" ht="15" thickBot="1">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="39" thickBot="1">
+    <row r="45" spans="1:3" ht="26.25" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1">
+    <row r="46" spans="1:3" ht="15" thickBot="1">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -7192,7 +7219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" ht="14.25">
       <c r="A47" s="156" t="s">
         <v>62</v>
       </c>
@@ -7203,24 +7230,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1">
+    <row r="48" spans="1:3" ht="15" thickBot="1">
       <c r="A48" s="157"/>
       <c r="B48" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C48" s="157"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+    <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="39" thickBot="1">
+    <row r="50" spans="1:3" ht="26.25" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1">
+    <row r="51" spans="1:3" ht="15" thickBot="1">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
@@ -7231,7 +7258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" ht="14.25">
       <c r="A52" s="156" t="s">
         <v>62</v>
       </c>
@@ -7242,24 +7269,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1">
+    <row r="53" spans="1:3" ht="15" thickBot="1">
       <c r="A53" s="157"/>
       <c r="B53" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C53" s="157"/>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1">
+    <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="26.25" thickBot="1">
+    <row r="55" spans="1:3" ht="14.25" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1">
+    <row r="56" spans="1:3" ht="15" thickBot="1">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -7270,7 +7297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" ht="14.25">
       <c r="A57" s="156" t="s">
         <v>62</v>
       </c>
@@ -7281,7 +7308,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1">
+    <row r="58" spans="1:3" ht="15" thickBot="1">
       <c r="A58" s="157"/>
       <c r="B58" s="6" t="s">
         <v>79</v>
@@ -7290,6 +7317,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -7298,12 +7331,6 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7312,28 +7339,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:BX117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.375" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
     <col min="33" max="38" width="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.28515625" customWidth="1"/>
+    <col min="45" max="45" width="5.25" customWidth="1"/>
     <col min="46" max="47" width="4" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="5.42578125" customWidth="1"/>
+    <col min="61" max="61" width="5.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:48">
@@ -7341,7 +7368,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="4:48" ht="15.75" thickBot="1">
+    <row r="4" spans="4:48" ht="14.25" thickBot="1">
       <c r="Z4">
         <v>800</v>
       </c>
@@ -7438,7 +7465,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="4:48" ht="15.75" thickBot="1">
+    <row r="8" spans="4:48" ht="14.25" thickBot="1">
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -7814,7 +7841,7 @@
       <c r="AU16" s="12"/>
       <c r="AV16" s="20"/>
     </row>
-    <row r="17" spans="3:48" ht="15.75" thickBot="1">
+    <row r="17" spans="3:48" ht="14.25" thickBot="1">
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -8027,7 +8054,7 @@
       <c r="AU21" s="22"/>
       <c r="AV21" s="23"/>
     </row>
-    <row r="22" spans="3:48" ht="15.75" thickBot="1">
+    <row r="22" spans="3:48" ht="14.25" thickBot="1">
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -8284,7 +8311,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="3:49" ht="15.75" thickBot="1"/>
+    <row r="38" spans="3:49" ht="14.25" thickBot="1"/>
     <row r="39" spans="3:49">
       <c r="E39" s="24">
         <v>2000</v>
@@ -8629,7 +8656,7 @@
       <c r="AV46" s="12"/>
       <c r="AW46" s="13"/>
     </row>
-    <row r="47" spans="3:49" ht="15.75" thickBot="1">
+    <row r="47" spans="3:49" ht="14.25" thickBot="1">
       <c r="E47" s="14"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
@@ -9011,7 +9038,7 @@
       <c r="AV55" s="12"/>
       <c r="AW55" s="13"/>
     </row>
-    <row r="56" spans="5:49" ht="15.75" thickBot="1">
+    <row r="56" spans="5:49" ht="14.25" thickBot="1">
       <c r="E56" s="14"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
@@ -9058,7 +9085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="5:49" ht="15.75" thickBot="1"/>
+    <row r="60" spans="5:49" ht="14.25" thickBot="1"/>
     <row r="61" spans="5:49">
       <c r="AD61" s="8"/>
       <c r="AE61" s="9"/>
@@ -9237,7 +9264,7 @@
       <c r="AV68" s="12"/>
       <c r="AW68" s="13"/>
     </row>
-    <row r="69" spans="30:49" ht="15.75" thickBot="1">
+    <row r="69" spans="30:49" ht="14.25" thickBot="1">
       <c r="AD69" s="14"/>
       <c r="AE69" s="15"/>
       <c r="AF69" s="15"/>
@@ -9435,7 +9462,7 @@
       <c r="AV77" s="12"/>
       <c r="AW77" s="13"/>
     </row>
-    <row r="78" spans="30:49" ht="15.75" thickBot="1">
+    <row r="78" spans="30:49" ht="14.25" thickBot="1">
       <c r="AD78" s="14"/>
       <c r="AE78" s="15"/>
       <c r="AF78" s="15"/>
@@ -9473,7 +9500,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="6:76" ht="15.75" thickBot="1">
+    <row r="83" spans="6:76" ht="14.25" thickBot="1">
       <c r="O83">
         <v>128</v>
       </c>
@@ -10575,7 +10602,7 @@
       <c r="BW99" s="12"/>
       <c r="BX99" s="13"/>
     </row>
-    <row r="100" spans="7:76" ht="15.75" thickBot="1">
+    <row r="100" spans="7:76" ht="14.25" thickBot="1">
       <c r="G100" s="14"/>
       <c r="H100" s="15"/>
       <c r="I100" s="15"/>
@@ -11729,7 +11756,7 @@
       <c r="BW116" s="12"/>
       <c r="BX116" s="13"/>
     </row>
-    <row r="117" spans="7:76" ht="15.75" thickBot="1">
+    <row r="117" spans="7:76" ht="14.25" thickBot="1">
       <c r="G117" s="14"/>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
@@ -11803,41 +11830,41 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CF125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AL50" sqref="AL50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.140625" customWidth="1"/>
-    <col min="36" max="36" width="4.28515625" customWidth="1"/>
-    <col min="38" max="38" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="2.5703125" customWidth="1"/>
-    <col min="48" max="48" width="4.85546875" customWidth="1"/>
-    <col min="49" max="49" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4.140625" customWidth="1"/>
-    <col min="52" max="53" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.875" customWidth="1"/>
+    <col min="5" max="5" width="4.75" customWidth="1"/>
+    <col min="9" max="9" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.125" customWidth="1"/>
+    <col min="36" max="36" width="4.25" customWidth="1"/>
+    <col min="38" max="38" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="2.625" customWidth="1"/>
+    <col min="48" max="48" width="4.875" customWidth="1"/>
+    <col min="49" max="49" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="4.125" customWidth="1"/>
+    <col min="52" max="53" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="2.875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="4" customWidth="1"/>
-    <col min="69" max="69" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
@@ -11845,7 +11872,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="10:84" s="27" customFormat="1" ht="46.5">
+    <row r="32" spans="10:84" s="27" customFormat="1" ht="42">
       <c r="J32" s="27">
         <v>0</v>
       </c>
@@ -12059,62 +12086,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="160" t="s">
+      <c r="K33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="160"/>
-      <c r="M33" s="160" t="s">
+      <c r="L33" s="158"/>
+      <c r="M33" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="160"/>
-      <c r="O33" s="160" t="s">
+      <c r="N33" s="158"/>
+      <c r="O33" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="160"/>
-      <c r="Q33" s="160" t="s">
+      <c r="P33" s="158"/>
+      <c r="Q33" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="160"/>
-      <c r="S33" s="160" t="s">
+      <c r="R33" s="158"/>
+      <c r="S33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="160"/>
-      <c r="U33" s="160" t="s">
+      <c r="T33" s="158"/>
+      <c r="U33" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="160"/>
-      <c r="W33" s="160" t="s">
+      <c r="V33" s="158"/>
+      <c r="W33" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="160"/>
-      <c r="Y33" s="160" t="s">
+      <c r="X33" s="158"/>
+      <c r="Y33" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="160"/>
-      <c r="AA33" s="160" t="s">
+      <c r="Z33" s="158"/>
+      <c r="AA33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="160"/>
+      <c r="AB33" s="158"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="160" t="s">
+      <c r="AG33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="160"/>
-      <c r="AI33" s="160" t="s">
+      <c r="AH33" s="158"/>
+      <c r="AI33" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="160"/>
-      <c r="AK33" s="160" t="s">
+      <c r="AJ33" s="158"/>
+      <c r="AK33" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="160"/>
-      <c r="AM33" s="160" t="s">
+      <c r="AL33" s="158"/>
+      <c r="AM33" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="160"/>
+      <c r="AN33" s="158"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -12137,104 +12164,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="158" t="s">
+      <c r="BO33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="159"/>
-      <c r="BQ33" s="158" t="s">
+      <c r="BP33" s="161"/>
+      <c r="BQ33" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="159"/>
-      <c r="BS33" s="158" t="s">
+      <c r="BR33" s="161"/>
+      <c r="BS33" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="159"/>
-      <c r="BU33" s="158" t="s">
+      <c r="BT33" s="161"/>
+      <c r="BU33" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="159"/>
-      <c r="BW33" s="158" t="s">
+      <c r="BV33" s="161"/>
+      <c r="BW33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="159"/>
-      <c r="BY33" s="158" t="s">
+      <c r="BX33" s="161"/>
+      <c r="BY33" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="159"/>
-      <c r="CA33" s="158" t="s">
+      <c r="BZ33" s="161"/>
+      <c r="CA33" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="159"/>
-      <c r="CC33" s="158" t="s">
+      <c r="CB33" s="161"/>
+      <c r="CC33" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="159"/>
-      <c r="CE33" s="158" t="s">
+      <c r="CD33" s="161"/>
+      <c r="CE33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="159"/>
+      <c r="CF33" s="161"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="160" t="s">
+      <c r="K34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="160"/>
-      <c r="M34" s="160" t="s">
+      <c r="L34" s="158"/>
+      <c r="M34" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="160"/>
-      <c r="O34" s="160" t="s">
+      <c r="N34" s="158"/>
+      <c r="O34" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="160"/>
-      <c r="Q34" s="160" t="s">
+      <c r="P34" s="158"/>
+      <c r="Q34" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="160"/>
-      <c r="S34" s="160" t="s">
+      <c r="R34" s="158"/>
+      <c r="S34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="160"/>
-      <c r="U34" s="160" t="s">
+      <c r="T34" s="158"/>
+      <c r="U34" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="160"/>
-      <c r="W34" s="160" t="s">
+      <c r="V34" s="158"/>
+      <c r="W34" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="160"/>
-      <c r="Y34" s="160" t="s">
+      <c r="X34" s="158"/>
+      <c r="Y34" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="160"/>
-      <c r="AA34" s="160" t="s">
+      <c r="Z34" s="158"/>
+      <c r="AA34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="160"/>
+      <c r="AB34" s="158"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="160" t="s">
+      <c r="AG34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="160"/>
-      <c r="AI34" s="160" t="s">
+      <c r="AH34" s="158"/>
+      <c r="AI34" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="160"/>
-      <c r="AK34" s="160" t="s">
+      <c r="AJ34" s="158"/>
+      <c r="AK34" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="160"/>
-      <c r="AM34" s="160" t="s">
+      <c r="AL34" s="158"/>
+      <c r="AM34" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="160"/>
+      <c r="AN34" s="158"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -12257,42 +12284,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="158" t="s">
+      <c r="BO34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="159"/>
-      <c r="BQ34" s="158" t="s">
+      <c r="BP34" s="161"/>
+      <c r="BQ34" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="159"/>
-      <c r="BS34" s="158" t="s">
+      <c r="BR34" s="161"/>
+      <c r="BS34" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="159"/>
-      <c r="BU34" s="158" t="s">
+      <c r="BT34" s="161"/>
+      <c r="BU34" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="159"/>
-      <c r="BW34" s="158" t="s">
+      <c r="BV34" s="161"/>
+      <c r="BW34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="159"/>
-      <c r="BY34" s="158" t="s">
+      <c r="BX34" s="161"/>
+      <c r="BY34" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="159"/>
-      <c r="CA34" s="158" t="s">
+      <c r="BZ34" s="161"/>
+      <c r="CA34" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="159"/>
-      <c r="CC34" s="158" t="s">
+      <c r="CB34" s="161"/>
+      <c r="CC34" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="159"/>
-      <c r="CE34" s="158" t="s">
+      <c r="CD34" s="161"/>
+      <c r="CE34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="159"/>
+      <c r="CF34" s="161"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -12306,62 +12333,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="165" t="s">
+      <c r="K36" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="165"/>
-      <c r="M36" s="165" t="s">
+      <c r="L36" s="159"/>
+      <c r="M36" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="165"/>
-      <c r="O36" s="165" t="s">
+      <c r="N36" s="159"/>
+      <c r="O36" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="165"/>
-      <c r="Q36" s="165" t="s">
+      <c r="P36" s="159"/>
+      <c r="Q36" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="165"/>
-      <c r="S36" s="165" t="s">
+      <c r="R36" s="159"/>
+      <c r="S36" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="165"/>
-      <c r="U36" s="165" t="s">
+      <c r="T36" s="159"/>
+      <c r="U36" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="165"/>
-      <c r="W36" s="165" t="s">
+      <c r="V36" s="159"/>
+      <c r="W36" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="165"/>
-      <c r="Y36" s="165" t="s">
+      <c r="X36" s="159"/>
+      <c r="Y36" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="165"/>
-      <c r="AA36" s="165" t="s">
+      <c r="Z36" s="159"/>
+      <c r="AA36" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="165"/>
+      <c r="AB36" s="159"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="165" t="s">
+      <c r="AG36" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="165"/>
-      <c r="AI36" s="165" t="s">
+      <c r="AH36" s="159"/>
+      <c r="AI36" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="165"/>
-      <c r="AK36" s="165" t="s">
+      <c r="AJ36" s="159"/>
+      <c r="AK36" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="165"/>
-      <c r="AM36" s="165" t="s">
+      <c r="AL36" s="159"/>
+      <c r="AM36" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="165"/>
+      <c r="AN36" s="159"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -12384,42 +12411,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="158" t="s">
+      <c r="BO36" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="159"/>
-      <c r="BQ36" s="158" t="s">
+      <c r="BP36" s="161"/>
+      <c r="BQ36" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="159"/>
-      <c r="BS36" s="158" t="s">
+      <c r="BR36" s="161"/>
+      <c r="BS36" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="159"/>
-      <c r="BU36" s="158" t="s">
+      <c r="BT36" s="161"/>
+      <c r="BU36" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="159"/>
-      <c r="BW36" s="158" t="s">
+      <c r="BV36" s="161"/>
+      <c r="BW36" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="159"/>
-      <c r="BY36" s="158" t="s">
+      <c r="BX36" s="161"/>
+      <c r="BY36" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="159"/>
-      <c r="CA36" s="158" t="s">
+      <c r="BZ36" s="161"/>
+      <c r="CA36" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="159"/>
-      <c r="CC36" s="158" t="s">
+      <c r="CB36" s="161"/>
+      <c r="CC36" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="159"/>
-      <c r="CE36" s="158" t="s">
+      <c r="CD36" s="161"/>
+      <c r="CE36" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="159"/>
+      <c r="CF36" s="161"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -12755,58 +12782,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="160" t="s">
+      <c r="M42" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="160"/>
-      <c r="O42" s="160" t="s">
+      <c r="N42" s="158"/>
+      <c r="O42" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="160"/>
-      <c r="Q42" s="160" t="s">
+      <c r="P42" s="158"/>
+      <c r="Q42" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="160"/>
-      <c r="S42" s="160" t="s">
+      <c r="R42" s="158"/>
+      <c r="S42" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="160"/>
-      <c r="U42" s="160" t="s">
+      <c r="T42" s="158"/>
+      <c r="U42" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="160"/>
-      <c r="W42" s="160" t="s">
+      <c r="V42" s="158"/>
+      <c r="W42" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="160"/>
-      <c r="Y42" s="160" t="s">
+      <c r="X42" s="158"/>
+      <c r="Y42" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="160"/>
-      <c r="AA42" s="160" t="s">
+      <c r="Z42" s="158"/>
+      <c r="AA42" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="160"/>
+      <c r="AB42" s="158"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="160" t="s">
+      <c r="AG42" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="160"/>
-      <c r="AI42" s="160" t="s">
+      <c r="AH42" s="158"/>
+      <c r="AI42" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="160"/>
-      <c r="AK42" s="160" t="s">
+      <c r="AJ42" s="158"/>
+      <c r="AK42" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="160"/>
-      <c r="AM42" s="160" t="s">
+      <c r="AL42" s="158"/>
+      <c r="AM42" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="160"/>
+      <c r="AN42" s="158"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -12829,42 +12856,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="158" t="s">
+      <c r="BO42" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="159"/>
-      <c r="BQ42" s="158" t="s">
+      <c r="BP42" s="161"/>
+      <c r="BQ42" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="159"/>
-      <c r="BS42" s="158" t="s">
+      <c r="BR42" s="161"/>
+      <c r="BS42" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="159"/>
-      <c r="BU42" s="158" t="s">
+      <c r="BT42" s="161"/>
+      <c r="BU42" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="159"/>
-      <c r="BW42" s="158" t="s">
+      <c r="BV42" s="161"/>
+      <c r="BW42" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="159"/>
-      <c r="BY42" s="158" t="s">
+      <c r="BX42" s="161"/>
+      <c r="BY42" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="159"/>
-      <c r="CA42" s="158" t="s">
+      <c r="BZ42" s="161"/>
+      <c r="CA42" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="159"/>
-      <c r="CC42" s="158" t="s">
+      <c r="CB42" s="161"/>
+      <c r="CC42" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="159"/>
-      <c r="CE42" s="158" t="s">
+      <c r="CD42" s="161"/>
+      <c r="CE42" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="159"/>
+      <c r="CF42" s="161"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -12897,71 +12924,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="164" t="s">
+      <c r="K46" s="165" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="164"/>
-      <c r="M46" s="164"/>
-      <c r="N46" s="164"/>
-      <c r="O46" s="164"/>
-      <c r="P46" s="164"/>
-      <c r="Q46" s="164"/>
-      <c r="R46" s="164"/>
-      <c r="S46" s="164"/>
-      <c r="T46" s="164"/>
-      <c r="U46" s="164"/>
-      <c r="V46" s="164"/>
-      <c r="W46" s="164"/>
-      <c r="X46" s="164"/>
-      <c r="Y46" s="164"/>
-      <c r="Z46" s="164"/>
-      <c r="AA46" s="164"/>
-      <c r="AB46" s="164"/>
-      <c r="AC46" s="164"/>
-      <c r="AD46" s="164"/>
-      <c r="AE46" s="164" t="s">
+      <c r="L46" s="165"/>
+      <c r="M46" s="165"/>
+      <c r="N46" s="165"/>
+      <c r="O46" s="165"/>
+      <c r="P46" s="165"/>
+      <c r="Q46" s="165"/>
+      <c r="R46" s="165"/>
+      <c r="S46" s="165"/>
+      <c r="T46" s="165"/>
+      <c r="U46" s="165"/>
+      <c r="V46" s="165"/>
+      <c r="W46" s="165"/>
+      <c r="X46" s="165"/>
+      <c r="Y46" s="165"/>
+      <c r="Z46" s="165"/>
+      <c r="AA46" s="165"/>
+      <c r="AB46" s="165"/>
+      <c r="AC46" s="165"/>
+      <c r="AD46" s="165"/>
+      <c r="AE46" s="165" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="164"/>
-      <c r="AG46" s="164"/>
-      <c r="AH46" s="164"/>
-      <c r="AI46" s="164"/>
-      <c r="AJ46" s="164"/>
-      <c r="AK46" s="164"/>
-      <c r="AL46" s="164"/>
-      <c r="AM46" s="164"/>
-      <c r="AN46" s="164"/>
-      <c r="AO46" s="160" t="s">
+      <c r="AF46" s="165"/>
+      <c r="AG46" s="165"/>
+      <c r="AH46" s="165"/>
+      <c r="AI46" s="165"/>
+      <c r="AJ46" s="165"/>
+      <c r="AK46" s="165"/>
+      <c r="AL46" s="165"/>
+      <c r="AM46" s="165"/>
+      <c r="AN46" s="165"/>
+      <c r="AO46" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="160"/>
-      <c r="AQ46" s="160" t="s">
+      <c r="AP46" s="158"/>
+      <c r="AQ46" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="160"/>
-      <c r="AS46" s="160" t="s">
+      <c r="AR46" s="158"/>
+      <c r="AS46" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="160"/>
-      <c r="AU46" s="160" t="s">
+      <c r="AT46" s="158"/>
+      <c r="AU46" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="160"/>
-      <c r="AW46" s="161" t="s">
+      <c r="AV46" s="158"/>
+      <c r="AW46" s="162" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="162"/>
-      <c r="AY46" s="162"/>
-      <c r="AZ46" s="162"/>
-      <c r="BA46" s="162"/>
-      <c r="BB46" s="162"/>
-      <c r="BC46" s="162"/>
-      <c r="BD46" s="162"/>
-      <c r="BE46" s="163"/>
-      <c r="BF46" s="160" t="s">
+      <c r="AX46" s="163"/>
+      <c r="AY46" s="163"/>
+      <c r="AZ46" s="163"/>
+      <c r="BA46" s="163"/>
+      <c r="BB46" s="163"/>
+      <c r="BC46" s="163"/>
+      <c r="BD46" s="163"/>
+      <c r="BE46" s="164"/>
+      <c r="BF46" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="160"/>
+      <c r="BG46" s="158"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -13015,7 +13042,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="5:71" ht="15.75" thickBot="1">
+    <row r="52" spans="5:71" ht="14.25" thickBot="1">
       <c r="E52" t="s">
         <v>108</v>
       </c>
@@ -13757,7 +13784,7 @@
       <c r="BP63" s="12"/>
       <c r="BQ63" s="20"/>
     </row>
-    <row r="64" spans="5:71" ht="15.75" thickBot="1">
+    <row r="64" spans="5:71" ht="14.25" thickBot="1">
       <c r="F64" s="11"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -14424,7 +14451,7 @@
       <c r="AU76" s="12"/>
       <c r="AV76" s="20"/>
     </row>
-    <row r="77" spans="5:69" ht="15.75" thickBot="1">
+    <row r="77" spans="5:69" ht="14.25" thickBot="1">
       <c r="E77">
         <v>480</v>
       </c>
@@ -14939,7 +14966,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="90" spans="4:48" ht="15.75" thickBot="1">
+    <row r="90" spans="4:48" ht="14.25" thickBot="1">
       <c r="E90" t="s">
         <v>109</v>
       </c>
@@ -16042,7 +16069,7 @@
       <c r="AU114" s="12"/>
       <c r="AV114" s="20"/>
     </row>
-    <row r="115" spans="4:48" ht="15.75" thickBot="1">
+    <row r="115" spans="4:48" ht="14.25" thickBot="1">
       <c r="D115">
         <v>240</v>
       </c>
@@ -16551,11 +16578,80 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="BO33:BP33"/>
+    <mergeCell ref="BO34:BP34"/>
+    <mergeCell ref="CA33:CB33"/>
+    <mergeCell ref="CC33:CD33"/>
+    <mergeCell ref="BQ33:BR33"/>
+    <mergeCell ref="BS33:BT33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BW33:BX33"/>
+    <mergeCell ref="BY33:BZ33"/>
+    <mergeCell ref="BQ34:BR34"/>
+    <mergeCell ref="BS34:BT34"/>
+    <mergeCell ref="BU34:BV34"/>
+    <mergeCell ref="BW34:BX34"/>
+    <mergeCell ref="BY34:BZ34"/>
+    <mergeCell ref="CA34:CB34"/>
+    <mergeCell ref="CC34:CD34"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
     <mergeCell ref="U34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:Z34"/>
@@ -16572,80 +16668,11 @@
     <mergeCell ref="AI34:AJ34"/>
     <mergeCell ref="AK34:AL34"/>
     <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="BO33:BP33"/>
-    <mergeCell ref="BO34:BP34"/>
-    <mergeCell ref="CA33:CB33"/>
-    <mergeCell ref="CC33:CD33"/>
-    <mergeCell ref="BQ33:BR33"/>
-    <mergeCell ref="BS33:BT33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="BW33:BX33"/>
-    <mergeCell ref="BY33:BZ33"/>
-    <mergeCell ref="BQ34:BR34"/>
-    <mergeCell ref="BS34:BT34"/>
-    <mergeCell ref="BU34:BV34"/>
-    <mergeCell ref="BW34:BX34"/>
-    <mergeCell ref="BY34:BZ34"/>
-    <mergeCell ref="CA34:CB34"/>
-    <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16655,18 +16682,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:EC67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:EC90"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD56" sqref="AD56"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X82" sqref="X82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="17" max="17" width="2.5703125" customWidth="1"/>
-    <col min="33" max="33" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.5703125" customWidth="1"/>
+    <col min="17" max="17" width="2.625" customWidth="1"/>
+    <col min="33" max="33" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="9:49">
@@ -17533,7 +17560,7 @@
       <c r="AY45" s="167"/>
       <c r="AZ45" s="168"/>
     </row>
-    <row r="46" spans="1:133" ht="46.5">
+    <row r="46" spans="1:133" ht="42">
       <c r="A46" t="s">
         <v>422</v>
       </c>
@@ -17926,262 +17953,262 @@
       </c>
     </row>
     <row r="47" spans="1:133">
-      <c r="F47" s="160" t="s">
+      <c r="F47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="160"/>
-      <c r="H47" s="160" t="s">
+      <c r="G47" s="158"/>
+      <c r="H47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="I47" s="160"/>
-      <c r="J47" s="160" t="s">
+      <c r="I47" s="158"/>
+      <c r="J47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="K47" s="160"/>
-      <c r="L47" s="160" t="s">
+      <c r="K47" s="158"/>
+      <c r="L47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="M47" s="160"/>
-      <c r="N47" s="160" t="s">
+      <c r="M47" s="158"/>
+      <c r="N47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="O47" s="160"/>
-      <c r="P47" s="160" t="s">
+      <c r="O47" s="158"/>
+      <c r="P47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="Q47" s="160"/>
-      <c r="R47" s="160" t="s">
+      <c r="Q47" s="158"/>
+      <c r="R47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="S47" s="160"/>
-      <c r="T47" s="160" t="s">
+      <c r="S47" s="158"/>
+      <c r="T47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="U47" s="160"/>
-      <c r="V47" s="160" t="s">
+      <c r="U47" s="158"/>
+      <c r="V47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="W47" s="160"/>
-      <c r="X47" s="160" t="s">
+      <c r="W47" s="158"/>
+      <c r="X47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="Y47" s="160"/>
-      <c r="Z47" s="160" t="s">
+      <c r="Y47" s="158"/>
+      <c r="Z47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AA47" s="160"/>
-      <c r="AB47" s="160" t="s">
+      <c r="AA47" s="158"/>
+      <c r="AB47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AC47" s="160"/>
-      <c r="AD47" s="160" t="s">
+      <c r="AC47" s="158"/>
+      <c r="AD47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AE47" s="160"/>
-      <c r="AF47" s="160" t="s">
+      <c r="AE47" s="158"/>
+      <c r="AF47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AG47" s="160"/>
-      <c r="AH47" s="160" t="s">
+      <c r="AG47" s="158"/>
+      <c r="AH47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AI47" s="160"/>
-      <c r="AJ47" s="160" t="s">
+      <c r="AI47" s="158"/>
+      <c r="AJ47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AK47" s="160"/>
-      <c r="AL47" s="160" t="s">
+      <c r="AK47" s="158"/>
+      <c r="AL47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AM47" s="160"/>
-      <c r="AN47" s="160" t="s">
+      <c r="AM47" s="158"/>
+      <c r="AN47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AO47" s="160"/>
-      <c r="AP47" s="160" t="s">
+      <c r="AO47" s="158"/>
+      <c r="AP47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AQ47" s="160"/>
-      <c r="AR47" s="160" t="s">
+      <c r="AQ47" s="158"/>
+      <c r="AR47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AS47" s="160"/>
-      <c r="AT47" s="160" t="s">
+      <c r="AS47" s="158"/>
+      <c r="AT47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AU47" s="160"/>
-      <c r="AV47" s="160" t="s">
+      <c r="AU47" s="158"/>
+      <c r="AV47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AW47" s="160"/>
-      <c r="AX47" s="160" t="s">
+      <c r="AW47" s="158"/>
+      <c r="AX47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AY47" s="160"/>
-      <c r="AZ47" s="160" t="s">
+      <c r="AY47" s="158"/>
+      <c r="AZ47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BA47" s="160"/>
-      <c r="BB47" s="160" t="s">
+      <c r="BA47" s="158"/>
+      <c r="BB47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BC47" s="160"/>
-      <c r="BD47" s="160" t="s">
+      <c r="BC47" s="158"/>
+      <c r="BD47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BE47" s="160"/>
-      <c r="BF47" s="160" t="s">
+      <c r="BE47" s="158"/>
+      <c r="BF47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BG47" s="160"/>
-      <c r="BH47" s="160" t="s">
+      <c r="BG47" s="158"/>
+      <c r="BH47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BI47" s="160"/>
-      <c r="BJ47" s="160" t="s">
+      <c r="BI47" s="158"/>
+      <c r="BJ47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BK47" s="160"/>
-      <c r="BL47" s="160" t="s">
+      <c r="BK47" s="158"/>
+      <c r="BL47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BM47" s="160"/>
-      <c r="BN47" s="160" t="s">
+      <c r="BM47" s="158"/>
+      <c r="BN47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BO47" s="160"/>
-      <c r="BP47" s="160" t="s">
+      <c r="BO47" s="158"/>
+      <c r="BP47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BQ47" s="160"/>
-      <c r="BR47" s="160" t="s">
+      <c r="BQ47" s="158"/>
+      <c r="BR47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BS47" s="160"/>
-      <c r="BT47" s="160" t="s">
+      <c r="BS47" s="158"/>
+      <c r="BT47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BU47" s="160"/>
-      <c r="BV47" s="160" t="s">
+      <c r="BU47" s="158"/>
+      <c r="BV47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BW47" s="160"/>
-      <c r="BX47" s="160" t="s">
+      <c r="BW47" s="158"/>
+      <c r="BX47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BY47" s="160"/>
-      <c r="BZ47" s="160" t="s">
+      <c r="BY47" s="158"/>
+      <c r="BZ47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CA47" s="160"/>
-      <c r="CB47" s="160" t="s">
+      <c r="CA47" s="158"/>
+      <c r="CB47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="CC47" s="160"/>
-      <c r="CD47" s="160" t="s">
+      <c r="CC47" s="158"/>
+      <c r="CD47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CE47" s="160"/>
-      <c r="CF47" s="160" t="s">
+      <c r="CE47" s="158"/>
+      <c r="CF47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CG47" s="160"/>
-      <c r="CH47" s="160" t="s">
+      <c r="CG47" s="158"/>
+      <c r="CH47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CI47" s="160"/>
-      <c r="CJ47" s="160" t="s">
+      <c r="CI47" s="158"/>
+      <c r="CJ47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="CK47" s="160"/>
-      <c r="CL47" s="160" t="s">
+      <c r="CK47" s="158"/>
+      <c r="CL47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CM47" s="160"/>
-      <c r="CN47" s="160" t="s">
+      <c r="CM47" s="158"/>
+      <c r="CN47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CO47" s="160"/>
-      <c r="CP47" s="160" t="s">
+      <c r="CO47" s="158"/>
+      <c r="CP47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CQ47" s="160"/>
-      <c r="CR47" s="160" t="s">
+      <c r="CQ47" s="158"/>
+      <c r="CR47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="CS47" s="160"/>
-      <c r="CT47" s="160" t="s">
+      <c r="CS47" s="158"/>
+      <c r="CT47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CU47" s="160"/>
-      <c r="CV47" s="160" t="s">
+      <c r="CU47" s="158"/>
+      <c r="CV47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CW47" s="160"/>
-      <c r="CX47" s="160" t="s">
+      <c r="CW47" s="158"/>
+      <c r="CX47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CY47" s="160"/>
-      <c r="CZ47" s="160" t="s">
+      <c r="CY47" s="158"/>
+      <c r="CZ47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="DA47" s="160"/>
-      <c r="DB47" s="160" t="s">
+      <c r="DA47" s="158"/>
+      <c r="DB47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="DC47" s="160"/>
-      <c r="DD47" s="160" t="s">
+      <c r="DC47" s="158"/>
+      <c r="DD47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="DE47" s="160"/>
-      <c r="DF47" s="160" t="s">
+      <c r="DE47" s="158"/>
+      <c r="DF47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="DG47" s="160"/>
-      <c r="DH47" s="160" t="s">
+      <c r="DG47" s="158"/>
+      <c r="DH47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="DI47" s="160"/>
-      <c r="DJ47" s="160" t="s">
+      <c r="DI47" s="158"/>
+      <c r="DJ47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="DK47" s="160"/>
-      <c r="DL47" s="160" t="s">
+      <c r="DK47" s="158"/>
+      <c r="DL47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="DM47" s="160"/>
-      <c r="DN47" s="160" t="s">
+      <c r="DM47" s="158"/>
+      <c r="DN47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="DO47" s="160"/>
-      <c r="DP47" s="160" t="s">
+      <c r="DO47" s="158"/>
+      <c r="DP47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="DQ47" s="160"/>
-      <c r="DR47" s="160" t="s">
+      <c r="DQ47" s="158"/>
+      <c r="DR47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="DS47" s="160"/>
-      <c r="DT47" s="160" t="s">
+      <c r="DS47" s="158"/>
+      <c r="DT47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="DU47" s="160"/>
-      <c r="DV47" s="160" t="s">
+      <c r="DU47" s="158"/>
+      <c r="DV47" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="DW47" s="160"/>
-      <c r="DX47" s="160" t="s">
+      <c r="DW47" s="158"/>
+      <c r="DX47" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="DY47" s="160"/>
-      <c r="DZ47" s="160" t="s">
+      <c r="DY47" s="158"/>
+      <c r="DZ47" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="EA47" s="160"/>
-      <c r="EB47" s="160" t="s">
+      <c r="EA47" s="158"/>
+      <c r="EB47" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="EC47" s="160"/>
+      <c r="EC47" s="158"/>
     </row>
     <row r="49" spans="11:36">
       <c r="K49" t="s">
@@ -18304,74 +18331,285 @@
         <v>448</v>
       </c>
     </row>
-    <row r="65" spans="27:29">
+    <row r="65" spans="4:29">
       <c r="AA65" s="45" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="66" spans="27:29">
+    <row r="66" spans="4:29">
       <c r="AB66" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="67" spans="27:29">
+    <row r="67" spans="4:29">
       <c r="AC67" t="s">
         <v>424</v>
       </c>
     </row>
+    <row r="78" spans="4:29">
+      <c r="D78" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="79" spans="4:29">
+      <c r="X79" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="80" spans="4:29">
+      <c r="I80">
+        <v>7</v>
+      </c>
+      <c r="J80">
+        <v>6</v>
+      </c>
+      <c r="K80">
+        <v>5</v>
+      </c>
+      <c r="L80">
+        <v>4</v>
+      </c>
+      <c r="M80">
+        <v>3</v>
+      </c>
+      <c r="N80">
+        <v>2</v>
+      </c>
+      <c r="O80">
+        <v>1</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="3:32">
+      <c r="D81" t="s">
+        <v>455</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" s="42"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="43"/>
+      <c r="L81" s="41"/>
+      <c r="M81" s="41"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="42"/>
+      <c r="P81" s="43"/>
+      <c r="T81" t="s">
+        <v>455</v>
+      </c>
+      <c r="X81">
+        <v>7</v>
+      </c>
+      <c r="Y81" s="43"/>
+      <c r="Z81" s="43"/>
+      <c r="AA81" s="43"/>
+      <c r="AB81" s="41"/>
+      <c r="AC81" s="41"/>
+      <c r="AD81" s="43"/>
+      <c r="AE81" s="43"/>
+      <c r="AF81" s="43"/>
+    </row>
+    <row r="82" spans="3:32">
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82" s="42"/>
+      <c r="J82" s="42"/>
+      <c r="K82" s="43"/>
+      <c r="L82" s="41"/>
+      <c r="M82" s="41"/>
+      <c r="N82" s="42"/>
+      <c r="O82" s="42"/>
+      <c r="P82" s="43"/>
+      <c r="X82">
+        <v>6</v>
+      </c>
+      <c r="Y82" s="42"/>
+      <c r="Z82" s="42"/>
+      <c r="AA82" s="43"/>
+      <c r="AB82" s="41"/>
+      <c r="AC82" s="41"/>
+      <c r="AD82" s="42"/>
+      <c r="AE82" s="42"/>
+      <c r="AF82" s="43"/>
+    </row>
+    <row r="83" spans="3:32">
+      <c r="D83" t="s">
+        <v>454</v>
+      </c>
+      <c r="H83">
+        <v>2</v>
+      </c>
+      <c r="I83" s="42"/>
+      <c r="J83" s="42"/>
+      <c r="K83" s="42"/>
+      <c r="L83" s="43"/>
+      <c r="M83" s="42"/>
+      <c r="N83" s="42"/>
+      <c r="O83" s="42"/>
+      <c r="P83" s="43"/>
+      <c r="T83" t="s">
+        <v>454</v>
+      </c>
+      <c r="X83">
+        <v>5</v>
+      </c>
+      <c r="Y83" s="42"/>
+      <c r="Z83" s="42"/>
+      <c r="AA83" s="43"/>
+      <c r="AB83" s="41"/>
+      <c r="AC83" s="41"/>
+      <c r="AD83" s="42"/>
+      <c r="AE83" s="42"/>
+      <c r="AF83" s="43"/>
+    </row>
+    <row r="84" spans="3:32">
+      <c r="D84" t="s">
+        <v>456</v>
+      </c>
+      <c r="H84">
+        <v>3</v>
+      </c>
+      <c r="I84" s="42"/>
+      <c r="J84" s="42"/>
+      <c r="K84" s="43"/>
+      <c r="L84" s="42"/>
+      <c r="M84" s="43"/>
+      <c r="N84" s="42"/>
+      <c r="O84" s="42"/>
+      <c r="P84" s="43"/>
+      <c r="T84" t="s">
+        <v>456</v>
+      </c>
+      <c r="X84">
+        <v>4</v>
+      </c>
+      <c r="Y84" s="42"/>
+      <c r="Z84" s="42"/>
+      <c r="AA84" s="43"/>
+      <c r="AB84" s="43"/>
+      <c r="AC84" s="43"/>
+      <c r="AD84" s="42"/>
+      <c r="AE84" s="42"/>
+      <c r="AF84" s="43"/>
+    </row>
+    <row r="85" spans="3:32">
+      <c r="H85">
+        <v>4</v>
+      </c>
+      <c r="I85" s="42"/>
+      <c r="J85" s="42"/>
+      <c r="K85" s="43"/>
+      <c r="L85" s="43"/>
+      <c r="M85" s="43"/>
+      <c r="N85" s="42"/>
+      <c r="O85" s="42"/>
+      <c r="P85" s="43"/>
+      <c r="X85">
+        <v>3</v>
+      </c>
+      <c r="Y85" s="42"/>
+      <c r="Z85" s="42"/>
+      <c r="AA85" s="43"/>
+      <c r="AB85" s="42"/>
+      <c r="AC85" s="43"/>
+      <c r="AD85" s="42"/>
+      <c r="AE85" s="42"/>
+      <c r="AF85" s="43"/>
+    </row>
+    <row r="86" spans="3:32">
+      <c r="H86">
+        <v>5</v>
+      </c>
+      <c r="I86" s="42"/>
+      <c r="J86" s="42"/>
+      <c r="K86" s="43"/>
+      <c r="L86" s="41"/>
+      <c r="M86" s="41"/>
+      <c r="N86" s="42"/>
+      <c r="O86" s="42"/>
+      <c r="P86" s="43"/>
+      <c r="X86">
+        <v>2</v>
+      </c>
+      <c r="Y86" s="42"/>
+      <c r="Z86" s="42"/>
+      <c r="AA86" s="42"/>
+      <c r="AB86" s="43"/>
+      <c r="AC86" s="42"/>
+      <c r="AD86" s="42"/>
+      <c r="AE86" s="42"/>
+      <c r="AF86" s="43"/>
+    </row>
+    <row r="87" spans="3:32">
+      <c r="H87">
+        <v>6</v>
+      </c>
+      <c r="I87" s="42"/>
+      <c r="J87" s="42"/>
+      <c r="K87" s="43"/>
+      <c r="L87" s="41"/>
+      <c r="M87" s="41"/>
+      <c r="N87" s="42"/>
+      <c r="O87" s="42"/>
+      <c r="P87" s="43"/>
+      <c r="X87">
+        <v>1</v>
+      </c>
+      <c r="Y87" s="42"/>
+      <c r="Z87" s="42"/>
+      <c r="AA87" s="43"/>
+      <c r="AB87" s="41"/>
+      <c r="AC87" s="41"/>
+      <c r="AD87" s="42"/>
+      <c r="AE87" s="42"/>
+      <c r="AF87" s="43"/>
+    </row>
+    <row r="88" spans="3:32">
+      <c r="H88">
+        <v>7</v>
+      </c>
+      <c r="I88" s="43"/>
+      <c r="J88" s="43"/>
+      <c r="K88" s="43"/>
+      <c r="L88" s="41"/>
+      <c r="M88" s="41"/>
+      <c r="N88" s="43"/>
+      <c r="O88" s="43"/>
+      <c r="P88" s="43"/>
+      <c r="X88">
+        <v>0</v>
+      </c>
+      <c r="Y88" s="42"/>
+      <c r="Z88" s="42"/>
+      <c r="AA88" s="43"/>
+      <c r="AB88" s="41"/>
+      <c r="AC88" s="41"/>
+      <c r="AD88" s="42"/>
+      <c r="AE88" s="42"/>
+      <c r="AF88" s="43"/>
+    </row>
+    <row r="89" spans="3:32">
+      <c r="C89" t="s">
+        <v>459</v>
+      </c>
+      <c r="U89" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="90" spans="3:32">
+      <c r="E90" t="s">
+        <v>457</v>
+      </c>
+      <c r="W90" t="s">
+        <v>460</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="AN47:AO47"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="X47:Y47"/>
-    <mergeCell ref="Z47:AA47"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AD47:AE47"/>
-    <mergeCell ref="AF47:AG47"/>
-    <mergeCell ref="AH47:AI47"/>
-    <mergeCell ref="AJ47:AK47"/>
-    <mergeCell ref="AL47:AM47"/>
-    <mergeCell ref="BL47:BM47"/>
-    <mergeCell ref="AP47:AQ47"/>
-    <mergeCell ref="AR47:AS47"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="AV47:AW47"/>
-    <mergeCell ref="AX47:AY47"/>
-    <mergeCell ref="AZ47:BA47"/>
-    <mergeCell ref="BB47:BC47"/>
-    <mergeCell ref="BD47:BE47"/>
-    <mergeCell ref="BF47:BG47"/>
-    <mergeCell ref="BH47:BI47"/>
-    <mergeCell ref="BJ47:BK47"/>
-    <mergeCell ref="CJ47:CK47"/>
-    <mergeCell ref="BN47:BO47"/>
-    <mergeCell ref="BP47:BQ47"/>
-    <mergeCell ref="BR47:BS47"/>
-    <mergeCell ref="BT47:BU47"/>
-    <mergeCell ref="BV47:BW47"/>
-    <mergeCell ref="BX47:BY47"/>
-    <mergeCell ref="BZ47:CA47"/>
-    <mergeCell ref="CB47:CC47"/>
-    <mergeCell ref="CD47:CE47"/>
-    <mergeCell ref="CF47:CG47"/>
-    <mergeCell ref="CH47:CI47"/>
-    <mergeCell ref="DD47:DE47"/>
-    <mergeCell ref="DF47:DG47"/>
-    <mergeCell ref="DH47:DI47"/>
-    <mergeCell ref="CL47:CM47"/>
-    <mergeCell ref="CN47:CO47"/>
-    <mergeCell ref="CP47:CQ47"/>
-    <mergeCell ref="CR47:CS47"/>
-    <mergeCell ref="CT47:CU47"/>
-    <mergeCell ref="CV47:CW47"/>
     <mergeCell ref="DV47:DW47"/>
     <mergeCell ref="DX47:DY47"/>
     <mergeCell ref="DZ47:EA47"/>
@@ -18388,6 +18626,57 @@
     <mergeCell ref="CX47:CY47"/>
     <mergeCell ref="CZ47:DA47"/>
     <mergeCell ref="DB47:DC47"/>
+    <mergeCell ref="DD47:DE47"/>
+    <mergeCell ref="DF47:DG47"/>
+    <mergeCell ref="DH47:DI47"/>
+    <mergeCell ref="CL47:CM47"/>
+    <mergeCell ref="CN47:CO47"/>
+    <mergeCell ref="CP47:CQ47"/>
+    <mergeCell ref="CR47:CS47"/>
+    <mergeCell ref="CT47:CU47"/>
+    <mergeCell ref="CV47:CW47"/>
+    <mergeCell ref="CJ47:CK47"/>
+    <mergeCell ref="BN47:BO47"/>
+    <mergeCell ref="BP47:BQ47"/>
+    <mergeCell ref="BR47:BS47"/>
+    <mergeCell ref="BT47:BU47"/>
+    <mergeCell ref="BV47:BW47"/>
+    <mergeCell ref="BX47:BY47"/>
+    <mergeCell ref="BZ47:CA47"/>
+    <mergeCell ref="CB47:CC47"/>
+    <mergeCell ref="CD47:CE47"/>
+    <mergeCell ref="CF47:CG47"/>
+    <mergeCell ref="CH47:CI47"/>
+    <mergeCell ref="BL47:BM47"/>
+    <mergeCell ref="AP47:AQ47"/>
+    <mergeCell ref="AR47:AS47"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="AV47:AW47"/>
+    <mergeCell ref="AX47:AY47"/>
+    <mergeCell ref="AZ47:BA47"/>
+    <mergeCell ref="BB47:BC47"/>
+    <mergeCell ref="BD47:BE47"/>
+    <mergeCell ref="BF47:BG47"/>
+    <mergeCell ref="BH47:BI47"/>
+    <mergeCell ref="BJ47:BK47"/>
+    <mergeCell ref="AN47:AO47"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="AF47:AG47"/>
+    <mergeCell ref="AH47:AI47"/>
+    <mergeCell ref="AJ47:AK47"/>
+    <mergeCell ref="AL47:AM47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18397,19 +18686,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:CB37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AK37" sqref="AK37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
   <cols>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:80" s="27" customFormat="1" ht="46.5">
+    <row r="2" spans="2:80" s="27" customFormat="1" ht="42">
       <c r="F2" s="27">
         <v>0</v>
       </c>
@@ -18623,62 +18912,62 @@
         <v>0</v>
       </c>
       <c r="F3" s="39"/>
-      <c r="G3" s="160" t="s">
+      <c r="G3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160" t="s">
+      <c r="H3" s="158"/>
+      <c r="I3" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160" t="s">
+      <c r="J3" s="158"/>
+      <c r="K3" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="160"/>
-      <c r="M3" s="160" t="s">
+      <c r="L3" s="158"/>
+      <c r="M3" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="160"/>
-      <c r="O3" s="160" t="s">
+      <c r="N3" s="158"/>
+      <c r="O3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="160"/>
-      <c r="Q3" s="160" t="s">
+      <c r="P3" s="158"/>
+      <c r="Q3" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="160"/>
-      <c r="S3" s="160" t="s">
+      <c r="R3" s="158"/>
+      <c r="S3" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="160"/>
-      <c r="U3" s="160" t="s">
+      <c r="T3" s="158"/>
+      <c r="U3" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="160"/>
-      <c r="W3" s="160" t="s">
+      <c r="V3" s="158"/>
+      <c r="W3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="X3" s="160"/>
+      <c r="X3" s="158"/>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="160" t="s">
+      <c r="AC3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="160"/>
-      <c r="AE3" s="160" t="s">
+      <c r="AD3" s="158"/>
+      <c r="AE3" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AF3" s="160"/>
-      <c r="AG3" s="160" t="s">
+      <c r="AF3" s="158"/>
+      <c r="AG3" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="160"/>
-      <c r="AI3" s="160" t="s">
+      <c r="AH3" s="158"/>
+      <c r="AI3" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AJ3" s="160"/>
+      <c r="AJ3" s="158"/>
       <c r="AK3" s="34"/>
       <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
@@ -18701,104 +18990,104 @@
       <c r="BH3" s="34"/>
       <c r="BI3" s="34"/>
       <c r="BJ3" s="34"/>
-      <c r="BK3" s="158" t="s">
+      <c r="BK3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BL3" s="159"/>
-      <c r="BM3" s="158" t="s">
+      <c r="BL3" s="161"/>
+      <c r="BM3" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BN3" s="159"/>
-      <c r="BO3" s="158" t="s">
+      <c r="BN3" s="161"/>
+      <c r="BO3" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" s="159"/>
-      <c r="BQ3" s="158" t="s">
+      <c r="BP3" s="161"/>
+      <c r="BQ3" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BR3" s="159"/>
-      <c r="BS3" s="158" t="s">
+      <c r="BR3" s="161"/>
+      <c r="BS3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="159"/>
-      <c r="BU3" s="158" t="s">
+      <c r="BT3" s="161"/>
+      <c r="BU3" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BV3" s="159"/>
-      <c r="BW3" s="158" t="s">
+      <c r="BV3" s="161"/>
+      <c r="BW3" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BX3" s="159"/>
-      <c r="BY3" s="158" t="s">
+      <c r="BX3" s="161"/>
+      <c r="BY3" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BZ3" s="159"/>
-      <c r="CA3" s="158" t="s">
+      <c r="BZ3" s="161"/>
+      <c r="CA3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CB3" s="159"/>
+      <c r="CB3" s="161"/>
     </row>
     <row r="4" spans="2:80">
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="34"/>
-      <c r="G4" s="160" t="s">
+      <c r="G4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160" t="s">
+      <c r="H4" s="158"/>
+      <c r="I4" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160" t="s">
+      <c r="J4" s="158"/>
+      <c r="K4" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="160"/>
-      <c r="M4" s="160" t="s">
+      <c r="L4" s="158"/>
+      <c r="M4" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="160"/>
-      <c r="O4" s="160" t="s">
+      <c r="N4" s="158"/>
+      <c r="O4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="P4" s="160"/>
-      <c r="Q4" s="160" t="s">
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="R4" s="160"/>
-      <c r="S4" s="160" t="s">
+      <c r="R4" s="158"/>
+      <c r="S4" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="160"/>
-      <c r="U4" s="160" t="s">
+      <c r="T4" s="158"/>
+      <c r="U4" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160" t="s">
+      <c r="V4" s="158"/>
+      <c r="W4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="160"/>
+      <c r="X4" s="158"/>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="160" t="s">
+      <c r="AC4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AD4" s="160"/>
-      <c r="AE4" s="160" t="s">
+      <c r="AD4" s="158"/>
+      <c r="AE4" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="160"/>
-      <c r="AG4" s="160" t="s">
+      <c r="AF4" s="158"/>
+      <c r="AG4" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AH4" s="160"/>
-      <c r="AI4" s="160" t="s">
+      <c r="AH4" s="158"/>
+      <c r="AI4" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="160"/>
+      <c r="AJ4" s="158"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
@@ -18821,42 +19110,42 @@
       <c r="BH4" s="34"/>
       <c r="BI4" s="34"/>
       <c r="BJ4" s="34"/>
-      <c r="BK4" s="158" t="s">
+      <c r="BK4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BL4" s="159"/>
-      <c r="BM4" s="158" t="s">
+      <c r="BL4" s="161"/>
+      <c r="BM4" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BN4" s="159"/>
-      <c r="BO4" s="158" t="s">
+      <c r="BN4" s="161"/>
+      <c r="BO4" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BP4" s="159"/>
-      <c r="BQ4" s="158" t="s">
+      <c r="BP4" s="161"/>
+      <c r="BQ4" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BR4" s="159"/>
-      <c r="BS4" s="158" t="s">
+      <c r="BR4" s="161"/>
+      <c r="BS4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BT4" s="159"/>
-      <c r="BU4" s="158" t="s">
+      <c r="BT4" s="161"/>
+      <c r="BU4" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BV4" s="159"/>
-      <c r="BW4" s="158" t="s">
+      <c r="BV4" s="161"/>
+      <c r="BW4" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="159"/>
-      <c r="BY4" s="158" t="s">
+      <c r="BX4" s="161"/>
+      <c r="BY4" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BZ4" s="159"/>
-      <c r="CA4" s="158" t="s">
+      <c r="BZ4" s="161"/>
+      <c r="CA4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CB4" s="159"/>
+      <c r="CB4" s="161"/>
     </row>
     <row r="5" spans="2:80">
       <c r="BX5" s="27"/>
@@ -18870,62 +19159,62 @@
         <v>239</v>
       </c>
       <c r="F6" s="36"/>
-      <c r="G6" s="165" t="s">
+      <c r="G6" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="165"/>
-      <c r="I6" s="165" t="s">
+      <c r="H6" s="159"/>
+      <c r="I6" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="165"/>
-      <c r="K6" s="165" t="s">
+      <c r="J6" s="159"/>
+      <c r="K6" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="165"/>
-      <c r="M6" s="165" t="s">
+      <c r="L6" s="159"/>
+      <c r="M6" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="165"/>
-      <c r="O6" s="165" t="s">
+      <c r="N6" s="159"/>
+      <c r="O6" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="165"/>
-      <c r="Q6" s="165" t="s">
+      <c r="P6" s="159"/>
+      <c r="Q6" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="R6" s="165"/>
-      <c r="S6" s="165" t="s">
+      <c r="R6" s="159"/>
+      <c r="S6" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="165"/>
-      <c r="U6" s="165" t="s">
+      <c r="T6" s="159"/>
+      <c r="U6" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="V6" s="165"/>
-      <c r="W6" s="165" t="s">
+      <c r="V6" s="159"/>
+      <c r="W6" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="X6" s="165"/>
+      <c r="X6" s="159"/>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AC6" s="165" t="s">
+      <c r="AC6" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" s="165"/>
-      <c r="AE6" s="165" t="s">
+      <c r="AD6" s="159"/>
+      <c r="AE6" s="159" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="165"/>
-      <c r="AG6" s="165" t="s">
+      <c r="AF6" s="159"/>
+      <c r="AG6" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="AH6" s="165"/>
-      <c r="AI6" s="165" t="s">
+      <c r="AH6" s="159"/>
+      <c r="AI6" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="AJ6" s="165"/>
+      <c r="AJ6" s="159"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -18948,42 +19237,42 @@
       <c r="BH6" s="34"/>
       <c r="BI6" s="34"/>
       <c r="BJ6" s="34"/>
-      <c r="BK6" s="158" t="s">
+      <c r="BK6" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BL6" s="159"/>
-      <c r="BM6" s="158" t="s">
+      <c r="BL6" s="161"/>
+      <c r="BM6" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BN6" s="159"/>
-      <c r="BO6" s="158" t="s">
+      <c r="BN6" s="161"/>
+      <c r="BO6" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BP6" s="159"/>
-      <c r="BQ6" s="158" t="s">
+      <c r="BP6" s="161"/>
+      <c r="BQ6" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BR6" s="159"/>
-      <c r="BS6" s="158" t="s">
+      <c r="BR6" s="161"/>
+      <c r="BS6" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BT6" s="159"/>
-      <c r="BU6" s="158" t="s">
+      <c r="BT6" s="161"/>
+      <c r="BU6" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BV6" s="159"/>
-      <c r="BW6" s="158" t="s">
+      <c r="BV6" s="161"/>
+      <c r="BW6" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BX6" s="159"/>
-      <c r="BY6" s="158" t="s">
+      <c r="BX6" s="161"/>
+      <c r="BY6" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BZ6" s="159"/>
-      <c r="CA6" s="158" t="s">
+      <c r="BZ6" s="161"/>
+      <c r="CA6" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CB6" s="159"/>
+      <c r="CB6" s="161"/>
     </row>
     <row r="7" spans="2:80">
       <c r="E7">
@@ -19319,58 +19608,58 @@
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="160" t="s">
+      <c r="I12" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="160"/>
-      <c r="K12" s="160" t="s">
+      <c r="J12" s="158"/>
+      <c r="K12" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="160"/>
-      <c r="M12" s="160" t="s">
+      <c r="L12" s="158"/>
+      <c r="M12" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="160"/>
-      <c r="O12" s="160" t="s">
+      <c r="N12" s="158"/>
+      <c r="O12" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="P12" s="160"/>
-      <c r="Q12" s="160" t="s">
+      <c r="P12" s="158"/>
+      <c r="Q12" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="160"/>
-      <c r="S12" s="160" t="s">
+      <c r="R12" s="158"/>
+      <c r="S12" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="T12" s="160"/>
-      <c r="U12" s="160" t="s">
+      <c r="T12" s="158"/>
+      <c r="U12" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="160"/>
-      <c r="W12" s="160" t="s">
+      <c r="V12" s="158"/>
+      <c r="W12" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="160"/>
+      <c r="X12" s="158"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="160" t="s">
+      <c r="AC12" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="160"/>
-      <c r="AE12" s="160" t="s">
+      <c r="AD12" s="158"/>
+      <c r="AE12" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AF12" s="160"/>
-      <c r="AG12" s="160" t="s">
+      <c r="AF12" s="158"/>
+      <c r="AG12" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="AH12" s="160"/>
-      <c r="AI12" s="160" t="s">
+      <c r="AH12" s="158"/>
+      <c r="AI12" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="AJ12" s="160"/>
+      <c r="AJ12" s="158"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="34"/>
       <c r="AM12" s="34"/>
@@ -19393,42 +19682,42 @@
       <c r="BH12" s="34"/>
       <c r="BI12" s="34"/>
       <c r="BJ12" s="34"/>
-      <c r="BK12" s="158" t="s">
+      <c r="BK12" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BL12" s="159"/>
-      <c r="BM12" s="158" t="s">
+      <c r="BL12" s="161"/>
+      <c r="BM12" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BN12" s="159"/>
-      <c r="BO12" s="158" t="s">
+      <c r="BN12" s="161"/>
+      <c r="BO12" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BP12" s="159"/>
-      <c r="BQ12" s="158" t="s">
+      <c r="BP12" s="161"/>
+      <c r="BQ12" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BR12" s="159"/>
-      <c r="BS12" s="158" t="s">
+      <c r="BR12" s="161"/>
+      <c r="BS12" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BT12" s="159"/>
-      <c r="BU12" s="158" t="s">
+      <c r="BT12" s="161"/>
+      <c r="BU12" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BV12" s="159"/>
-      <c r="BW12" s="158" t="s">
+      <c r="BV12" s="161"/>
+      <c r="BW12" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BX12" s="159"/>
-      <c r="BY12" s="158" t="s">
+      <c r="BX12" s="161"/>
+      <c r="BY12" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BZ12" s="159"/>
-      <c r="CA12" s="158" t="s">
+      <c r="BZ12" s="161"/>
+      <c r="CA12" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CB12" s="159"/>
+      <c r="CB12" s="161"/>
     </row>
     <row r="13" spans="2:80">
       <c r="BX13" s="27"/>
@@ -19461,71 +19750,71 @@
         <v>120</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="164" t="s">
+      <c r="G16" s="165" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="164"/>
-      <c r="I16" s="164"/>
-      <c r="J16" s="164"/>
-      <c r="K16" s="164"/>
-      <c r="L16" s="164"/>
-      <c r="M16" s="164"/>
-      <c r="N16" s="164"/>
-      <c r="O16" s="164"/>
-      <c r="P16" s="164"/>
-      <c r="Q16" s="164"/>
-      <c r="R16" s="164"/>
-      <c r="S16" s="164"/>
-      <c r="T16" s="164"/>
-      <c r="U16" s="164"/>
-      <c r="V16" s="164"/>
-      <c r="W16" s="164"/>
-      <c r="X16" s="164"/>
-      <c r="Y16" s="164"/>
-      <c r="Z16" s="164"/>
-      <c r="AA16" s="164" t="s">
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
+      <c r="M16" s="165"/>
+      <c r="N16" s="165"/>
+      <c r="O16" s="165"/>
+      <c r="P16" s="165"/>
+      <c r="Q16" s="165"/>
+      <c r="R16" s="165"/>
+      <c r="S16" s="165"/>
+      <c r="T16" s="165"/>
+      <c r="U16" s="165"/>
+      <c r="V16" s="165"/>
+      <c r="W16" s="165"/>
+      <c r="X16" s="165"/>
+      <c r="Y16" s="165"/>
+      <c r="Z16" s="165"/>
+      <c r="AA16" s="165" t="s">
         <v>116</v>
       </c>
-      <c r="AB16" s="164"/>
-      <c r="AC16" s="164"/>
-      <c r="AD16" s="164"/>
-      <c r="AE16" s="164"/>
-      <c r="AF16" s="164"/>
-      <c r="AG16" s="164"/>
-      <c r="AH16" s="164"/>
-      <c r="AI16" s="164"/>
-      <c r="AJ16" s="164"/>
-      <c r="AK16" s="160" t="s">
+      <c r="AB16" s="165"/>
+      <c r="AC16" s="165"/>
+      <c r="AD16" s="165"/>
+      <c r="AE16" s="165"/>
+      <c r="AF16" s="165"/>
+      <c r="AG16" s="165"/>
+      <c r="AH16" s="165"/>
+      <c r="AI16" s="165"/>
+      <c r="AJ16" s="165"/>
+      <c r="AK16" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="AL16" s="160"/>
-      <c r="AM16" s="160" t="s">
+      <c r="AL16" s="158"/>
+      <c r="AM16" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="AN16" s="160"/>
-      <c r="AO16" s="160" t="s">
+      <c r="AN16" s="158"/>
+      <c r="AO16" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="AP16" s="160"/>
-      <c r="AQ16" s="160" t="s">
+      <c r="AP16" s="158"/>
+      <c r="AQ16" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="AR16" s="160"/>
-      <c r="AS16" s="161" t="s">
+      <c r="AR16" s="158"/>
+      <c r="AS16" s="162" t="s">
         <v>119</v>
       </c>
-      <c r="AT16" s="162"/>
-      <c r="AU16" s="162"/>
-      <c r="AV16" s="162"/>
-      <c r="AW16" s="162"/>
-      <c r="AX16" s="162"/>
-      <c r="AY16" s="162"/>
-      <c r="AZ16" s="162"/>
-      <c r="BA16" s="163"/>
-      <c r="BB16" s="160" t="s">
+      <c r="AT16" s="163"/>
+      <c r="AU16" s="163"/>
+      <c r="AV16" s="163"/>
+      <c r="AW16" s="163"/>
+      <c r="AX16" s="163"/>
+      <c r="AY16" s="163"/>
+      <c r="AZ16" s="163"/>
+      <c r="BA16" s="164"/>
+      <c r="BB16" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="BC16" s="160"/>
+      <c r="BC16" s="158"/>
       <c r="BE16" s="38"/>
       <c r="BF16" s="38"/>
       <c r="BG16" s="38"/>
@@ -20074,18 +20363,73 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="BB16:BC16"/>
+    <mergeCell ref="BW12:BX12"/>
+    <mergeCell ref="BY12:BZ12"/>
+    <mergeCell ref="CA12:CB12"/>
+    <mergeCell ref="G16:Z16"/>
+    <mergeCell ref="AA16:AJ16"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AM16:AN16"/>
+    <mergeCell ref="AO16:AP16"/>
+    <mergeCell ref="AQ16:AR16"/>
+    <mergeCell ref="AS16:BA16"/>
+    <mergeCell ref="BK12:BL12"/>
+    <mergeCell ref="BM12:BN12"/>
+    <mergeCell ref="BO12:BP12"/>
+    <mergeCell ref="BQ12:BR12"/>
+    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AC6:AD6"/>
     <mergeCell ref="BU3:BV3"/>
     <mergeCell ref="BW3:BX3"/>
     <mergeCell ref="BY3:BZ3"/>
@@ -20102,73 +20446,18 @@
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="BQ3:BR3"/>
     <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="BB16:BC16"/>
-    <mergeCell ref="BW12:BX12"/>
-    <mergeCell ref="BY12:BZ12"/>
-    <mergeCell ref="CA12:CB12"/>
-    <mergeCell ref="G16:Z16"/>
-    <mergeCell ref="AA16:AJ16"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AM16:AN16"/>
-    <mergeCell ref="AO16:AP16"/>
-    <mergeCell ref="AQ16:AR16"/>
-    <mergeCell ref="AS16:BA16"/>
-    <mergeCell ref="BK12:BL12"/>
-    <mergeCell ref="BM12:BN12"/>
-    <mergeCell ref="BO12:BP12"/>
-    <mergeCell ref="BQ12:BR12"/>
-    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20178,14 +20467,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F50"/>
   <sheetViews>
     <sheetView topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" t="s">
@@ -20215,17 +20504,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:AB16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="20" max="20" width="5.140625" customWidth="1"/>
-    <col min="21" max="28" width="3.42578125" customWidth="1"/>
+    <col min="20" max="20" width="5.125" customWidth="1"/>
+    <col min="21" max="28" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:28">
@@ -20236,7 +20525,7 @@
     <row r="5" spans="1:28" ht="17.25">
       <c r="A5" s="48"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="14.25">
       <c r="A6" s="49"/>
       <c r="B6" s="50">
         <v>0</v>
@@ -20287,7 +20576,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="28.5">
+    <row r="7" spans="1:28" ht="14.25">
       <c r="A7" s="106" t="s">
         <v>227</v>
       </c>
@@ -20343,7 +20632,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="28.5">
+    <row r="8" spans="1:28" ht="14.25">
       <c r="A8" s="50">
         <v>10</v>
       </c>
@@ -20397,7 +20686,7 @@
       </c>
       <c r="R8" s="169"/>
     </row>
-    <row r="9" spans="1:28" ht="28.5">
+    <row r="9" spans="1:28" ht="14.25">
       <c r="A9" s="50">
         <v>20</v>
       </c>
@@ -20453,7 +20742,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="28.5">
+    <row r="10" spans="1:28" ht="14.25">
       <c r="A10" s="50">
         <v>30</v>
       </c>
@@ -20623,17 +20912,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="5.25" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="2" spans="2:25" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:25">
+    <row r="2" spans="2:25" ht="14.25" thickBot="1"/>
+    <row r="3" spans="2:25" ht="14.25">
       <c r="B3" s="114" t="s">
         <v>238</v>
       </c>
@@ -20707,7 +20996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:25" ht="15.75" thickBot="1">
+    <row r="4" spans="2:25" ht="15" thickBot="1">
       <c r="B4" s="117" t="s">
         <v>239</v>
       </c>
@@ -20781,7 +21070,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="15.75" thickBot="1">
+    <row r="5" spans="2:25" ht="15" thickBot="1">
       <c r="B5" s="119" t="s">
         <v>241</v>
       </c>
@@ -20855,7 +21144,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="15.75" thickBot="1">
+    <row r="6" spans="2:25" ht="15" thickBot="1">
       <c r="B6" s="121" t="s">
         <v>242</v>
       </c>
@@ -20929,7 +21218,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="15.75" thickBot="1">
+    <row r="7" spans="2:25" ht="15" thickBot="1">
       <c r="B7" s="119" t="s">
         <v>243</v>
       </c>
@@ -21003,7 +21292,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:25" ht="15.75" thickBot="1">
+    <row r="8" spans="2:25" ht="15" thickBot="1">
       <c r="B8" s="121" t="s">
         <v>244</v>
       </c>
@@ -21077,7 +21366,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:25" ht="15.75" thickBot="1">
+    <row r="9" spans="2:25" ht="15" thickBot="1">
       <c r="B9" s="119" t="s">
         <v>245</v>
       </c>
@@ -21151,7 +21440,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:25" ht="15.75" thickBot="1">
+    <row r="10" spans="2:25" ht="15" thickBot="1">
       <c r="B10" s="121" t="s">
         <v>246</v>
       </c>
@@ -21225,7 +21514,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:25" ht="15.75" thickBot="1">
+    <row r="11" spans="2:25" ht="15" thickBot="1">
       <c r="B11" s="119" t="s">
         <v>247</v>
       </c>
@@ -21299,7 +21588,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:25" ht="15.75" thickBot="1">
+    <row r="12" spans="2:25" ht="15" thickBot="1">
       <c r="B12" s="121" t="s">
         <v>248</v>
       </c>
@@ -21373,7 +21662,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="15.75" thickBot="1">
+    <row r="13" spans="2:25" ht="15" thickBot="1">
       <c r="B13" s="119" t="s">
         <v>249</v>
       </c>
@@ -21447,7 +21736,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="15.75" thickBot="1">
+    <row r="14" spans="2:25" ht="15" thickBot="1">
       <c r="B14" s="121" t="s">
         <v>250</v>
       </c>
@@ -21521,7 +21810,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:25" ht="15.75" thickBot="1">
+    <row r="15" spans="2:25" ht="15" thickBot="1">
       <c r="B15" s="119" t="s">
         <v>251</v>
       </c>
@@ -21595,7 +21884,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="15.75" thickBot="1">
+    <row r="16" spans="2:25" ht="15" thickBot="1">
       <c r="B16" s="121" t="s">
         <v>253</v>
       </c>
@@ -21669,7 +21958,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="15.75" thickBot="1">
+    <row r="17" spans="2:25" ht="15" thickBot="1">
       <c r="B17" s="119" t="s">
         <v>255</v>
       </c>
@@ -21743,7 +22032,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="15.75" thickBot="1">
+    <row r="18" spans="2:25" ht="15" thickBot="1">
       <c r="B18" s="121" t="s">
         <v>257</v>
       </c>
@@ -21817,7 +22106,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="15.75" thickBot="1">
+    <row r="19" spans="2:25" ht="15" thickBot="1">
       <c r="B19" s="119" t="s">
         <v>259</v>
       </c>
@@ -21891,7 +22180,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="2:25" ht="15.75" thickBot="1">
+    <row r="20" spans="2:25" ht="15" thickBot="1">
       <c r="B20" s="123" t="s">
         <v>261</v>
       </c>
@@ -21965,7 +22254,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="21" spans="2:25">
+    <row r="21" spans="2:25" ht="14.25">
       <c r="B21" s="154" t="s">
         <v>407</v>
       </c>

</xml_diff>

<commit_message>
doc update, more work investigation...
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="464">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -1544,6 +1544,18 @@
   </si>
   <si>
     <t>M - N + 6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hsync</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>vsync</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>vblank</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2531,7 +2543,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3006,16 +3018,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3030,6 +3039,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3041,6 +3053,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5078,7 +5111,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>68</xdr:col>
-      <xdr:colOff>225425</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>49825</xdr:rowOff>
     </xdr:to>
@@ -5449,6 +5482,65 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3999442" y="10616142"/>
+          <a:ext cx="1972733" cy="1431925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="7200"/>
+            <a:t>VGA</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="7200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7317,12 +7409,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -7331,6 +7417,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7342,7 +7434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:BX117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -11831,10 +11923,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:CF125"/>
+  <dimension ref="A2:CF166"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AL50" sqref="AL50"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
@@ -11848,8 +11940,9 @@
     <col min="31" max="31" width="2.875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="4.125" customWidth="1"/>
     <col min="36" max="36" width="4.25" customWidth="1"/>
-    <col min="38" max="38" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.625" customWidth="1"/>
     <col min="47" max="47" width="2.625" customWidth="1"/>
     <col min="48" max="48" width="4.875" customWidth="1"/>
     <col min="49" max="49" width="2.875" bestFit="1" customWidth="1"/>
@@ -12086,62 +12179,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="158" t="s">
+      <c r="K33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="158"/>
-      <c r="M33" s="158" t="s">
+      <c r="L33" s="160"/>
+      <c r="M33" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="158"/>
-      <c r="O33" s="158" t="s">
+      <c r="N33" s="160"/>
+      <c r="O33" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="158"/>
-      <c r="Q33" s="158" t="s">
+      <c r="P33" s="160"/>
+      <c r="Q33" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="158"/>
-      <c r="S33" s="158" t="s">
+      <c r="R33" s="160"/>
+      <c r="S33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="158"/>
-      <c r="U33" s="158" t="s">
+      <c r="T33" s="160"/>
+      <c r="U33" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="158"/>
-      <c r="W33" s="158" t="s">
+      <c r="V33" s="160"/>
+      <c r="W33" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="158"/>
-      <c r="Y33" s="158" t="s">
+      <c r="X33" s="160"/>
+      <c r="Y33" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="158"/>
-      <c r="AA33" s="158" t="s">
+      <c r="Z33" s="160"/>
+      <c r="AA33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="158"/>
+      <c r="AB33" s="160"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="158" t="s">
+      <c r="AG33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="158"/>
-      <c r="AI33" s="158" t="s">
+      <c r="AH33" s="160"/>
+      <c r="AI33" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="158"/>
-      <c r="AK33" s="158" t="s">
+      <c r="AJ33" s="160"/>
+      <c r="AK33" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="158"/>
-      <c r="AM33" s="158" t="s">
+      <c r="AL33" s="160"/>
+      <c r="AM33" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="158"/>
+      <c r="AN33" s="160"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -12164,104 +12257,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="160" t="s">
+      <c r="BO33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="161"/>
-      <c r="BQ33" s="160" t="s">
+      <c r="BP33" s="159"/>
+      <c r="BQ33" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="161"/>
-      <c r="BS33" s="160" t="s">
+      <c r="BR33" s="159"/>
+      <c r="BS33" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="161"/>
-      <c r="BU33" s="160" t="s">
+      <c r="BT33" s="159"/>
+      <c r="BU33" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="161"/>
-      <c r="BW33" s="160" t="s">
+      <c r="BV33" s="159"/>
+      <c r="BW33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="161"/>
-      <c r="BY33" s="160" t="s">
+      <c r="BX33" s="159"/>
+      <c r="BY33" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="161"/>
-      <c r="CA33" s="160" t="s">
+      <c r="BZ33" s="159"/>
+      <c r="CA33" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="161"/>
-      <c r="CC33" s="160" t="s">
+      <c r="CB33" s="159"/>
+      <c r="CC33" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="161"/>
-      <c r="CE33" s="160" t="s">
+      <c r="CD33" s="159"/>
+      <c r="CE33" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="161"/>
+      <c r="CF33" s="159"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="158" t="s">
+      <c r="K34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="158"/>
-      <c r="M34" s="158" t="s">
+      <c r="L34" s="160"/>
+      <c r="M34" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="158"/>
-      <c r="O34" s="158" t="s">
+      <c r="N34" s="160"/>
+      <c r="O34" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="158"/>
-      <c r="Q34" s="158" t="s">
+      <c r="P34" s="160"/>
+      <c r="Q34" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="158"/>
-      <c r="S34" s="158" t="s">
+      <c r="R34" s="160"/>
+      <c r="S34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="158"/>
-      <c r="U34" s="158" t="s">
+      <c r="T34" s="160"/>
+      <c r="U34" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="158"/>
-      <c r="W34" s="158" t="s">
+      <c r="V34" s="160"/>
+      <c r="W34" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="158"/>
-      <c r="Y34" s="158" t="s">
+      <c r="X34" s="160"/>
+      <c r="Y34" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="158"/>
-      <c r="AA34" s="158" t="s">
+      <c r="Z34" s="160"/>
+      <c r="AA34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="158"/>
+      <c r="AB34" s="160"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="158" t="s">
+      <c r="AG34" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="158"/>
-      <c r="AI34" s="158" t="s">
+      <c r="AH34" s="160"/>
+      <c r="AI34" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="158"/>
-      <c r="AK34" s="158" t="s">
+      <c r="AJ34" s="160"/>
+      <c r="AK34" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="158"/>
-      <c r="AM34" s="158" t="s">
+      <c r="AL34" s="160"/>
+      <c r="AM34" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="158"/>
+      <c r="AN34" s="160"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -12284,42 +12377,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="160" t="s">
+      <c r="BO34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="161"/>
-      <c r="BQ34" s="160" t="s">
+      <c r="BP34" s="159"/>
+      <c r="BQ34" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="161"/>
-      <c r="BS34" s="160" t="s">
+      <c r="BR34" s="159"/>
+      <c r="BS34" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="161"/>
-      <c r="BU34" s="160" t="s">
+      <c r="BT34" s="159"/>
+      <c r="BU34" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="161"/>
-      <c r="BW34" s="160" t="s">
+      <c r="BV34" s="159"/>
+      <c r="BW34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="161"/>
-      <c r="BY34" s="160" t="s">
+      <c r="BX34" s="159"/>
+      <c r="BY34" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="161"/>
-      <c r="CA34" s="160" t="s">
+      <c r="BZ34" s="159"/>
+      <c r="CA34" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="161"/>
-      <c r="CC34" s="160" t="s">
+      <c r="CB34" s="159"/>
+      <c r="CC34" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="161"/>
-      <c r="CE34" s="160" t="s">
+      <c r="CD34" s="159"/>
+      <c r="CE34" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="161"/>
+      <c r="CF34" s="159"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -12333,62 +12426,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="159" t="s">
+      <c r="K36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="159"/>
-      <c r="M36" s="159" t="s">
+      <c r="L36" s="165"/>
+      <c r="M36" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="159"/>
-      <c r="O36" s="159" t="s">
+      <c r="N36" s="165"/>
+      <c r="O36" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="159"/>
-      <c r="Q36" s="159" t="s">
+      <c r="P36" s="165"/>
+      <c r="Q36" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="159"/>
-      <c r="S36" s="159" t="s">
+      <c r="R36" s="165"/>
+      <c r="S36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="159"/>
-      <c r="U36" s="159" t="s">
+      <c r="T36" s="165"/>
+      <c r="U36" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="159"/>
-      <c r="W36" s="159" t="s">
+      <c r="V36" s="165"/>
+      <c r="W36" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="159"/>
-      <c r="Y36" s="159" t="s">
+      <c r="X36" s="165"/>
+      <c r="Y36" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="159"/>
-      <c r="AA36" s="159" t="s">
+      <c r="Z36" s="165"/>
+      <c r="AA36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="159"/>
+      <c r="AB36" s="165"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="159" t="s">
+      <c r="AG36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="159"/>
-      <c r="AI36" s="159" t="s">
+      <c r="AH36" s="165"/>
+      <c r="AI36" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="159"/>
-      <c r="AK36" s="159" t="s">
+      <c r="AJ36" s="165"/>
+      <c r="AK36" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="159"/>
-      <c r="AM36" s="159" t="s">
+      <c r="AL36" s="165"/>
+      <c r="AM36" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="159"/>
+      <c r="AN36" s="165"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -12411,42 +12504,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="160" t="s">
+      <c r="BO36" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="161"/>
-      <c r="BQ36" s="160" t="s">
+      <c r="BP36" s="159"/>
+      <c r="BQ36" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="161"/>
-      <c r="BS36" s="160" t="s">
+      <c r="BR36" s="159"/>
+      <c r="BS36" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="161"/>
-      <c r="BU36" s="160" t="s">
+      <c r="BT36" s="159"/>
+      <c r="BU36" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="161"/>
-      <c r="BW36" s="160" t="s">
+      <c r="BV36" s="159"/>
+      <c r="BW36" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="161"/>
-      <c r="BY36" s="160" t="s">
+      <c r="BX36" s="159"/>
+      <c r="BY36" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="161"/>
-      <c r="CA36" s="160" t="s">
+      <c r="BZ36" s="159"/>
+      <c r="CA36" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="161"/>
-      <c r="CC36" s="160" t="s">
+      <c r="CB36" s="159"/>
+      <c r="CC36" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="161"/>
-      <c r="CE36" s="160" t="s">
+      <c r="CD36" s="159"/>
+      <c r="CE36" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="161"/>
+      <c r="CF36" s="159"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -12782,58 +12875,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="158" t="s">
+      <c r="M42" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="158"/>
-      <c r="O42" s="158" t="s">
+      <c r="N42" s="160"/>
+      <c r="O42" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="158"/>
-      <c r="Q42" s="158" t="s">
+      <c r="P42" s="160"/>
+      <c r="Q42" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="158"/>
-      <c r="S42" s="158" t="s">
+      <c r="R42" s="160"/>
+      <c r="S42" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="158"/>
-      <c r="U42" s="158" t="s">
+      <c r="T42" s="160"/>
+      <c r="U42" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="158"/>
-      <c r="W42" s="158" t="s">
+      <c r="V42" s="160"/>
+      <c r="W42" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="158"/>
-      <c r="Y42" s="158" t="s">
+      <c r="X42" s="160"/>
+      <c r="Y42" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="158"/>
-      <c r="AA42" s="158" t="s">
+      <c r="Z42" s="160"/>
+      <c r="AA42" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="158"/>
+      <c r="AB42" s="160"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="158" t="s">
+      <c r="AG42" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="158"/>
-      <c r="AI42" s="158" t="s">
+      <c r="AH42" s="160"/>
+      <c r="AI42" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="158"/>
-      <c r="AK42" s="158" t="s">
+      <c r="AJ42" s="160"/>
+      <c r="AK42" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="158"/>
-      <c r="AM42" s="158" t="s">
+      <c r="AL42" s="160"/>
+      <c r="AM42" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="158"/>
+      <c r="AN42" s="160"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -12856,42 +12949,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="160" t="s">
+      <c r="BO42" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="161"/>
-      <c r="BQ42" s="160" t="s">
+      <c r="BP42" s="159"/>
+      <c r="BQ42" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="161"/>
-      <c r="BS42" s="160" t="s">
+      <c r="BR42" s="159"/>
+      <c r="BS42" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="161"/>
-      <c r="BU42" s="160" t="s">
+      <c r="BT42" s="159"/>
+      <c r="BU42" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="161"/>
-      <c r="BW42" s="160" t="s">
+      <c r="BV42" s="159"/>
+      <c r="BW42" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="161"/>
-      <c r="BY42" s="160" t="s">
+      <c r="BX42" s="159"/>
+      <c r="BY42" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="161"/>
-      <c r="CA42" s="160" t="s">
+      <c r="BZ42" s="159"/>
+      <c r="CA42" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="161"/>
-      <c r="CC42" s="160" t="s">
+      <c r="CB42" s="159"/>
+      <c r="CC42" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="161"/>
-      <c r="CE42" s="160" t="s">
+      <c r="CD42" s="159"/>
+      <c r="CE42" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="161"/>
+      <c r="CF42" s="159"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -12924,71 +13017,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="165" t="s">
+      <c r="K46" s="164" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="165"/>
-      <c r="M46" s="165"/>
-      <c r="N46" s="165"/>
-      <c r="O46" s="165"/>
-      <c r="P46" s="165"/>
-      <c r="Q46" s="165"/>
-      <c r="R46" s="165"/>
-      <c r="S46" s="165"/>
-      <c r="T46" s="165"/>
-      <c r="U46" s="165"/>
-      <c r="V46" s="165"/>
-      <c r="W46" s="165"/>
-      <c r="X46" s="165"/>
-      <c r="Y46" s="165"/>
-      <c r="Z46" s="165"/>
-      <c r="AA46" s="165"/>
-      <c r="AB46" s="165"/>
-      <c r="AC46" s="165"/>
-      <c r="AD46" s="165"/>
-      <c r="AE46" s="165" t="s">
+      <c r="L46" s="164"/>
+      <c r="M46" s="164"/>
+      <c r="N46" s="164"/>
+      <c r="O46" s="164"/>
+      <c r="P46" s="164"/>
+      <c r="Q46" s="164"/>
+      <c r="R46" s="164"/>
+      <c r="S46" s="164"/>
+      <c r="T46" s="164"/>
+      <c r="U46" s="164"/>
+      <c r="V46" s="164"/>
+      <c r="W46" s="164"/>
+      <c r="X46" s="164"/>
+      <c r="Y46" s="164"/>
+      <c r="Z46" s="164"/>
+      <c r="AA46" s="164"/>
+      <c r="AB46" s="164"/>
+      <c r="AC46" s="164"/>
+      <c r="AD46" s="164"/>
+      <c r="AE46" s="164" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="165"/>
-      <c r="AG46" s="165"/>
-      <c r="AH46" s="165"/>
-      <c r="AI46" s="165"/>
-      <c r="AJ46" s="165"/>
-      <c r="AK46" s="165"/>
-      <c r="AL46" s="165"/>
-      <c r="AM46" s="165"/>
-      <c r="AN46" s="165"/>
-      <c r="AO46" s="158" t="s">
+      <c r="AF46" s="164"/>
+      <c r="AG46" s="164"/>
+      <c r="AH46" s="164"/>
+      <c r="AI46" s="164"/>
+      <c r="AJ46" s="164"/>
+      <c r="AK46" s="164"/>
+      <c r="AL46" s="164"/>
+      <c r="AM46" s="164"/>
+      <c r="AN46" s="164"/>
+      <c r="AO46" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="158"/>
-      <c r="AQ46" s="158" t="s">
+      <c r="AP46" s="160"/>
+      <c r="AQ46" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="158"/>
-      <c r="AS46" s="158" t="s">
+      <c r="AR46" s="160"/>
+      <c r="AS46" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="158"/>
-      <c r="AU46" s="158" t="s">
+      <c r="AT46" s="160"/>
+      <c r="AU46" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="158"/>
-      <c r="AW46" s="162" t="s">
+      <c r="AV46" s="160"/>
+      <c r="AW46" s="161" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="163"/>
-      <c r="AY46" s="163"/>
-      <c r="AZ46" s="163"/>
-      <c r="BA46" s="163"/>
-      <c r="BB46" s="163"/>
-      <c r="BC46" s="163"/>
-      <c r="BD46" s="163"/>
-      <c r="BE46" s="164"/>
-      <c r="BF46" s="158" t="s">
+      <c r="AX46" s="162"/>
+      <c r="AY46" s="162"/>
+      <c r="AZ46" s="162"/>
+      <c r="BA46" s="162"/>
+      <c r="BB46" s="162"/>
+      <c r="BC46" s="162"/>
+      <c r="BD46" s="162"/>
+      <c r="BE46" s="163"/>
+      <c r="BF46" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="158"/>
+      <c r="BG46" s="160"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -16576,22 +16669,1706 @@
       <c r="AU125" s="22"/>
       <c r="AV125" s="23"/>
     </row>
+    <row r="130" spans="4:48">
+      <c r="D130" t="s">
+        <v>110</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="AF130">
+        <v>256</v>
+      </c>
+      <c r="AV130">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="131" spans="4:48" ht="14.25" thickBot="1">
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="AJ131">
+        <v>640</v>
+      </c>
+      <c r="AL131">
+        <v>660</v>
+      </c>
+      <c r="AS131" s="110">
+        <v>756</v>
+      </c>
+      <c r="AV131">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="132" spans="4:48">
+      <c r="F132" s="8"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="9"/>
+      <c r="M132" s="9"/>
+      <c r="N132" s="9"/>
+      <c r="O132" s="9"/>
+      <c r="P132" s="9"/>
+      <c r="Q132" s="9"/>
+      <c r="R132" s="9"/>
+      <c r="S132" s="9"/>
+      <c r="T132" s="9"/>
+      <c r="U132" s="9"/>
+      <c r="V132" s="9"/>
+      <c r="W132" s="9"/>
+      <c r="X132" s="9"/>
+      <c r="Y132" s="9"/>
+      <c r="Z132" s="9"/>
+      <c r="AA132" s="9"/>
+      <c r="AB132" s="9"/>
+      <c r="AC132" s="9"/>
+      <c r="AD132" s="9"/>
+      <c r="AE132" s="9"/>
+      <c r="AF132" s="9"/>
+      <c r="AG132" s="9"/>
+      <c r="AH132" s="9"/>
+      <c r="AI132" s="9"/>
+      <c r="AJ132" s="10"/>
+      <c r="AK132" s="17"/>
+      <c r="AL132" s="170" t="s">
+        <v>461</v>
+      </c>
+      <c r="AM132" s="170"/>
+      <c r="AN132" s="170"/>
+      <c r="AO132" s="170"/>
+      <c r="AP132" s="170"/>
+      <c r="AQ132" s="170"/>
+      <c r="AR132" s="170"/>
+      <c r="AS132" s="17"/>
+      <c r="AT132" s="17"/>
+      <c r="AU132" s="17"/>
+      <c r="AV132" s="18"/>
+    </row>
+    <row r="133" spans="4:48">
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133" s="11"/>
+      <c r="G133" s="12"/>
+      <c r="H133" s="12"/>
+      <c r="I133" s="12"/>
+      <c r="J133" s="12"/>
+      <c r="K133" s="12"/>
+      <c r="L133" s="12"/>
+      <c r="M133" s="12"/>
+      <c r="N133" s="12"/>
+      <c r="O133" s="12"/>
+      <c r="P133" s="12"/>
+      <c r="Q133" s="12"/>
+      <c r="R133" s="12"/>
+      <c r="S133" s="12"/>
+      <c r="T133" s="12"/>
+      <c r="U133" s="12"/>
+      <c r="V133" s="12"/>
+      <c r="W133" s="12"/>
+      <c r="X133" s="12"/>
+      <c r="Y133" s="12"/>
+      <c r="Z133" s="12"/>
+      <c r="AA133" s="12"/>
+      <c r="AB133" s="12"/>
+      <c r="AC133" s="12"/>
+      <c r="AD133" s="12"/>
+      <c r="AE133" s="12"/>
+      <c r="AF133" s="12"/>
+      <c r="AG133" s="12"/>
+      <c r="AH133" s="12"/>
+      <c r="AI133" s="12"/>
+      <c r="AJ133" s="13"/>
+      <c r="AK133" s="12"/>
+      <c r="AL133" s="171"/>
+      <c r="AM133" s="171"/>
+      <c r="AN133" s="171"/>
+      <c r="AO133" s="171"/>
+      <c r="AP133" s="171"/>
+      <c r="AQ133" s="171"/>
+      <c r="AR133" s="171"/>
+      <c r="AS133" s="12"/>
+      <c r="AT133" s="12"/>
+      <c r="AU133" s="12"/>
+      <c r="AV133" s="20"/>
+    </row>
+    <row r="134" spans="4:48">
+      <c r="F134" s="11"/>
+      <c r="G134" s="12"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="12"/>
+      <c r="J134" s="12"/>
+      <c r="K134" s="12"/>
+      <c r="L134" s="12"/>
+      <c r="M134" s="12"/>
+      <c r="N134" s="12"/>
+      <c r="O134" s="12"/>
+      <c r="P134" s="12"/>
+      <c r="Q134" s="12"/>
+      <c r="R134" s="12"/>
+      <c r="S134" s="12"/>
+      <c r="T134" s="12"/>
+      <c r="U134" s="12"/>
+      <c r="V134" s="12"/>
+      <c r="W134" s="12"/>
+      <c r="X134" s="12"/>
+      <c r="Y134" s="12"/>
+      <c r="Z134" s="12"/>
+      <c r="AA134" s="12"/>
+      <c r="AB134" s="12"/>
+      <c r="AC134" s="12"/>
+      <c r="AD134" s="12"/>
+      <c r="AE134" s="12"/>
+      <c r="AF134" s="12"/>
+      <c r="AG134" s="12"/>
+      <c r="AH134" s="12"/>
+      <c r="AI134" s="12"/>
+      <c r="AJ134" s="13"/>
+      <c r="AK134" s="12"/>
+      <c r="AL134" s="171"/>
+      <c r="AM134" s="171"/>
+      <c r="AN134" s="171"/>
+      <c r="AO134" s="171"/>
+      <c r="AP134" s="171"/>
+      <c r="AQ134" s="171"/>
+      <c r="AR134" s="171"/>
+      <c r="AS134" s="12"/>
+      <c r="AT134" s="12"/>
+      <c r="AU134" s="12"/>
+      <c r="AV134" s="20"/>
+    </row>
+    <row r="135" spans="4:48">
+      <c r="F135" s="11"/>
+      <c r="G135" s="12"/>
+      <c r="H135" s="12"/>
+      <c r="I135" s="12"/>
+      <c r="J135" s="12"/>
+      <c r="K135" s="12"/>
+      <c r="L135" s="12"/>
+      <c r="M135" s="12"/>
+      <c r="N135" s="12"/>
+      <c r="O135" s="12"/>
+      <c r="P135" s="12"/>
+      <c r="Q135" s="12"/>
+      <c r="R135" s="12"/>
+      <c r="S135" s="12"/>
+      <c r="T135" s="12"/>
+      <c r="U135" s="12"/>
+      <c r="V135" s="12"/>
+      <c r="W135" s="12"/>
+      <c r="X135" s="12"/>
+      <c r="Y135" s="12"/>
+      <c r="Z135" s="12"/>
+      <c r="AA135" s="12"/>
+      <c r="AB135" s="12"/>
+      <c r="AC135" s="12"/>
+      <c r="AD135" s="12"/>
+      <c r="AE135" s="12"/>
+      <c r="AF135" s="12"/>
+      <c r="AG135" s="12"/>
+      <c r="AH135" s="12"/>
+      <c r="AI135" s="12"/>
+      <c r="AJ135" s="13"/>
+      <c r="AK135" s="12"/>
+      <c r="AL135" s="171"/>
+      <c r="AM135" s="171"/>
+      <c r="AN135" s="171"/>
+      <c r="AO135" s="171"/>
+      <c r="AP135" s="171"/>
+      <c r="AQ135" s="171"/>
+      <c r="AR135" s="171"/>
+      <c r="AS135" s="12"/>
+      <c r="AT135" s="12"/>
+      <c r="AU135" s="12"/>
+      <c r="AV135" s="20"/>
+    </row>
+    <row r="136" spans="4:48">
+      <c r="F136" s="11"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="12"/>
+      <c r="I136" s="12"/>
+      <c r="J136" s="12"/>
+      <c r="K136" s="12"/>
+      <c r="L136" s="12"/>
+      <c r="M136" s="12"/>
+      <c r="N136" s="12"/>
+      <c r="O136" s="12"/>
+      <c r="P136" s="12"/>
+      <c r="Q136" s="12"/>
+      <c r="R136" s="12"/>
+      <c r="S136" s="12"/>
+      <c r="T136" s="12"/>
+      <c r="U136" s="12"/>
+      <c r="V136" s="12"/>
+      <c r="W136" s="12"/>
+      <c r="X136" s="12"/>
+      <c r="Y136" s="12"/>
+      <c r="Z136" s="12"/>
+      <c r="AA136" s="12"/>
+      <c r="AB136" s="12"/>
+      <c r="AC136" s="12"/>
+      <c r="AD136" s="12"/>
+      <c r="AE136" s="12"/>
+      <c r="AF136" s="12"/>
+      <c r="AG136" s="12"/>
+      <c r="AH136" s="12"/>
+      <c r="AI136" s="12"/>
+      <c r="AJ136" s="13"/>
+      <c r="AK136" s="12"/>
+      <c r="AL136" s="171"/>
+      <c r="AM136" s="171"/>
+      <c r="AN136" s="171"/>
+      <c r="AO136" s="171"/>
+      <c r="AP136" s="171"/>
+      <c r="AQ136" s="171"/>
+      <c r="AR136" s="171"/>
+      <c r="AS136" s="12"/>
+      <c r="AT136" s="12"/>
+      <c r="AU136" s="12"/>
+      <c r="AV136" s="20"/>
+    </row>
+    <row r="137" spans="4:48">
+      <c r="F137" s="11"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="12"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="12"/>
+      <c r="L137" s="12"/>
+      <c r="M137" s="12"/>
+      <c r="N137" s="12"/>
+      <c r="O137" s="12"/>
+      <c r="P137" s="12"/>
+      <c r="Q137" s="12"/>
+      <c r="R137" s="12"/>
+      <c r="S137" s="12"/>
+      <c r="T137" s="12"/>
+      <c r="U137" s="12"/>
+      <c r="V137" s="12"/>
+      <c r="W137" s="12"/>
+      <c r="X137" s="12"/>
+      <c r="Y137" s="12"/>
+      <c r="Z137" s="12"/>
+      <c r="AA137" s="12"/>
+      <c r="AB137" s="12"/>
+      <c r="AC137" s="12"/>
+      <c r="AD137" s="12"/>
+      <c r="AE137" s="12"/>
+      <c r="AF137" s="12"/>
+      <c r="AG137" s="12"/>
+      <c r="AH137" s="12"/>
+      <c r="AI137" s="12"/>
+      <c r="AJ137" s="13"/>
+      <c r="AK137" s="12"/>
+      <c r="AL137" s="171"/>
+      <c r="AM137" s="171"/>
+      <c r="AN137" s="171"/>
+      <c r="AO137" s="171"/>
+      <c r="AP137" s="171"/>
+      <c r="AQ137" s="171"/>
+      <c r="AR137" s="171"/>
+      <c r="AS137" s="12"/>
+      <c r="AT137" s="12"/>
+      <c r="AU137" s="12"/>
+      <c r="AV137" s="20"/>
+    </row>
+    <row r="138" spans="4:48">
+      <c r="F138" s="11"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="12"/>
+      <c r="J138" s="12"/>
+      <c r="K138" s="12"/>
+      <c r="L138" s="12"/>
+      <c r="M138" s="12"/>
+      <c r="N138" s="12"/>
+      <c r="O138" s="12"/>
+      <c r="P138" s="12"/>
+      <c r="Q138" s="12"/>
+      <c r="R138" s="12"/>
+      <c r="S138" s="12"/>
+      <c r="T138" s="12"/>
+      <c r="U138" s="12"/>
+      <c r="V138" s="12"/>
+      <c r="W138" s="12"/>
+      <c r="X138" s="12"/>
+      <c r="Y138" s="12"/>
+      <c r="Z138" s="12"/>
+      <c r="AA138" s="12"/>
+      <c r="AB138" s="12"/>
+      <c r="AC138" s="12"/>
+      <c r="AD138" s="12"/>
+      <c r="AE138" s="12"/>
+      <c r="AF138" s="12"/>
+      <c r="AG138" s="12"/>
+      <c r="AH138" s="12"/>
+      <c r="AI138" s="12"/>
+      <c r="AJ138" s="13"/>
+      <c r="AK138" s="12"/>
+      <c r="AL138" s="171"/>
+      <c r="AM138" s="171"/>
+      <c r="AN138" s="171"/>
+      <c r="AO138" s="171"/>
+      <c r="AP138" s="171"/>
+      <c r="AQ138" s="171"/>
+      <c r="AR138" s="171"/>
+      <c r="AS138" s="12"/>
+      <c r="AT138" s="12"/>
+      <c r="AU138" s="12"/>
+      <c r="AV138" s="20"/>
+    </row>
+    <row r="139" spans="4:48">
+      <c r="F139" s="11"/>
+      <c r="G139" s="12"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="12"/>
+      <c r="J139" s="12"/>
+      <c r="K139" s="12"/>
+      <c r="L139" s="12"/>
+      <c r="M139" s="12"/>
+      <c r="N139" s="12"/>
+      <c r="O139" s="12"/>
+      <c r="P139" s="12"/>
+      <c r="Q139" s="12"/>
+      <c r="R139" s="12"/>
+      <c r="S139" s="12"/>
+      <c r="T139" s="12"/>
+      <c r="U139" s="12"/>
+      <c r="V139" s="12"/>
+      <c r="W139" s="12"/>
+      <c r="X139" s="12"/>
+      <c r="Y139" s="12"/>
+      <c r="Z139" s="12"/>
+      <c r="AA139" s="12"/>
+      <c r="AB139" s="12"/>
+      <c r="AC139" s="12"/>
+      <c r="AD139" s="12"/>
+      <c r="AE139" s="12"/>
+      <c r="AF139" s="12"/>
+      <c r="AG139" s="12"/>
+      <c r="AH139" s="12"/>
+      <c r="AI139" s="12"/>
+      <c r="AJ139" s="13"/>
+      <c r="AK139" s="12"/>
+      <c r="AL139" s="171"/>
+      <c r="AM139" s="171"/>
+      <c r="AN139" s="171"/>
+      <c r="AO139" s="171"/>
+      <c r="AP139" s="171"/>
+      <c r="AQ139" s="171"/>
+      <c r="AR139" s="171"/>
+      <c r="AS139" s="12"/>
+      <c r="AT139" s="12"/>
+      <c r="AU139" s="12"/>
+      <c r="AV139" s="20"/>
+    </row>
+    <row r="140" spans="4:48">
+      <c r="F140" s="11"/>
+      <c r="G140" s="12"/>
+      <c r="H140" s="12"/>
+      <c r="I140" s="12"/>
+      <c r="J140" s="12"/>
+      <c r="K140" s="12"/>
+      <c r="L140" s="12"/>
+      <c r="M140" s="12"/>
+      <c r="N140" s="12"/>
+      <c r="O140" s="12"/>
+      <c r="P140" s="12"/>
+      <c r="Q140" s="12"/>
+      <c r="R140" s="12"/>
+      <c r="S140" s="12"/>
+      <c r="T140" s="12"/>
+      <c r="U140" s="12"/>
+      <c r="V140" s="12"/>
+      <c r="W140" s="12"/>
+      <c r="X140" s="12"/>
+      <c r="Y140" s="12"/>
+      <c r="Z140" s="12"/>
+      <c r="AA140" s="12"/>
+      <c r="AB140" s="12"/>
+      <c r="AC140" s="12"/>
+      <c r="AD140" s="12"/>
+      <c r="AE140" s="12"/>
+      <c r="AF140" s="12"/>
+      <c r="AG140" s="12"/>
+      <c r="AH140" s="12"/>
+      <c r="AI140" s="12"/>
+      <c r="AJ140" s="13"/>
+      <c r="AK140" s="12"/>
+      <c r="AL140" s="171"/>
+      <c r="AM140" s="171"/>
+      <c r="AN140" s="171"/>
+      <c r="AO140" s="171"/>
+      <c r="AP140" s="171"/>
+      <c r="AQ140" s="171"/>
+      <c r="AR140" s="171"/>
+      <c r="AS140" s="12"/>
+      <c r="AT140" s="12"/>
+      <c r="AU140" s="12"/>
+      <c r="AV140" s="20"/>
+    </row>
+    <row r="141" spans="4:48">
+      <c r="F141" s="11"/>
+      <c r="G141" s="12"/>
+      <c r="H141" s="12"/>
+      <c r="I141" s="12"/>
+      <c r="J141" s="12"/>
+      <c r="K141" s="12"/>
+      <c r="L141" s="12"/>
+      <c r="M141" s="12"/>
+      <c r="N141" s="12"/>
+      <c r="O141" s="12"/>
+      <c r="P141" s="12"/>
+      <c r="Q141" s="12"/>
+      <c r="R141" s="12"/>
+      <c r="S141" s="12"/>
+      <c r="T141" s="12"/>
+      <c r="U141" s="12"/>
+      <c r="V141" s="12"/>
+      <c r="W141" s="12"/>
+      <c r="X141" s="12"/>
+      <c r="Y141" s="12"/>
+      <c r="Z141" s="12"/>
+      <c r="AA141" s="12"/>
+      <c r="AB141" s="12"/>
+      <c r="AC141" s="12"/>
+      <c r="AD141" s="12"/>
+      <c r="AE141" s="12"/>
+      <c r="AF141" s="12"/>
+      <c r="AG141" s="12"/>
+      <c r="AH141" s="12"/>
+      <c r="AI141" s="12"/>
+      <c r="AJ141" s="13"/>
+      <c r="AK141" s="12"/>
+      <c r="AL141" s="171"/>
+      <c r="AM141" s="171"/>
+      <c r="AN141" s="171"/>
+      <c r="AO141" s="171"/>
+      <c r="AP141" s="171"/>
+      <c r="AQ141" s="171"/>
+      <c r="AR141" s="171"/>
+      <c r="AS141" s="12"/>
+      <c r="AT141" s="12"/>
+      <c r="AU141" s="12"/>
+      <c r="AV141" s="20"/>
+    </row>
+    <row r="142" spans="4:48">
+      <c r="F142" s="11"/>
+      <c r="G142" s="12"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="12"/>
+      <c r="J142" s="12"/>
+      <c r="K142" s="12"/>
+      <c r="L142" s="12"/>
+      <c r="M142" s="12"/>
+      <c r="N142" s="12"/>
+      <c r="O142" s="12"/>
+      <c r="P142" s="12"/>
+      <c r="Q142" s="12"/>
+      <c r="R142" s="12"/>
+      <c r="S142" s="12"/>
+      <c r="T142" s="12"/>
+      <c r="U142" s="12"/>
+      <c r="V142" s="12"/>
+      <c r="W142" s="12"/>
+      <c r="X142" s="12"/>
+      <c r="Y142" s="12"/>
+      <c r="Z142" s="12"/>
+      <c r="AA142" s="12"/>
+      <c r="AB142" s="12"/>
+      <c r="AC142" s="12"/>
+      <c r="AD142" s="12"/>
+      <c r="AE142" s="12"/>
+      <c r="AF142" s="12"/>
+      <c r="AG142" s="12"/>
+      <c r="AH142" s="12"/>
+      <c r="AI142" s="12"/>
+      <c r="AJ142" s="13"/>
+      <c r="AK142" s="12"/>
+      <c r="AL142" s="171"/>
+      <c r="AM142" s="171"/>
+      <c r="AN142" s="171"/>
+      <c r="AO142" s="171"/>
+      <c r="AP142" s="171"/>
+      <c r="AQ142" s="171"/>
+      <c r="AR142" s="171"/>
+      <c r="AS142" s="12"/>
+      <c r="AT142" s="12"/>
+      <c r="AU142" s="12"/>
+      <c r="AV142" s="20"/>
+    </row>
+    <row r="143" spans="4:48">
+      <c r="F143" s="11"/>
+      <c r="G143" s="12"/>
+      <c r="H143" s="12"/>
+      <c r="I143" s="12"/>
+      <c r="J143" s="12"/>
+      <c r="K143" s="12"/>
+      <c r="L143" s="12"/>
+      <c r="M143" s="12"/>
+      <c r="N143" s="12"/>
+      <c r="O143" s="12"/>
+      <c r="P143" s="12"/>
+      <c r="Q143" s="12"/>
+      <c r="R143" s="12"/>
+      <c r="S143" s="12"/>
+      <c r="T143" s="12"/>
+      <c r="U143" s="12"/>
+      <c r="V143" s="12"/>
+      <c r="W143" s="12"/>
+      <c r="X143" s="12"/>
+      <c r="Y143" s="12"/>
+      <c r="Z143" s="12"/>
+      <c r="AA143" s="12"/>
+      <c r="AB143" s="12"/>
+      <c r="AC143" s="12"/>
+      <c r="AD143" s="12"/>
+      <c r="AE143" s="12"/>
+      <c r="AF143" s="12"/>
+      <c r="AG143" s="12"/>
+      <c r="AH143" s="12"/>
+      <c r="AI143" s="12"/>
+      <c r="AJ143" s="13"/>
+      <c r="AK143" s="12"/>
+      <c r="AL143" s="171"/>
+      <c r="AM143" s="171"/>
+      <c r="AN143" s="171"/>
+      <c r="AO143" s="171"/>
+      <c r="AP143" s="171"/>
+      <c r="AQ143" s="171"/>
+      <c r="AR143" s="171"/>
+      <c r="AS143" s="12"/>
+      <c r="AT143" s="12"/>
+      <c r="AU143" s="12"/>
+      <c r="AV143" s="20"/>
+    </row>
+    <row r="144" spans="4:48">
+      <c r="F144" s="11"/>
+      <c r="G144" s="12"/>
+      <c r="H144" s="12"/>
+      <c r="I144" s="12"/>
+      <c r="J144" s="12"/>
+      <c r="K144" s="12"/>
+      <c r="L144" s="12"/>
+      <c r="M144" s="12"/>
+      <c r="N144" s="12"/>
+      <c r="O144" s="12"/>
+      <c r="P144" s="12"/>
+      <c r="Q144" s="12"/>
+      <c r="R144" s="12"/>
+      <c r="S144" s="12"/>
+      <c r="T144" s="12"/>
+      <c r="U144" s="12"/>
+      <c r="V144" s="12"/>
+      <c r="W144" s="12"/>
+      <c r="X144" s="12"/>
+      <c r="Y144" s="12"/>
+      <c r="Z144" s="12"/>
+      <c r="AA144" s="12"/>
+      <c r="AB144" s="12"/>
+      <c r="AC144" s="12"/>
+      <c r="AD144" s="12"/>
+      <c r="AE144" s="12"/>
+      <c r="AF144" s="12"/>
+      <c r="AG144" s="12"/>
+      <c r="AH144" s="12"/>
+      <c r="AI144" s="12"/>
+      <c r="AJ144" s="13"/>
+      <c r="AK144" s="12"/>
+      <c r="AL144" s="171"/>
+      <c r="AM144" s="171"/>
+      <c r="AN144" s="171"/>
+      <c r="AO144" s="171"/>
+      <c r="AP144" s="171"/>
+      <c r="AQ144" s="171"/>
+      <c r="AR144" s="171"/>
+      <c r="AS144" s="12"/>
+      <c r="AT144" s="12"/>
+      <c r="AU144" s="12"/>
+      <c r="AV144" s="20"/>
+    </row>
+    <row r="145" spans="4:48">
+      <c r="F145" s="11"/>
+      <c r="G145" s="12"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="12"/>
+      <c r="J145" s="12"/>
+      <c r="K145" s="12"/>
+      <c r="L145" s="12"/>
+      <c r="M145" s="12"/>
+      <c r="N145" s="12"/>
+      <c r="O145" s="12"/>
+      <c r="P145" s="12"/>
+      <c r="Q145" s="12"/>
+      <c r="R145" s="12"/>
+      <c r="S145" s="12"/>
+      <c r="T145" s="12"/>
+      <c r="U145" s="12"/>
+      <c r="V145" s="12"/>
+      <c r="W145" s="12"/>
+      <c r="X145" s="12"/>
+      <c r="Y145" s="12"/>
+      <c r="Z145" s="12"/>
+      <c r="AA145" s="12"/>
+      <c r="AB145" s="12"/>
+      <c r="AC145" s="12"/>
+      <c r="AD145" s="12"/>
+      <c r="AE145" s="12"/>
+      <c r="AF145" s="12"/>
+      <c r="AG145" s="12"/>
+      <c r="AH145" s="12"/>
+      <c r="AI145" s="12"/>
+      <c r="AJ145" s="13"/>
+      <c r="AK145" s="12"/>
+      <c r="AL145" s="171"/>
+      <c r="AM145" s="171"/>
+      <c r="AN145" s="171"/>
+      <c r="AO145" s="171"/>
+      <c r="AP145" s="171"/>
+      <c r="AQ145" s="171"/>
+      <c r="AR145" s="171"/>
+      <c r="AS145" s="12"/>
+      <c r="AT145" s="12"/>
+      <c r="AU145" s="12"/>
+      <c r="AV145" s="20"/>
+    </row>
+    <row r="146" spans="4:48">
+      <c r="F146" s="11"/>
+      <c r="G146" s="12"/>
+      <c r="H146" s="12"/>
+      <c r="I146" s="12"/>
+      <c r="J146" s="12"/>
+      <c r="K146" s="12"/>
+      <c r="L146" s="12"/>
+      <c r="M146" s="12"/>
+      <c r="N146" s="12"/>
+      <c r="O146" s="12"/>
+      <c r="P146" s="12"/>
+      <c r="Q146" s="12"/>
+      <c r="R146" s="12"/>
+      <c r="S146" s="12"/>
+      <c r="T146" s="12"/>
+      <c r="U146" s="12"/>
+      <c r="V146" s="12"/>
+      <c r="W146" s="12"/>
+      <c r="X146" s="12"/>
+      <c r="Y146" s="12"/>
+      <c r="Z146" s="12"/>
+      <c r="AA146" s="12"/>
+      <c r="AB146" s="12"/>
+      <c r="AC146" s="12"/>
+      <c r="AD146" s="12"/>
+      <c r="AE146" s="12"/>
+      <c r="AF146" s="12"/>
+      <c r="AG146" s="12"/>
+      <c r="AH146" s="12"/>
+      <c r="AI146" s="12"/>
+      <c r="AJ146" s="13"/>
+      <c r="AK146" s="12"/>
+      <c r="AL146" s="171"/>
+      <c r="AM146" s="171"/>
+      <c r="AN146" s="171"/>
+      <c r="AO146" s="171"/>
+      <c r="AP146" s="171"/>
+      <c r="AQ146" s="171"/>
+      <c r="AR146" s="171"/>
+      <c r="AS146" s="12"/>
+      <c r="AT146" s="12"/>
+      <c r="AU146" s="12"/>
+      <c r="AV146" s="20"/>
+    </row>
+    <row r="147" spans="4:48">
+      <c r="F147" s="11"/>
+      <c r="G147" s="12"/>
+      <c r="H147" s="12"/>
+      <c r="I147" s="12"/>
+      <c r="J147" s="12"/>
+      <c r="K147" s="12"/>
+      <c r="L147" s="12"/>
+      <c r="M147" s="12"/>
+      <c r="N147" s="12"/>
+      <c r="O147" s="12"/>
+      <c r="P147" s="12"/>
+      <c r="Q147" s="12"/>
+      <c r="R147" s="12"/>
+      <c r="S147" s="12"/>
+      <c r="T147" s="12"/>
+      <c r="U147" s="12"/>
+      <c r="V147" s="12"/>
+      <c r="W147" s="12"/>
+      <c r="X147" s="12"/>
+      <c r="Y147" s="12"/>
+      <c r="Z147" s="12"/>
+      <c r="AA147" s="12"/>
+      <c r="AB147" s="12"/>
+      <c r="AC147" s="12"/>
+      <c r="AD147" s="12"/>
+      <c r="AE147" s="12"/>
+      <c r="AF147" s="12"/>
+      <c r="AG147" s="12"/>
+      <c r="AH147" s="12"/>
+      <c r="AI147" s="12"/>
+      <c r="AJ147" s="13"/>
+      <c r="AK147" s="12"/>
+      <c r="AL147" s="171"/>
+      <c r="AM147" s="171"/>
+      <c r="AN147" s="171"/>
+      <c r="AO147" s="171"/>
+      <c r="AP147" s="171"/>
+      <c r="AQ147" s="171"/>
+      <c r="AR147" s="171"/>
+      <c r="AS147" s="12"/>
+      <c r="AT147" s="12"/>
+      <c r="AU147" s="12"/>
+      <c r="AV147" s="20"/>
+    </row>
+    <row r="148" spans="4:48">
+      <c r="F148" s="11"/>
+      <c r="G148" s="12"/>
+      <c r="H148" s="12"/>
+      <c r="I148" s="12"/>
+      <c r="J148" s="12"/>
+      <c r="K148" s="12"/>
+      <c r="L148" s="12"/>
+      <c r="M148" s="12"/>
+      <c r="N148" s="12"/>
+      <c r="O148" s="12"/>
+      <c r="P148" s="12"/>
+      <c r="Q148" s="12"/>
+      <c r="R148" s="12"/>
+      <c r="S148" s="12"/>
+      <c r="T148" s="12"/>
+      <c r="U148" s="12"/>
+      <c r="V148" s="12"/>
+      <c r="W148" s="12"/>
+      <c r="X148" s="12"/>
+      <c r="Y148" s="12"/>
+      <c r="Z148" s="12"/>
+      <c r="AA148" s="12"/>
+      <c r="AB148" s="12"/>
+      <c r="AC148" s="12"/>
+      <c r="AD148" s="12"/>
+      <c r="AE148" s="12"/>
+      <c r="AF148" s="12"/>
+      <c r="AG148" s="12"/>
+      <c r="AH148" s="12"/>
+      <c r="AI148" s="12"/>
+      <c r="AJ148" s="13"/>
+      <c r="AK148" s="12"/>
+      <c r="AL148" s="171"/>
+      <c r="AM148" s="171"/>
+      <c r="AN148" s="171"/>
+      <c r="AO148" s="171"/>
+      <c r="AP148" s="171"/>
+      <c r="AQ148" s="171"/>
+      <c r="AR148" s="171"/>
+      <c r="AS148" s="12"/>
+      <c r="AT148" s="12"/>
+      <c r="AU148" s="12"/>
+      <c r="AV148" s="20"/>
+    </row>
+    <row r="149" spans="4:48">
+      <c r="F149" s="11"/>
+      <c r="G149" s="12"/>
+      <c r="H149" s="12"/>
+      <c r="I149" s="12"/>
+      <c r="J149" s="12"/>
+      <c r="K149" s="12"/>
+      <c r="L149" s="12"/>
+      <c r="M149" s="12"/>
+      <c r="N149" s="12"/>
+      <c r="O149" s="12"/>
+      <c r="P149" s="12"/>
+      <c r="Q149" s="12"/>
+      <c r="R149" s="12"/>
+      <c r="S149" s="12"/>
+      <c r="T149" s="12"/>
+      <c r="U149" s="12"/>
+      <c r="V149" s="12"/>
+      <c r="W149" s="12"/>
+      <c r="X149" s="12"/>
+      <c r="Y149" s="12"/>
+      <c r="Z149" s="12"/>
+      <c r="AA149" s="12"/>
+      <c r="AB149" s="12"/>
+      <c r="AC149" s="12"/>
+      <c r="AD149" s="12"/>
+      <c r="AE149" s="12"/>
+      <c r="AF149" s="12"/>
+      <c r="AG149" s="12"/>
+      <c r="AH149" s="12"/>
+      <c r="AI149" s="12"/>
+      <c r="AJ149" s="13"/>
+      <c r="AK149" s="12"/>
+      <c r="AL149" s="171"/>
+      <c r="AM149" s="171"/>
+      <c r="AN149" s="171"/>
+      <c r="AO149" s="171"/>
+      <c r="AP149" s="171"/>
+      <c r="AQ149" s="171"/>
+      <c r="AR149" s="171"/>
+      <c r="AS149" s="12"/>
+      <c r="AT149" s="12"/>
+      <c r="AU149" s="12"/>
+      <c r="AV149" s="20"/>
+    </row>
+    <row r="150" spans="4:48">
+      <c r="F150" s="11"/>
+      <c r="G150" s="12"/>
+      <c r="H150" s="12"/>
+      <c r="I150" s="12"/>
+      <c r="J150" s="12"/>
+      <c r="K150" s="12"/>
+      <c r="L150" s="12"/>
+      <c r="M150" s="12"/>
+      <c r="N150" s="12"/>
+      <c r="O150" s="12"/>
+      <c r="P150" s="12"/>
+      <c r="Q150" s="12"/>
+      <c r="R150" s="12"/>
+      <c r="S150" s="12"/>
+      <c r="T150" s="12"/>
+      <c r="U150" s="12"/>
+      <c r="V150" s="12"/>
+      <c r="W150" s="12"/>
+      <c r="X150" s="12"/>
+      <c r="Y150" s="12"/>
+      <c r="Z150" s="12"/>
+      <c r="AA150" s="12"/>
+      <c r="AB150" s="12"/>
+      <c r="AC150" s="12"/>
+      <c r="AD150" s="12"/>
+      <c r="AE150" s="12"/>
+      <c r="AF150" s="12"/>
+      <c r="AG150" s="12"/>
+      <c r="AH150" s="12"/>
+      <c r="AI150" s="12"/>
+      <c r="AJ150" s="13"/>
+      <c r="AK150" s="12"/>
+      <c r="AL150" s="171"/>
+      <c r="AM150" s="171"/>
+      <c r="AN150" s="171"/>
+      <c r="AO150" s="171"/>
+      <c r="AP150" s="171"/>
+      <c r="AQ150" s="171"/>
+      <c r="AR150" s="171"/>
+      <c r="AS150" s="12"/>
+      <c r="AT150" s="12"/>
+      <c r="AU150" s="12"/>
+      <c r="AV150" s="20"/>
+    </row>
+    <row r="151" spans="4:48">
+      <c r="F151" s="11"/>
+      <c r="G151" s="12"/>
+      <c r="H151" s="12"/>
+      <c r="I151" s="12"/>
+      <c r="J151" s="12"/>
+      <c r="K151" s="12"/>
+      <c r="L151" s="12"/>
+      <c r="M151" s="12"/>
+      <c r="N151" s="12"/>
+      <c r="O151" s="12"/>
+      <c r="P151" s="12"/>
+      <c r="Q151" s="12"/>
+      <c r="R151" s="12"/>
+      <c r="S151" s="12"/>
+      <c r="T151" s="12"/>
+      <c r="U151" s="12"/>
+      <c r="V151" s="12"/>
+      <c r="W151" s="12"/>
+      <c r="X151" s="12"/>
+      <c r="Y151" s="12"/>
+      <c r="Z151" s="12"/>
+      <c r="AA151" s="12"/>
+      <c r="AB151" s="12"/>
+      <c r="AC151" s="12"/>
+      <c r="AD151" s="12"/>
+      <c r="AE151" s="12"/>
+      <c r="AF151" s="12"/>
+      <c r="AG151" s="12"/>
+      <c r="AH151" s="12"/>
+      <c r="AI151" s="12"/>
+      <c r="AJ151" s="13"/>
+      <c r="AK151" s="12"/>
+      <c r="AL151" s="171"/>
+      <c r="AM151" s="171"/>
+      <c r="AN151" s="171"/>
+      <c r="AO151" s="171"/>
+      <c r="AP151" s="171"/>
+      <c r="AQ151" s="171"/>
+      <c r="AR151" s="171"/>
+      <c r="AS151" s="12"/>
+      <c r="AT151" s="12"/>
+      <c r="AU151" s="12"/>
+      <c r="AV151" s="20"/>
+    </row>
+    <row r="152" spans="4:48">
+      <c r="F152" s="11"/>
+      <c r="G152" s="12"/>
+      <c r="H152" s="12"/>
+      <c r="I152" s="12"/>
+      <c r="J152" s="12"/>
+      <c r="K152" s="12"/>
+      <c r="L152" s="12"/>
+      <c r="M152" s="12"/>
+      <c r="N152" s="12"/>
+      <c r="O152" s="12"/>
+      <c r="P152" s="12"/>
+      <c r="Q152" s="12"/>
+      <c r="R152" s="12"/>
+      <c r="S152" s="12"/>
+      <c r="T152" s="12"/>
+      <c r="U152" s="12"/>
+      <c r="V152" s="12"/>
+      <c r="W152" s="12"/>
+      <c r="X152" s="12"/>
+      <c r="Y152" s="12"/>
+      <c r="Z152" s="12"/>
+      <c r="AA152" s="12"/>
+      <c r="AB152" s="12"/>
+      <c r="AC152" s="12"/>
+      <c r="AD152" s="12"/>
+      <c r="AE152" s="12"/>
+      <c r="AF152" s="12"/>
+      <c r="AG152" s="12"/>
+      <c r="AH152" s="12"/>
+      <c r="AI152" s="12"/>
+      <c r="AJ152" s="13"/>
+      <c r="AK152" s="12"/>
+      <c r="AL152" s="171"/>
+      <c r="AM152" s="171"/>
+      <c r="AN152" s="171"/>
+      <c r="AO152" s="171"/>
+      <c r="AP152" s="171"/>
+      <c r="AQ152" s="171"/>
+      <c r="AR152" s="171"/>
+      <c r="AS152" s="12"/>
+      <c r="AT152" s="12"/>
+      <c r="AU152" s="12"/>
+      <c r="AV152" s="20"/>
+    </row>
+    <row r="153" spans="4:48">
+      <c r="F153" s="11"/>
+      <c r="G153" s="12"/>
+      <c r="H153" s="12"/>
+      <c r="I153" s="12"/>
+      <c r="J153" s="12"/>
+      <c r="K153" s="12"/>
+      <c r="L153" s="12"/>
+      <c r="M153" s="12"/>
+      <c r="N153" s="12"/>
+      <c r="O153" s="12"/>
+      <c r="P153" s="12"/>
+      <c r="Q153" s="12"/>
+      <c r="R153" s="12"/>
+      <c r="S153" s="12"/>
+      <c r="T153" s="12"/>
+      <c r="U153" s="12"/>
+      <c r="V153" s="12"/>
+      <c r="W153" s="12"/>
+      <c r="X153" s="12"/>
+      <c r="Y153" s="12"/>
+      <c r="Z153" s="12"/>
+      <c r="AA153" s="12"/>
+      <c r="AB153" s="12"/>
+      <c r="AC153" s="12"/>
+      <c r="AD153" s="12"/>
+      <c r="AE153" s="12"/>
+      <c r="AF153" s="12"/>
+      <c r="AG153" s="12"/>
+      <c r="AH153" s="12"/>
+      <c r="AI153" s="12"/>
+      <c r="AJ153" s="13"/>
+      <c r="AK153" s="12"/>
+      <c r="AL153" s="171"/>
+      <c r="AM153" s="171"/>
+      <c r="AN153" s="171"/>
+      <c r="AO153" s="171"/>
+      <c r="AP153" s="171"/>
+      <c r="AQ153" s="171"/>
+      <c r="AR153" s="171"/>
+      <c r="AS153" s="12"/>
+      <c r="AT153" s="12"/>
+      <c r="AU153" s="12"/>
+      <c r="AV153" s="20"/>
+    </row>
+    <row r="154" spans="4:48">
+      <c r="F154" s="11"/>
+      <c r="G154" s="12"/>
+      <c r="H154" s="12"/>
+      <c r="I154" s="12"/>
+      <c r="J154" s="12"/>
+      <c r="K154" s="12"/>
+      <c r="L154" s="12"/>
+      <c r="M154" s="12"/>
+      <c r="N154" s="12"/>
+      <c r="O154" s="12"/>
+      <c r="P154" s="12"/>
+      <c r="Q154" s="12"/>
+      <c r="R154" s="12"/>
+      <c r="S154" s="12"/>
+      <c r="T154" s="12"/>
+      <c r="U154" s="12"/>
+      <c r="V154" s="12"/>
+      <c r="W154" s="12"/>
+      <c r="X154" s="12"/>
+      <c r="Y154" s="12"/>
+      <c r="Z154" s="12"/>
+      <c r="AA154" s="12"/>
+      <c r="AB154" s="12"/>
+      <c r="AC154" s="12"/>
+      <c r="AD154" s="12"/>
+      <c r="AE154" s="12"/>
+      <c r="AF154" s="12"/>
+      <c r="AG154" s="12"/>
+      <c r="AH154" s="12"/>
+      <c r="AI154" s="12"/>
+      <c r="AJ154" s="13"/>
+      <c r="AK154" s="12"/>
+      <c r="AL154" s="171"/>
+      <c r="AM154" s="171"/>
+      <c r="AN154" s="171"/>
+      <c r="AO154" s="171"/>
+      <c r="AP154" s="171"/>
+      <c r="AQ154" s="171"/>
+      <c r="AR154" s="171"/>
+      <c r="AS154" s="12"/>
+      <c r="AT154" s="12"/>
+      <c r="AU154" s="12"/>
+      <c r="AV154" s="20"/>
+    </row>
+    <row r="155" spans="4:48">
+      <c r="F155" s="11"/>
+      <c r="G155" s="12"/>
+      <c r="H155" s="12"/>
+      <c r="I155" s="12"/>
+      <c r="J155" s="12"/>
+      <c r="K155" s="12"/>
+      <c r="L155" s="12"/>
+      <c r="M155" s="12"/>
+      <c r="N155" s="12"/>
+      <c r="O155" s="12"/>
+      <c r="P155" s="12"/>
+      <c r="Q155" s="12"/>
+      <c r="R155" s="12"/>
+      <c r="S155" s="12"/>
+      <c r="T155" s="12"/>
+      <c r="U155" s="12"/>
+      <c r="V155" s="12"/>
+      <c r="W155" s="12"/>
+      <c r="X155" s="12"/>
+      <c r="Y155" s="12"/>
+      <c r="Z155" s="12"/>
+      <c r="AA155" s="12"/>
+      <c r="AB155" s="12"/>
+      <c r="AC155" s="12"/>
+      <c r="AD155" s="12"/>
+      <c r="AE155" s="12"/>
+      <c r="AF155" s="12"/>
+      <c r="AG155" s="12"/>
+      <c r="AH155" s="12"/>
+      <c r="AI155" s="12"/>
+      <c r="AJ155" s="13"/>
+      <c r="AK155" s="12"/>
+      <c r="AL155" s="171"/>
+      <c r="AM155" s="171"/>
+      <c r="AN155" s="171"/>
+      <c r="AO155" s="171"/>
+      <c r="AP155" s="171"/>
+      <c r="AQ155" s="171"/>
+      <c r="AR155" s="171"/>
+      <c r="AS155" s="12"/>
+      <c r="AT155" s="12"/>
+      <c r="AU155" s="12"/>
+      <c r="AV155" s="20"/>
+    </row>
+    <row r="156" spans="4:48" ht="14.25" thickBot="1">
+      <c r="D156">
+        <v>240</v>
+      </c>
+      <c r="E156">
+        <v>480</v>
+      </c>
+      <c r="F156" s="14"/>
+      <c r="G156" s="15"/>
+      <c r="H156" s="15"/>
+      <c r="I156" s="15"/>
+      <c r="J156" s="15"/>
+      <c r="K156" s="15"/>
+      <c r="L156" s="15"/>
+      <c r="M156" s="15"/>
+      <c r="N156" s="15"/>
+      <c r="O156" s="15"/>
+      <c r="P156" s="15"/>
+      <c r="Q156" s="15"/>
+      <c r="R156" s="15"/>
+      <c r="S156" s="15"/>
+      <c r="T156" s="15"/>
+      <c r="U156" s="15"/>
+      <c r="V156" s="15"/>
+      <c r="W156" s="15"/>
+      <c r="X156" s="15"/>
+      <c r="Y156" s="15"/>
+      <c r="Z156" s="15"/>
+      <c r="AA156" s="15"/>
+      <c r="AB156" s="15"/>
+      <c r="AC156" s="15"/>
+      <c r="AD156" s="15"/>
+      <c r="AE156" s="15"/>
+      <c r="AF156" s="15"/>
+      <c r="AG156" s="15"/>
+      <c r="AH156" s="15"/>
+      <c r="AI156" s="15"/>
+      <c r="AJ156" s="16"/>
+      <c r="AK156" s="12"/>
+      <c r="AL156" s="171"/>
+      <c r="AM156" s="171"/>
+      <c r="AN156" s="171"/>
+      <c r="AO156" s="171"/>
+      <c r="AP156" s="171"/>
+      <c r="AQ156" s="171"/>
+      <c r="AR156" s="171"/>
+      <c r="AS156" s="12"/>
+      <c r="AT156" s="12"/>
+      <c r="AU156" s="12"/>
+      <c r="AV156" s="20"/>
+    </row>
+    <row r="157" spans="4:48">
+      <c r="F157" s="175" t="s">
+        <v>463</v>
+      </c>
+      <c r="G157" s="25"/>
+      <c r="H157" s="25"/>
+      <c r="I157" s="25"/>
+      <c r="J157" s="25"/>
+      <c r="K157" s="25"/>
+      <c r="L157" s="25"/>
+      <c r="M157" s="25"/>
+      <c r="N157" s="25"/>
+      <c r="O157" s="25"/>
+      <c r="P157" s="25"/>
+      <c r="Q157" s="25"/>
+      <c r="R157" s="25"/>
+      <c r="S157" s="25"/>
+      <c r="T157" s="25"/>
+      <c r="U157" s="25"/>
+      <c r="V157" s="25"/>
+      <c r="W157" s="25"/>
+      <c r="X157" s="25"/>
+      <c r="Y157" s="25"/>
+      <c r="Z157" s="25"/>
+      <c r="AA157" s="25"/>
+      <c r="AB157" s="25"/>
+      <c r="AC157" s="25"/>
+      <c r="AD157" s="25"/>
+      <c r="AE157" s="25"/>
+      <c r="AF157" s="25"/>
+      <c r="AG157" s="25"/>
+      <c r="AH157" s="25"/>
+      <c r="AI157" s="25"/>
+      <c r="AJ157" s="25"/>
+      <c r="AK157" s="25"/>
+      <c r="AL157" s="171"/>
+      <c r="AM157" s="171"/>
+      <c r="AN157" s="171"/>
+      <c r="AO157" s="171"/>
+      <c r="AP157" s="171"/>
+      <c r="AQ157" s="171"/>
+      <c r="AR157" s="171"/>
+      <c r="AS157" s="25"/>
+      <c r="AT157" s="25"/>
+      <c r="AU157" s="25"/>
+      <c r="AV157" s="176"/>
+    </row>
+    <row r="158" spans="4:48">
+      <c r="F158" s="175"/>
+      <c r="G158" s="25"/>
+      <c r="H158" s="25"/>
+      <c r="I158" s="25"/>
+      <c r="J158" s="25"/>
+      <c r="K158" s="25"/>
+      <c r="L158" s="25"/>
+      <c r="M158" s="25"/>
+      <c r="N158" s="25"/>
+      <c r="O158" s="25"/>
+      <c r="P158" s="25"/>
+      <c r="Q158" s="25"/>
+      <c r="R158" s="25"/>
+      <c r="S158" s="25"/>
+      <c r="T158" s="25"/>
+      <c r="U158" s="25"/>
+      <c r="V158" s="25"/>
+      <c r="W158" s="25"/>
+      <c r="X158" s="25"/>
+      <c r="Y158" s="25"/>
+      <c r="Z158" s="25"/>
+      <c r="AA158" s="25"/>
+      <c r="AB158" s="25"/>
+      <c r="AC158" s="25"/>
+      <c r="AD158" s="25"/>
+      <c r="AE158" s="25"/>
+      <c r="AF158" s="25"/>
+      <c r="AG158" s="25"/>
+      <c r="AH158" s="25"/>
+      <c r="AI158" s="25"/>
+      <c r="AJ158" s="25"/>
+      <c r="AK158" s="25"/>
+      <c r="AL158" s="171"/>
+      <c r="AM158" s="171"/>
+      <c r="AN158" s="171"/>
+      <c r="AO158" s="171"/>
+      <c r="AP158" s="171"/>
+      <c r="AQ158" s="171"/>
+      <c r="AR158" s="171"/>
+      <c r="AS158" s="25"/>
+      <c r="AT158" s="25"/>
+      <c r="AU158" s="25"/>
+      <c r="AV158" s="176"/>
+    </row>
+    <row r="159" spans="4:48">
+      <c r="F159" s="175"/>
+      <c r="G159" s="25"/>
+      <c r="H159" s="25"/>
+      <c r="I159" s="25"/>
+      <c r="J159" s="25"/>
+      <c r="K159" s="25"/>
+      <c r="L159" s="25"/>
+      <c r="M159" s="25"/>
+      <c r="N159" s="25"/>
+      <c r="O159" s="25"/>
+      <c r="P159" s="25"/>
+      <c r="Q159" s="25"/>
+      <c r="R159" s="25"/>
+      <c r="S159" s="25"/>
+      <c r="T159" s="25"/>
+      <c r="U159" s="25"/>
+      <c r="V159" s="25"/>
+      <c r="W159" s="25"/>
+      <c r="X159" s="25"/>
+      <c r="Y159" s="25"/>
+      <c r="Z159" s="25"/>
+      <c r="AA159" s="25"/>
+      <c r="AB159" s="25"/>
+      <c r="AC159" s="25"/>
+      <c r="AD159" s="25"/>
+      <c r="AE159" s="25"/>
+      <c r="AF159" s="25"/>
+      <c r="AG159" s="25"/>
+      <c r="AH159" s="25"/>
+      <c r="AI159" s="25"/>
+      <c r="AJ159" s="25"/>
+      <c r="AK159" s="25"/>
+      <c r="AL159" s="171"/>
+      <c r="AM159" s="171"/>
+      <c r="AN159" s="171"/>
+      <c r="AO159" s="171"/>
+      <c r="AP159" s="171"/>
+      <c r="AQ159" s="171"/>
+      <c r="AR159" s="171"/>
+      <c r="AS159" s="25"/>
+      <c r="AT159" s="25"/>
+      <c r="AU159" s="25"/>
+      <c r="AV159" s="176"/>
+    </row>
+    <row r="160" spans="4:48">
+      <c r="F160" s="175"/>
+      <c r="G160" s="25"/>
+      <c r="H160" s="25"/>
+      <c r="I160" s="25"/>
+      <c r="J160" s="25"/>
+      <c r="K160" s="25"/>
+      <c r="L160" s="25"/>
+      <c r="M160" s="25"/>
+      <c r="N160" s="25"/>
+      <c r="O160" s="25"/>
+      <c r="P160" s="25"/>
+      <c r="Q160" s="25"/>
+      <c r="R160" s="25"/>
+      <c r="S160" s="25"/>
+      <c r="T160" s="25"/>
+      <c r="U160" s="25"/>
+      <c r="V160" s="25"/>
+      <c r="W160" s="25"/>
+      <c r="X160" s="25"/>
+      <c r="Y160" s="25"/>
+      <c r="Z160" s="25"/>
+      <c r="AA160" s="25"/>
+      <c r="AB160" s="25"/>
+      <c r="AC160" s="25"/>
+      <c r="AD160" s="25"/>
+      <c r="AE160" s="25"/>
+      <c r="AF160" s="25"/>
+      <c r="AG160" s="25"/>
+      <c r="AH160" s="25"/>
+      <c r="AI160" s="25"/>
+      <c r="AJ160" s="25"/>
+      <c r="AK160" s="25"/>
+      <c r="AL160" s="171"/>
+      <c r="AM160" s="171"/>
+      <c r="AN160" s="171"/>
+      <c r="AO160" s="171"/>
+      <c r="AP160" s="171"/>
+      <c r="AQ160" s="171"/>
+      <c r="AR160" s="171"/>
+      <c r="AS160" s="25"/>
+      <c r="AT160" s="25"/>
+      <c r="AU160" s="25"/>
+      <c r="AV160" s="176"/>
+    </row>
+    <row r="161" spans="4:48">
+      <c r="E161">
+        <v>494</v>
+      </c>
+      <c r="F161" s="173" t="s">
+        <v>462</v>
+      </c>
+      <c r="G161" s="171"/>
+      <c r="H161" s="171"/>
+      <c r="I161" s="171"/>
+      <c r="J161" s="171"/>
+      <c r="K161" s="171"/>
+      <c r="L161" s="171"/>
+      <c r="M161" s="171"/>
+      <c r="N161" s="171"/>
+      <c r="O161" s="171"/>
+      <c r="P161" s="171"/>
+      <c r="Q161" s="171"/>
+      <c r="R161" s="171"/>
+      <c r="S161" s="171"/>
+      <c r="T161" s="171"/>
+      <c r="U161" s="171"/>
+      <c r="V161" s="171"/>
+      <c r="W161" s="171"/>
+      <c r="X161" s="171"/>
+      <c r="Y161" s="171"/>
+      <c r="Z161" s="171"/>
+      <c r="AA161" s="171"/>
+      <c r="AB161" s="171"/>
+      <c r="AC161" s="171"/>
+      <c r="AD161" s="171"/>
+      <c r="AE161" s="171"/>
+      <c r="AF161" s="171"/>
+      <c r="AG161" s="171"/>
+      <c r="AH161" s="171"/>
+      <c r="AI161" s="171"/>
+      <c r="AJ161" s="171"/>
+      <c r="AK161" s="171"/>
+      <c r="AL161" s="171"/>
+      <c r="AM161" s="171"/>
+      <c r="AN161" s="171"/>
+      <c r="AO161" s="171"/>
+      <c r="AP161" s="171"/>
+      <c r="AQ161" s="171"/>
+      <c r="AR161" s="171"/>
+      <c r="AS161" s="171"/>
+      <c r="AT161" s="171"/>
+      <c r="AU161" s="171"/>
+      <c r="AV161" s="174"/>
+    </row>
+    <row r="162" spans="4:48">
+      <c r="F162" s="175"/>
+      <c r="G162" s="25"/>
+      <c r="H162" s="25"/>
+      <c r="I162" s="25"/>
+      <c r="J162" s="25"/>
+      <c r="K162" s="25"/>
+      <c r="L162" s="25"/>
+      <c r="M162" s="25"/>
+      <c r="N162" s="25"/>
+      <c r="O162" s="25"/>
+      <c r="P162" s="25"/>
+      <c r="Q162" s="25"/>
+      <c r="R162" s="25"/>
+      <c r="S162" s="25"/>
+      <c r="T162" s="25"/>
+      <c r="U162" s="25"/>
+      <c r="V162" s="25"/>
+      <c r="W162" s="25"/>
+      <c r="X162" s="25"/>
+      <c r="Y162" s="25"/>
+      <c r="Z162" s="25"/>
+      <c r="AA162" s="25"/>
+      <c r="AB162" s="25"/>
+      <c r="AC162" s="25"/>
+      <c r="AD162" s="25"/>
+      <c r="AE162" s="25"/>
+      <c r="AF162" s="25"/>
+      <c r="AG162" s="25"/>
+      <c r="AH162" s="25"/>
+      <c r="AI162" s="25"/>
+      <c r="AJ162" s="25"/>
+      <c r="AK162" s="25"/>
+      <c r="AL162" s="171"/>
+      <c r="AM162" s="171"/>
+      <c r="AN162" s="171"/>
+      <c r="AO162" s="171"/>
+      <c r="AP162" s="171"/>
+      <c r="AQ162" s="171"/>
+      <c r="AR162" s="171"/>
+      <c r="AS162" s="25"/>
+      <c r="AT162" s="25"/>
+      <c r="AU162" s="25"/>
+      <c r="AV162" s="176"/>
+    </row>
+    <row r="163" spans="4:48">
+      <c r="F163" s="175"/>
+      <c r="G163" s="25"/>
+      <c r="H163" s="25"/>
+      <c r="I163" s="25"/>
+      <c r="J163" s="25"/>
+      <c r="K163" s="25"/>
+      <c r="L163" s="25"/>
+      <c r="M163" s="25"/>
+      <c r="N163" s="25"/>
+      <c r="O163" s="25"/>
+      <c r="P163" s="25"/>
+      <c r="Q163" s="25"/>
+      <c r="R163" s="25"/>
+      <c r="S163" s="25"/>
+      <c r="T163" s="25"/>
+      <c r="U163" s="25"/>
+      <c r="V163" s="25"/>
+      <c r="W163" s="25"/>
+      <c r="X163" s="25"/>
+      <c r="Y163" s="25"/>
+      <c r="Z163" s="25"/>
+      <c r="AA163" s="25"/>
+      <c r="AB163" s="25"/>
+      <c r="AC163" s="25"/>
+      <c r="AD163" s="25"/>
+      <c r="AE163" s="25"/>
+      <c r="AF163" s="25"/>
+      <c r="AG163" s="25"/>
+      <c r="AH163" s="25"/>
+      <c r="AI163" s="25"/>
+      <c r="AJ163" s="25"/>
+      <c r="AK163" s="25"/>
+      <c r="AL163" s="171"/>
+      <c r="AM163" s="171"/>
+      <c r="AN163" s="171"/>
+      <c r="AO163" s="171"/>
+      <c r="AP163" s="171"/>
+      <c r="AQ163" s="171"/>
+      <c r="AR163" s="171"/>
+      <c r="AS163" s="25"/>
+      <c r="AT163" s="25"/>
+      <c r="AU163" s="25"/>
+      <c r="AV163" s="176"/>
+    </row>
+    <row r="164" spans="4:48">
+      <c r="F164" s="175"/>
+      <c r="G164" s="25"/>
+      <c r="H164" s="25"/>
+      <c r="I164" s="25"/>
+      <c r="J164" s="25"/>
+      <c r="K164" s="25"/>
+      <c r="L164" s="25"/>
+      <c r="M164" s="25"/>
+      <c r="N164" s="25"/>
+      <c r="O164" s="25"/>
+      <c r="P164" s="25"/>
+      <c r="Q164" s="25"/>
+      <c r="R164" s="25"/>
+      <c r="S164" s="25"/>
+      <c r="T164" s="25"/>
+      <c r="U164" s="25"/>
+      <c r="V164" s="25"/>
+      <c r="W164" s="25"/>
+      <c r="X164" s="25"/>
+      <c r="Y164" s="25"/>
+      <c r="Z164" s="25"/>
+      <c r="AA164" s="25"/>
+      <c r="AB164" s="25"/>
+      <c r="AC164" s="25"/>
+      <c r="AD164" s="25"/>
+      <c r="AE164" s="25"/>
+      <c r="AF164" s="25"/>
+      <c r="AG164" s="25"/>
+      <c r="AH164" s="25"/>
+      <c r="AI164" s="25"/>
+      <c r="AJ164" s="25"/>
+      <c r="AK164" s="25"/>
+      <c r="AL164" s="171"/>
+      <c r="AM164" s="171"/>
+      <c r="AN164" s="171"/>
+      <c r="AO164" s="171"/>
+      <c r="AP164" s="171"/>
+      <c r="AQ164" s="171"/>
+      <c r="AR164" s="171"/>
+      <c r="AS164" s="25"/>
+      <c r="AT164" s="25"/>
+      <c r="AU164" s="25"/>
+      <c r="AV164" s="176"/>
+    </row>
+    <row r="165" spans="4:48">
+      <c r="F165" s="175"/>
+      <c r="G165" s="25"/>
+      <c r="H165" s="25"/>
+      <c r="I165" s="25"/>
+      <c r="J165" s="25"/>
+      <c r="K165" s="25"/>
+      <c r="L165" s="25"/>
+      <c r="M165" s="25"/>
+      <c r="N165" s="25"/>
+      <c r="O165" s="25"/>
+      <c r="P165" s="25"/>
+      <c r="Q165" s="25"/>
+      <c r="R165" s="25"/>
+      <c r="S165" s="25"/>
+      <c r="T165" s="25"/>
+      <c r="U165" s="25"/>
+      <c r="V165" s="25"/>
+      <c r="W165" s="25"/>
+      <c r="X165" s="25"/>
+      <c r="Y165" s="25"/>
+      <c r="Z165" s="25"/>
+      <c r="AA165" s="25"/>
+      <c r="AB165" s="25"/>
+      <c r="AC165" s="25"/>
+      <c r="AD165" s="25"/>
+      <c r="AE165" s="25"/>
+      <c r="AF165" s="25"/>
+      <c r="AG165" s="25"/>
+      <c r="AH165" s="25"/>
+      <c r="AI165" s="25"/>
+      <c r="AJ165" s="25"/>
+      <c r="AK165" s="25"/>
+      <c r="AL165" s="171"/>
+      <c r="AM165" s="171"/>
+      <c r="AN165" s="171"/>
+      <c r="AO165" s="171"/>
+      <c r="AP165" s="171"/>
+      <c r="AQ165" s="171"/>
+      <c r="AR165" s="171"/>
+      <c r="AS165" s="25"/>
+      <c r="AT165" s="25"/>
+      <c r="AU165" s="25"/>
+      <c r="AV165" s="176"/>
+    </row>
+    <row r="166" spans="4:48">
+      <c r="D166">
+        <v>263</v>
+      </c>
+      <c r="E166">
+        <v>525</v>
+      </c>
+      <c r="F166" s="21"/>
+      <c r="G166" s="22"/>
+      <c r="H166" s="22"/>
+      <c r="I166" s="22"/>
+      <c r="J166" s="22"/>
+      <c r="K166" s="22"/>
+      <c r="L166" s="22"/>
+      <c r="M166" s="22"/>
+      <c r="N166" s="22"/>
+      <c r="O166" s="22"/>
+      <c r="P166" s="22"/>
+      <c r="Q166" s="22"/>
+      <c r="R166" s="22"/>
+      <c r="S166" s="22"/>
+      <c r="T166" s="22"/>
+      <c r="U166" s="22"/>
+      <c r="V166" s="22"/>
+      <c r="W166" s="22"/>
+      <c r="X166" s="22"/>
+      <c r="Y166" s="22"/>
+      <c r="Z166" s="22"/>
+      <c r="AA166" s="22"/>
+      <c r="AB166" s="22"/>
+      <c r="AC166" s="22"/>
+      <c r="AD166" s="22"/>
+      <c r="AE166" s="22"/>
+      <c r="AF166" s="22"/>
+      <c r="AG166" s="22"/>
+      <c r="AH166" s="22"/>
+      <c r="AI166" s="22"/>
+      <c r="AJ166" s="22"/>
+      <c r="AK166" s="22"/>
+      <c r="AL166" s="172"/>
+      <c r="AM166" s="172"/>
+      <c r="AN166" s="172"/>
+      <c r="AO166" s="172"/>
+      <c r="AP166" s="172"/>
+      <c r="AQ166" s="172"/>
+      <c r="AR166" s="172"/>
+      <c r="AS166" s="22"/>
+      <c r="AT166" s="22"/>
+      <c r="AU166" s="22"/>
+      <c r="AV166" s="23"/>
+    </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AG34:AH34"/>
+    <mergeCell ref="AI34:AJ34"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
     <mergeCell ref="BO33:BP33"/>
     <mergeCell ref="BO34:BP34"/>
     <mergeCell ref="CA33:CB33"/>
@@ -16608,71 +18385,20 @@
     <mergeCell ref="BY34:BZ34"/>
     <mergeCell ref="CA34:CB34"/>
     <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AG34:AH34"/>
-    <mergeCell ref="AI34:AJ34"/>
-    <mergeCell ref="AK34:AL34"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BY36:BZ36"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16685,7 +18411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:EC90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="X82" sqref="X82"/>
     </sheetView>
   </sheetViews>
@@ -17953,262 +19679,262 @@
       </c>
     </row>
     <row r="47" spans="1:133">
-      <c r="F47" s="158" t="s">
+      <c r="F47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="158"/>
-      <c r="H47" s="158" t="s">
+      <c r="G47" s="160"/>
+      <c r="H47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="I47" s="158"/>
-      <c r="J47" s="158" t="s">
+      <c r="I47" s="160"/>
+      <c r="J47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="K47" s="158"/>
-      <c r="L47" s="158" t="s">
+      <c r="K47" s="160"/>
+      <c r="L47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="M47" s="158"/>
-      <c r="N47" s="158" t="s">
+      <c r="M47" s="160"/>
+      <c r="N47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="O47" s="158"/>
-      <c r="P47" s="158" t="s">
+      <c r="O47" s="160"/>
+      <c r="P47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="Q47" s="158"/>
-      <c r="R47" s="158" t="s">
+      <c r="Q47" s="160"/>
+      <c r="R47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="S47" s="158"/>
-      <c r="T47" s="158" t="s">
+      <c r="S47" s="160"/>
+      <c r="T47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="U47" s="158"/>
-      <c r="V47" s="158" t="s">
+      <c r="U47" s="160"/>
+      <c r="V47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="W47" s="158"/>
-      <c r="X47" s="158" t="s">
+      <c r="W47" s="160"/>
+      <c r="X47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="Y47" s="158"/>
-      <c r="Z47" s="158" t="s">
+      <c r="Y47" s="160"/>
+      <c r="Z47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AA47" s="158"/>
-      <c r="AB47" s="158" t="s">
+      <c r="AA47" s="160"/>
+      <c r="AB47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AC47" s="158"/>
-      <c r="AD47" s="158" t="s">
+      <c r="AC47" s="160"/>
+      <c r="AD47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AE47" s="158"/>
-      <c r="AF47" s="158" t="s">
+      <c r="AE47" s="160"/>
+      <c r="AF47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AG47" s="158"/>
-      <c r="AH47" s="158" t="s">
+      <c r="AG47" s="160"/>
+      <c r="AH47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AI47" s="158"/>
-      <c r="AJ47" s="158" t="s">
+      <c r="AI47" s="160"/>
+      <c r="AJ47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AK47" s="158"/>
-      <c r="AL47" s="158" t="s">
+      <c r="AK47" s="160"/>
+      <c r="AL47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AM47" s="158"/>
-      <c r="AN47" s="158" t="s">
+      <c r="AM47" s="160"/>
+      <c r="AN47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AO47" s="158"/>
-      <c r="AP47" s="158" t="s">
+      <c r="AO47" s="160"/>
+      <c r="AP47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AQ47" s="158"/>
-      <c r="AR47" s="158" t="s">
+      <c r="AQ47" s="160"/>
+      <c r="AR47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AS47" s="158"/>
-      <c r="AT47" s="158" t="s">
+      <c r="AS47" s="160"/>
+      <c r="AT47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AU47" s="158"/>
-      <c r="AV47" s="158" t="s">
+      <c r="AU47" s="160"/>
+      <c r="AV47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AW47" s="158"/>
-      <c r="AX47" s="158" t="s">
+      <c r="AW47" s="160"/>
+      <c r="AX47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AY47" s="158"/>
-      <c r="AZ47" s="158" t="s">
+      <c r="AY47" s="160"/>
+      <c r="AZ47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BA47" s="158"/>
-      <c r="BB47" s="158" t="s">
+      <c r="BA47" s="160"/>
+      <c r="BB47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BC47" s="158"/>
-      <c r="BD47" s="158" t="s">
+      <c r="BC47" s="160"/>
+      <c r="BD47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BE47" s="158"/>
-      <c r="BF47" s="158" t="s">
+      <c r="BE47" s="160"/>
+      <c r="BF47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BG47" s="158"/>
-      <c r="BH47" s="158" t="s">
+      <c r="BG47" s="160"/>
+      <c r="BH47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BI47" s="158"/>
-      <c r="BJ47" s="158" t="s">
+      <c r="BI47" s="160"/>
+      <c r="BJ47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BK47" s="158"/>
-      <c r="BL47" s="158" t="s">
+      <c r="BK47" s="160"/>
+      <c r="BL47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BM47" s="158"/>
-      <c r="BN47" s="158" t="s">
+      <c r="BM47" s="160"/>
+      <c r="BN47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BO47" s="158"/>
-      <c r="BP47" s="158" t="s">
+      <c r="BO47" s="160"/>
+      <c r="BP47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BQ47" s="158"/>
-      <c r="BR47" s="158" t="s">
+      <c r="BQ47" s="160"/>
+      <c r="BR47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="BS47" s="158"/>
-      <c r="BT47" s="158" t="s">
+      <c r="BS47" s="160"/>
+      <c r="BT47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="BU47" s="158"/>
-      <c r="BV47" s="158" t="s">
+      <c r="BU47" s="160"/>
+      <c r="BV47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="BW47" s="158"/>
-      <c r="BX47" s="158" t="s">
+      <c r="BW47" s="160"/>
+      <c r="BX47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="BY47" s="158"/>
-      <c r="BZ47" s="158" t="s">
+      <c r="BY47" s="160"/>
+      <c r="BZ47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CA47" s="158"/>
-      <c r="CB47" s="158" t="s">
+      <c r="CA47" s="160"/>
+      <c r="CB47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="CC47" s="158"/>
-      <c r="CD47" s="158" t="s">
+      <c r="CC47" s="160"/>
+      <c r="CD47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CE47" s="158"/>
-      <c r="CF47" s="158" t="s">
+      <c r="CE47" s="160"/>
+      <c r="CF47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CG47" s="158"/>
-      <c r="CH47" s="158" t="s">
+      <c r="CG47" s="160"/>
+      <c r="CH47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CI47" s="158"/>
-      <c r="CJ47" s="158" t="s">
+      <c r="CI47" s="160"/>
+      <c r="CJ47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="CK47" s="158"/>
-      <c r="CL47" s="158" t="s">
+      <c r="CK47" s="160"/>
+      <c r="CL47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CM47" s="158"/>
-      <c r="CN47" s="158" t="s">
+      <c r="CM47" s="160"/>
+      <c r="CN47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CO47" s="158"/>
-      <c r="CP47" s="158" t="s">
+      <c r="CO47" s="160"/>
+      <c r="CP47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CQ47" s="158"/>
-      <c r="CR47" s="158" t="s">
+      <c r="CQ47" s="160"/>
+      <c r="CR47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="CS47" s="158"/>
-      <c r="CT47" s="158" t="s">
+      <c r="CS47" s="160"/>
+      <c r="CT47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="CU47" s="158"/>
-      <c r="CV47" s="158" t="s">
+      <c r="CU47" s="160"/>
+      <c r="CV47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="CW47" s="158"/>
-      <c r="CX47" s="158" t="s">
+      <c r="CW47" s="160"/>
+      <c r="CX47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="CY47" s="158"/>
-      <c r="CZ47" s="158" t="s">
+      <c r="CY47" s="160"/>
+      <c r="CZ47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="DA47" s="158"/>
-      <c r="DB47" s="158" t="s">
+      <c r="DA47" s="160"/>
+      <c r="DB47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="DC47" s="158"/>
-      <c r="DD47" s="158" t="s">
+      <c r="DC47" s="160"/>
+      <c r="DD47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="DE47" s="158"/>
-      <c r="DF47" s="158" t="s">
+      <c r="DE47" s="160"/>
+      <c r="DF47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="DG47" s="158"/>
-      <c r="DH47" s="158" t="s">
+      <c r="DG47" s="160"/>
+      <c r="DH47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="DI47" s="158"/>
-      <c r="DJ47" s="158" t="s">
+      <c r="DI47" s="160"/>
+      <c r="DJ47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="DK47" s="158"/>
-      <c r="DL47" s="158" t="s">
+      <c r="DK47" s="160"/>
+      <c r="DL47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="DM47" s="158"/>
-      <c r="DN47" s="158" t="s">
+      <c r="DM47" s="160"/>
+      <c r="DN47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="DO47" s="158"/>
-      <c r="DP47" s="158" t="s">
+      <c r="DO47" s="160"/>
+      <c r="DP47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="DQ47" s="158"/>
-      <c r="DR47" s="158" t="s">
+      <c r="DQ47" s="160"/>
+      <c r="DR47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="DS47" s="158"/>
-      <c r="DT47" s="158" t="s">
+      <c r="DS47" s="160"/>
+      <c r="DT47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="DU47" s="158"/>
-      <c r="DV47" s="158" t="s">
+      <c r="DU47" s="160"/>
+      <c r="DV47" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="DW47" s="158"/>
-      <c r="DX47" s="158" t="s">
+      <c r="DW47" s="160"/>
+      <c r="DX47" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="DY47" s="158"/>
-      <c r="DZ47" s="158" t="s">
+      <c r="DY47" s="160"/>
+      <c r="DZ47" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="EA47" s="158"/>
-      <c r="EB47" s="158" t="s">
+      <c r="EA47" s="160"/>
+      <c r="EB47" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="EC47" s="158"/>
+      <c r="EC47" s="160"/>
     </row>
     <row r="49" spans="11:36">
       <c r="K49" t="s">
@@ -18610,6 +20336,57 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="AN47:AO47"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="AF47:AG47"/>
+    <mergeCell ref="AH47:AI47"/>
+    <mergeCell ref="AJ47:AK47"/>
+    <mergeCell ref="AL47:AM47"/>
+    <mergeCell ref="BL47:BM47"/>
+    <mergeCell ref="AP47:AQ47"/>
+    <mergeCell ref="AR47:AS47"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="AV47:AW47"/>
+    <mergeCell ref="AX47:AY47"/>
+    <mergeCell ref="AZ47:BA47"/>
+    <mergeCell ref="BB47:BC47"/>
+    <mergeCell ref="BD47:BE47"/>
+    <mergeCell ref="BF47:BG47"/>
+    <mergeCell ref="BH47:BI47"/>
+    <mergeCell ref="BJ47:BK47"/>
+    <mergeCell ref="CJ47:CK47"/>
+    <mergeCell ref="BN47:BO47"/>
+    <mergeCell ref="BP47:BQ47"/>
+    <mergeCell ref="BR47:BS47"/>
+    <mergeCell ref="BT47:BU47"/>
+    <mergeCell ref="BV47:BW47"/>
+    <mergeCell ref="BX47:BY47"/>
+    <mergeCell ref="BZ47:CA47"/>
+    <mergeCell ref="CB47:CC47"/>
+    <mergeCell ref="CD47:CE47"/>
+    <mergeCell ref="CF47:CG47"/>
+    <mergeCell ref="CH47:CI47"/>
+    <mergeCell ref="DD47:DE47"/>
+    <mergeCell ref="DF47:DG47"/>
+    <mergeCell ref="DH47:DI47"/>
+    <mergeCell ref="CL47:CM47"/>
+    <mergeCell ref="CN47:CO47"/>
+    <mergeCell ref="CP47:CQ47"/>
+    <mergeCell ref="CR47:CS47"/>
+    <mergeCell ref="CT47:CU47"/>
+    <mergeCell ref="CV47:CW47"/>
     <mergeCell ref="DV47:DW47"/>
     <mergeCell ref="DX47:DY47"/>
     <mergeCell ref="DZ47:EA47"/>
@@ -18626,57 +20403,6 @@
     <mergeCell ref="CX47:CY47"/>
     <mergeCell ref="CZ47:DA47"/>
     <mergeCell ref="DB47:DC47"/>
-    <mergeCell ref="DD47:DE47"/>
-    <mergeCell ref="DF47:DG47"/>
-    <mergeCell ref="DH47:DI47"/>
-    <mergeCell ref="CL47:CM47"/>
-    <mergeCell ref="CN47:CO47"/>
-    <mergeCell ref="CP47:CQ47"/>
-    <mergeCell ref="CR47:CS47"/>
-    <mergeCell ref="CT47:CU47"/>
-    <mergeCell ref="CV47:CW47"/>
-    <mergeCell ref="CJ47:CK47"/>
-    <mergeCell ref="BN47:BO47"/>
-    <mergeCell ref="BP47:BQ47"/>
-    <mergeCell ref="BR47:BS47"/>
-    <mergeCell ref="BT47:BU47"/>
-    <mergeCell ref="BV47:BW47"/>
-    <mergeCell ref="BX47:BY47"/>
-    <mergeCell ref="BZ47:CA47"/>
-    <mergeCell ref="CB47:CC47"/>
-    <mergeCell ref="CD47:CE47"/>
-    <mergeCell ref="CF47:CG47"/>
-    <mergeCell ref="CH47:CI47"/>
-    <mergeCell ref="BL47:BM47"/>
-    <mergeCell ref="AP47:AQ47"/>
-    <mergeCell ref="AR47:AS47"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="AV47:AW47"/>
-    <mergeCell ref="AX47:AY47"/>
-    <mergeCell ref="AZ47:BA47"/>
-    <mergeCell ref="BB47:BC47"/>
-    <mergeCell ref="BD47:BE47"/>
-    <mergeCell ref="BF47:BG47"/>
-    <mergeCell ref="BH47:BI47"/>
-    <mergeCell ref="BJ47:BK47"/>
-    <mergeCell ref="AN47:AO47"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="X47:Y47"/>
-    <mergeCell ref="Z47:AA47"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AD47:AE47"/>
-    <mergeCell ref="AF47:AG47"/>
-    <mergeCell ref="AH47:AI47"/>
-    <mergeCell ref="AJ47:AK47"/>
-    <mergeCell ref="AL47:AM47"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18912,62 +20638,62 @@
         <v>0</v>
       </c>
       <c r="F3" s="39"/>
-      <c r="G3" s="158" t="s">
+      <c r="G3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158" t="s">
+      <c r="H3" s="160"/>
+      <c r="I3" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158" t="s">
+      <c r="J3" s="160"/>
+      <c r="K3" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="158"/>
-      <c r="M3" s="158" t="s">
+      <c r="L3" s="160"/>
+      <c r="M3" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158" t="s">
+      <c r="N3" s="160"/>
+      <c r="O3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="158"/>
-      <c r="Q3" s="158" t="s">
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="158"/>
-      <c r="S3" s="158" t="s">
+      <c r="R3" s="160"/>
+      <c r="S3" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="158"/>
-      <c r="U3" s="158" t="s">
+      <c r="T3" s="160"/>
+      <c r="U3" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="158"/>
-      <c r="W3" s="158" t="s">
+      <c r="V3" s="160"/>
+      <c r="W3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="X3" s="158"/>
+      <c r="X3" s="160"/>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="158" t="s">
+      <c r="AC3" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="158"/>
-      <c r="AE3" s="158" t="s">
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AF3" s="158"/>
-      <c r="AG3" s="158" t="s">
+      <c r="AF3" s="160"/>
+      <c r="AG3" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="158"/>
-      <c r="AI3" s="158" t="s">
+      <c r="AH3" s="160"/>
+      <c r="AI3" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AJ3" s="158"/>
+      <c r="AJ3" s="160"/>
       <c r="AK3" s="34"/>
       <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
@@ -18990,104 +20716,104 @@
       <c r="BH3" s="34"/>
       <c r="BI3" s="34"/>
       <c r="BJ3" s="34"/>
-      <c r="BK3" s="160" t="s">
+      <c r="BK3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BL3" s="161"/>
-      <c r="BM3" s="160" t="s">
+      <c r="BL3" s="159"/>
+      <c r="BM3" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BN3" s="161"/>
-      <c r="BO3" s="160" t="s">
+      <c r="BN3" s="159"/>
+      <c r="BO3" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" s="161"/>
-      <c r="BQ3" s="160" t="s">
+      <c r="BP3" s="159"/>
+      <c r="BQ3" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BR3" s="161"/>
-      <c r="BS3" s="160" t="s">
+      <c r="BR3" s="159"/>
+      <c r="BS3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="161"/>
-      <c r="BU3" s="160" t="s">
+      <c r="BT3" s="159"/>
+      <c r="BU3" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BV3" s="161"/>
-      <c r="BW3" s="160" t="s">
+      <c r="BV3" s="159"/>
+      <c r="BW3" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BX3" s="161"/>
-      <c r="BY3" s="160" t="s">
+      <c r="BX3" s="159"/>
+      <c r="BY3" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BZ3" s="161"/>
-      <c r="CA3" s="160" t="s">
+      <c r="BZ3" s="159"/>
+      <c r="CA3" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CB3" s="161"/>
+      <c r="CB3" s="159"/>
     </row>
     <row r="4" spans="2:80">
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="34"/>
-      <c r="G4" s="158" t="s">
+      <c r="G4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158" t="s">
+      <c r="H4" s="160"/>
+      <c r="I4" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158" t="s">
+      <c r="J4" s="160"/>
+      <c r="K4" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158" t="s">
+      <c r="L4" s="160"/>
+      <c r="M4" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158" t="s">
+      <c r="N4" s="160"/>
+      <c r="O4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="P4" s="158"/>
-      <c r="Q4" s="158" t="s">
+      <c r="P4" s="160"/>
+      <c r="Q4" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="R4" s="158"/>
-      <c r="S4" s="158" t="s">
+      <c r="R4" s="160"/>
+      <c r="S4" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="158"/>
-      <c r="U4" s="158" t="s">
+      <c r="T4" s="160"/>
+      <c r="U4" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="V4" s="158"/>
-      <c r="W4" s="158" t="s">
+      <c r="V4" s="160"/>
+      <c r="W4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="158"/>
+      <c r="X4" s="160"/>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="158" t="s">
+      <c r="AC4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AD4" s="158"/>
-      <c r="AE4" s="158" t="s">
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="158"/>
-      <c r="AG4" s="158" t="s">
+      <c r="AF4" s="160"/>
+      <c r="AG4" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AH4" s="158"/>
-      <c r="AI4" s="158" t="s">
+      <c r="AH4" s="160"/>
+      <c r="AI4" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="158"/>
+      <c r="AJ4" s="160"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
@@ -19110,42 +20836,42 @@
       <c r="BH4" s="34"/>
       <c r="BI4" s="34"/>
       <c r="BJ4" s="34"/>
-      <c r="BK4" s="160" t="s">
+      <c r="BK4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BL4" s="161"/>
-      <c r="BM4" s="160" t="s">
+      <c r="BL4" s="159"/>
+      <c r="BM4" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BN4" s="161"/>
-      <c r="BO4" s="160" t="s">
+      <c r="BN4" s="159"/>
+      <c r="BO4" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BP4" s="161"/>
-      <c r="BQ4" s="160" t="s">
+      <c r="BP4" s="159"/>
+      <c r="BQ4" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BR4" s="161"/>
-      <c r="BS4" s="160" t="s">
+      <c r="BR4" s="159"/>
+      <c r="BS4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BT4" s="161"/>
-      <c r="BU4" s="160" t="s">
+      <c r="BT4" s="159"/>
+      <c r="BU4" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BV4" s="161"/>
-      <c r="BW4" s="160" t="s">
+      <c r="BV4" s="159"/>
+      <c r="BW4" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="161"/>
-      <c r="BY4" s="160" t="s">
+      <c r="BX4" s="159"/>
+      <c r="BY4" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BZ4" s="161"/>
-      <c r="CA4" s="160" t="s">
+      <c r="BZ4" s="159"/>
+      <c r="CA4" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CB4" s="161"/>
+      <c r="CB4" s="159"/>
     </row>
     <row r="5" spans="2:80">
       <c r="BX5" s="27"/>
@@ -19159,62 +20885,62 @@
         <v>239</v>
       </c>
       <c r="F6" s="36"/>
-      <c r="G6" s="159" t="s">
+      <c r="G6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159" t="s">
+      <c r="H6" s="165"/>
+      <c r="I6" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="159"/>
-      <c r="K6" s="159" t="s">
+      <c r="J6" s="165"/>
+      <c r="K6" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159" t="s">
+      <c r="L6" s="165"/>
+      <c r="M6" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="159"/>
-      <c r="O6" s="159" t="s">
+      <c r="N6" s="165"/>
+      <c r="O6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="159"/>
-      <c r="Q6" s="159" t="s">
+      <c r="P6" s="165"/>
+      <c r="Q6" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="R6" s="159"/>
-      <c r="S6" s="159" t="s">
+      <c r="R6" s="165"/>
+      <c r="S6" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="159"/>
-      <c r="U6" s="159" t="s">
+      <c r="T6" s="165"/>
+      <c r="U6" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="V6" s="159"/>
-      <c r="W6" s="159" t="s">
+      <c r="V6" s="165"/>
+      <c r="W6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="X6" s="159"/>
+      <c r="X6" s="165"/>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AC6" s="159" t="s">
+      <c r="AC6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" s="159"/>
-      <c r="AE6" s="159" t="s">
+      <c r="AD6" s="165"/>
+      <c r="AE6" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="159"/>
-      <c r="AG6" s="159" t="s">
+      <c r="AF6" s="165"/>
+      <c r="AG6" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="AH6" s="159"/>
-      <c r="AI6" s="159" t="s">
+      <c r="AH6" s="165"/>
+      <c r="AI6" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="AJ6" s="159"/>
+      <c r="AJ6" s="165"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -19237,42 +20963,42 @@
       <c r="BH6" s="34"/>
       <c r="BI6" s="34"/>
       <c r="BJ6" s="34"/>
-      <c r="BK6" s="160" t="s">
+      <c r="BK6" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BL6" s="161"/>
-      <c r="BM6" s="160" t="s">
+      <c r="BL6" s="159"/>
+      <c r="BM6" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BN6" s="161"/>
-      <c r="BO6" s="160" t="s">
+      <c r="BN6" s="159"/>
+      <c r="BO6" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BP6" s="161"/>
-      <c r="BQ6" s="160" t="s">
+      <c r="BP6" s="159"/>
+      <c r="BQ6" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BR6" s="161"/>
-      <c r="BS6" s="160" t="s">
+      <c r="BR6" s="159"/>
+      <c r="BS6" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BT6" s="161"/>
-      <c r="BU6" s="160" t="s">
+      <c r="BT6" s="159"/>
+      <c r="BU6" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BV6" s="161"/>
-      <c r="BW6" s="160" t="s">
+      <c r="BV6" s="159"/>
+      <c r="BW6" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BX6" s="161"/>
-      <c r="BY6" s="160" t="s">
+      <c r="BX6" s="159"/>
+      <c r="BY6" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BZ6" s="161"/>
-      <c r="CA6" s="160" t="s">
+      <c r="BZ6" s="159"/>
+      <c r="CA6" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CB6" s="161"/>
+      <c r="CB6" s="159"/>
     </row>
     <row r="7" spans="2:80">
       <c r="E7">
@@ -19608,58 +21334,58 @@
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="158" t="s">
+      <c r="I12" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="158"/>
-      <c r="K12" s="158" t="s">
+      <c r="J12" s="160"/>
+      <c r="K12" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="158"/>
-      <c r="M12" s="158" t="s">
+      <c r="L12" s="160"/>
+      <c r="M12" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="158"/>
-      <c r="O12" s="158" t="s">
+      <c r="N12" s="160"/>
+      <c r="O12" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="P12" s="158"/>
-      <c r="Q12" s="158" t="s">
+      <c r="P12" s="160"/>
+      <c r="Q12" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="158"/>
-      <c r="S12" s="158" t="s">
+      <c r="R12" s="160"/>
+      <c r="S12" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="T12" s="158"/>
-      <c r="U12" s="158" t="s">
+      <c r="T12" s="160"/>
+      <c r="U12" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="158"/>
-      <c r="W12" s="158" t="s">
+      <c r="V12" s="160"/>
+      <c r="W12" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="158"/>
+      <c r="X12" s="160"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="158" t="s">
+      <c r="AC12" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="158"/>
-      <c r="AE12" s="158" t="s">
+      <c r="AD12" s="160"/>
+      <c r="AE12" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AF12" s="158"/>
-      <c r="AG12" s="158" t="s">
+      <c r="AF12" s="160"/>
+      <c r="AG12" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="AH12" s="158"/>
-      <c r="AI12" s="158" t="s">
+      <c r="AH12" s="160"/>
+      <c r="AI12" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="AJ12" s="158"/>
+      <c r="AJ12" s="160"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="34"/>
       <c r="AM12" s="34"/>
@@ -19682,42 +21408,42 @@
       <c r="BH12" s="34"/>
       <c r="BI12" s="34"/>
       <c r="BJ12" s="34"/>
-      <c r="BK12" s="160" t="s">
+      <c r="BK12" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BL12" s="161"/>
-      <c r="BM12" s="160" t="s">
+      <c r="BL12" s="159"/>
+      <c r="BM12" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BN12" s="161"/>
-      <c r="BO12" s="160" t="s">
+      <c r="BN12" s="159"/>
+      <c r="BO12" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BP12" s="161"/>
-      <c r="BQ12" s="160" t="s">
+      <c r="BP12" s="159"/>
+      <c r="BQ12" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BR12" s="161"/>
-      <c r="BS12" s="160" t="s">
+      <c r="BR12" s="159"/>
+      <c r="BS12" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="BT12" s="161"/>
-      <c r="BU12" s="160" t="s">
+      <c r="BT12" s="159"/>
+      <c r="BU12" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="BV12" s="161"/>
-      <c r="BW12" s="160" t="s">
+      <c r="BV12" s="159"/>
+      <c r="BW12" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="BX12" s="161"/>
-      <c r="BY12" s="160" t="s">
+      <c r="BX12" s="159"/>
+      <c r="BY12" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="BZ12" s="161"/>
-      <c r="CA12" s="160" t="s">
+      <c r="BZ12" s="159"/>
+      <c r="CA12" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="CB12" s="161"/>
+      <c r="CB12" s="159"/>
     </row>
     <row r="13" spans="2:80">
       <c r="BX13" s="27"/>
@@ -19750,71 +21476,71 @@
         <v>120</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="165" t="s">
+      <c r="G16" s="164" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="165"/>
-      <c r="I16" s="165"/>
-      <c r="J16" s="165"/>
-      <c r="K16" s="165"/>
-      <c r="L16" s="165"/>
-      <c r="M16" s="165"/>
-      <c r="N16" s="165"/>
-      <c r="O16" s="165"/>
-      <c r="P16" s="165"/>
-      <c r="Q16" s="165"/>
-      <c r="R16" s="165"/>
-      <c r="S16" s="165"/>
-      <c r="T16" s="165"/>
-      <c r="U16" s="165"/>
-      <c r="V16" s="165"/>
-      <c r="W16" s="165"/>
-      <c r="X16" s="165"/>
-      <c r="Y16" s="165"/>
-      <c r="Z16" s="165"/>
-      <c r="AA16" s="165" t="s">
+      <c r="H16" s="164"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="164"/>
+      <c r="K16" s="164"/>
+      <c r="L16" s="164"/>
+      <c r="M16" s="164"/>
+      <c r="N16" s="164"/>
+      <c r="O16" s="164"/>
+      <c r="P16" s="164"/>
+      <c r="Q16" s="164"/>
+      <c r="R16" s="164"/>
+      <c r="S16" s="164"/>
+      <c r="T16" s="164"/>
+      <c r="U16" s="164"/>
+      <c r="V16" s="164"/>
+      <c r="W16" s="164"/>
+      <c r="X16" s="164"/>
+      <c r="Y16" s="164"/>
+      <c r="Z16" s="164"/>
+      <c r="AA16" s="164" t="s">
         <v>116</v>
       </c>
-      <c r="AB16" s="165"/>
-      <c r="AC16" s="165"/>
-      <c r="AD16" s="165"/>
-      <c r="AE16" s="165"/>
-      <c r="AF16" s="165"/>
-      <c r="AG16" s="165"/>
-      <c r="AH16" s="165"/>
-      <c r="AI16" s="165"/>
-      <c r="AJ16" s="165"/>
-      <c r="AK16" s="158" t="s">
+      <c r="AB16" s="164"/>
+      <c r="AC16" s="164"/>
+      <c r="AD16" s="164"/>
+      <c r="AE16" s="164"/>
+      <c r="AF16" s="164"/>
+      <c r="AG16" s="164"/>
+      <c r="AH16" s="164"/>
+      <c r="AI16" s="164"/>
+      <c r="AJ16" s="164"/>
+      <c r="AK16" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="AL16" s="158"/>
-      <c r="AM16" s="158" t="s">
+      <c r="AL16" s="160"/>
+      <c r="AM16" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="AN16" s="158"/>
-      <c r="AO16" s="158" t="s">
+      <c r="AN16" s="160"/>
+      <c r="AO16" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="AP16" s="158"/>
-      <c r="AQ16" s="158" t="s">
+      <c r="AP16" s="160"/>
+      <c r="AQ16" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="AR16" s="158"/>
-      <c r="AS16" s="162" t="s">
+      <c r="AR16" s="160"/>
+      <c r="AS16" s="161" t="s">
         <v>119</v>
       </c>
-      <c r="AT16" s="163"/>
-      <c r="AU16" s="163"/>
-      <c r="AV16" s="163"/>
-      <c r="AW16" s="163"/>
-      <c r="AX16" s="163"/>
-      <c r="AY16" s="163"/>
-      <c r="AZ16" s="163"/>
-      <c r="BA16" s="164"/>
-      <c r="BB16" s="158" t="s">
+      <c r="AT16" s="162"/>
+      <c r="AU16" s="162"/>
+      <c r="AV16" s="162"/>
+      <c r="AW16" s="162"/>
+      <c r="AX16" s="162"/>
+      <c r="AY16" s="162"/>
+      <c r="AZ16" s="162"/>
+      <c r="BA16" s="163"/>
+      <c r="BB16" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="BC16" s="158"/>
+      <c r="BC16" s="160"/>
       <c r="BE16" s="38"/>
       <c r="BF16" s="38"/>
       <c r="BG16" s="38"/>
@@ -20363,6 +22089,85 @@
     </row>
   </sheetData>
   <mergeCells count="95">
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="BU3:BV3"/>
+    <mergeCell ref="BW3:BX3"/>
+    <mergeCell ref="BY3:BZ3"/>
+    <mergeCell ref="CA3:CB3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
     <mergeCell ref="BB16:BC16"/>
     <mergeCell ref="BW12:BX12"/>
     <mergeCell ref="BY12:BZ12"/>
@@ -20379,85 +22184,6 @@
     <mergeCell ref="BO12:BP12"/>
     <mergeCell ref="BQ12:BR12"/>
     <mergeCell ref="BS12:BT12"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="BU3:BV3"/>
-    <mergeCell ref="BW3:BX3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="CA3:CB3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test smb rom update
</commit_message>
<xml_diff>
--- a/doc/mos6502-ppu.xlsx
+++ b/doc/mos6502-ppu.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16110" windowHeight="11655" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="moto nes ppu design" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="470">
   <si>
     <t>ppu register handling</t>
     <phoneticPr fontId="1"/>
@@ -1565,27 +1570,39 @@
   <si>
     <t>(262 once.)</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pl</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>sp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
   </numFmts>
   <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1644,7 +1661,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -2702,7 +2719,7 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="24" fontId="8" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2870,7 +2887,7 @@
     <xf numFmtId="0" fontId="7" fillId="63" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="24" fontId="8" fillId="10" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3047,16 +3064,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3069,6 +3083,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3085,7 +3102,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6580,7 +6597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6622,7 +6639,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6654,9 +6671,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6688,6 +6706,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6863,14 +6882,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AO6:AO11"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="6" spans="41:41">
       <c r="AO6" t="s">
@@ -6900,18 +6919,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.25" customWidth="1"/>
-    <col min="2" max="2" width="42.625" customWidth="1"/>
-    <col min="3" max="3" width="64.25" customWidth="1"/>
+    <col min="1" max="1" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="15.75" thickBot="1">
@@ -6919,7 +6938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" thickBot="1">
+    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -6927,12 +6946,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" thickBot="1">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -6943,7 +6962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -6954,7 +6973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -6965,7 +6984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="163" t="s">
         <v>16</v>
       </c>
@@ -6976,14 +6995,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
       <c r="A9" s="164"/>
       <c r="B9" s="164"/>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -6994,7 +7013,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1">
+    <row r="11" spans="1:3" ht="29.25" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -7005,7 +7024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -7016,7 +7035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="163" t="s">
         <v>28</v>
       </c>
@@ -7027,14 +7046,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1">
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
       <c r="A14" s="164"/>
       <c r="B14" s="164"/>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -7042,12 +7061,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" thickBot="1">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -7058,7 +7077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -7069,7 +7088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -7080,7 +7099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -7091,7 +7110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -7102,7 +7121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
@@ -7113,7 +7132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
+    <row r="23" spans="1:3" ht="29.25" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -7124,7 +7143,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
         <v>41</v>
       </c>
@@ -7135,7 +7154,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
@@ -7146,17 +7165,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" thickBot="1">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -7167,7 +7186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="163" t="s">
         <v>10</v>
       </c>
@@ -7178,14 +7197,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
       <c r="A30" s="164"/>
       <c r="B30" s="164"/>
       <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1">
+    <row r="31" spans="1:3" ht="29.25" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>13</v>
       </c>
@@ -7196,7 +7215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
+    <row r="32" spans="1:3" ht="29.25" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -7207,7 +7226,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="163" t="s">
         <v>20</v>
       </c>
@@ -7218,14 +7237,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1">
+    <row r="34" spans="1:3" ht="15.75" thickBot="1">
       <c r="A34" s="164"/>
       <c r="B34" s="164"/>
       <c r="C34" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1">
       <c r="A35" s="4" t="s">
         <v>58</v>
       </c>
@@ -7234,17 +7253,17 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" thickBot="1">
+    <row r="37" spans="1:3" ht="15.75" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -7255,7 +7274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1">
+    <row r="39" spans="1:3" ht="15.75" thickBot="1">
       <c r="A39" s="4" t="s">
         <v>62</v>
       </c>
@@ -7266,17 +7285,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1">
       <c r="A40" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" thickBot="1">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1">
+    <row r="42" spans="1:3" ht="15.75" thickBot="1">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -7287,7 +7306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -7298,17 +7317,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="26.25" thickBot="1">
+    <row r="45" spans="1:3" ht="39" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1">
+    <row r="46" spans="1:3" ht="15.75" thickBot="1">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -7319,7 +7338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="163" t="s">
         <v>62</v>
       </c>
@@ -7330,24 +7349,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1">
+    <row r="48" spans="1:3" ht="15.75" thickBot="1">
       <c r="A48" s="164"/>
       <c r="B48" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C48" s="164"/>
     </row>
-    <row r="49" spans="1:3" ht="15" thickBot="1">
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
       <c r="A49" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="26.25" thickBot="1">
+    <row r="50" spans="1:3" ht="39" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1">
+    <row r="51" spans="1:3" ht="15.75" thickBot="1">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
@@ -7358,7 +7377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="163" t="s">
         <v>62</v>
       </c>
@@ -7369,24 +7388,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1">
+    <row r="53" spans="1:3" ht="15.75" thickBot="1">
       <c r="A53" s="164"/>
       <c r="B53" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C53" s="164"/>
     </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1">
+    <row r="54" spans="1:3" ht="15.75" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" thickBot="1">
+    <row r="55" spans="1:3" ht="26.25" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1">
+    <row r="56" spans="1:3" ht="15.75" thickBot="1">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -7397,7 +7416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="163" t="s">
         <v>62</v>
       </c>
@@ -7408,7 +7427,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" thickBot="1">
+    <row r="58" spans="1:3" ht="15.75" thickBot="1">
       <c r="A58" s="164"/>
       <c r="B58" s="6" t="s">
         <v>79</v>
@@ -7417,12 +7436,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A33:A34"/>
@@ -7431,6 +7444,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7439,28 +7458,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:BX117"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
     <col min="33" max="38" width="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.25" customWidth="1"/>
+    <col min="45" max="45" width="5.28515625" customWidth="1"/>
     <col min="46" max="47" width="4" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="5.375" customWidth="1"/>
+    <col min="61" max="61" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:48">
@@ -7468,7 +7487,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="4:48" ht="14.25" thickBot="1">
+    <row r="4" spans="4:48" ht="15.75" thickBot="1">
       <c r="Z4">
         <v>800</v>
       </c>
@@ -7565,7 +7584,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="4:48" ht="14.25" thickBot="1">
+    <row r="8" spans="4:48" ht="15.75" thickBot="1">
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -7941,7 +7960,7 @@
       <c r="AU16" s="12"/>
       <c r="AV16" s="20"/>
     </row>
-    <row r="17" spans="3:48" ht="14.25" thickBot="1">
+    <row r="17" spans="3:48" ht="15.75" thickBot="1">
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -8154,7 +8173,7 @@
       <c r="AU21" s="22"/>
       <c r="AV21" s="23"/>
     </row>
-    <row r="22" spans="3:48" ht="14.25" thickBot="1">
+    <row r="22" spans="3:48" ht="15.75" thickBot="1">
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -8411,7 +8430,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="3:49" ht="14.25" thickBot="1"/>
+    <row r="38" spans="3:49" ht="15.75" thickBot="1"/>
     <row r="39" spans="3:49">
       <c r="E39" s="24">
         <v>2000</v>
@@ -8756,7 +8775,7 @@
       <c r="AV46" s="12"/>
       <c r="AW46" s="13"/>
     </row>
-    <row r="47" spans="3:49" ht="14.25" thickBot="1">
+    <row r="47" spans="3:49" ht="15.75" thickBot="1">
       <c r="E47" s="14"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
@@ -9138,7 +9157,7 @@
       <c r="AV55" s="12"/>
       <c r="AW55" s="13"/>
     </row>
-    <row r="56" spans="5:49" ht="14.25" thickBot="1">
+    <row r="56" spans="5:49" ht="15.75" thickBot="1">
       <c r="E56" s="14"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
@@ -9185,7 +9204,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="5:49" ht="14.25" thickBot="1"/>
+    <row r="60" spans="5:49" ht="15.75" thickBot="1"/>
     <row r="61" spans="5:49">
       <c r="AD61" s="8"/>
       <c r="AE61" s="9"/>
@@ -9364,7 +9383,7 @@
       <c r="AV68" s="12"/>
       <c r="AW68" s="13"/>
     </row>
-    <row r="69" spans="30:49" ht="14.25" thickBot="1">
+    <row r="69" spans="30:49" ht="15.75" thickBot="1">
       <c r="AD69" s="14"/>
       <c r="AE69" s="15"/>
       <c r="AF69" s="15"/>
@@ -9562,7 +9581,7 @@
       <c r="AV77" s="12"/>
       <c r="AW77" s="13"/>
     </row>
-    <row r="78" spans="30:49" ht="14.25" thickBot="1">
+    <row r="78" spans="30:49" ht="15.75" thickBot="1">
       <c r="AD78" s="14"/>
       <c r="AE78" s="15"/>
       <c r="AF78" s="15"/>
@@ -9600,7 +9619,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="6:76" ht="14.25" thickBot="1">
+    <row r="83" spans="6:76" ht="15.75" thickBot="1">
       <c r="O83">
         <v>128</v>
       </c>
@@ -10702,7 +10721,7 @@
       <c r="BW99" s="12"/>
       <c r="BX99" s="13"/>
     </row>
-    <row r="100" spans="7:76" ht="14.25" thickBot="1">
+    <row r="100" spans="7:76" ht="15.75" thickBot="1">
       <c r="G100" s="14"/>
       <c r="H100" s="15"/>
       <c r="I100" s="15"/>
@@ -11856,7 +11875,7 @@
       <c r="BW116" s="12"/>
       <c r="BX116" s="13"/>
     </row>
-    <row r="117" spans="7:76" ht="14.25" thickBot="1">
+    <row r="117" spans="7:76" ht="15.75" thickBot="1">
       <c r="G117" s="14"/>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
@@ -11930,42 +11949,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:CF167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A125" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="4.875" customWidth="1"/>
-    <col min="5" max="5" width="4.75" customWidth="1"/>
-    <col min="9" max="9" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.125" customWidth="1"/>
-    <col min="36" max="36" width="4.25" customWidth="1"/>
-    <col min="38" max="38" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.625" customWidth="1"/>
-    <col min="47" max="47" width="2.625" customWidth="1"/>
-    <col min="48" max="48" width="4.875" customWidth="1"/>
-    <col min="49" max="49" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4.125" customWidth="1"/>
-    <col min="52" max="53" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.140625" customWidth="1"/>
+    <col min="36" max="36" width="4.28515625" customWidth="1"/>
+    <col min="38" max="38" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.5703125" customWidth="1"/>
+    <col min="47" max="47" width="2.5703125" customWidth="1"/>
+    <col min="48" max="48" width="4.85546875" customWidth="1"/>
+    <col min="49" max="49" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="4.140625" customWidth="1"/>
+    <col min="52" max="53" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="4" customWidth="1"/>
-    <col min="69" max="69" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="3.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
@@ -11973,7 +11992,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="10:84" s="27" customFormat="1" ht="42">
+    <row r="32" spans="10:84" s="27" customFormat="1" ht="46.5">
       <c r="J32" s="27">
         <v>0</v>
       </c>
@@ -12187,62 +12206,62 @@
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="165" t="s">
+      <c r="K33" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="165"/>
-      <c r="M33" s="165" t="s">
+      <c r="L33" s="167"/>
+      <c r="M33" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="N33" s="165"/>
-      <c r="O33" s="165" t="s">
+      <c r="N33" s="167"/>
+      <c r="O33" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="P33" s="165"/>
-      <c r="Q33" s="165" t="s">
+      <c r="P33" s="167"/>
+      <c r="Q33" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="165"/>
-      <c r="S33" s="165" t="s">
+      <c r="R33" s="167"/>
+      <c r="S33" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="T33" s="165"/>
-      <c r="U33" s="165" t="s">
+      <c r="T33" s="167"/>
+      <c r="U33" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="V33" s="165"/>
-      <c r="W33" s="165" t="s">
+      <c r="V33" s="167"/>
+      <c r="W33" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="X33" s="165"/>
-      <c r="Y33" s="165" t="s">
+      <c r="X33" s="167"/>
+      <c r="Y33" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="Z33" s="165"/>
-      <c r="AA33" s="165" t="s">
+      <c r="Z33" s="167"/>
+      <c r="AA33" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AB33" s="165"/>
+      <c r="AB33" s="167"/>
       <c r="AD33" s="35"/>
       <c r="AE33" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG33" s="165" t="s">
+      <c r="AG33" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AH33" s="165"/>
-      <c r="AI33" s="165" t="s">
+      <c r="AH33" s="167"/>
+      <c r="AI33" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AJ33" s="165"/>
-      <c r="AK33" s="165" t="s">
+      <c r="AJ33" s="167"/>
+      <c r="AK33" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AL33" s="165"/>
-      <c r="AM33" s="165" t="s">
+      <c r="AL33" s="167"/>
+      <c r="AM33" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AN33" s="165"/>
+      <c r="AN33" s="167"/>
       <c r="AO33" s="34"/>
       <c r="AP33" s="34"/>
       <c r="AQ33" s="34"/>
@@ -12265,104 +12284,104 @@
       <c r="BL33" s="34"/>
       <c r="BM33" s="34"/>
       <c r="BN33" s="34"/>
-      <c r="BO33" s="167" t="s">
+      <c r="BO33" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BP33" s="168"/>
-      <c r="BQ33" s="167" t="s">
+      <c r="BP33" s="166"/>
+      <c r="BQ33" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BR33" s="168"/>
-      <c r="BS33" s="167" t="s">
+      <c r="BR33" s="166"/>
+      <c r="BS33" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BT33" s="168"/>
-      <c r="BU33" s="167" t="s">
+      <c r="BT33" s="166"/>
+      <c r="BU33" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BV33" s="168"/>
-      <c r="BW33" s="167" t="s">
+      <c r="BV33" s="166"/>
+      <c r="BW33" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BX33" s="168"/>
-      <c r="BY33" s="167" t="s">
+      <c r="BX33" s="166"/>
+      <c r="BY33" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BZ33" s="168"/>
-      <c r="CA33" s="167" t="s">
+      <c r="BZ33" s="166"/>
+      <c r="CA33" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="CB33" s="168"/>
-      <c r="CC33" s="167" t="s">
+      <c r="CB33" s="166"/>
+      <c r="CC33" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="CD33" s="168"/>
-      <c r="CE33" s="167" t="s">
+      <c r="CD33" s="166"/>
+      <c r="CE33" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CF33" s="168"/>
+      <c r="CF33" s="166"/>
     </row>
     <row r="34" spans="6:84">
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="34"/>
-      <c r="K34" s="165" t="s">
+      <c r="K34" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="165"/>
-      <c r="M34" s="165" t="s">
+      <c r="L34" s="167"/>
+      <c r="M34" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="165"/>
-      <c r="O34" s="165" t="s">
+      <c r="N34" s="167"/>
+      <c r="O34" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="P34" s="165"/>
-      <c r="Q34" s="165" t="s">
+      <c r="P34" s="167"/>
+      <c r="Q34" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="165"/>
-      <c r="S34" s="165" t="s">
+      <c r="R34" s="167"/>
+      <c r="S34" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="165"/>
-      <c r="U34" s="165" t="s">
+      <c r="T34" s="167"/>
+      <c r="U34" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="V34" s="165"/>
-      <c r="W34" s="165" t="s">
+      <c r="V34" s="167"/>
+      <c r="W34" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="X34" s="165"/>
-      <c r="Y34" s="165" t="s">
+      <c r="X34" s="167"/>
+      <c r="Y34" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="Z34" s="165"/>
-      <c r="AA34" s="165" t="s">
+      <c r="Z34" s="167"/>
+      <c r="AA34" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="165"/>
+      <c r="AB34" s="167"/>
       <c r="AD34" s="35"/>
       <c r="AE34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG34" s="165" t="s">
+      <c r="AG34" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AH34" s="165"/>
-      <c r="AI34" s="165" t="s">
+      <c r="AH34" s="167"/>
+      <c r="AI34" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AJ34" s="165"/>
-      <c r="AK34" s="165" t="s">
+      <c r="AJ34" s="167"/>
+      <c r="AK34" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AL34" s="165"/>
-      <c r="AM34" s="165" t="s">
+      <c r="AL34" s="167"/>
+      <c r="AM34" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AN34" s="165"/>
+      <c r="AN34" s="167"/>
       <c r="AO34" s="34"/>
       <c r="AP34" s="34"/>
       <c r="AQ34" s="34"/>
@@ -12385,42 +12404,42 @@
       <c r="BL34" s="34"/>
       <c r="BM34" s="34"/>
       <c r="BN34" s="34"/>
-      <c r="BO34" s="167" t="s">
+      <c r="BO34" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BP34" s="168"/>
-      <c r="BQ34" s="167" t="s">
+      <c r="BP34" s="166"/>
+      <c r="BQ34" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BR34" s="168"/>
-      <c r="BS34" s="167" t="s">
+      <c r="BR34" s="166"/>
+      <c r="BS34" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BT34" s="168"/>
-      <c r="BU34" s="167" t="s">
+      <c r="BT34" s="166"/>
+      <c r="BU34" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BV34" s="168"/>
-      <c r="BW34" s="167" t="s">
+      <c r="BV34" s="166"/>
+      <c r="BW34" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BX34" s="168"/>
-      <c r="BY34" s="167" t="s">
+      <c r="BX34" s="166"/>
+      <c r="BY34" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BZ34" s="168"/>
-      <c r="CA34" s="167" t="s">
+      <c r="BZ34" s="166"/>
+      <c r="CA34" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="CB34" s="168"/>
-      <c r="CC34" s="167" t="s">
+      <c r="CB34" s="166"/>
+      <c r="CC34" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="CD34" s="168"/>
-      <c r="CE34" s="167" t="s">
+      <c r="CD34" s="166"/>
+      <c r="CE34" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CF34" s="168"/>
+      <c r="CF34" s="166"/>
     </row>
     <row r="35" spans="6:84">
       <c r="CB35" s="27"/>
@@ -12434,62 +12453,62 @@
         <v>239</v>
       </c>
       <c r="J36" s="36"/>
-      <c r="K36" s="166" t="s">
+      <c r="K36" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="L36" s="166"/>
-      <c r="M36" s="166" t="s">
+      <c r="L36" s="172"/>
+      <c r="M36" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="N36" s="166"/>
-      <c r="O36" s="166" t="s">
+      <c r="N36" s="172"/>
+      <c r="O36" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="P36" s="166"/>
-      <c r="Q36" s="166" t="s">
+      <c r="P36" s="172"/>
+      <c r="Q36" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="R36" s="166"/>
-      <c r="S36" s="166" t="s">
+      <c r="R36" s="172"/>
+      <c r="S36" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="T36" s="166"/>
-      <c r="U36" s="166" t="s">
+      <c r="T36" s="172"/>
+      <c r="U36" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="V36" s="166"/>
-      <c r="W36" s="166" t="s">
+      <c r="V36" s="172"/>
+      <c r="W36" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="X36" s="166"/>
-      <c r="Y36" s="166" t="s">
+      <c r="X36" s="172"/>
+      <c r="Y36" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="Z36" s="166"/>
-      <c r="AA36" s="166" t="s">
+      <c r="Z36" s="172"/>
+      <c r="AA36" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="AB36" s="166"/>
+      <c r="AB36" s="172"/>
       <c r="AD36" s="37"/>
       <c r="AE36" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AG36" s="166" t="s">
+      <c r="AG36" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="AH36" s="166"/>
-      <c r="AI36" s="166" t="s">
+      <c r="AH36" s="172"/>
+      <c r="AI36" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="AJ36" s="166"/>
-      <c r="AK36" s="166" t="s">
+      <c r="AJ36" s="172"/>
+      <c r="AK36" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="AL36" s="166"/>
-      <c r="AM36" s="166" t="s">
+      <c r="AL36" s="172"/>
+      <c r="AM36" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="AN36" s="166"/>
+      <c r="AN36" s="172"/>
       <c r="AO36" s="36"/>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -12512,42 +12531,42 @@
       <c r="BL36" s="34"/>
       <c r="BM36" s="34"/>
       <c r="BN36" s="34"/>
-      <c r="BO36" s="167" t="s">
+      <c r="BO36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BP36" s="168"/>
-      <c r="BQ36" s="167" t="s">
+      <c r="BP36" s="166"/>
+      <c r="BQ36" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BR36" s="168"/>
-      <c r="BS36" s="167" t="s">
+      <c r="BR36" s="166"/>
+      <c r="BS36" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BT36" s="168"/>
-      <c r="BU36" s="167" t="s">
+      <c r="BT36" s="166"/>
+      <c r="BU36" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BV36" s="168"/>
-      <c r="BW36" s="167" t="s">
+      <c r="BV36" s="166"/>
+      <c r="BW36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BX36" s="168"/>
-      <c r="BY36" s="167" t="s">
+      <c r="BX36" s="166"/>
+      <c r="BY36" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BZ36" s="168"/>
-      <c r="CA36" s="167" t="s">
+      <c r="BZ36" s="166"/>
+      <c r="CA36" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="CB36" s="168"/>
-      <c r="CC36" s="167" t="s">
+      <c r="CB36" s="166"/>
+      <c r="CC36" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="CD36" s="168"/>
-      <c r="CE36" s="167" t="s">
+      <c r="CD36" s="166"/>
+      <c r="CE36" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CF36" s="168"/>
+      <c r="CF36" s="166"/>
     </row>
     <row r="37" spans="6:84">
       <c r="I37">
@@ -12883,58 +12902,58 @@
       <c r="J42" s="38"/>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
-      <c r="M42" s="165" t="s">
+      <c r="M42" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="N42" s="165"/>
-      <c r="O42" s="165" t="s">
+      <c r="N42" s="167"/>
+      <c r="O42" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="P42" s="165"/>
-      <c r="Q42" s="165" t="s">
+      <c r="P42" s="167"/>
+      <c r="Q42" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="R42" s="165"/>
-      <c r="S42" s="165" t="s">
+      <c r="R42" s="167"/>
+      <c r="S42" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="T42" s="165"/>
-      <c r="U42" s="165" t="s">
+      <c r="T42" s="167"/>
+      <c r="U42" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="V42" s="165"/>
-      <c r="W42" s="165" t="s">
+      <c r="V42" s="167"/>
+      <c r="W42" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="X42" s="165"/>
-      <c r="Y42" s="165" t="s">
+      <c r="X42" s="167"/>
+      <c r="Y42" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="Z42" s="165"/>
-      <c r="AA42" s="165" t="s">
+      <c r="Z42" s="167"/>
+      <c r="AA42" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AB42" s="165"/>
+      <c r="AB42" s="167"/>
       <c r="AD42" s="35"/>
       <c r="AE42" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AG42" s="165" t="s">
+      <c r="AG42" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AH42" s="165"/>
-      <c r="AI42" s="165" t="s">
+      <c r="AH42" s="167"/>
+      <c r="AI42" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AJ42" s="165"/>
-      <c r="AK42" s="165" t="s">
+      <c r="AJ42" s="167"/>
+      <c r="AK42" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AL42" s="165"/>
-      <c r="AM42" s="165" t="s">
+      <c r="AL42" s="167"/>
+      <c r="AM42" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AN42" s="165"/>
+      <c r="AN42" s="167"/>
       <c r="AO42" s="34"/>
       <c r="AP42" s="34"/>
       <c r="AQ42" s="34"/>
@@ -12957,42 +12976,42 @@
       <c r="BL42" s="34"/>
       <c r="BM42" s="34"/>
       <c r="BN42" s="34"/>
-      <c r="BO42" s="167" t="s">
+      <c r="BO42" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BP42" s="168"/>
-      <c r="BQ42" s="167" t="s">
+      <c r="BP42" s="166"/>
+      <c r="BQ42" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BR42" s="168"/>
-      <c r="BS42" s="167" t="s">
+      <c r="BR42" s="166"/>
+      <c r="BS42" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BT42" s="168"/>
-      <c r="BU42" s="167" t="s">
+      <c r="BT42" s="166"/>
+      <c r="BU42" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BV42" s="168"/>
-      <c r="BW42" s="167" t="s">
+      <c r="BV42" s="166"/>
+      <c r="BW42" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BX42" s="168"/>
-      <c r="BY42" s="167" t="s">
+      <c r="BX42" s="166"/>
+      <c r="BY42" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BZ42" s="168"/>
-      <c r="CA42" s="167" t="s">
+      <c r="BZ42" s="166"/>
+      <c r="CA42" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="CB42" s="168"/>
-      <c r="CC42" s="167" t="s">
+      <c r="CB42" s="166"/>
+      <c r="CC42" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="CD42" s="168"/>
-      <c r="CE42" s="167" t="s">
+      <c r="CD42" s="166"/>
+      <c r="CE42" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CF42" s="168"/>
+      <c r="CF42" s="166"/>
     </row>
     <row r="43" spans="6:84">
       <c r="CB43" s="27"/>
@@ -13025,71 +13044,71 @@
         <v>120</v>
       </c>
       <c r="J46" s="34"/>
-      <c r="K46" s="172" t="s">
+      <c r="K46" s="171" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="172"/>
-      <c r="M46" s="172"/>
-      <c r="N46" s="172"/>
-      <c r="O46" s="172"/>
-      <c r="P46" s="172"/>
-      <c r="Q46" s="172"/>
-      <c r="R46" s="172"/>
-      <c r="S46" s="172"/>
-      <c r="T46" s="172"/>
-      <c r="U46" s="172"/>
-      <c r="V46" s="172"/>
-      <c r="W46" s="172"/>
-      <c r="X46" s="172"/>
-      <c r="Y46" s="172"/>
-      <c r="Z46" s="172"/>
-      <c r="AA46" s="172"/>
-      <c r="AB46" s="172"/>
-      <c r="AC46" s="172"/>
-      <c r="AD46" s="172"/>
-      <c r="AE46" s="172" t="s">
+      <c r="L46" s="171"/>
+      <c r="M46" s="171"/>
+      <c r="N46" s="171"/>
+      <c r="O46" s="171"/>
+      <c r="P46" s="171"/>
+      <c r="Q46" s="171"/>
+      <c r="R46" s="171"/>
+      <c r="S46" s="171"/>
+      <c r="T46" s="171"/>
+      <c r="U46" s="171"/>
+      <c r="V46" s="171"/>
+      <c r="W46" s="171"/>
+      <c r="X46" s="171"/>
+      <c r="Y46" s="171"/>
+      <c r="Z46" s="171"/>
+      <c r="AA46" s="171"/>
+      <c r="AB46" s="171"/>
+      <c r="AC46" s="171"/>
+      <c r="AD46" s="171"/>
+      <c r="AE46" s="171" t="s">
         <v>116</v>
       </c>
-      <c r="AF46" s="172"/>
-      <c r="AG46" s="172"/>
-      <c r="AH46" s="172"/>
-      <c r="AI46" s="172"/>
-      <c r="AJ46" s="172"/>
-      <c r="AK46" s="172"/>
-      <c r="AL46" s="172"/>
-      <c r="AM46" s="172"/>
-      <c r="AN46" s="172"/>
-      <c r="AO46" s="165" t="s">
+      <c r="AF46" s="171"/>
+      <c r="AG46" s="171"/>
+      <c r="AH46" s="171"/>
+      <c r="AI46" s="171"/>
+      <c r="AJ46" s="171"/>
+      <c r="AK46" s="171"/>
+      <c r="AL46" s="171"/>
+      <c r="AM46" s="171"/>
+      <c r="AN46" s="171"/>
+      <c r="AO46" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AP46" s="165"/>
-      <c r="AQ46" s="165" t="s">
+      <c r="AP46" s="167"/>
+      <c r="AQ46" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AR46" s="165"/>
-      <c r="AS46" s="165" t="s">
+      <c r="AR46" s="167"/>
+      <c r="AS46" s="167" t="s">
         <v>117</v>
       </c>
-      <c r="AT46" s="165"/>
-      <c r="AU46" s="165" t="s">
+      <c r="AT46" s="167"/>
+      <c r="AU46" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="AV46" s="165"/>
-      <c r="AW46" s="169" t="s">
+      <c r="AV46" s="167"/>
+      <c r="AW46" s="168" t="s">
         <v>119</v>
       </c>
-      <c r="AX46" s="170"/>
-      <c r="AY46" s="170"/>
-      <c r="AZ46" s="170"/>
-      <c r="BA46" s="170"/>
-      <c r="BB46" s="170"/>
-      <c r="BC46" s="170"/>
-      <c r="BD46" s="170"/>
-      <c r="BE46" s="171"/>
-      <c r="BF46" s="165" t="s">
+      <c r="AX46" s="169"/>
+      <c r="AY46" s="169"/>
+      <c r="AZ46" s="169"/>
+      <c r="BA46" s="169"/>
+      <c r="BB46" s="169"/>
+      <c r="BC46" s="169"/>
+      <c r="BD46" s="169"/>
+      <c r="BE46" s="170"/>
+      <c r="BF46" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="BG46" s="165"/>
+      <c r="BG46" s="167"/>
       <c r="BI46" s="38"/>
       <c r="BJ46" s="38"/>
       <c r="BK46" s="38"/>
@@ -13143,7 +13162,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="5:71" ht="14.25" thickBot="1">
+    <row r="52" spans="5:71" ht="15.75" thickBot="1">
       <c r="E52" t="s">
         <v>108</v>
       </c>
@@ -13885,7 +13904,7 @@
       <c r="BP63" s="12"/>
       <c r="BQ63" s="20"/>
     </row>
-    <row r="64" spans="5:71" ht="14.25" thickBot="1">
+    <row r="64" spans="5:71" ht="15.75" thickBot="1">
       <c r="F64" s="11"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -14552,7 +14571,7 @@
       <c r="AU76" s="12"/>
       <c r="AV76" s="20"/>
     </row>
-    <row r="77" spans="5:69" ht="14.25" thickBot="1">
+    <row r="77" spans="5:69" ht="15.75" thickBot="1">
       <c r="E77">
         <v>480</v>
       </c>
@@ -15067,7 +15086,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="90" spans="4:48" ht="14.25" thickBot="1">
+    <row r="90" spans="4:48" ht="15.75" thickBot="1">
       <c r="E90" t="s">
         <v>109</v>
       </c>
@@ -16170,7 +16189,7 @@
       <c r="AU114" s="12"/>
       <c r="AV114" s="20"/>
     </row>
-    <row r="115" spans="4:48" ht="14.25" thickBot="1">
+    <row r="115" spans="4:48" ht="15.75" thickBot="1">
       <c r="D115">
         <v>240</v>
       </c>
@@ -16691,7 +16710,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="131" spans="4:48" ht="14.25" thickBot="1">
+    <row r="131" spans="4:48" ht="15.75" thickBot="1">
       <c r="F131">
         <v>0</v>
       </c>
@@ -17796,7 +17815,7 @@
       <c r="AU155" s="12"/>
       <c r="AV155" s="20"/>
     </row>
-    <row r="156" spans="4:48" ht="14.25" thickBot="1">
+    <row r="156" spans="4:48" ht="15.75" thickBot="1">
       <c r="D156">
         <v>240</v>
       </c>
@@ -18317,20 +18336,71 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="BQ42:BR42"/>
-    <mergeCell ref="BS42:BT42"/>
-    <mergeCell ref="BU42:BV42"/>
-    <mergeCell ref="BW42:BX42"/>
-    <mergeCell ref="CE33:CF33"/>
-    <mergeCell ref="CE34:CF34"/>
-    <mergeCell ref="CE36:CF36"/>
-    <mergeCell ref="CE42:CF42"/>
-    <mergeCell ref="BY42:BZ42"/>
-    <mergeCell ref="CA42:CB42"/>
-    <mergeCell ref="CC42:CD42"/>
-    <mergeCell ref="CA36:CB36"/>
-    <mergeCell ref="CC36:CD36"/>
-    <mergeCell ref="BY36:BZ36"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AG34:AH34"/>
+    <mergeCell ref="AI34:AJ34"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W36:X36"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="BW36:BX36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AI36:AJ36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AG42:AH42"/>
+    <mergeCell ref="AI42:AJ42"/>
+    <mergeCell ref="AK42:AL42"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="BO36:BP36"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BS36:BT36"/>
+    <mergeCell ref="BU36:BV36"/>
+    <mergeCell ref="BO42:BP42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="AS46:AT46"/>
+    <mergeCell ref="AU46:AV46"/>
+    <mergeCell ref="BF46:BG46"/>
+    <mergeCell ref="AW46:BE46"/>
+    <mergeCell ref="K46:AD46"/>
+    <mergeCell ref="AE46:AN46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AQ46:AR46"/>
     <mergeCell ref="BO33:BP33"/>
     <mergeCell ref="BO34:BP34"/>
     <mergeCell ref="CA33:CB33"/>
@@ -18347,71 +18417,20 @@
     <mergeCell ref="BY34:BZ34"/>
     <mergeCell ref="CA34:CB34"/>
     <mergeCell ref="CC34:CD34"/>
-    <mergeCell ref="AS46:AT46"/>
-    <mergeCell ref="AU46:AV46"/>
-    <mergeCell ref="BF46:BG46"/>
-    <mergeCell ref="AW46:BE46"/>
-    <mergeCell ref="K46:AD46"/>
-    <mergeCell ref="AE46:AN46"/>
-    <mergeCell ref="AO46:AP46"/>
-    <mergeCell ref="AQ46:AR46"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="BW36:BX36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AM36:AN36"/>
-    <mergeCell ref="AI36:AJ36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AG42:AH42"/>
-    <mergeCell ref="AI42:AJ42"/>
-    <mergeCell ref="AK42:AL42"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="BO36:BP36"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BS36:BT36"/>
-    <mergeCell ref="BU36:BV36"/>
-    <mergeCell ref="BO42:BP42"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AG36:AH36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AM33:AN33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AG34:AH34"/>
-    <mergeCell ref="AI34:AJ34"/>
-    <mergeCell ref="AK34:AL34"/>
-    <mergeCell ref="AM34:AN34"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="BQ42:BR42"/>
+    <mergeCell ref="BS42:BT42"/>
+    <mergeCell ref="BU42:BV42"/>
+    <mergeCell ref="BW42:BX42"/>
+    <mergeCell ref="CE33:CF33"/>
+    <mergeCell ref="CE34:CF34"/>
+    <mergeCell ref="CE36:CF36"/>
+    <mergeCell ref="CE42:CF42"/>
+    <mergeCell ref="BY42:BZ42"/>
+    <mergeCell ref="CA42:CB42"/>
+    <mergeCell ref="CC42:CD42"/>
+    <mergeCell ref="CA36:CB36"/>
+    <mergeCell ref="CC36:CD36"/>
+    <mergeCell ref="BY36:BZ36"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18421,18 +18440,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:EC90"/>
   <sheetViews>
     <sheetView topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="X82" sqref="X82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="17" max="17" width="2.625" customWidth="1"/>
-    <col min="33" max="33" width="2.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.625" customWidth="1"/>
+    <col min="17" max="17" width="2.5703125" customWidth="1"/>
+    <col min="33" max="33" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="9:49">
@@ -19299,7 +19318,7 @@
       <c r="AY45" s="174"/>
       <c r="AZ45" s="175"/>
     </row>
-    <row r="46" spans="1:133" ht="42">
+    <row r="46" spans="1:133" ht="46.5">
       <c r="A46" t="s">
         <v>422</v>
       </c>
@@ -19692,262 +19711,262 @@
       </c>
     </row>
     <row r="47" spans="1:133">
-      <c r="F47" s="165" t="s">
+      <c r="F47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="165"/>
-      <c r="H47" s="165" t="s">
+      <c r="G47" s="167"/>
+      <c r="H47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="I47" s="165"/>
-      <c r="J47" s="165" t="s">
+      <c r="I47" s="167"/>
+      <c r="J47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="K47" s="165"/>
-      <c r="L47" s="165" t="s">
+      <c r="K47" s="167"/>
+      <c r="L47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="M47" s="165"/>
-      <c r="N47" s="165" t="s">
+      <c r="M47" s="167"/>
+      <c r="N47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="O47" s="165"/>
-      <c r="P47" s="165" t="s">
+      <c r="O47" s="167"/>
+      <c r="P47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="Q47" s="165"/>
-      <c r="R47" s="165" t="s">
+      <c r="Q47" s="167"/>
+      <c r="R47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="S47" s="165"/>
-      <c r="T47" s="165" t="s">
+      <c r="S47" s="167"/>
+      <c r="T47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="U47" s="165"/>
-      <c r="V47" s="165" t="s">
+      <c r="U47" s="167"/>
+      <c r="V47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="W47" s="165"/>
-      <c r="X47" s="165" t="s">
+      <c r="W47" s="167"/>
+      <c r="X47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="Y47" s="165"/>
-      <c r="Z47" s="165" t="s">
+      <c r="Y47" s="167"/>
+      <c r="Z47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AA47" s="165"/>
-      <c r="AB47" s="165" t="s">
+      <c r="AA47" s="167"/>
+      <c r="AB47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AC47" s="165"/>
-      <c r="AD47" s="165" t="s">
+      <c r="AC47" s="167"/>
+      <c r="AD47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AE47" s="165"/>
-      <c r="AF47" s="165" t="s">
+      <c r="AE47" s="167"/>
+      <c r="AF47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AG47" s="165"/>
-      <c r="AH47" s="165" t="s">
+      <c r="AG47" s="167"/>
+      <c r="AH47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AI47" s="165"/>
-      <c r="AJ47" s="165" t="s">
+      <c r="AI47" s="167"/>
+      <c r="AJ47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AK47" s="165"/>
-      <c r="AL47" s="165" t="s">
+      <c r="AK47" s="167"/>
+      <c r="AL47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AM47" s="165"/>
-      <c r="AN47" s="165" t="s">
+      <c r="AM47" s="167"/>
+      <c r="AN47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AO47" s="165"/>
-      <c r="AP47" s="165" t="s">
+      <c r="AO47" s="167"/>
+      <c r="AP47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AQ47" s="165"/>
-      <c r="AR47" s="165" t="s">
+      <c r="AQ47" s="167"/>
+      <c r="AR47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AS47" s="165"/>
-      <c r="AT47" s="165" t="s">
+      <c r="AS47" s="167"/>
+      <c r="AT47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AU47" s="165"/>
-      <c r="AV47" s="165" t="s">
+      <c r="AU47" s="167"/>
+      <c r="AV47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AW47" s="165"/>
-      <c r="AX47" s="165" t="s">
+      <c r="AW47" s="167"/>
+      <c r="AX47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AY47" s="165"/>
-      <c r="AZ47" s="165" t="s">
+      <c r="AY47" s="167"/>
+      <c r="AZ47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="BA47" s="165"/>
-      <c r="BB47" s="165" t="s">
+      <c r="BA47" s="167"/>
+      <c r="BB47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="BC47" s="165"/>
-      <c r="BD47" s="165" t="s">
+      <c r="BC47" s="167"/>
+      <c r="BD47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="BE47" s="165"/>
-      <c r="BF47" s="165" t="s">
+      <c r="BE47" s="167"/>
+      <c r="BF47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="BG47" s="165"/>
-      <c r="BH47" s="165" t="s">
+      <c r="BG47" s="167"/>
+      <c r="BH47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="BI47" s="165"/>
-      <c r="BJ47" s="165" t="s">
+      <c r="BI47" s="167"/>
+      <c r="BJ47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="BK47" s="165"/>
-      <c r="BL47" s="165" t="s">
+      <c r="BK47" s="167"/>
+      <c r="BL47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="BM47" s="165"/>
-      <c r="BN47" s="165" t="s">
+      <c r="BM47" s="167"/>
+      <c r="BN47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="BO47" s="165"/>
-      <c r="BP47" s="165" t="s">
+      <c r="BO47" s="167"/>
+      <c r="BP47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="BQ47" s="165"/>
-      <c r="BR47" s="165" t="s">
+      <c r="BQ47" s="167"/>
+      <c r="BR47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="BS47" s="165"/>
-      <c r="BT47" s="165" t="s">
+      <c r="BS47" s="167"/>
+      <c r="BT47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="BU47" s="165"/>
-      <c r="BV47" s="165" t="s">
+      <c r="BU47" s="167"/>
+      <c r="BV47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="BW47" s="165"/>
-      <c r="BX47" s="165" t="s">
+      <c r="BW47" s="167"/>
+      <c r="BX47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="BY47" s="165"/>
-      <c r="BZ47" s="165" t="s">
+      <c r="BY47" s="167"/>
+      <c r="BZ47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="CA47" s="165"/>
-      <c r="CB47" s="165" t="s">
+      <c r="CA47" s="167"/>
+      <c r="CB47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="CC47" s="165"/>
-      <c r="CD47" s="165" t="s">
+      <c r="CC47" s="167"/>
+      <c r="CD47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="CE47" s="165"/>
-      <c r="CF47" s="165" t="s">
+      <c r="CE47" s="167"/>
+      <c r="CF47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="CG47" s="165"/>
-      <c r="CH47" s="165" t="s">
+      <c r="CG47" s="167"/>
+      <c r="CH47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="CI47" s="165"/>
-      <c r="CJ47" s="165" t="s">
+      <c r="CI47" s="167"/>
+      <c r="CJ47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="CK47" s="165"/>
-      <c r="CL47" s="165" t="s">
+      <c r="CK47" s="167"/>
+      <c r="CL47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="CM47" s="165"/>
-      <c r="CN47" s="165" t="s">
+      <c r="CM47" s="167"/>
+      <c r="CN47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="CO47" s="165"/>
-      <c r="CP47" s="165" t="s">
+      <c r="CO47" s="167"/>
+      <c r="CP47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="CQ47" s="165"/>
-      <c r="CR47" s="165" t="s">
+      <c r="CQ47" s="167"/>
+      <c r="CR47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="CS47" s="165"/>
-      <c r="CT47" s="165" t="s">
+      <c r="CS47" s="167"/>
+      <c r="CT47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="CU47" s="165"/>
-      <c r="CV47" s="165" t="s">
+      <c r="CU47" s="167"/>
+      <c r="CV47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="CW47" s="165"/>
-      <c r="CX47" s="165" t="s">
+      <c r="CW47" s="167"/>
+      <c r="CX47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="CY47" s="165"/>
-      <c r="CZ47" s="165" t="s">
+      <c r="CY47" s="167"/>
+      <c r="CZ47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="DA47" s="165"/>
-      <c r="DB47" s="165" t="s">
+      <c r="DA47" s="167"/>
+      <c r="DB47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="DC47" s="165"/>
-      <c r="DD47" s="165" t="s">
+      <c r="DC47" s="167"/>
+      <c r="DD47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="DE47" s="165"/>
-      <c r="DF47" s="165" t="s">
+      <c r="DE47" s="167"/>
+      <c r="DF47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="DG47" s="165"/>
-      <c r="DH47" s="165" t="s">
+      <c r="DG47" s="167"/>
+      <c r="DH47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="DI47" s="165"/>
-      <c r="DJ47" s="165" t="s">
+      <c r="DI47" s="167"/>
+      <c r="DJ47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="DK47" s="165"/>
-      <c r="DL47" s="165" t="s">
+      <c r="DK47" s="167"/>
+      <c r="DL47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="DM47" s="165"/>
-      <c r="DN47" s="165" t="s">
+      <c r="DM47" s="167"/>
+      <c r="DN47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="DO47" s="165"/>
-      <c r="DP47" s="165" t="s">
+      <c r="DO47" s="167"/>
+      <c r="DP47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="DQ47" s="165"/>
-      <c r="DR47" s="165" t="s">
+      <c r="DQ47" s="167"/>
+      <c r="DR47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="DS47" s="165"/>
-      <c r="DT47" s="165" t="s">
+      <c r="DS47" s="167"/>
+      <c r="DT47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="DU47" s="165"/>
-      <c r="DV47" s="165" t="s">
+      <c r="DU47" s="167"/>
+      <c r="DV47" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="DW47" s="165"/>
-      <c r="DX47" s="165" t="s">
+      <c r="DW47" s="167"/>
+      <c r="DX47" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="DY47" s="165"/>
-      <c r="DZ47" s="165" t="s">
+      <c r="DY47" s="167"/>
+      <c r="DZ47" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="EA47" s="165"/>
-      <c r="EB47" s="165" t="s">
+      <c r="EA47" s="167"/>
+      <c r="EB47" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="EC47" s="165"/>
+      <c r="EC47" s="167"/>
     </row>
     <row r="49" spans="11:36">
       <c r="K49" t="s">
@@ -20349,6 +20368,57 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="AN47:AO47"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="AF47:AG47"/>
+    <mergeCell ref="AH47:AI47"/>
+    <mergeCell ref="AJ47:AK47"/>
+    <mergeCell ref="AL47:AM47"/>
+    <mergeCell ref="BL47:BM47"/>
+    <mergeCell ref="AP47:AQ47"/>
+    <mergeCell ref="AR47:AS47"/>
+    <mergeCell ref="AT47:AU47"/>
+    <mergeCell ref="AV47:AW47"/>
+    <mergeCell ref="AX47:AY47"/>
+    <mergeCell ref="AZ47:BA47"/>
+    <mergeCell ref="BB47:BC47"/>
+    <mergeCell ref="BD47:BE47"/>
+    <mergeCell ref="BF47:BG47"/>
+    <mergeCell ref="BH47:BI47"/>
+    <mergeCell ref="BJ47:BK47"/>
+    <mergeCell ref="CJ47:CK47"/>
+    <mergeCell ref="BN47:BO47"/>
+    <mergeCell ref="BP47:BQ47"/>
+    <mergeCell ref="BR47:BS47"/>
+    <mergeCell ref="BT47:BU47"/>
+    <mergeCell ref="BV47:BW47"/>
+    <mergeCell ref="BX47:BY47"/>
+    <mergeCell ref="BZ47:CA47"/>
+    <mergeCell ref="CB47:CC47"/>
+    <mergeCell ref="CD47:CE47"/>
+    <mergeCell ref="CF47:CG47"/>
+    <mergeCell ref="CH47:CI47"/>
+    <mergeCell ref="DD47:DE47"/>
+    <mergeCell ref="DF47:DG47"/>
+    <mergeCell ref="DH47:DI47"/>
+    <mergeCell ref="CL47:CM47"/>
+    <mergeCell ref="CN47:CO47"/>
+    <mergeCell ref="CP47:CQ47"/>
+    <mergeCell ref="CR47:CS47"/>
+    <mergeCell ref="CT47:CU47"/>
+    <mergeCell ref="CV47:CW47"/>
     <mergeCell ref="DV47:DW47"/>
     <mergeCell ref="DX47:DY47"/>
     <mergeCell ref="DZ47:EA47"/>
@@ -20365,57 +20435,6 @@
     <mergeCell ref="CX47:CY47"/>
     <mergeCell ref="CZ47:DA47"/>
     <mergeCell ref="DB47:DC47"/>
-    <mergeCell ref="DD47:DE47"/>
-    <mergeCell ref="DF47:DG47"/>
-    <mergeCell ref="DH47:DI47"/>
-    <mergeCell ref="CL47:CM47"/>
-    <mergeCell ref="CN47:CO47"/>
-    <mergeCell ref="CP47:CQ47"/>
-    <mergeCell ref="CR47:CS47"/>
-    <mergeCell ref="CT47:CU47"/>
-    <mergeCell ref="CV47:CW47"/>
-    <mergeCell ref="CJ47:CK47"/>
-    <mergeCell ref="BN47:BO47"/>
-    <mergeCell ref="BP47:BQ47"/>
-    <mergeCell ref="BR47:BS47"/>
-    <mergeCell ref="BT47:BU47"/>
-    <mergeCell ref="BV47:BW47"/>
-    <mergeCell ref="BX47:BY47"/>
-    <mergeCell ref="BZ47:CA47"/>
-    <mergeCell ref="CB47:CC47"/>
-    <mergeCell ref="CD47:CE47"/>
-    <mergeCell ref="CF47:CG47"/>
-    <mergeCell ref="CH47:CI47"/>
-    <mergeCell ref="BL47:BM47"/>
-    <mergeCell ref="AP47:AQ47"/>
-    <mergeCell ref="AR47:AS47"/>
-    <mergeCell ref="AT47:AU47"/>
-    <mergeCell ref="AV47:AW47"/>
-    <mergeCell ref="AX47:AY47"/>
-    <mergeCell ref="AZ47:BA47"/>
-    <mergeCell ref="BB47:BC47"/>
-    <mergeCell ref="BD47:BE47"/>
-    <mergeCell ref="BF47:BG47"/>
-    <mergeCell ref="BH47:BI47"/>
-    <mergeCell ref="BJ47:BK47"/>
-    <mergeCell ref="AN47:AO47"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="X47:Y47"/>
-    <mergeCell ref="Z47:AA47"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AD47:AE47"/>
-    <mergeCell ref="AF47:AG47"/>
-    <mergeCell ref="AH47:AI47"/>
-    <mergeCell ref="AJ47:AK47"/>
-    <mergeCell ref="AL47:AM47"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20425,19 +20444,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:CB37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AK37" sqref="AK37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:80" s="27" customFormat="1" ht="42">
+    <row r="2" spans="2:80" s="27" customFormat="1" ht="46.5">
       <c r="F2" s="27">
         <v>0</v>
       </c>
@@ -20651,62 +20670,62 @@
         <v>0</v>
       </c>
       <c r="F3" s="39"/>
-      <c r="G3" s="165" t="s">
+      <c r="G3" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165" t="s">
+      <c r="H3" s="167"/>
+      <c r="I3" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="165"/>
-      <c r="K3" s="165" t="s">
+      <c r="J3" s="167"/>
+      <c r="K3" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="165"/>
-      <c r="M3" s="165" t="s">
+      <c r="L3" s="167"/>
+      <c r="M3" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="165"/>
-      <c r="O3" s="165" t="s">
+      <c r="N3" s="167"/>
+      <c r="O3" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="165"/>
-      <c r="Q3" s="165" t="s">
+      <c r="P3" s="167"/>
+      <c r="Q3" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="165"/>
-      <c r="S3" s="165" t="s">
+      <c r="R3" s="167"/>
+      <c r="S3" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="165"/>
-      <c r="U3" s="165" t="s">
+      <c r="T3" s="167"/>
+      <c r="U3" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="V3" s="165"/>
-      <c r="W3" s="165" t="s">
+      <c r="V3" s="167"/>
+      <c r="W3" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="X3" s="165"/>
+      <c r="X3" s="167"/>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="165" t="s">
+      <c r="AC3" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="165"/>
-      <c r="AE3" s="165" t="s">
+      <c r="AD3" s="167"/>
+      <c r="AE3" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AF3" s="165"/>
-      <c r="AG3" s="165" t="s">
+      <c r="AF3" s="167"/>
+      <c r="AG3" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="165"/>
-      <c r="AI3" s="165" t="s">
+      <c r="AH3" s="167"/>
+      <c r="AI3" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AJ3" s="165"/>
+      <c r="AJ3" s="167"/>
       <c r="AK3" s="34"/>
       <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
@@ -20729,104 +20748,104 @@
       <c r="BH3" s="34"/>
       <c r="BI3" s="34"/>
       <c r="BJ3" s="34"/>
-      <c r="BK3" s="167" t="s">
+      <c r="BK3" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BL3" s="168"/>
-      <c r="BM3" s="167" t="s">
+      <c r="BL3" s="166"/>
+      <c r="BM3" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BN3" s="168"/>
-      <c r="BO3" s="167" t="s">
+      <c r="BN3" s="166"/>
+      <c r="BO3" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" s="168"/>
-      <c r="BQ3" s="167" t="s">
+      <c r="BP3" s="166"/>
+      <c r="BQ3" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BR3" s="168"/>
-      <c r="BS3" s="167" t="s">
+      <c r="BR3" s="166"/>
+      <c r="BS3" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="168"/>
-      <c r="BU3" s="167" t="s">
+      <c r="BT3" s="166"/>
+      <c r="BU3" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BV3" s="168"/>
-      <c r="BW3" s="167" t="s">
+      <c r="BV3" s="166"/>
+      <c r="BW3" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BX3" s="168"/>
-      <c r="BY3" s="167" t="s">
+      <c r="BX3" s="166"/>
+      <c r="BY3" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BZ3" s="168"/>
-      <c r="CA3" s="167" t="s">
+      <c r="BZ3" s="166"/>
+      <c r="CA3" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CB3" s="168"/>
+      <c r="CB3" s="166"/>
     </row>
     <row r="4" spans="2:80">
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="34"/>
-      <c r="G4" s="165" t="s">
+      <c r="G4" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165" t="s">
+      <c r="H4" s="167"/>
+      <c r="I4" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="165"/>
-      <c r="K4" s="165" t="s">
+      <c r="J4" s="167"/>
+      <c r="K4" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="165"/>
-      <c r="M4" s="165" t="s">
+      <c r="L4" s="167"/>
+      <c r="M4" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="165"/>
-      <c r="O4" s="165" t="s">
+      <c r="N4" s="167"/>
+      <c r="O4" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="P4" s="165"/>
-      <c r="Q4" s="165" t="s">
+      <c r="P4" s="167"/>
+      <c r="Q4" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="R4" s="165"/>
-      <c r="S4" s="165" t="s">
+      <c r="R4" s="167"/>
+      <c r="S4" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="165"/>
-      <c r="U4" s="165" t="s">
+      <c r="T4" s="167"/>
+      <c r="U4" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="V4" s="165"/>
-      <c r="W4" s="165" t="s">
+      <c r="V4" s="167"/>
+      <c r="W4" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="165"/>
+      <c r="X4" s="167"/>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="165" t="s">
+      <c r="AC4" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AD4" s="165"/>
-      <c r="AE4" s="165" t="s">
+      <c r="AD4" s="167"/>
+      <c r="AE4" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AF4" s="165"/>
-      <c r="AG4" s="165" t="s">
+      <c r="AF4" s="167"/>
+      <c r="AG4" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="165" t="s">
+      <c r="AH4" s="167"/>
+      <c r="AI4" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="165"/>
+      <c r="AJ4" s="167"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="34"/>
@@ -20849,42 +20868,42 @@
       <c r="BH4" s="34"/>
       <c r="BI4" s="34"/>
       <c r="BJ4" s="34"/>
-      <c r="BK4" s="167" t="s">
+      <c r="BK4" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BL4" s="168"/>
-      <c r="BM4" s="167" t="s">
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BN4" s="168"/>
-      <c r="BO4" s="167" t="s">
+      <c r="BN4" s="166"/>
+      <c r="BO4" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BP4" s="168"/>
-      <c r="BQ4" s="167" t="s">
+      <c r="BP4" s="166"/>
+      <c r="BQ4" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BR4" s="168"/>
-      <c r="BS4" s="167" t="s">
+      <c r="BR4" s="166"/>
+      <c r="BS4" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BT4" s="168"/>
-      <c r="BU4" s="167" t="s">
+      <c r="BT4" s="166"/>
+      <c r="BU4" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BV4" s="168"/>
-      <c r="BW4" s="167" t="s">
+      <c r="BV4" s="166"/>
+      <c r="BW4" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BX4" s="168"/>
-      <c r="BY4" s="167" t="s">
+      <c r="BX4" s="166"/>
+      <c r="BY4" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BZ4" s="168"/>
-      <c r="CA4" s="167" t="s">
+      <c r="BZ4" s="166"/>
+      <c r="CA4" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CB4" s="168"/>
+      <c r="CB4" s="166"/>
     </row>
     <row r="5" spans="2:80">
       <c r="BX5" s="27"/>
@@ -20898,62 +20917,62 @@
         <v>239</v>
       </c>
       <c r="F6" s="36"/>
-      <c r="G6" s="166" t="s">
+      <c r="G6" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="166"/>
-      <c r="I6" s="166" t="s">
+      <c r="H6" s="172"/>
+      <c r="I6" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="166"/>
-      <c r="K6" s="166" t="s">
+      <c r="J6" s="172"/>
+      <c r="K6" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="166"/>
-      <c r="M6" s="166" t="s">
+      <c r="L6" s="172"/>
+      <c r="M6" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="166"/>
-      <c r="O6" s="166" t="s">
+      <c r="N6" s="172"/>
+      <c r="O6" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="166"/>
-      <c r="Q6" s="166" t="s">
+      <c r="P6" s="172"/>
+      <c r="Q6" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="R6" s="166"/>
-      <c r="S6" s="166" t="s">
+      <c r="R6" s="172"/>
+      <c r="S6" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="T6" s="166"/>
-      <c r="U6" s="166" t="s">
+      <c r="T6" s="172"/>
+      <c r="U6" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="V6" s="166"/>
-      <c r="W6" s="166" t="s">
+      <c r="V6" s="172"/>
+      <c r="W6" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="X6" s="166"/>
+      <c r="X6" s="172"/>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AC6" s="166" t="s">
+      <c r="AC6" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" s="166"/>
-      <c r="AE6" s="166" t="s">
+      <c r="AD6" s="172"/>
+      <c r="AE6" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="AF6" s="166"/>
-      <c r="AG6" s="166" t="s">
+      <c r="AF6" s="172"/>
+      <c r="AG6" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="AH6" s="166"/>
-      <c r="AI6" s="166" t="s">
+      <c r="AH6" s="172"/>
+      <c r="AI6" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="AJ6" s="166"/>
+      <c r="AJ6" s="172"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -20976,42 +20995,42 @@
       <c r="BH6" s="34"/>
       <c r="BI6" s="34"/>
       <c r="BJ6" s="34"/>
-      <c r="BK6" s="167" t="s">
+      <c r="BK6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BL6" s="168"/>
-      <c r="BM6" s="167" t="s">
+      <c r="BL6" s="166"/>
+      <c r="BM6" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BN6" s="168"/>
-      <c r="BO6" s="167" t="s">
+      <c r="BN6" s="166"/>
+      <c r="BO6" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BP6" s="168"/>
-      <c r="BQ6" s="167" t="s">
+      <c r="BP6" s="166"/>
+      <c r="BQ6" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BR6" s="168"/>
-      <c r="BS6" s="167" t="s">
+      <c r="BR6" s="166"/>
+      <c r="BS6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BT6" s="168"/>
-      <c r="BU6" s="167" t="s">
+      <c r="BT6" s="166"/>
+      <c r="BU6" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BV6" s="168"/>
-      <c r="BW6" s="167" t="s">
+      <c r="BV6" s="166"/>
+      <c r="BW6" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BX6" s="168"/>
-      <c r="BY6" s="167" t="s">
+      <c r="BX6" s="166"/>
+      <c r="BY6" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BZ6" s="168"/>
-      <c r="CA6" s="167" t="s">
+      <c r="BZ6" s="166"/>
+      <c r="CA6" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CB6" s="168"/>
+      <c r="CB6" s="166"/>
     </row>
     <row r="7" spans="2:80">
       <c r="E7">
@@ -21347,58 +21366,58 @@
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="165" t="s">
+      <c r="I12" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="165"/>
-      <c r="K12" s="165" t="s">
+      <c r="J12" s="167"/>
+      <c r="K12" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="165"/>
-      <c r="M12" s="165" t="s">
+      <c r="L12" s="167"/>
+      <c r="M12" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="165"/>
-      <c r="O12" s="165" t="s">
+      <c r="N12" s="167"/>
+      <c r="O12" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="P12" s="165"/>
-      <c r="Q12" s="165" t="s">
+      <c r="P12" s="167"/>
+      <c r="Q12" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="165"/>
-      <c r="S12" s="165" t="s">
+      <c r="R12" s="167"/>
+      <c r="S12" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="T12" s="165"/>
-      <c r="U12" s="165" t="s">
+      <c r="T12" s="167"/>
+      <c r="U12" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="165"/>
-      <c r="W12" s="165" t="s">
+      <c r="V12" s="167"/>
+      <c r="W12" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="165"/>
+      <c r="X12" s="167"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="165" t="s">
+      <c r="AC12" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="165"/>
-      <c r="AE12" s="165" t="s">
+      <c r="AD12" s="167"/>
+      <c r="AE12" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AF12" s="165"/>
-      <c r="AG12" s="165" t="s">
+      <c r="AF12" s="167"/>
+      <c r="AG12" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="AH12" s="165"/>
-      <c r="AI12" s="165" t="s">
+      <c r="AH12" s="167"/>
+      <c r="AI12" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="AJ12" s="165"/>
+      <c r="AJ12" s="167"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="34"/>
       <c r="AM12" s="34"/>
@@ -21421,42 +21440,42 @@
       <c r="BH12" s="34"/>
       <c r="BI12" s="34"/>
       <c r="BJ12" s="34"/>
-      <c r="BK12" s="167" t="s">
+      <c r="BK12" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BL12" s="168"/>
-      <c r="BM12" s="167" t="s">
+      <c r="BL12" s="166"/>
+      <c r="BM12" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BN12" s="168"/>
-      <c r="BO12" s="167" t="s">
+      <c r="BN12" s="166"/>
+      <c r="BO12" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BP12" s="168"/>
-      <c r="BQ12" s="167" t="s">
+      <c r="BP12" s="166"/>
+      <c r="BQ12" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BR12" s="168"/>
-      <c r="BS12" s="167" t="s">
+      <c r="BR12" s="166"/>
+      <c r="BS12" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="BT12" s="168"/>
-      <c r="BU12" s="167" t="s">
+      <c r="BT12" s="166"/>
+      <c r="BU12" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="BV12" s="168"/>
-      <c r="BW12" s="167" t="s">
+      <c r="BV12" s="166"/>
+      <c r="BW12" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="BX12" s="168"/>
-      <c r="BY12" s="167" t="s">
+      <c r="BX12" s="166"/>
+      <c r="BY12" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="BZ12" s="168"/>
-      <c r="CA12" s="167" t="s">
+      <c r="BZ12" s="166"/>
+      <c r="CA12" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="CB12" s="168"/>
+      <c r="CB12" s="166"/>
     </row>
     <row r="13" spans="2:80">
       <c r="BX13" s="27"/>
@@ -21489,71 +21508,71 @@
         <v>120</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="172" t="s">
+      <c r="G16" s="171" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="172"/>
-      <c r="I16" s="172"/>
-      <c r="J16" s="172"/>
-      <c r="K16" s="172"/>
-      <c r="L16" s="172"/>
-      <c r="M16" s="172"/>
-      <c r="N16" s="172"/>
-      <c r="O16" s="172"/>
-      <c r="P16" s="172"/>
-      <c r="Q16" s="172"/>
-      <c r="R16" s="172"/>
-      <c r="S16" s="172"/>
-      <c r="T16" s="172"/>
-      <c r="U16" s="172"/>
-      <c r="V16" s="172"/>
-      <c r="W16" s="172"/>
-      <c r="X16" s="172"/>
-      <c r="Y16" s="172"/>
-      <c r="Z16" s="172"/>
-      <c r="AA16" s="172" t="s">
+      <c r="H16" s="171"/>
+      <c r="I16" s="171"/>
+      <c r="J16" s="171"/>
+      <c r="K16" s="171"/>
+      <c r="L16" s="171"/>
+      <c r="M16" s="171"/>
+      <c r="N16" s="171"/>
+      <c r="O16" s="171"/>
+      <c r="P16" s="171"/>
+      <c r="Q16" s="171"/>
+      <c r="R16" s="171"/>
+      <c r="S16" s="171"/>
+      <c r="T16" s="171"/>
+      <c r="U16" s="171"/>
+      <c r="V16" s="171"/>
+      <c r="W16" s="171"/>
+      <c r="X16" s="171"/>
+      <c r="Y16" s="171"/>
+      <c r="Z16" s="171"/>
+      <c r="AA16" s="171" t="s">
         <v>116</v>
       </c>
-      <c r="AB16" s="172"/>
-      <c r="AC16" s="172"/>
-      <c r="AD16" s="172"/>
-      <c r="AE16" s="172"/>
-      <c r="AF16" s="172"/>
-      <c r="AG16" s="172"/>
-      <c r="AH16" s="172"/>
-      <c r="AI16" s="172"/>
-      <c r="AJ16" s="172"/>
-      <c r="AK16" s="165" t="s">
+      <c r="AB16" s="171"/>
+      <c r="AC16" s="171"/>
+      <c r="AD16" s="171"/>
+      <c r="AE16" s="171"/>
+      <c r="AF16" s="171"/>
+      <c r="AG16" s="171"/>
+      <c r="AH16" s="171"/>
+      <c r="AI16" s="171"/>
+      <c r="AJ16" s="171"/>
+      <c r="AK16" s="167" t="s">
         <v>111</v>
       </c>
-      <c r="AL16" s="165"/>
-      <c r="AM16" s="165" t="s">
+      <c r="AL16" s="167"/>
+      <c r="AM16" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="AN16" s="165"/>
-      <c r="AO16" s="165" t="s">
+      <c r="AN16" s="167"/>
+      <c r="AO16" s="167" t="s">
         <v>117</v>
       </c>
-      <c r="AP16" s="165"/>
-      <c r="AQ16" s="165" t="s">
+      <c r="AP16" s="167"/>
+      <c r="AQ16" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="AR16" s="165"/>
-      <c r="AS16" s="169" t="s">
+      <c r="AR16" s="167"/>
+      <c r="AS16" s="168" t="s">
         <v>119</v>
       </c>
-      <c r="AT16" s="170"/>
-      <c r="AU16" s="170"/>
-      <c r="AV16" s="170"/>
-      <c r="AW16" s="170"/>
-      <c r="AX16" s="170"/>
-      <c r="AY16" s="170"/>
-      <c r="AZ16" s="170"/>
-      <c r="BA16" s="171"/>
-      <c r="BB16" s="165" t="s">
+      <c r="AT16" s="169"/>
+      <c r="AU16" s="169"/>
+      <c r="AV16" s="169"/>
+      <c r="AW16" s="169"/>
+      <c r="AX16" s="169"/>
+      <c r="AY16" s="169"/>
+      <c r="AZ16" s="169"/>
+      <c r="BA16" s="170"/>
+      <c r="BB16" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="BC16" s="165"/>
+      <c r="BC16" s="167"/>
       <c r="BE16" s="38"/>
       <c r="BF16" s="38"/>
       <c r="BG16" s="38"/>
@@ -22102,6 +22121,85 @@
     </row>
   </sheetData>
   <mergeCells count="95">
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="BU3:BV3"/>
+    <mergeCell ref="BW3:BX3"/>
+    <mergeCell ref="BY3:BZ3"/>
+    <mergeCell ref="CA3:CB3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="BO3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BW4:BX4"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
     <mergeCell ref="BB16:BC16"/>
     <mergeCell ref="BW12:BX12"/>
     <mergeCell ref="BY12:BZ12"/>
@@ -22118,85 +22216,6 @@
     <mergeCell ref="BO12:BP12"/>
     <mergeCell ref="BQ12:BR12"/>
     <mergeCell ref="BS12:BT12"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BW4:BX4"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="BU3:BV3"/>
-    <mergeCell ref="BW3:BX3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="CA3:CB3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BM3:BN3"/>
-    <mergeCell ref="BO3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22206,14 +22225,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F50"/>
   <sheetViews>
     <sheetView topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" t="s">
@@ -22243,17 +22262,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:AB16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:AB20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="20" max="20" width="5.125" customWidth="1"/>
-    <col min="21" max="28" width="3.375" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" customWidth="1"/>
+    <col min="21" max="28" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:28">
@@ -22264,7 +22283,7 @@
     <row r="5" spans="1:28" ht="17.25">
       <c r="A5" s="48"/>
     </row>
-    <row r="6" spans="1:28" ht="14.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="49"/>
       <c r="B6" s="50">
         <v>0</v>
@@ -22315,7 +22334,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="14.25">
+    <row r="7" spans="1:28" ht="28.5">
       <c r="A7" s="106" t="s">
         <v>227</v>
       </c>
@@ -22371,7 +22390,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="14.25">
+    <row r="8" spans="1:28" ht="28.5">
       <c r="A8" s="50">
         <v>10</v>
       </c>
@@ -22425,7 +22444,7 @@
       </c>
       <c r="R8" s="176"/>
     </row>
-    <row r="9" spans="1:28" ht="14.25">
+    <row r="9" spans="1:28" ht="28.5">
       <c r="A9" s="50">
         <v>20</v>
       </c>
@@ -22481,7 +22500,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="14.25">
+    <row r="10" spans="1:28" ht="28.5">
       <c r="A10" s="50">
         <v>30</v>
       </c>
@@ -22636,6 +22655,38 @@
         <v>1</v>
       </c>
       <c r="Y16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13">
+      <c r="L17" t="s">
+        <v>469</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13">
+      <c r="L18" t="s">
+        <v>468</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="12:13">
+      <c r="L19" t="s">
+        <v>466</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="12:13">
+      <c r="L20" t="s">
+        <v>467</v>
+      </c>
+      <c r="M20">
         <v>1</v>
       </c>
     </row>
@@ -22651,17 +22702,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.25" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:25" ht="14.25" thickBot="1"/>
-    <row r="3" spans="2:25" ht="14.25">
+    <row r="2" spans="2:25" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:25">
       <c r="B3" s="114" t="s">
         <v>238</v>
       </c>
@@ -22735,7 +22786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:25" ht="15" thickBot="1">
+    <row r="4" spans="2:25" ht="15.75" thickBot="1">
       <c r="B4" s="117" t="s">
         <v>239</v>
       </c>
@@ -22809,7 +22860,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="15" thickBot="1">
+    <row r="5" spans="2:25" ht="15.75" thickBot="1">
       <c r="B5" s="119" t="s">
         <v>241</v>
       </c>
@@ -22883,7 +22934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="15" thickBot="1">
+    <row r="6" spans="2:25" ht="15.75" thickBot="1">
       <c r="B6" s="121" t="s">
         <v>242</v>
       </c>
@@ -22957,7 +23008,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="15" thickBot="1">
+    <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="B7" s="119" t="s">
         <v>243</v>
       </c>
@@ -23031,7 +23082,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:25" ht="15" thickBot="1">
+    <row r="8" spans="2:25" ht="15.75" thickBot="1">
       <c r="B8" s="121" t="s">
         <v>244</v>
       </c>
@@ -23105,7 +23156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:25" ht="15" thickBot="1">
+    <row r="9" spans="2:25" ht="15.75" thickBot="1">
       <c r="B9" s="119" t="s">
         <v>245</v>
       </c>
@@ -23179,7 +23230,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:25" ht="15" thickBot="1">
+    <row r="10" spans="2:25" ht="15.75" thickBot="1">
       <c r="B10" s="121" t="s">
         <v>246</v>
       </c>
@@ -23253,7 +23304,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:25" ht="15" thickBot="1">
+    <row r="11" spans="2:25" ht="15.75" thickBot="1">
       <c r="B11" s="119" t="s">
         <v>247</v>
       </c>
@@ -23327,7 +23378,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:25" ht="15" thickBot="1">
+    <row r="12" spans="2:25" ht="15.75" thickBot="1">
       <c r="B12" s="121" t="s">
         <v>248</v>
       </c>
@@ -23401,7 +23452,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="15" thickBot="1">
+    <row r="13" spans="2:25" ht="15.75" thickBot="1">
       <c r="B13" s="119" t="s">
         <v>249</v>
       </c>
@@ -23475,7 +23526,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="15" thickBot="1">
+    <row r="14" spans="2:25" ht="15.75" thickBot="1">
       <c r="B14" s="121" t="s">
         <v>250</v>
       </c>
@@ -23549,7 +23600,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:25" ht="15" thickBot="1">
+    <row r="15" spans="2:25" ht="15.75" thickBot="1">
       <c r="B15" s="119" t="s">
         <v>251</v>
       </c>
@@ -23623,7 +23674,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="15" thickBot="1">
+    <row r="16" spans="2:25" ht="15.75" thickBot="1">
       <c r="B16" s="121" t="s">
         <v>253</v>
       </c>
@@ -23697,7 +23748,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="15" thickBot="1">
+    <row r="17" spans="2:25" ht="15.75" thickBot="1">
       <c r="B17" s="119" t="s">
         <v>255</v>
       </c>
@@ -23771,7 +23822,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="15" thickBot="1">
+    <row r="18" spans="2:25" ht="15.75" thickBot="1">
       <c r="B18" s="121" t="s">
         <v>257</v>
       </c>
@@ -23845,7 +23896,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="15" thickBot="1">
+    <row r="19" spans="2:25" ht="15.75" thickBot="1">
       <c r="B19" s="119" t="s">
         <v>259</v>
       </c>
@@ -23919,7 +23970,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="2:25" ht="15" thickBot="1">
+    <row r="20" spans="2:25" ht="15.75" thickBot="1">
       <c r="B20" s="123" t="s">
         <v>261</v>
       </c>
@@ -23993,7 +24044,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="14.25">
+    <row r="21" spans="2:25">
       <c r="B21" s="154" t="s">
         <v>407</v>
       </c>

</xml_diff>